<commit_message>
OAB : Laporan Riwayat Pengobatan Dalam 1 bulan terakhir
</commit_message>
<xml_diff>
--- a/Laravel-InaLUTS/resources/templates/Report_OAB.xlsx
+++ b/Laravel-InaLUTS/resources/templates/Report_OAB.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="73">
   <si>
     <t>No</t>
   </si>
@@ -209,6 +209,30 @@
   </si>
   <si>
     <t>MSA (multiple system atrophy)</t>
+  </si>
+  <si>
+    <t>Antihipertensi</t>
+  </si>
+  <si>
+    <t>Obat diabetik</t>
+  </si>
+  <si>
+    <t>Obat-obatan psikiatri</t>
+  </si>
+  <si>
+    <t>Obat-obatan COPD</t>
+  </si>
+  <si>
+    <t>Obat-obatan asma</t>
+  </si>
+  <si>
+    <t>Obat-obatan alergi</t>
+  </si>
+  <si>
+    <t>Obat-obatan saraf</t>
+  </si>
+  <si>
+    <t>Riwayat Pengobatan Dalam 1 bulan terakhir</t>
   </si>
 </sst>
 </file>
@@ -255,7 +279,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -319,6 +343,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -335,7 +371,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -355,6 +391,24 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -370,23 +424,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -689,7 +731,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BJ6"/>
+  <dimension ref="A1:BQ6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
@@ -718,92 +760,92 @@
     <col min="42" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:62" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="9"/>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
+    <row r="1" spans="1:69" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="15"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
     </row>
-    <row r="2" spans="1:62" x14ac:dyDescent="0.25">
-      <c r="A2" s="10"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10"/>
+    <row r="2" spans="1:69" x14ac:dyDescent="0.25">
+      <c r="A2" s="16"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="16"/>
     </row>
-    <row r="3" spans="1:62" x14ac:dyDescent="0.25">
-      <c r="A3" s="11"/>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
-      <c r="J3" s="11"/>
-      <c r="K3" s="11"/>
+    <row r="3" spans="1:69" x14ac:dyDescent="0.25">
+      <c r="A3" s="17"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="17"/>
+      <c r="K3" s="17"/>
     </row>
-    <row r="4" spans="1:62" s="4" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+    <row r="4" spans="1:69" s="4" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:69" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="7"/>
-      <c r="L5" s="7"/>
-      <c r="M5" s="7"/>
-      <c r="N5" s="7"/>
-      <c r="O5" s="7"/>
-      <c r="P5" s="7"/>
-      <c r="Q5" s="7"/>
-      <c r="R5" s="7"/>
-      <c r="S5" s="7"/>
-      <c r="T5" s="7"/>
-      <c r="U5" s="7"/>
-      <c r="V5" s="7"/>
-      <c r="W5" s="7"/>
-      <c r="X5" s="7"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="13"/>
+      <c r="L5" s="13"/>
+      <c r="M5" s="13"/>
+      <c r="N5" s="13"/>
+      <c r="O5" s="13"/>
+      <c r="P5" s="13"/>
+      <c r="Q5" s="13"/>
+      <c r="R5" s="13"/>
+      <c r="S5" s="13"/>
+      <c r="T5" s="13"/>
+      <c r="U5" s="13"/>
+      <c r="V5" s="13"/>
+      <c r="W5" s="13"/>
+      <c r="X5" s="13"/>
       <c r="Y5" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="Z5" s="13" t="s">
+      <c r="Z5" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="AA5" s="13"/>
-      <c r="AB5" s="13"/>
-      <c r="AC5" s="13"/>
-      <c r="AD5" s="13"/>
-      <c r="AE5" s="13"/>
-      <c r="AF5" s="13"/>
-      <c r="AG5" s="13"/>
-      <c r="AH5" s="13"/>
-      <c r="AI5" s="13"/>
-      <c r="AJ5" s="13"/>
-      <c r="AK5" s="13"/>
+      <c r="AA5" s="11"/>
+      <c r="AB5" s="11"/>
+      <c r="AC5" s="11"/>
+      <c r="AD5" s="11"/>
+      <c r="AE5" s="11"/>
+      <c r="AF5" s="11"/>
+      <c r="AG5" s="11"/>
+      <c r="AH5" s="11"/>
+      <c r="AI5" s="11"/>
+      <c r="AJ5" s="11"/>
+      <c r="AK5" s="11"/>
       <c r="AL5" s="12" t="s">
         <v>40</v>
       </c>
@@ -831,9 +873,18 @@
       <c r="BH5" s="12"/>
       <c r="BI5" s="12"/>
       <c r="BJ5" s="12"/>
+      <c r="BK5" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="BL5" s="18"/>
+      <c r="BM5" s="18"/>
+      <c r="BN5" s="18"/>
+      <c r="BO5" s="18"/>
+      <c r="BP5" s="18"/>
+      <c r="BQ5" s="18"/>
     </row>
-    <row r="6" spans="1:62" s="2" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A6" s="8"/>
+    <row r="6" spans="1:69" s="2" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A6" s="14"/>
       <c r="B6" s="3" t="s">
         <v>2</v>
       </c>
@@ -906,120 +957,142 @@
       <c r="Y6" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="Z6" s="15" t="s">
+      <c r="Z6" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="AA6" s="15" t="s">
+      <c r="AA6" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="AB6" s="15" t="s">
+      <c r="AB6" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="AC6" s="15" t="s">
+      <c r="AC6" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="AD6" s="15" t="s">
+      <c r="AD6" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="AE6" s="15" t="s">
+      <c r="AE6" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="AF6" s="15" t="s">
+      <c r="AF6" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="AG6" s="15" t="s">
+      <c r="AG6" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="AH6" s="15" t="s">
+      <c r="AH6" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="AI6" s="15" t="s">
+      <c r="AI6" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="AJ6" s="15" t="s">
+      <c r="AJ6" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="AK6" s="15" t="s">
+      <c r="AK6" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="AL6" s="14" t="s">
+      <c r="AL6" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="AM6" s="14" t="s">
+      <c r="AM6" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="AN6" s="14" t="s">
+      <c r="AN6" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="AO6" s="17" t="s">
+      <c r="AO6" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="AP6" s="14" t="s">
+      <c r="AP6" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="AQ6" s="14" t="s">
+      <c r="AQ6" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="AR6" s="14" t="s">
+      <c r="AR6" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="AS6" s="14" t="s">
+      <c r="AS6" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="AT6" s="14" t="s">
+      <c r="AT6" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="AU6" s="14" t="s">
+      <c r="AU6" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="AV6" s="14" t="s">
+      <c r="AV6" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="AW6" s="14" t="s">
+      <c r="AW6" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="AX6" s="14" t="s">
+      <c r="AX6" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="AY6" s="14" t="s">
+      <c r="AY6" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="AZ6" s="16" t="s">
+      <c r="AZ6" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="BA6" s="16" t="s">
+      <c r="BA6" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="BB6" s="16" t="s">
+      <c r="BB6" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="BC6" s="16" t="s">
+      <c r="BC6" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="BD6" s="16" t="s">
+      <c r="BD6" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="BE6" s="16" t="s">
+      <c r="BE6" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="BF6" s="16" t="s">
+      <c r="BF6" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="BG6" s="16" t="s">
+      <c r="BG6" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="BH6" s="16" t="s">
+      <c r="BH6" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="BI6" s="16" t="s">
+      <c r="BI6" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="BJ6" s="16" t="s">
+      <c r="BJ6" s="9" t="s">
         <v>64</v>
+      </c>
+      <c r="BK6" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="BL6" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="BM6" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="BN6" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="BO6" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="BP6" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="BQ6" s="19" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="8">
+    <mergeCell ref="BK5:BQ5"/>
     <mergeCell ref="Z5:AK5"/>
     <mergeCell ref="AL5:BJ5"/>
     <mergeCell ref="B5:X5"/>

</xml_diff>

<commit_message>
OAB : Laporan Riwayat Pengobatan LUTS sebelumnya
</commit_message>
<xml_diff>
--- a/Laravel-InaLUTS/resources/templates/Report_OAB.xlsx
+++ b/Laravel-InaLUTS/resources/templates/Report_OAB.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="94">
   <si>
     <t>No</t>
   </si>
@@ -233,6 +233,69 @@
   </si>
   <si>
     <t>Riwayat Pengobatan Dalam 1 bulan terakhir</t>
+  </si>
+  <si>
+    <t>Riwayat Pengobatan LUTS sebelumnya</t>
+  </si>
+  <si>
+    <t>Tamsulosin</t>
+  </si>
+  <si>
+    <t>Penghambat alfa</t>
+  </si>
+  <si>
+    <t>Alfuzosin</t>
+  </si>
+  <si>
+    <t>Doxazosin</t>
+  </si>
+  <si>
+    <t>Terazosin</t>
+  </si>
+  <si>
+    <t>Silodosin</t>
+  </si>
+  <si>
+    <t>5 — ARI</t>
+  </si>
+  <si>
+    <t>Finasteride</t>
+  </si>
+  <si>
+    <t>Dutasteride</t>
+  </si>
+  <si>
+    <t>PDE-5 inhibitor</t>
+  </si>
+  <si>
+    <t>Lamanya</t>
+  </si>
+  <si>
+    <t>Tadalafil</t>
+  </si>
+  <si>
+    <t>Antimuskarinik</t>
+  </si>
+  <si>
+    <t>Solifenacin</t>
+  </si>
+  <si>
+    <t>Imidafenacin</t>
+  </si>
+  <si>
+    <t>Tolterodine</t>
+  </si>
+  <si>
+    <t>Propiverine</t>
+  </si>
+  <si>
+    <t>Flavoxate</t>
+  </si>
+  <si>
+    <t>Beta 3 agonis</t>
+  </si>
+  <si>
+    <t>Mirabegron</t>
   </si>
 </sst>
 </file>
@@ -279,7 +342,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -355,6 +418,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -371,7 +452,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -412,6 +493,24 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -424,11 +523,17 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -731,10 +836,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BQ6"/>
+  <dimension ref="A1:CT7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" topLeftCell="BT1" workbookViewId="0">
+      <selection activeCell="CT7" sqref="CT7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -760,346 +865,580 @@
     <col min="42" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:69" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="15"/>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
+    <row r="1" spans="1:98" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="21"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
     </row>
-    <row r="2" spans="1:69" x14ac:dyDescent="0.25">
-      <c r="A2" s="16"/>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
-      <c r="K2" s="16"/>
+    <row r="2" spans="1:98" x14ac:dyDescent="0.25">
+      <c r="A2" s="22"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="22"/>
+      <c r="K2" s="22"/>
     </row>
-    <row r="3" spans="1:69" x14ac:dyDescent="0.25">
-      <c r="A3" s="17"/>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
-      <c r="J3" s="17"/>
-      <c r="K3" s="17"/>
+    <row r="3" spans="1:98" x14ac:dyDescent="0.25">
+      <c r="A3" s="23"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="23"/>
+      <c r="K3" s="23"/>
     </row>
-    <row r="4" spans="1:69" s="4" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:69" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
+    <row r="4" spans="1:98" s="4" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:98" s="2" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13"/>
-      <c r="K5" s="13"/>
-      <c r="L5" s="13"/>
-      <c r="M5" s="13"/>
-      <c r="N5" s="13"/>
-      <c r="O5" s="13"/>
-      <c r="P5" s="13"/>
-      <c r="Q5" s="13"/>
-      <c r="R5" s="13"/>
-      <c r="S5" s="13"/>
-      <c r="T5" s="13"/>
-      <c r="U5" s="13"/>
-      <c r="V5" s="13"/>
-      <c r="W5" s="13"/>
-      <c r="X5" s="13"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="19"/>
+      <c r="J5" s="19"/>
+      <c r="K5" s="19"/>
+      <c r="L5" s="19"/>
+      <c r="M5" s="19"/>
+      <c r="N5" s="19"/>
+      <c r="O5" s="19"/>
+      <c r="P5" s="19"/>
+      <c r="Q5" s="19"/>
+      <c r="R5" s="19"/>
+      <c r="S5" s="19"/>
+      <c r="T5" s="19"/>
+      <c r="U5" s="19"/>
+      <c r="V5" s="19"/>
+      <c r="W5" s="19"/>
+      <c r="X5" s="19"/>
       <c r="Y5" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="Z5" s="11" t="s">
+      <c r="Z5" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="AA5" s="11"/>
-      <c r="AB5" s="11"/>
-      <c r="AC5" s="11"/>
-      <c r="AD5" s="11"/>
-      <c r="AE5" s="11"/>
-      <c r="AF5" s="11"/>
-      <c r="AG5" s="11"/>
-      <c r="AH5" s="11"/>
-      <c r="AI5" s="11"/>
-      <c r="AJ5" s="11"/>
-      <c r="AK5" s="11"/>
-      <c r="AL5" s="12" t="s">
+      <c r="AA5" s="17"/>
+      <c r="AB5" s="17"/>
+      <c r="AC5" s="17"/>
+      <c r="AD5" s="17"/>
+      <c r="AE5" s="17"/>
+      <c r="AF5" s="17"/>
+      <c r="AG5" s="17"/>
+      <c r="AH5" s="17"/>
+      <c r="AI5" s="17"/>
+      <c r="AJ5" s="17"/>
+      <c r="AK5" s="17"/>
+      <c r="AL5" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="AM5" s="12"/>
-      <c r="AN5" s="12"/>
-      <c r="AO5" s="12"/>
-      <c r="AP5" s="12"/>
-      <c r="AQ5" s="12"/>
-      <c r="AR5" s="12"/>
-      <c r="AS5" s="12"/>
-      <c r="AT5" s="12"/>
-      <c r="AU5" s="12"/>
-      <c r="AV5" s="12"/>
-      <c r="AW5" s="12"/>
-      <c r="AX5" s="12"/>
-      <c r="AY5" s="12"/>
-      <c r="AZ5" s="12"/>
-      <c r="BA5" s="12"/>
-      <c r="BB5" s="12"/>
-      <c r="BC5" s="12"/>
-      <c r="BD5" s="12"/>
-      <c r="BE5" s="12"/>
-      <c r="BF5" s="12"/>
-      <c r="BG5" s="12"/>
-      <c r="BH5" s="12"/>
-      <c r="BI5" s="12"/>
-      <c r="BJ5" s="12"/>
-      <c r="BK5" s="18" t="s">
+      <c r="AM5" s="18"/>
+      <c r="AN5" s="18"/>
+      <c r="AO5" s="18"/>
+      <c r="AP5" s="18"/>
+      <c r="AQ5" s="18"/>
+      <c r="AR5" s="18"/>
+      <c r="AS5" s="18"/>
+      <c r="AT5" s="18"/>
+      <c r="AU5" s="18"/>
+      <c r="AV5" s="18"/>
+      <c r="AW5" s="18"/>
+      <c r="AX5" s="18"/>
+      <c r="AY5" s="18"/>
+      <c r="AZ5" s="18"/>
+      <c r="BA5" s="18"/>
+      <c r="BB5" s="18"/>
+      <c r="BC5" s="18"/>
+      <c r="BD5" s="18"/>
+      <c r="BE5" s="18"/>
+      <c r="BF5" s="18"/>
+      <c r="BG5" s="18"/>
+      <c r="BH5" s="18"/>
+      <c r="BI5" s="18"/>
+      <c r="BJ5" s="18"/>
+      <c r="BK5" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="BL5" s="18"/>
-      <c r="BM5" s="18"/>
-      <c r="BN5" s="18"/>
-      <c r="BO5" s="18"/>
-      <c r="BP5" s="18"/>
-      <c r="BQ5" s="18"/>
+      <c r="BL5" s="16"/>
+      <c r="BM5" s="16"/>
+      <c r="BN5" s="16"/>
+      <c r="BO5" s="16"/>
+      <c r="BP5" s="16"/>
+      <c r="BQ5" s="16"/>
+      <c r="BR5" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="BS5" s="27"/>
+      <c r="BT5" s="27"/>
+      <c r="BU5" s="27"/>
+      <c r="BV5" s="27"/>
+      <c r="BW5" s="27"/>
+      <c r="BX5" s="27"/>
+      <c r="BY5" s="27"/>
+      <c r="BZ5" s="27"/>
+      <c r="CA5" s="27"/>
+      <c r="CB5" s="27"/>
+      <c r="CC5" s="27"/>
+      <c r="CD5" s="27"/>
+      <c r="CE5" s="27"/>
+      <c r="CF5" s="27"/>
+      <c r="CG5" s="27"/>
+      <c r="CH5" s="27"/>
+      <c r="CI5" s="27"/>
+      <c r="CJ5" s="27"/>
+      <c r="CK5" s="27"/>
+      <c r="CL5" s="27"/>
+      <c r="CM5" s="27"/>
+      <c r="CN5" s="27"/>
+      <c r="CO5" s="27"/>
+      <c r="CP5" s="27"/>
+      <c r="CQ5" s="27"/>
+      <c r="CR5" s="27"/>
+      <c r="CS5" s="27"/>
+      <c r="CT5" s="27"/>
     </row>
-    <row r="6" spans="1:69" s="2" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A6" s="14"/>
-      <c r="B6" s="3" t="s">
+    <row r="6" spans="1:98" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="20"/>
+      <c r="B6" s="13"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="13"/>
+      <c r="L6" s="13"/>
+      <c r="M6" s="13"/>
+      <c r="N6" s="13"/>
+      <c r="O6" s="13"/>
+      <c r="P6" s="13"/>
+      <c r="Q6" s="13"/>
+      <c r="R6" s="13"/>
+      <c r="S6" s="13"/>
+      <c r="T6" s="13"/>
+      <c r="U6" s="13"/>
+      <c r="V6" s="13"/>
+      <c r="W6" s="13"/>
+      <c r="X6" s="13"/>
+      <c r="Y6" s="6"/>
+      <c r="Z6" s="11"/>
+      <c r="AA6" s="11"/>
+      <c r="AB6" s="11"/>
+      <c r="AC6" s="11"/>
+      <c r="AD6" s="11"/>
+      <c r="AE6" s="11"/>
+      <c r="AF6" s="11"/>
+      <c r="AG6" s="11"/>
+      <c r="AH6" s="11"/>
+      <c r="AI6" s="11"/>
+      <c r="AJ6" s="11"/>
+      <c r="AK6" s="11"/>
+      <c r="AL6" s="12"/>
+      <c r="AM6" s="12"/>
+      <c r="AN6" s="12"/>
+      <c r="AO6" s="12"/>
+      <c r="AP6" s="12"/>
+      <c r="AQ6" s="12"/>
+      <c r="AR6" s="12"/>
+      <c r="AS6" s="12"/>
+      <c r="AT6" s="12"/>
+      <c r="AU6" s="12"/>
+      <c r="AV6" s="12"/>
+      <c r="AW6" s="12"/>
+      <c r="AX6" s="12"/>
+      <c r="AY6" s="12"/>
+      <c r="AZ6" s="12"/>
+      <c r="BA6" s="12"/>
+      <c r="BB6" s="12"/>
+      <c r="BC6" s="12"/>
+      <c r="BD6" s="12"/>
+      <c r="BE6" s="12"/>
+      <c r="BF6" s="12"/>
+      <c r="BG6" s="12"/>
+      <c r="BH6" s="12"/>
+      <c r="BI6" s="12"/>
+      <c r="BJ6" s="12"/>
+      <c r="BK6" s="14"/>
+      <c r="BL6" s="14"/>
+      <c r="BM6" s="14"/>
+      <c r="BN6" s="14"/>
+      <c r="BO6" s="14"/>
+      <c r="BP6" s="14"/>
+      <c r="BQ6" s="14"/>
+      <c r="BR6" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="BS6" s="26"/>
+      <c r="BT6" s="26"/>
+      <c r="BU6" s="26"/>
+      <c r="BV6" s="26"/>
+      <c r="BW6" s="26"/>
+      <c r="BX6" s="26"/>
+      <c r="BY6" s="26"/>
+      <c r="BZ6" s="26"/>
+      <c r="CA6" s="26"/>
+      <c r="CB6" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="CC6" s="26"/>
+      <c r="CD6" s="26"/>
+      <c r="CE6" s="26"/>
+      <c r="CF6" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="CG6" s="26"/>
+      <c r="CH6" s="26"/>
+      <c r="CI6" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="CJ6" s="26"/>
+      <c r="CK6" s="26"/>
+      <c r="CL6" s="26"/>
+      <c r="CM6" s="26"/>
+      <c r="CN6" s="26"/>
+      <c r="CO6" s="26"/>
+      <c r="CP6" s="26"/>
+      <c r="CQ6" s="26"/>
+      <c r="CR6" s="26"/>
+      <c r="CS6" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="CT6" s="26"/>
+    </row>
+    <row r="7" spans="1:98" s="2" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A7" s="20"/>
+      <c r="B7" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C7" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D7" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="G7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="H7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="I6" s="3" t="s">
+      <c r="I7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="J6" s="3" t="s">
+      <c r="J7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="K6" s="3" t="s">
+      <c r="K7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="L6" s="3" t="s">
+      <c r="L7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="M6" s="3" t="s">
+      <c r="M7" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="N6" s="3" t="s">
+      <c r="N7" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="O6" s="3" t="s">
+      <c r="O7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="P6" s="3" t="s">
+      <c r="P7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="Q6" s="3" t="s">
+      <c r="Q7" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="R6" s="3" t="s">
+      <c r="R7" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="S6" s="3" t="s">
+      <c r="S7" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="T6" s="3" t="s">
+      <c r="T7" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="U6" s="3" t="s">
+      <c r="U7" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="V6" s="3" t="s">
+      <c r="V7" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="W6" s="3" t="s">
+      <c r="W7" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="X6" s="3" t="s">
+      <c r="X7" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="Y6" s="5" t="s">
+      <c r="Y7" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="Z6" s="8" t="s">
+      <c r="Z7" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="AA6" s="8" t="s">
+      <c r="AA7" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="AB6" s="8" t="s">
+      <c r="AB7" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="AC6" s="8" t="s">
+      <c r="AC7" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="AD6" s="8" t="s">
+      <c r="AD7" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="AE6" s="8" t="s">
+      <c r="AE7" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="AF6" s="8" t="s">
+      <c r="AF7" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="AG6" s="8" t="s">
+      <c r="AG7" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="AH6" s="8" t="s">
+      <c r="AH7" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="AI6" s="8" t="s">
+      <c r="AI7" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="AJ6" s="8" t="s">
+      <c r="AJ7" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="AK6" s="8" t="s">
+      <c r="AK7" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="AL6" s="7" t="s">
+      <c r="AL7" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="AM6" s="7" t="s">
+      <c r="AM7" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="AN6" s="7" t="s">
+      <c r="AN7" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="AO6" s="10" t="s">
+      <c r="AO7" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="AP6" s="7" t="s">
+      <c r="AP7" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="AQ6" s="7" t="s">
+      <c r="AQ7" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="AR6" s="7" t="s">
+      <c r="AR7" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="AS6" s="7" t="s">
+      <c r="AS7" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="AT6" s="7" t="s">
+      <c r="AT7" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="AU6" s="7" t="s">
+      <c r="AU7" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="AV6" s="7" t="s">
+      <c r="AV7" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="AW6" s="7" t="s">
+      <c r="AW7" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="AX6" s="7" t="s">
+      <c r="AX7" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="AY6" s="7" t="s">
+      <c r="AY7" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="AZ6" s="9" t="s">
+      <c r="AZ7" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="BA6" s="9" t="s">
+      <c r="BA7" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="BB6" s="9" t="s">
+      <c r="BB7" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="BC6" s="9" t="s">
+      <c r="BC7" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="BD6" s="9" t="s">
+      <c r="BD7" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="BE6" s="9" t="s">
+      <c r="BE7" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="BF6" s="9" t="s">
+      <c r="BF7" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="BG6" s="9" t="s">
+      <c r="BG7" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="BH6" s="9" t="s">
+      <c r="BH7" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="BI6" s="9" t="s">
+      <c r="BI7" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="BJ6" s="9" t="s">
+      <c r="BJ7" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="BK6" s="19" t="s">
+      <c r="BK7" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="BL6" s="19" t="s">
+      <c r="BL7" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="BM6" s="19" t="s">
+      <c r="BM7" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="BN6" s="19" t="s">
+      <c r="BN7" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="BO6" s="19" t="s">
+      <c r="BO7" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="BP6" s="19" t="s">
+      <c r="BP7" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="BQ6" s="19" t="s">
+      <c r="BQ7" s="15" t="s">
         <v>71</v>
+      </c>
+      <c r="BR7" s="24" t="s">
+        <v>74</v>
+      </c>
+      <c r="BS7" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="BT7" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="BU7" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="BV7" s="25" t="s">
+        <v>77</v>
+      </c>
+      <c r="BW7" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="BX7" s="25" t="s">
+        <v>78</v>
+      </c>
+      <c r="BY7" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="BZ7" s="25" t="s">
+        <v>79</v>
+      </c>
+      <c r="CA7" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="CB7" s="25" t="s">
+        <v>81</v>
+      </c>
+      <c r="CC7" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="CD7" s="25" t="s">
+        <v>82</v>
+      </c>
+      <c r="CE7" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="CF7" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="CG7" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="CH7" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="CI7" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="CJ7" s="25" t="s">
+        <v>84</v>
+      </c>
+      <c r="CK7" s="25" t="s">
+        <v>88</v>
+      </c>
+      <c r="CL7" s="25" t="s">
+        <v>84</v>
+      </c>
+      <c r="CM7" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="CN7" s="25" t="s">
+        <v>84</v>
+      </c>
+      <c r="CO7" s="25" t="s">
+        <v>90</v>
+      </c>
+      <c r="CP7" s="25" t="s">
+        <v>84</v>
+      </c>
+      <c r="CQ7" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="CR7" s="25" t="s">
+        <v>84</v>
+      </c>
+      <c r="CS7" s="25" t="s">
+        <v>93</v>
+      </c>
+      <c r="CT7" s="25" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="14">
+    <mergeCell ref="CB6:CE6"/>
+    <mergeCell ref="CF6:CH6"/>
+    <mergeCell ref="CI6:CR6"/>
+    <mergeCell ref="CS6:CT6"/>
+    <mergeCell ref="BR5:CT5"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="BR6:CA6"/>
     <mergeCell ref="BK5:BQ5"/>
     <mergeCell ref="Z5:AK5"/>
     <mergeCell ref="AL5:BJ5"/>
     <mergeCell ref="B5:X5"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A5:A7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
OAB : Laporan Riwayat operasi / endoskopi urologi
</commit_message>
<xml_diff>
--- a/Laravel-InaLUTS/resources/templates/Report_OAB.xlsx
+++ b/Laravel-InaLUTS/resources/templates/Report_OAB.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="104">
   <si>
     <t>No</t>
   </si>
@@ -296,6 +296,36 @@
   </si>
   <si>
     <t>Mirabegron</t>
+  </si>
+  <si>
+    <t>Riwayat operasi / endoskopi urologi</t>
+  </si>
+  <si>
+    <t>Tanggal</t>
+  </si>
+  <si>
+    <t>TUR Prostat</t>
+  </si>
+  <si>
+    <t>Radikal prostat</t>
+  </si>
+  <si>
+    <t>Rekonstruksi uretra</t>
+  </si>
+  <si>
+    <t>TUR Buli</t>
+  </si>
+  <si>
+    <t>Operasi POP</t>
+  </si>
+  <si>
+    <t>Injeksi Botox</t>
+  </si>
+  <si>
+    <t>Sistoskopi</t>
+  </si>
+  <si>
+    <t>Operasi anti inkontinensia urine</t>
   </si>
 </sst>
 </file>
@@ -452,7 +482,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -499,6 +529,27 @@
     <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -514,25 +565,10 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -836,10 +872,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CT7"/>
+  <dimension ref="A1:DI7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BT1" workbookViewId="0">
-      <selection activeCell="CT7" sqref="CT7"/>
+    <sheetView tabSelected="1" topLeftCell="CQ1" workbookViewId="0">
+      <selection activeCell="CU8" sqref="CU8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -865,162 +901,179 @@
     <col min="42" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:98" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="21"/>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
+    <row r="1" spans="1:113" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="20"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
     </row>
-    <row r="2" spans="1:98" x14ac:dyDescent="0.25">
-      <c r="A2" s="22"/>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
-      <c r="I2" s="22"/>
-      <c r="J2" s="22"/>
-      <c r="K2" s="22"/>
+    <row r="2" spans="1:113" x14ac:dyDescent="0.25">
+      <c r="A2" s="21"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="21"/>
+      <c r="K2" s="21"/>
     </row>
-    <row r="3" spans="1:98" x14ac:dyDescent="0.25">
-      <c r="A3" s="23"/>
-      <c r="B3" s="23"/>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="23"/>
-      <c r="I3" s="23"/>
-      <c r="J3" s="23"/>
-      <c r="K3" s="23"/>
+    <row r="3" spans="1:113" x14ac:dyDescent="0.25">
+      <c r="A3" s="22"/>
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="22"/>
+      <c r="I3" s="22"/>
+      <c r="J3" s="22"/>
+      <c r="K3" s="22"/>
     </row>
-    <row r="4" spans="1:98" s="4" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:98" s="2" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="20" t="s">
+    <row r="4" spans="1:113" s="4" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:113" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="19"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="19"/>
-      <c r="H5" s="19"/>
-      <c r="I5" s="19"/>
-      <c r="J5" s="19"/>
-      <c r="K5" s="19"/>
-      <c r="L5" s="19"/>
-      <c r="M5" s="19"/>
-      <c r="N5" s="19"/>
-      <c r="O5" s="19"/>
-      <c r="P5" s="19"/>
-      <c r="Q5" s="19"/>
-      <c r="R5" s="19"/>
-      <c r="S5" s="19"/>
-      <c r="T5" s="19"/>
-      <c r="U5" s="19"/>
-      <c r="V5" s="19"/>
-      <c r="W5" s="19"/>
-      <c r="X5" s="19"/>
+      <c r="C5" s="26"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="26"/>
+      <c r="H5" s="26"/>
+      <c r="I5" s="26"/>
+      <c r="J5" s="26"/>
+      <c r="K5" s="26"/>
+      <c r="L5" s="26"/>
+      <c r="M5" s="26"/>
+      <c r="N5" s="26"/>
+      <c r="O5" s="26"/>
+      <c r="P5" s="26"/>
+      <c r="Q5" s="26"/>
+      <c r="R5" s="26"/>
+      <c r="S5" s="26"/>
+      <c r="T5" s="26"/>
+      <c r="U5" s="26"/>
+      <c r="V5" s="26"/>
+      <c r="W5" s="26"/>
+      <c r="X5" s="26"/>
       <c r="Y5" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="Z5" s="17" t="s">
+      <c r="Z5" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="AA5" s="17"/>
-      <c r="AB5" s="17"/>
-      <c r="AC5" s="17"/>
-      <c r="AD5" s="17"/>
-      <c r="AE5" s="17"/>
-      <c r="AF5" s="17"/>
-      <c r="AG5" s="17"/>
-      <c r="AH5" s="17"/>
-      <c r="AI5" s="17"/>
-      <c r="AJ5" s="17"/>
-      <c r="AK5" s="17"/>
-      <c r="AL5" s="18" t="s">
+      <c r="AA5" s="24"/>
+      <c r="AB5" s="24"/>
+      <c r="AC5" s="24"/>
+      <c r="AD5" s="24"/>
+      <c r="AE5" s="24"/>
+      <c r="AF5" s="24"/>
+      <c r="AG5" s="24"/>
+      <c r="AH5" s="24"/>
+      <c r="AI5" s="24"/>
+      <c r="AJ5" s="24"/>
+      <c r="AK5" s="24"/>
+      <c r="AL5" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="AM5" s="18"/>
-      <c r="AN5" s="18"/>
-      <c r="AO5" s="18"/>
-      <c r="AP5" s="18"/>
-      <c r="AQ5" s="18"/>
-      <c r="AR5" s="18"/>
-      <c r="AS5" s="18"/>
-      <c r="AT5" s="18"/>
-      <c r="AU5" s="18"/>
-      <c r="AV5" s="18"/>
-      <c r="AW5" s="18"/>
-      <c r="AX5" s="18"/>
-      <c r="AY5" s="18"/>
-      <c r="AZ5" s="18"/>
-      <c r="BA5" s="18"/>
-      <c r="BB5" s="18"/>
-      <c r="BC5" s="18"/>
-      <c r="BD5" s="18"/>
-      <c r="BE5" s="18"/>
-      <c r="BF5" s="18"/>
-      <c r="BG5" s="18"/>
-      <c r="BH5" s="18"/>
-      <c r="BI5" s="18"/>
-      <c r="BJ5" s="18"/>
-      <c r="BK5" s="16" t="s">
+      <c r="AM5" s="25"/>
+      <c r="AN5" s="25"/>
+      <c r="AO5" s="25"/>
+      <c r="AP5" s="25"/>
+      <c r="AQ5" s="25"/>
+      <c r="AR5" s="25"/>
+      <c r="AS5" s="25"/>
+      <c r="AT5" s="25"/>
+      <c r="AU5" s="25"/>
+      <c r="AV5" s="25"/>
+      <c r="AW5" s="25"/>
+      <c r="AX5" s="25"/>
+      <c r="AY5" s="25"/>
+      <c r="AZ5" s="25"/>
+      <c r="BA5" s="25"/>
+      <c r="BB5" s="25"/>
+      <c r="BC5" s="25"/>
+      <c r="BD5" s="25"/>
+      <c r="BE5" s="25"/>
+      <c r="BF5" s="25"/>
+      <c r="BG5" s="25"/>
+      <c r="BH5" s="25"/>
+      <c r="BI5" s="25"/>
+      <c r="BJ5" s="25"/>
+      <c r="BK5" s="23" t="s">
         <v>72</v>
       </c>
-      <c r="BL5" s="16"/>
-      <c r="BM5" s="16"/>
-      <c r="BN5" s="16"/>
-      <c r="BO5" s="16"/>
-      <c r="BP5" s="16"/>
-      <c r="BQ5" s="16"/>
-      <c r="BR5" s="27" t="s">
+      <c r="BL5" s="23"/>
+      <c r="BM5" s="23"/>
+      <c r="BN5" s="23"/>
+      <c r="BO5" s="23"/>
+      <c r="BP5" s="23"/>
+      <c r="BQ5" s="23"/>
+      <c r="BR5" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="BS5" s="27"/>
-      <c r="BT5" s="27"/>
-      <c r="BU5" s="27"/>
-      <c r="BV5" s="27"/>
-      <c r="BW5" s="27"/>
-      <c r="BX5" s="27"/>
-      <c r="BY5" s="27"/>
-      <c r="BZ5" s="27"/>
-      <c r="CA5" s="27"/>
-      <c r="CB5" s="27"/>
-      <c r="CC5" s="27"/>
-      <c r="CD5" s="27"/>
-      <c r="CE5" s="27"/>
-      <c r="CF5" s="27"/>
-      <c r="CG5" s="27"/>
-      <c r="CH5" s="27"/>
-      <c r="CI5" s="27"/>
-      <c r="CJ5" s="27"/>
-      <c r="CK5" s="27"/>
-      <c r="CL5" s="27"/>
-      <c r="CM5" s="27"/>
-      <c r="CN5" s="27"/>
-      <c r="CO5" s="27"/>
-      <c r="CP5" s="27"/>
-      <c r="CQ5" s="27"/>
-      <c r="CR5" s="27"/>
-      <c r="CS5" s="27"/>
-      <c r="CT5" s="27"/>
+      <c r="BS5" s="19"/>
+      <c r="BT5" s="19"/>
+      <c r="BU5" s="19"/>
+      <c r="BV5" s="19"/>
+      <c r="BW5" s="19"/>
+      <c r="BX5" s="19"/>
+      <c r="BY5" s="19"/>
+      <c r="BZ5" s="19"/>
+      <c r="CA5" s="19"/>
+      <c r="CB5" s="19"/>
+      <c r="CC5" s="19"/>
+      <c r="CD5" s="19"/>
+      <c r="CE5" s="19"/>
+      <c r="CF5" s="19"/>
+      <c r="CG5" s="19"/>
+      <c r="CH5" s="19"/>
+      <c r="CI5" s="19"/>
+      <c r="CJ5" s="19"/>
+      <c r="CK5" s="19"/>
+      <c r="CL5" s="19"/>
+      <c r="CM5" s="19"/>
+      <c r="CN5" s="19"/>
+      <c r="CO5" s="19"/>
+      <c r="CP5" s="19"/>
+      <c r="CQ5" s="19"/>
+      <c r="CR5" s="19"/>
+      <c r="CS5" s="19"/>
+      <c r="CT5" s="19"/>
+      <c r="CU5" s="29" t="s">
+        <v>94</v>
+      </c>
+      <c r="CV5" s="29"/>
+      <c r="CW5" s="29"/>
+      <c r="CX5" s="29"/>
+      <c r="CY5" s="29"/>
+      <c r="CZ5" s="29"/>
+      <c r="DA5" s="29"/>
+      <c r="DB5" s="29"/>
+      <c r="DC5" s="29"/>
+      <c r="DD5" s="29"/>
+      <c r="DE5" s="29"/>
+      <c r="DF5" s="29"/>
+      <c r="DG5" s="29"/>
+      <c r="DH5" s="29"/>
+      <c r="DI5" s="29"/>
     </row>
-    <row r="6" spans="1:98" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="20"/>
+    <row r="6" spans="1:113" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="27"/>
       <c r="B6" s="13"/>
       <c r="C6" s="13"/>
       <c r="D6" s="13"/>
@@ -1089,48 +1142,63 @@
       <c r="BO6" s="14"/>
       <c r="BP6" s="14"/>
       <c r="BQ6" s="14"/>
-      <c r="BR6" s="26" t="s">
+      <c r="BR6" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="BS6" s="26"/>
-      <c r="BT6" s="26"/>
-      <c r="BU6" s="26"/>
-      <c r="BV6" s="26"/>
-      <c r="BW6" s="26"/>
-      <c r="BX6" s="26"/>
-      <c r="BY6" s="26"/>
-      <c r="BZ6" s="26"/>
-      <c r="CA6" s="26"/>
-      <c r="CB6" s="26" t="s">
+      <c r="BS6" s="18"/>
+      <c r="BT6" s="18"/>
+      <c r="BU6" s="18"/>
+      <c r="BV6" s="18"/>
+      <c r="BW6" s="18"/>
+      <c r="BX6" s="18"/>
+      <c r="BY6" s="18"/>
+      <c r="BZ6" s="18"/>
+      <c r="CA6" s="18"/>
+      <c r="CB6" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="CC6" s="26"/>
-      <c r="CD6" s="26"/>
-      <c r="CE6" s="26"/>
-      <c r="CF6" s="26" t="s">
+      <c r="CC6" s="18"/>
+      <c r="CD6" s="18"/>
+      <c r="CE6" s="18"/>
+      <c r="CF6" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="CG6" s="26"/>
-      <c r="CH6" s="26"/>
-      <c r="CI6" s="26" t="s">
+      <c r="CG6" s="18"/>
+      <c r="CH6" s="18"/>
+      <c r="CI6" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="CJ6" s="26"/>
-      <c r="CK6" s="26"/>
-      <c r="CL6" s="26"/>
-      <c r="CM6" s="26"/>
-      <c r="CN6" s="26"/>
-      <c r="CO6" s="26"/>
-      <c r="CP6" s="26"/>
-      <c r="CQ6" s="26"/>
-      <c r="CR6" s="26"/>
-      <c r="CS6" s="26" t="s">
+      <c r="CJ6" s="18"/>
+      <c r="CK6" s="18"/>
+      <c r="CL6" s="18"/>
+      <c r="CM6" s="18"/>
+      <c r="CN6" s="18"/>
+      <c r="CO6" s="18"/>
+      <c r="CP6" s="18"/>
+      <c r="CQ6" s="18"/>
+      <c r="CR6" s="18"/>
+      <c r="CS6" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="CT6" s="26"/>
+      <c r="CT6" s="18"/>
+      <c r="CU6" s="28"/>
+      <c r="CV6" s="28"/>
+      <c r="CW6" s="28"/>
+      <c r="CX6" s="28"/>
+      <c r="CY6" s="28"/>
+      <c r="CZ6" s="28"/>
+      <c r="DA6" s="28"/>
+      <c r="DB6" s="28"/>
+      <c r="DC6" s="28"/>
+      <c r="DD6" s="28"/>
+      <c r="DE6" s="28"/>
+      <c r="DF6" s="28"/>
+      <c r="DG6" s="28"/>
+      <c r="DH6" s="28"/>
+      <c r="DI6" s="28"/>
     </row>
-    <row r="7" spans="1:98" s="2" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A7" s="20"/>
+    <row r="7" spans="1:113" s="2" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A7" s="27"/>
       <c r="B7" s="3" t="s">
         <v>2</v>
       </c>
@@ -1335,101 +1403,142 @@
       <c r="BQ7" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="BR7" s="24" t="s">
+      <c r="BR7" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="BS7" s="24" t="s">
+      <c r="BS7" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="BT7" s="25" t="s">
+      <c r="BT7" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="BU7" s="24" t="s">
+      <c r="BU7" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="BV7" s="25" t="s">
+      <c r="BV7" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="BW7" s="24" t="s">
+      <c r="BW7" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="BX7" s="25" t="s">
+      <c r="BX7" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="BY7" s="24" t="s">
+      <c r="BY7" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="BZ7" s="25" t="s">
+      <c r="BZ7" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="CA7" s="24" t="s">
+      <c r="CA7" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="CB7" s="25" t="s">
+      <c r="CB7" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="CC7" s="24" t="s">
+      <c r="CC7" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="CD7" s="25" t="s">
+      <c r="CD7" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="CE7" s="24" t="s">
+      <c r="CE7" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="CF7" s="25" t="s">
+      <c r="CF7" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="CG7" s="25" t="s">
+      <c r="CG7" s="17" t="s">
         <v>85</v>
       </c>
-      <c r="CH7" s="24" t="s">
+      <c r="CH7" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="CI7" s="25" t="s">
+      <c r="CI7" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="CJ7" s="25" t="s">
+      <c r="CJ7" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="CK7" s="25" t="s">
+      <c r="CK7" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="CL7" s="25" t="s">
+      <c r="CL7" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="CM7" s="25" t="s">
+      <c r="CM7" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="CN7" s="25" t="s">
+      <c r="CN7" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="CO7" s="25" t="s">
+      <c r="CO7" s="17" t="s">
         <v>90</v>
       </c>
-      <c r="CP7" s="25" t="s">
+      <c r="CP7" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="CQ7" s="25" t="s">
+      <c r="CQ7" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="CR7" s="25" t="s">
+      <c r="CR7" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="CS7" s="25" t="s">
+      <c r="CS7" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="CT7" s="25" t="s">
+      <c r="CT7" s="17" t="s">
         <v>84</v>
+      </c>
+      <c r="CU7" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="CV7" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="CW7" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="CX7" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="CY7" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="CZ7" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="DA7" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="DB7" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="DC7" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="DD7" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="DE7" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="DF7" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="DG7" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="DH7" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="DI7" s="7" t="s">
+        <v>95</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="14">
-    <mergeCell ref="CB6:CE6"/>
-    <mergeCell ref="CF6:CH6"/>
-    <mergeCell ref="CI6:CR6"/>
-    <mergeCell ref="CS6:CT6"/>
-    <mergeCell ref="BR5:CT5"/>
+  <mergeCells count="15">
+    <mergeCell ref="CU5:DI5"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="A2:K2"/>
     <mergeCell ref="A3:K3"/>
@@ -1439,6 +1548,11 @@
     <mergeCell ref="AL5:BJ5"/>
     <mergeCell ref="B5:X5"/>
     <mergeCell ref="A5:A7"/>
+    <mergeCell ref="CB6:CE6"/>
+    <mergeCell ref="CF6:CH6"/>
+    <mergeCell ref="CI6:CR6"/>
+    <mergeCell ref="CS6:CT6"/>
+    <mergeCell ref="BR5:CT5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
OAB : Laporan Riwayat Operasi Non Urologi
</commit_message>
<xml_diff>
--- a/Laravel-InaLUTS/resources/templates/Report_OAB.xlsx
+++ b/Laravel-InaLUTS/resources/templates/Report_OAB.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="109">
   <si>
     <t>No</t>
   </si>
@@ -326,6 +326,21 @@
   </si>
   <si>
     <t>Operasi anti inkontinensia urine</t>
+  </si>
+  <si>
+    <t>Operasi tulang belakang</t>
+  </si>
+  <si>
+    <t>Operasi area pelvik</t>
+  </si>
+  <si>
+    <t>Operasi di daerah pelvis</t>
+  </si>
+  <si>
+    <t>Operasi kraniotomi</t>
+  </si>
+  <si>
+    <t>Riwayat Operasi Non Urologi</t>
   </si>
 </sst>
 </file>
@@ -482,7 +497,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -535,41 +550,47 @@
     <xf numFmtId="0" fontId="1" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -872,10 +893,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:DI7"/>
+  <dimension ref="A1:DM7"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="CQ1" workbookViewId="0">
-      <selection activeCell="CU8" sqref="CU8"/>
+      <selection activeCell="DJ8" sqref="DJ8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -901,7 +922,7 @@
     <col min="42" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:113" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:117" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A1" s="20"/>
       <c r="B1" s="20"/>
       <c r="C1" s="20"/>
@@ -914,7 +935,7 @@
       <c r="J1" s="20"/>
       <c r="K1" s="20"/>
     </row>
-    <row r="2" spans="1:113" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:117" x14ac:dyDescent="0.25">
       <c r="A2" s="21"/>
       <c r="B2" s="21"/>
       <c r="C2" s="21"/>
@@ -927,7 +948,7 @@
       <c r="J2" s="21"/>
       <c r="K2" s="21"/>
     </row>
-    <row r="3" spans="1:113" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:117" x14ac:dyDescent="0.25">
       <c r="A3" s="22"/>
       <c r="B3" s="22"/>
       <c r="C3" s="22"/>
@@ -940,140 +961,146 @@
       <c r="J3" s="22"/>
       <c r="K3" s="22"/>
     </row>
-    <row r="4" spans="1:113" s="4" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:113" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="27" t="s">
+    <row r="4" spans="1:117" s="4" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:117" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="26" t="s">
+      <c r="B5" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="26"/>
-      <c r="D5" s="26"/>
-      <c r="E5" s="26"/>
-      <c r="F5" s="26"/>
-      <c r="G5" s="26"/>
-      <c r="H5" s="26"/>
-      <c r="I5" s="26"/>
-      <c r="J5" s="26"/>
-      <c r="K5" s="26"/>
-      <c r="L5" s="26"/>
-      <c r="M5" s="26"/>
-      <c r="N5" s="26"/>
-      <c r="O5" s="26"/>
-      <c r="P5" s="26"/>
-      <c r="Q5" s="26"/>
-      <c r="R5" s="26"/>
-      <c r="S5" s="26"/>
-      <c r="T5" s="26"/>
-      <c r="U5" s="26"/>
-      <c r="V5" s="26"/>
-      <c r="W5" s="26"/>
-      <c r="X5" s="26"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="27"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="27"/>
+      <c r="H5" s="27"/>
+      <c r="I5" s="27"/>
+      <c r="J5" s="27"/>
+      <c r="K5" s="27"/>
+      <c r="L5" s="27"/>
+      <c r="M5" s="27"/>
+      <c r="N5" s="27"/>
+      <c r="O5" s="27"/>
+      <c r="P5" s="27"/>
+      <c r="Q5" s="27"/>
+      <c r="R5" s="27"/>
+      <c r="S5" s="27"/>
+      <c r="T5" s="27"/>
+      <c r="U5" s="27"/>
+      <c r="V5" s="27"/>
+      <c r="W5" s="27"/>
+      <c r="X5" s="27"/>
       <c r="Y5" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="Z5" s="24" t="s">
+      <c r="Z5" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="AA5" s="24"/>
-      <c r="AB5" s="24"/>
-      <c r="AC5" s="24"/>
-      <c r="AD5" s="24"/>
-      <c r="AE5" s="24"/>
-      <c r="AF5" s="24"/>
-      <c r="AG5" s="24"/>
-      <c r="AH5" s="24"/>
-      <c r="AI5" s="24"/>
-      <c r="AJ5" s="24"/>
-      <c r="AK5" s="24"/>
-      <c r="AL5" s="25" t="s">
+      <c r="AA5" s="25"/>
+      <c r="AB5" s="25"/>
+      <c r="AC5" s="25"/>
+      <c r="AD5" s="25"/>
+      <c r="AE5" s="25"/>
+      <c r="AF5" s="25"/>
+      <c r="AG5" s="25"/>
+      <c r="AH5" s="25"/>
+      <c r="AI5" s="25"/>
+      <c r="AJ5" s="25"/>
+      <c r="AK5" s="25"/>
+      <c r="AL5" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="AM5" s="25"/>
-      <c r="AN5" s="25"/>
-      <c r="AO5" s="25"/>
-      <c r="AP5" s="25"/>
-      <c r="AQ5" s="25"/>
-      <c r="AR5" s="25"/>
-      <c r="AS5" s="25"/>
-      <c r="AT5" s="25"/>
-      <c r="AU5" s="25"/>
-      <c r="AV5" s="25"/>
-      <c r="AW5" s="25"/>
-      <c r="AX5" s="25"/>
-      <c r="AY5" s="25"/>
-      <c r="AZ5" s="25"/>
-      <c r="BA5" s="25"/>
-      <c r="BB5" s="25"/>
-      <c r="BC5" s="25"/>
-      <c r="BD5" s="25"/>
-      <c r="BE5" s="25"/>
-      <c r="BF5" s="25"/>
-      <c r="BG5" s="25"/>
-      <c r="BH5" s="25"/>
-      <c r="BI5" s="25"/>
-      <c r="BJ5" s="25"/>
-      <c r="BK5" s="23" t="s">
+      <c r="AM5" s="26"/>
+      <c r="AN5" s="26"/>
+      <c r="AO5" s="26"/>
+      <c r="AP5" s="26"/>
+      <c r="AQ5" s="26"/>
+      <c r="AR5" s="26"/>
+      <c r="AS5" s="26"/>
+      <c r="AT5" s="26"/>
+      <c r="AU5" s="26"/>
+      <c r="AV5" s="26"/>
+      <c r="AW5" s="26"/>
+      <c r="AX5" s="26"/>
+      <c r="AY5" s="26"/>
+      <c r="AZ5" s="26"/>
+      <c r="BA5" s="26"/>
+      <c r="BB5" s="26"/>
+      <c r="BC5" s="26"/>
+      <c r="BD5" s="26"/>
+      <c r="BE5" s="26"/>
+      <c r="BF5" s="26"/>
+      <c r="BG5" s="26"/>
+      <c r="BH5" s="26"/>
+      <c r="BI5" s="26"/>
+      <c r="BJ5" s="26"/>
+      <c r="BK5" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="BL5" s="23"/>
-      <c r="BM5" s="23"/>
-      <c r="BN5" s="23"/>
-      <c r="BO5" s="23"/>
-      <c r="BP5" s="23"/>
-      <c r="BQ5" s="23"/>
-      <c r="BR5" s="19" t="s">
+      <c r="BL5" s="24"/>
+      <c r="BM5" s="24"/>
+      <c r="BN5" s="24"/>
+      <c r="BO5" s="24"/>
+      <c r="BP5" s="24"/>
+      <c r="BQ5" s="24"/>
+      <c r="BR5" s="29" t="s">
         <v>73</v>
       </c>
-      <c r="BS5" s="19"/>
-      <c r="BT5" s="19"/>
-      <c r="BU5" s="19"/>
-      <c r="BV5" s="19"/>
-      <c r="BW5" s="19"/>
-      <c r="BX5" s="19"/>
-      <c r="BY5" s="19"/>
-      <c r="BZ5" s="19"/>
-      <c r="CA5" s="19"/>
-      <c r="CB5" s="19"/>
-      <c r="CC5" s="19"/>
-      <c r="CD5" s="19"/>
-      <c r="CE5" s="19"/>
-      <c r="CF5" s="19"/>
-      <c r="CG5" s="19"/>
-      <c r="CH5" s="19"/>
-      <c r="CI5" s="19"/>
-      <c r="CJ5" s="19"/>
-      <c r="CK5" s="19"/>
-      <c r="CL5" s="19"/>
-      <c r="CM5" s="19"/>
-      <c r="CN5" s="19"/>
-      <c r="CO5" s="19"/>
-      <c r="CP5" s="19"/>
-      <c r="CQ5" s="19"/>
-      <c r="CR5" s="19"/>
-      <c r="CS5" s="19"/>
-      <c r="CT5" s="19"/>
-      <c r="CU5" s="29" t="s">
+      <c r="BS5" s="29"/>
+      <c r="BT5" s="29"/>
+      <c r="BU5" s="29"/>
+      <c r="BV5" s="29"/>
+      <c r="BW5" s="29"/>
+      <c r="BX5" s="29"/>
+      <c r="BY5" s="29"/>
+      <c r="BZ5" s="29"/>
+      <c r="CA5" s="29"/>
+      <c r="CB5" s="29"/>
+      <c r="CC5" s="29"/>
+      <c r="CD5" s="29"/>
+      <c r="CE5" s="29"/>
+      <c r="CF5" s="29"/>
+      <c r="CG5" s="29"/>
+      <c r="CH5" s="29"/>
+      <c r="CI5" s="29"/>
+      <c r="CJ5" s="29"/>
+      <c r="CK5" s="29"/>
+      <c r="CL5" s="29"/>
+      <c r="CM5" s="29"/>
+      <c r="CN5" s="29"/>
+      <c r="CO5" s="29"/>
+      <c r="CP5" s="29"/>
+      <c r="CQ5" s="29"/>
+      <c r="CR5" s="29"/>
+      <c r="CS5" s="29"/>
+      <c r="CT5" s="29"/>
+      <c r="CU5" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="CV5" s="29"/>
-      <c r="CW5" s="29"/>
-      <c r="CX5" s="29"/>
-      <c r="CY5" s="29"/>
-      <c r="CZ5" s="29"/>
-      <c r="DA5" s="29"/>
-      <c r="DB5" s="29"/>
-      <c r="DC5" s="29"/>
-      <c r="DD5" s="29"/>
-      <c r="DE5" s="29"/>
-      <c r="DF5" s="29"/>
-      <c r="DG5" s="29"/>
-      <c r="DH5" s="29"/>
-      <c r="DI5" s="29"/>
+      <c r="CV5" s="19"/>
+      <c r="CW5" s="19"/>
+      <c r="CX5" s="19"/>
+      <c r="CY5" s="19"/>
+      <c r="CZ5" s="19"/>
+      <c r="DA5" s="19"/>
+      <c r="DB5" s="19"/>
+      <c r="DC5" s="19"/>
+      <c r="DD5" s="19"/>
+      <c r="DE5" s="19"/>
+      <c r="DF5" s="19"/>
+      <c r="DG5" s="19"/>
+      <c r="DH5" s="19"/>
+      <c r="DI5" s="19"/>
+      <c r="DJ5" s="30" t="s">
+        <v>108</v>
+      </c>
+      <c r="DK5" s="30"/>
+      <c r="DL5" s="30"/>
+      <c r="DM5" s="30"/>
     </row>
-    <row r="6" spans="1:113" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="27"/>
+    <row r="6" spans="1:117" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="28"/>
       <c r="B6" s="13"/>
       <c r="C6" s="13"/>
       <c r="D6" s="13"/>
@@ -1142,63 +1169,67 @@
       <c r="BO6" s="14"/>
       <c r="BP6" s="14"/>
       <c r="BQ6" s="14"/>
-      <c r="BR6" s="18" t="s">
+      <c r="BR6" s="23" t="s">
         <v>75</v>
       </c>
-      <c r="BS6" s="18"/>
-      <c r="BT6" s="18"/>
-      <c r="BU6" s="18"/>
-      <c r="BV6" s="18"/>
-      <c r="BW6" s="18"/>
-      <c r="BX6" s="18"/>
-      <c r="BY6" s="18"/>
-      <c r="BZ6" s="18"/>
-      <c r="CA6" s="18"/>
-      <c r="CB6" s="18" t="s">
+      <c r="BS6" s="23"/>
+      <c r="BT6" s="23"/>
+      <c r="BU6" s="23"/>
+      <c r="BV6" s="23"/>
+      <c r="BW6" s="23"/>
+      <c r="BX6" s="23"/>
+      <c r="BY6" s="23"/>
+      <c r="BZ6" s="23"/>
+      <c r="CA6" s="23"/>
+      <c r="CB6" s="23" t="s">
         <v>80</v>
       </c>
-      <c r="CC6" s="18"/>
-      <c r="CD6" s="18"/>
-      <c r="CE6" s="18"/>
-      <c r="CF6" s="18" t="s">
+      <c r="CC6" s="23"/>
+      <c r="CD6" s="23"/>
+      <c r="CE6" s="23"/>
+      <c r="CF6" s="23" t="s">
         <v>83</v>
       </c>
-      <c r="CG6" s="18"/>
-      <c r="CH6" s="18"/>
-      <c r="CI6" s="18" t="s">
+      <c r="CG6" s="23"/>
+      <c r="CH6" s="23"/>
+      <c r="CI6" s="23" t="s">
         <v>86</v>
       </c>
-      <c r="CJ6" s="18"/>
-      <c r="CK6" s="18"/>
-      <c r="CL6" s="18"/>
-      <c r="CM6" s="18"/>
-      <c r="CN6" s="18"/>
-      <c r="CO6" s="18"/>
-      <c r="CP6" s="18"/>
-      <c r="CQ6" s="18"/>
-      <c r="CR6" s="18"/>
-      <c r="CS6" s="18" t="s">
+      <c r="CJ6" s="23"/>
+      <c r="CK6" s="23"/>
+      <c r="CL6" s="23"/>
+      <c r="CM6" s="23"/>
+      <c r="CN6" s="23"/>
+      <c r="CO6" s="23"/>
+      <c r="CP6" s="23"/>
+      <c r="CQ6" s="23"/>
+      <c r="CR6" s="23"/>
+      <c r="CS6" s="23" t="s">
         <v>92</v>
       </c>
-      <c r="CT6" s="18"/>
-      <c r="CU6" s="28"/>
-      <c r="CV6" s="28"/>
-      <c r="CW6" s="28"/>
-      <c r="CX6" s="28"/>
-      <c r="CY6" s="28"/>
-      <c r="CZ6" s="28"/>
-      <c r="DA6" s="28"/>
-      <c r="DB6" s="28"/>
-      <c r="DC6" s="28"/>
-      <c r="DD6" s="28"/>
-      <c r="DE6" s="28"/>
-      <c r="DF6" s="28"/>
-      <c r="DG6" s="28"/>
-      <c r="DH6" s="28"/>
-      <c r="DI6" s="28"/>
+      <c r="CT6" s="23"/>
+      <c r="CU6" s="18"/>
+      <c r="CV6" s="18"/>
+      <c r="CW6" s="18"/>
+      <c r="CX6" s="18"/>
+      <c r="CY6" s="18"/>
+      <c r="CZ6" s="18"/>
+      <c r="DA6" s="18"/>
+      <c r="DB6" s="18"/>
+      <c r="DC6" s="18"/>
+      <c r="DD6" s="18"/>
+      <c r="DE6" s="18"/>
+      <c r="DF6" s="18"/>
+      <c r="DG6" s="18"/>
+      <c r="DH6" s="18"/>
+      <c r="DI6" s="18"/>
+      <c r="DJ6" s="31"/>
+      <c r="DK6" s="31"/>
+      <c r="DL6" s="31"/>
+      <c r="DM6" s="31"/>
     </row>
-    <row r="7" spans="1:113" s="2" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A7" s="27"/>
+    <row r="7" spans="1:117" s="2" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A7" s="28"/>
       <c r="B7" s="3" t="s">
         <v>2</v>
       </c>
@@ -1535,9 +1566,22 @@
       <c r="DI7" s="7" t="s">
         <v>95</v>
       </c>
+      <c r="DJ7" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="DK7" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="DL7" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="DM7" s="5" t="s">
+        <v>107</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="16">
+    <mergeCell ref="DJ5:DM5"/>
     <mergeCell ref="CU5:DI5"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="A2:K2"/>

</xml_diff>

<commit_message>
OAB : Laporan Riwayat Radiasi dan Kemoterapi
</commit_message>
<xml_diff>
--- a/Laravel-InaLUTS/resources/templates/Report_OAB.xlsx
+++ b/Laravel-InaLUTS/resources/templates/Report_OAB.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="112">
   <si>
     <t>No</t>
   </si>
@@ -341,6 +341,15 @@
   </si>
   <si>
     <t>Riwayat Operasi Non Urologi</t>
+  </si>
+  <si>
+    <t>Riwayat Radiasi dan Kemoterapi</t>
+  </si>
+  <si>
+    <t>Riwayat radiasi pelvis</t>
+  </si>
+  <si>
+    <t>Riwayat kemoterapi</t>
   </si>
 </sst>
 </file>
@@ -497,7 +506,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -553,6 +562,12 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -586,11 +601,11 @@
     <xf numFmtId="0" fontId="1" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -893,10 +908,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:DM7"/>
+  <dimension ref="A1:DO7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="CQ1" workbookViewId="0">
-      <selection activeCell="DJ8" sqref="DJ8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -919,188 +934,194 @@
     <col min="26" max="37" width="10.7109375" style="1" customWidth="1"/>
     <col min="38" max="40" width="9.140625" style="1"/>
     <col min="41" max="41" width="18" style="1" bestFit="1" customWidth="1"/>
-    <col min="42" max="16384" width="9.140625" style="1"/>
+    <col min="42" max="117" width="9.140625" style="1"/>
+    <col min="118" max="119" width="15.7109375" style="1" customWidth="1"/>
+    <col min="120" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:117" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="20"/>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
+    <row r="1" spans="1:119" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="22"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
     </row>
-    <row r="2" spans="1:117" x14ac:dyDescent="0.25">
-      <c r="A2" s="21"/>
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="21"/>
-      <c r="J2" s="21"/>
-      <c r="K2" s="21"/>
+    <row r="2" spans="1:119" x14ac:dyDescent="0.25">
+      <c r="A2" s="23"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23"/>
+      <c r="K2" s="23"/>
     </row>
-    <row r="3" spans="1:117" x14ac:dyDescent="0.25">
-      <c r="A3" s="22"/>
-      <c r="B3" s="22"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="22"/>
-      <c r="H3" s="22"/>
-      <c r="I3" s="22"/>
-      <c r="J3" s="22"/>
-      <c r="K3" s="22"/>
+    <row r="3" spans="1:119" x14ac:dyDescent="0.25">
+      <c r="A3" s="24"/>
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="24"/>
+      <c r="J3" s="24"/>
+      <c r="K3" s="24"/>
     </row>
-    <row r="4" spans="1:117" s="4" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:117" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="28" t="s">
+    <row r="4" spans="1:119" s="4" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:119" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="27" t="s">
+      <c r="B5" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="27"/>
-      <c r="D5" s="27"/>
-      <c r="E5" s="27"/>
-      <c r="F5" s="27"/>
-      <c r="G5" s="27"/>
-      <c r="H5" s="27"/>
-      <c r="I5" s="27"/>
-      <c r="J5" s="27"/>
-      <c r="K5" s="27"/>
-      <c r="L5" s="27"/>
-      <c r="M5" s="27"/>
-      <c r="N5" s="27"/>
-      <c r="O5" s="27"/>
-      <c r="P5" s="27"/>
-      <c r="Q5" s="27"/>
-      <c r="R5" s="27"/>
-      <c r="S5" s="27"/>
-      <c r="T5" s="27"/>
-      <c r="U5" s="27"/>
-      <c r="V5" s="27"/>
-      <c r="W5" s="27"/>
-      <c r="X5" s="27"/>
+      <c r="C5" s="29"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="29"/>
+      <c r="G5" s="29"/>
+      <c r="H5" s="29"/>
+      <c r="I5" s="29"/>
+      <c r="J5" s="29"/>
+      <c r="K5" s="29"/>
+      <c r="L5" s="29"/>
+      <c r="M5" s="29"/>
+      <c r="N5" s="29"/>
+      <c r="O5" s="29"/>
+      <c r="P5" s="29"/>
+      <c r="Q5" s="29"/>
+      <c r="R5" s="29"/>
+      <c r="S5" s="29"/>
+      <c r="T5" s="29"/>
+      <c r="U5" s="29"/>
+      <c r="V5" s="29"/>
+      <c r="W5" s="29"/>
+      <c r="X5" s="29"/>
       <c r="Y5" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="Z5" s="25" t="s">
+      <c r="Z5" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="AA5" s="25"/>
-      <c r="AB5" s="25"/>
-      <c r="AC5" s="25"/>
-      <c r="AD5" s="25"/>
-      <c r="AE5" s="25"/>
-      <c r="AF5" s="25"/>
-      <c r="AG5" s="25"/>
-      <c r="AH5" s="25"/>
-      <c r="AI5" s="25"/>
-      <c r="AJ5" s="25"/>
-      <c r="AK5" s="25"/>
-      <c r="AL5" s="26" t="s">
+      <c r="AA5" s="27"/>
+      <c r="AB5" s="27"/>
+      <c r="AC5" s="27"/>
+      <c r="AD5" s="27"/>
+      <c r="AE5" s="27"/>
+      <c r="AF5" s="27"/>
+      <c r="AG5" s="27"/>
+      <c r="AH5" s="27"/>
+      <c r="AI5" s="27"/>
+      <c r="AJ5" s="27"/>
+      <c r="AK5" s="27"/>
+      <c r="AL5" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="AM5" s="26"/>
-      <c r="AN5" s="26"/>
-      <c r="AO5" s="26"/>
-      <c r="AP5" s="26"/>
-      <c r="AQ5" s="26"/>
-      <c r="AR5" s="26"/>
-      <c r="AS5" s="26"/>
-      <c r="AT5" s="26"/>
-      <c r="AU5" s="26"/>
-      <c r="AV5" s="26"/>
-      <c r="AW5" s="26"/>
-      <c r="AX5" s="26"/>
-      <c r="AY5" s="26"/>
-      <c r="AZ5" s="26"/>
-      <c r="BA5" s="26"/>
-      <c r="BB5" s="26"/>
-      <c r="BC5" s="26"/>
-      <c r="BD5" s="26"/>
-      <c r="BE5" s="26"/>
-      <c r="BF5" s="26"/>
-      <c r="BG5" s="26"/>
-      <c r="BH5" s="26"/>
-      <c r="BI5" s="26"/>
-      <c r="BJ5" s="26"/>
-      <c r="BK5" s="24" t="s">
+      <c r="AM5" s="28"/>
+      <c r="AN5" s="28"/>
+      <c r="AO5" s="28"/>
+      <c r="AP5" s="28"/>
+      <c r="AQ5" s="28"/>
+      <c r="AR5" s="28"/>
+      <c r="AS5" s="28"/>
+      <c r="AT5" s="28"/>
+      <c r="AU5" s="28"/>
+      <c r="AV5" s="28"/>
+      <c r="AW5" s="28"/>
+      <c r="AX5" s="28"/>
+      <c r="AY5" s="28"/>
+      <c r="AZ5" s="28"/>
+      <c r="BA5" s="28"/>
+      <c r="BB5" s="28"/>
+      <c r="BC5" s="28"/>
+      <c r="BD5" s="28"/>
+      <c r="BE5" s="28"/>
+      <c r="BF5" s="28"/>
+      <c r="BG5" s="28"/>
+      <c r="BH5" s="28"/>
+      <c r="BI5" s="28"/>
+      <c r="BJ5" s="28"/>
+      <c r="BK5" s="26" t="s">
         <v>72</v>
       </c>
-      <c r="BL5" s="24"/>
-      <c r="BM5" s="24"/>
-      <c r="BN5" s="24"/>
-      <c r="BO5" s="24"/>
-      <c r="BP5" s="24"/>
-      <c r="BQ5" s="24"/>
-      <c r="BR5" s="29" t="s">
+      <c r="BL5" s="26"/>
+      <c r="BM5" s="26"/>
+      <c r="BN5" s="26"/>
+      <c r="BO5" s="26"/>
+      <c r="BP5" s="26"/>
+      <c r="BQ5" s="26"/>
+      <c r="BR5" s="31" t="s">
         <v>73</v>
       </c>
-      <c r="BS5" s="29"/>
-      <c r="BT5" s="29"/>
-      <c r="BU5" s="29"/>
-      <c r="BV5" s="29"/>
-      <c r="BW5" s="29"/>
-      <c r="BX5" s="29"/>
-      <c r="BY5" s="29"/>
-      <c r="BZ5" s="29"/>
-      <c r="CA5" s="29"/>
-      <c r="CB5" s="29"/>
-      <c r="CC5" s="29"/>
-      <c r="CD5" s="29"/>
-      <c r="CE5" s="29"/>
-      <c r="CF5" s="29"/>
-      <c r="CG5" s="29"/>
-      <c r="CH5" s="29"/>
-      <c r="CI5" s="29"/>
-      <c r="CJ5" s="29"/>
-      <c r="CK5" s="29"/>
-      <c r="CL5" s="29"/>
-      <c r="CM5" s="29"/>
-      <c r="CN5" s="29"/>
-      <c r="CO5" s="29"/>
-      <c r="CP5" s="29"/>
-      <c r="CQ5" s="29"/>
-      <c r="CR5" s="29"/>
-      <c r="CS5" s="29"/>
-      <c r="CT5" s="29"/>
-      <c r="CU5" s="19" t="s">
+      <c r="BS5" s="31"/>
+      <c r="BT5" s="31"/>
+      <c r="BU5" s="31"/>
+      <c r="BV5" s="31"/>
+      <c r="BW5" s="31"/>
+      <c r="BX5" s="31"/>
+      <c r="BY5" s="31"/>
+      <c r="BZ5" s="31"/>
+      <c r="CA5" s="31"/>
+      <c r="CB5" s="31"/>
+      <c r="CC5" s="31"/>
+      <c r="CD5" s="31"/>
+      <c r="CE5" s="31"/>
+      <c r="CF5" s="31"/>
+      <c r="CG5" s="31"/>
+      <c r="CH5" s="31"/>
+      <c r="CI5" s="31"/>
+      <c r="CJ5" s="31"/>
+      <c r="CK5" s="31"/>
+      <c r="CL5" s="31"/>
+      <c r="CM5" s="31"/>
+      <c r="CN5" s="31"/>
+      <c r="CO5" s="31"/>
+      <c r="CP5" s="31"/>
+      <c r="CQ5" s="31"/>
+      <c r="CR5" s="31"/>
+      <c r="CS5" s="31"/>
+      <c r="CT5" s="31"/>
+      <c r="CU5" s="21" t="s">
         <v>94</v>
       </c>
-      <c r="CV5" s="19"/>
-      <c r="CW5" s="19"/>
-      <c r="CX5" s="19"/>
-      <c r="CY5" s="19"/>
-      <c r="CZ5" s="19"/>
-      <c r="DA5" s="19"/>
-      <c r="DB5" s="19"/>
-      <c r="DC5" s="19"/>
-      <c r="DD5" s="19"/>
-      <c r="DE5" s="19"/>
-      <c r="DF5" s="19"/>
-      <c r="DG5" s="19"/>
-      <c r="DH5" s="19"/>
-      <c r="DI5" s="19"/>
-      <c r="DJ5" s="30" t="s">
+      <c r="CV5" s="21"/>
+      <c r="CW5" s="21"/>
+      <c r="CX5" s="21"/>
+      <c r="CY5" s="21"/>
+      <c r="CZ5" s="21"/>
+      <c r="DA5" s="21"/>
+      <c r="DB5" s="21"/>
+      <c r="DC5" s="21"/>
+      <c r="DD5" s="21"/>
+      <c r="DE5" s="21"/>
+      <c r="DF5" s="21"/>
+      <c r="DG5" s="21"/>
+      <c r="DH5" s="21"/>
+      <c r="DI5" s="21"/>
+      <c r="DJ5" s="20" t="s">
         <v>108</v>
       </c>
-      <c r="DK5" s="30"/>
-      <c r="DL5" s="30"/>
-      <c r="DM5" s="30"/>
+      <c r="DK5" s="20"/>
+      <c r="DL5" s="20"/>
+      <c r="DM5" s="20"/>
+      <c r="DN5" s="33" t="s">
+        <v>109</v>
+      </c>
+      <c r="DO5" s="33"/>
     </row>
-    <row r="6" spans="1:117" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="28"/>
+    <row r="6" spans="1:119" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="30"/>
       <c r="B6" s="13"/>
       <c r="C6" s="13"/>
       <c r="D6" s="13"/>
@@ -1169,45 +1190,45 @@
       <c r="BO6" s="14"/>
       <c r="BP6" s="14"/>
       <c r="BQ6" s="14"/>
-      <c r="BR6" s="23" t="s">
+      <c r="BR6" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="BS6" s="23"/>
-      <c r="BT6" s="23"/>
-      <c r="BU6" s="23"/>
-      <c r="BV6" s="23"/>
-      <c r="BW6" s="23"/>
-      <c r="BX6" s="23"/>
-      <c r="BY6" s="23"/>
-      <c r="BZ6" s="23"/>
-      <c r="CA6" s="23"/>
-      <c r="CB6" s="23" t="s">
+      <c r="BS6" s="25"/>
+      <c r="BT6" s="25"/>
+      <c r="BU6" s="25"/>
+      <c r="BV6" s="25"/>
+      <c r="BW6" s="25"/>
+      <c r="BX6" s="25"/>
+      <c r="BY6" s="25"/>
+      <c r="BZ6" s="25"/>
+      <c r="CA6" s="25"/>
+      <c r="CB6" s="25" t="s">
         <v>80</v>
       </c>
-      <c r="CC6" s="23"/>
-      <c r="CD6" s="23"/>
-      <c r="CE6" s="23"/>
-      <c r="CF6" s="23" t="s">
+      <c r="CC6" s="25"/>
+      <c r="CD6" s="25"/>
+      <c r="CE6" s="25"/>
+      <c r="CF6" s="25" t="s">
         <v>83</v>
       </c>
-      <c r="CG6" s="23"/>
-      <c r="CH6" s="23"/>
-      <c r="CI6" s="23" t="s">
+      <c r="CG6" s="25"/>
+      <c r="CH6" s="25"/>
+      <c r="CI6" s="25" t="s">
         <v>86</v>
       </c>
-      <c r="CJ6" s="23"/>
-      <c r="CK6" s="23"/>
-      <c r="CL6" s="23"/>
-      <c r="CM6" s="23"/>
-      <c r="CN6" s="23"/>
-      <c r="CO6" s="23"/>
-      <c r="CP6" s="23"/>
-      <c r="CQ6" s="23"/>
-      <c r="CR6" s="23"/>
-      <c r="CS6" s="23" t="s">
+      <c r="CJ6" s="25"/>
+      <c r="CK6" s="25"/>
+      <c r="CL6" s="25"/>
+      <c r="CM6" s="25"/>
+      <c r="CN6" s="25"/>
+      <c r="CO6" s="25"/>
+      <c r="CP6" s="25"/>
+      <c r="CQ6" s="25"/>
+      <c r="CR6" s="25"/>
+      <c r="CS6" s="25" t="s">
         <v>92</v>
       </c>
-      <c r="CT6" s="23"/>
+      <c r="CT6" s="25"/>
       <c r="CU6" s="18"/>
       <c r="CV6" s="18"/>
       <c r="CW6" s="18"/>
@@ -1223,13 +1244,15 @@
       <c r="DG6" s="18"/>
       <c r="DH6" s="18"/>
       <c r="DI6" s="18"/>
-      <c r="DJ6" s="31"/>
-      <c r="DK6" s="31"/>
-      <c r="DL6" s="31"/>
-      <c r="DM6" s="31"/>
+      <c r="DJ6" s="19"/>
+      <c r="DK6" s="19"/>
+      <c r="DL6" s="19"/>
+      <c r="DM6" s="19"/>
+      <c r="DN6" s="32"/>
+      <c r="DO6" s="32"/>
     </row>
-    <row r="7" spans="1:117" s="2" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A7" s="28"/>
+    <row r="7" spans="1:119" s="2" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A7" s="30"/>
       <c r="B7" s="3" t="s">
         <v>2</v>
       </c>
@@ -1578,25 +1601,32 @@
       <c r="DM7" s="5" t="s">
         <v>107</v>
       </c>
+      <c r="DN7" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="DO7" s="8" t="s">
+        <v>111</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="16">
+  <mergeCells count="17">
+    <mergeCell ref="DN5:DO5"/>
+    <mergeCell ref="BR6:CA6"/>
+    <mergeCell ref="BK5:BQ5"/>
+    <mergeCell ref="Z5:AK5"/>
+    <mergeCell ref="AL5:BJ5"/>
+    <mergeCell ref="B5:X5"/>
+    <mergeCell ref="BR5:CT5"/>
     <mergeCell ref="DJ5:DM5"/>
     <mergeCell ref="CU5:DI5"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="A2:K2"/>
     <mergeCell ref="A3:K3"/>
-    <mergeCell ref="BR6:CA6"/>
-    <mergeCell ref="BK5:BQ5"/>
-    <mergeCell ref="Z5:AK5"/>
-    <mergeCell ref="AL5:BJ5"/>
-    <mergeCell ref="B5:X5"/>
     <mergeCell ref="A5:A7"/>
     <mergeCell ref="CB6:CE6"/>
     <mergeCell ref="CF6:CH6"/>
     <mergeCell ref="CI6:CR6"/>
     <mergeCell ref="CS6:CT6"/>
-    <mergeCell ref="BR5:CT5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
OAB : Laporan Sistem Skor
</commit_message>
<xml_diff>
--- a/Laravel-InaLUTS/resources/templates/Report_OAB.xlsx
+++ b/Laravel-InaLUTS/resources/templates/Report_OAB.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="113">
   <si>
     <t>No</t>
   </si>
@@ -350,6 +350,9 @@
   </si>
   <si>
     <t>Riwayat kemoterapi</t>
+  </si>
+  <si>
+    <t>Sistem skor</t>
   </si>
 </sst>
 </file>
@@ -506,7 +509,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -565,6 +568,30 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -580,32 +607,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -908,7 +914,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:DO7"/>
+  <dimension ref="A1:DP7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
@@ -936,192 +942,196 @@
     <col min="41" max="41" width="18" style="1" bestFit="1" customWidth="1"/>
     <col min="42" max="117" width="9.140625" style="1"/>
     <col min="118" max="119" width="15.7109375" style="1" customWidth="1"/>
-    <col min="120" max="16384" width="9.140625" style="1"/>
+    <col min="120" max="120" width="12.7109375" style="1" customWidth="1"/>
+    <col min="121" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:119" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="22"/>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
+    <row r="1" spans="1:120" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="30"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
     </row>
-    <row r="2" spans="1:119" x14ac:dyDescent="0.25">
-      <c r="A2" s="23"/>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23"/>
-      <c r="J2" s="23"/>
-      <c r="K2" s="23"/>
+    <row r="2" spans="1:120" x14ac:dyDescent="0.25">
+      <c r="A2" s="31"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="31"/>
     </row>
-    <row r="3" spans="1:119" x14ac:dyDescent="0.25">
-      <c r="A3" s="24"/>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="24"/>
-      <c r="I3" s="24"/>
-      <c r="J3" s="24"/>
-      <c r="K3" s="24"/>
+    <row r="3" spans="1:120" x14ac:dyDescent="0.25">
+      <c r="A3" s="32"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
+      <c r="K3" s="32"/>
     </row>
-    <row r="4" spans="1:119" s="4" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:119" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="30" t="s">
+    <row r="4" spans="1:120" s="4" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:120" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="29" t="s">
+      <c r="B5" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="29"/>
-      <c r="D5" s="29"/>
-      <c r="E5" s="29"/>
-      <c r="F5" s="29"/>
-      <c r="G5" s="29"/>
-      <c r="H5" s="29"/>
-      <c r="I5" s="29"/>
-      <c r="J5" s="29"/>
-      <c r="K5" s="29"/>
-      <c r="L5" s="29"/>
-      <c r="M5" s="29"/>
-      <c r="N5" s="29"/>
-      <c r="O5" s="29"/>
-      <c r="P5" s="29"/>
-      <c r="Q5" s="29"/>
-      <c r="R5" s="29"/>
-      <c r="S5" s="29"/>
-      <c r="T5" s="29"/>
-      <c r="U5" s="29"/>
-      <c r="V5" s="29"/>
-      <c r="W5" s="29"/>
-      <c r="X5" s="29"/>
+      <c r="C5" s="26"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="26"/>
+      <c r="H5" s="26"/>
+      <c r="I5" s="26"/>
+      <c r="J5" s="26"/>
+      <c r="K5" s="26"/>
+      <c r="L5" s="26"/>
+      <c r="M5" s="26"/>
+      <c r="N5" s="26"/>
+      <c r="O5" s="26"/>
+      <c r="P5" s="26"/>
+      <c r="Q5" s="26"/>
+      <c r="R5" s="26"/>
+      <c r="S5" s="26"/>
+      <c r="T5" s="26"/>
+      <c r="U5" s="26"/>
+      <c r="V5" s="26"/>
+      <c r="W5" s="26"/>
+      <c r="X5" s="26"/>
       <c r="Y5" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="Z5" s="27" t="s">
+      <c r="Z5" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="AA5" s="27"/>
-      <c r="AB5" s="27"/>
-      <c r="AC5" s="27"/>
-      <c r="AD5" s="27"/>
-      <c r="AE5" s="27"/>
-      <c r="AF5" s="27"/>
-      <c r="AG5" s="27"/>
-      <c r="AH5" s="27"/>
-      <c r="AI5" s="27"/>
-      <c r="AJ5" s="27"/>
-      <c r="AK5" s="27"/>
-      <c r="AL5" s="28" t="s">
+      <c r="AA5" s="24"/>
+      <c r="AB5" s="24"/>
+      <c r="AC5" s="24"/>
+      <c r="AD5" s="24"/>
+      <c r="AE5" s="24"/>
+      <c r="AF5" s="24"/>
+      <c r="AG5" s="24"/>
+      <c r="AH5" s="24"/>
+      <c r="AI5" s="24"/>
+      <c r="AJ5" s="24"/>
+      <c r="AK5" s="24"/>
+      <c r="AL5" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="AM5" s="28"/>
-      <c r="AN5" s="28"/>
-      <c r="AO5" s="28"/>
-      <c r="AP5" s="28"/>
-      <c r="AQ5" s="28"/>
-      <c r="AR5" s="28"/>
-      <c r="AS5" s="28"/>
-      <c r="AT5" s="28"/>
-      <c r="AU5" s="28"/>
-      <c r="AV5" s="28"/>
-      <c r="AW5" s="28"/>
-      <c r="AX5" s="28"/>
-      <c r="AY5" s="28"/>
-      <c r="AZ5" s="28"/>
-      <c r="BA5" s="28"/>
-      <c r="BB5" s="28"/>
-      <c r="BC5" s="28"/>
-      <c r="BD5" s="28"/>
-      <c r="BE5" s="28"/>
-      <c r="BF5" s="28"/>
-      <c r="BG5" s="28"/>
-      <c r="BH5" s="28"/>
-      <c r="BI5" s="28"/>
-      <c r="BJ5" s="28"/>
-      <c r="BK5" s="26" t="s">
+      <c r="AM5" s="25"/>
+      <c r="AN5" s="25"/>
+      <c r="AO5" s="25"/>
+      <c r="AP5" s="25"/>
+      <c r="AQ5" s="25"/>
+      <c r="AR5" s="25"/>
+      <c r="AS5" s="25"/>
+      <c r="AT5" s="25"/>
+      <c r="AU5" s="25"/>
+      <c r="AV5" s="25"/>
+      <c r="AW5" s="25"/>
+      <c r="AX5" s="25"/>
+      <c r="AY5" s="25"/>
+      <c r="AZ5" s="25"/>
+      <c r="BA5" s="25"/>
+      <c r="BB5" s="25"/>
+      <c r="BC5" s="25"/>
+      <c r="BD5" s="25"/>
+      <c r="BE5" s="25"/>
+      <c r="BF5" s="25"/>
+      <c r="BG5" s="25"/>
+      <c r="BH5" s="25"/>
+      <c r="BI5" s="25"/>
+      <c r="BJ5" s="25"/>
+      <c r="BK5" s="23" t="s">
         <v>72</v>
       </c>
-      <c r="BL5" s="26"/>
-      <c r="BM5" s="26"/>
-      <c r="BN5" s="26"/>
-      <c r="BO5" s="26"/>
-      <c r="BP5" s="26"/>
-      <c r="BQ5" s="26"/>
-      <c r="BR5" s="31" t="s">
+      <c r="BL5" s="23"/>
+      <c r="BM5" s="23"/>
+      <c r="BN5" s="23"/>
+      <c r="BO5" s="23"/>
+      <c r="BP5" s="23"/>
+      <c r="BQ5" s="23"/>
+      <c r="BR5" s="27" t="s">
         <v>73</v>
       </c>
-      <c r="BS5" s="31"/>
-      <c r="BT5" s="31"/>
-      <c r="BU5" s="31"/>
-      <c r="BV5" s="31"/>
-      <c r="BW5" s="31"/>
-      <c r="BX5" s="31"/>
-      <c r="BY5" s="31"/>
-      <c r="BZ5" s="31"/>
-      <c r="CA5" s="31"/>
-      <c r="CB5" s="31"/>
-      <c r="CC5" s="31"/>
-      <c r="CD5" s="31"/>
-      <c r="CE5" s="31"/>
-      <c r="CF5" s="31"/>
-      <c r="CG5" s="31"/>
-      <c r="CH5" s="31"/>
-      <c r="CI5" s="31"/>
-      <c r="CJ5" s="31"/>
-      <c r="CK5" s="31"/>
-      <c r="CL5" s="31"/>
-      <c r="CM5" s="31"/>
-      <c r="CN5" s="31"/>
-      <c r="CO5" s="31"/>
-      <c r="CP5" s="31"/>
-      <c r="CQ5" s="31"/>
-      <c r="CR5" s="31"/>
-      <c r="CS5" s="31"/>
-      <c r="CT5" s="31"/>
-      <c r="CU5" s="21" t="s">
+      <c r="BS5" s="27"/>
+      <c r="BT5" s="27"/>
+      <c r="BU5" s="27"/>
+      <c r="BV5" s="27"/>
+      <c r="BW5" s="27"/>
+      <c r="BX5" s="27"/>
+      <c r="BY5" s="27"/>
+      <c r="BZ5" s="27"/>
+      <c r="CA5" s="27"/>
+      <c r="CB5" s="27"/>
+      <c r="CC5" s="27"/>
+      <c r="CD5" s="27"/>
+      <c r="CE5" s="27"/>
+      <c r="CF5" s="27"/>
+      <c r="CG5" s="27"/>
+      <c r="CH5" s="27"/>
+      <c r="CI5" s="27"/>
+      <c r="CJ5" s="27"/>
+      <c r="CK5" s="27"/>
+      <c r="CL5" s="27"/>
+      <c r="CM5" s="27"/>
+      <c r="CN5" s="27"/>
+      <c r="CO5" s="27"/>
+      <c r="CP5" s="27"/>
+      <c r="CQ5" s="27"/>
+      <c r="CR5" s="27"/>
+      <c r="CS5" s="27"/>
+      <c r="CT5" s="27"/>
+      <c r="CU5" s="29" t="s">
         <v>94</v>
       </c>
-      <c r="CV5" s="21"/>
-      <c r="CW5" s="21"/>
-      <c r="CX5" s="21"/>
-      <c r="CY5" s="21"/>
-      <c r="CZ5" s="21"/>
-      <c r="DA5" s="21"/>
-      <c r="DB5" s="21"/>
-      <c r="DC5" s="21"/>
-      <c r="DD5" s="21"/>
-      <c r="DE5" s="21"/>
-      <c r="DF5" s="21"/>
-      <c r="DG5" s="21"/>
-      <c r="DH5" s="21"/>
-      <c r="DI5" s="21"/>
-      <c r="DJ5" s="20" t="s">
+      <c r="CV5" s="29"/>
+      <c r="CW5" s="29"/>
+      <c r="CX5" s="29"/>
+      <c r="CY5" s="29"/>
+      <c r="CZ5" s="29"/>
+      <c r="DA5" s="29"/>
+      <c r="DB5" s="29"/>
+      <c r="DC5" s="29"/>
+      <c r="DD5" s="29"/>
+      <c r="DE5" s="29"/>
+      <c r="DF5" s="29"/>
+      <c r="DG5" s="29"/>
+      <c r="DH5" s="29"/>
+      <c r="DI5" s="29"/>
+      <c r="DJ5" s="28" t="s">
         <v>108</v>
       </c>
-      <c r="DK5" s="20"/>
-      <c r="DL5" s="20"/>
-      <c r="DM5" s="20"/>
-      <c r="DN5" s="33" t="s">
+      <c r="DK5" s="28"/>
+      <c r="DL5" s="28"/>
+      <c r="DM5" s="28"/>
+      <c r="DN5" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="DO5" s="33"/>
+      <c r="DO5" s="21"/>
+      <c r="DP5" s="34" t="s">
+        <v>112</v>
+      </c>
     </row>
-    <row r="6" spans="1:119" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="30"/>
+    <row r="6" spans="1:120" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="33"/>
       <c r="B6" s="13"/>
       <c r="C6" s="13"/>
       <c r="D6" s="13"/>
@@ -1190,45 +1200,45 @@
       <c r="BO6" s="14"/>
       <c r="BP6" s="14"/>
       <c r="BQ6" s="14"/>
-      <c r="BR6" s="25" t="s">
+      <c r="BR6" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="BS6" s="25"/>
-      <c r="BT6" s="25"/>
-      <c r="BU6" s="25"/>
-      <c r="BV6" s="25"/>
-      <c r="BW6" s="25"/>
-      <c r="BX6" s="25"/>
-      <c r="BY6" s="25"/>
-      <c r="BZ6" s="25"/>
-      <c r="CA6" s="25"/>
-      <c r="CB6" s="25" t="s">
+      <c r="BS6" s="22"/>
+      <c r="BT6" s="22"/>
+      <c r="BU6" s="22"/>
+      <c r="BV6" s="22"/>
+      <c r="BW6" s="22"/>
+      <c r="BX6" s="22"/>
+      <c r="BY6" s="22"/>
+      <c r="BZ6" s="22"/>
+      <c r="CA6" s="22"/>
+      <c r="CB6" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="CC6" s="25"/>
-      <c r="CD6" s="25"/>
-      <c r="CE6" s="25"/>
-      <c r="CF6" s="25" t="s">
+      <c r="CC6" s="22"/>
+      <c r="CD6" s="22"/>
+      <c r="CE6" s="22"/>
+      <c r="CF6" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="CG6" s="25"/>
-      <c r="CH6" s="25"/>
-      <c r="CI6" s="25" t="s">
+      <c r="CG6" s="22"/>
+      <c r="CH6" s="22"/>
+      <c r="CI6" s="22" t="s">
         <v>86</v>
       </c>
-      <c r="CJ6" s="25"/>
-      <c r="CK6" s="25"/>
-      <c r="CL6" s="25"/>
-      <c r="CM6" s="25"/>
-      <c r="CN6" s="25"/>
-      <c r="CO6" s="25"/>
-      <c r="CP6" s="25"/>
-      <c r="CQ6" s="25"/>
-      <c r="CR6" s="25"/>
-      <c r="CS6" s="25" t="s">
+      <c r="CJ6" s="22"/>
+      <c r="CK6" s="22"/>
+      <c r="CL6" s="22"/>
+      <c r="CM6" s="22"/>
+      <c r="CN6" s="22"/>
+      <c r="CO6" s="22"/>
+      <c r="CP6" s="22"/>
+      <c r="CQ6" s="22"/>
+      <c r="CR6" s="22"/>
+      <c r="CS6" s="22" t="s">
         <v>92</v>
       </c>
-      <c r="CT6" s="25"/>
+      <c r="CT6" s="22"/>
       <c r="CU6" s="18"/>
       <c r="CV6" s="18"/>
       <c r="CW6" s="18"/>
@@ -1248,11 +1258,12 @@
       <c r="DK6" s="19"/>
       <c r="DL6" s="19"/>
       <c r="DM6" s="19"/>
-      <c r="DN6" s="32"/>
-      <c r="DO6" s="32"/>
+      <c r="DN6" s="20"/>
+      <c r="DO6" s="20"/>
+      <c r="DP6" s="34"/>
     </row>
-    <row r="7" spans="1:119" s="2" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A7" s="30"/>
+    <row r="7" spans="1:120" s="2" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A7" s="33"/>
       <c r="B7" s="3" t="s">
         <v>2</v>
       </c>
@@ -1606,15 +1617,13 @@
       </c>
       <c r="DO7" s="8" t="s">
         <v>111</v>
+      </c>
+      <c r="DP7" s="3" t="s">
+        <v>112</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="DN5:DO5"/>
-    <mergeCell ref="BR6:CA6"/>
-    <mergeCell ref="BK5:BQ5"/>
-    <mergeCell ref="Z5:AK5"/>
-    <mergeCell ref="AL5:BJ5"/>
     <mergeCell ref="B5:X5"/>
     <mergeCell ref="BR5:CT5"/>
     <mergeCell ref="DJ5:DM5"/>
@@ -1627,6 +1636,11 @@
     <mergeCell ref="CF6:CH6"/>
     <mergeCell ref="CI6:CR6"/>
     <mergeCell ref="CS6:CT6"/>
+    <mergeCell ref="DN5:DO5"/>
+    <mergeCell ref="BR6:CA6"/>
+    <mergeCell ref="BK5:BQ5"/>
+    <mergeCell ref="Z5:AK5"/>
+    <mergeCell ref="AL5:BJ5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Update menu sidebar detail OAB
</commit_message>
<xml_diff>
--- a/Laravel-InaLUTS/resources/templates/Report_OAB.xlsx
+++ b/Laravel-InaLUTS/resources/templates/Report_OAB.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="123">
   <si>
     <t>No</t>
   </si>
@@ -353,6 +353,36 @@
   </si>
   <si>
     <t>Sistem skor</t>
+  </si>
+  <si>
+    <t>Kuesioner OABSS</t>
+  </si>
+  <si>
+    <t>OABSS</t>
+  </si>
+  <si>
+    <t>QOL</t>
+  </si>
+  <si>
+    <t>IIEF</t>
+  </si>
+  <si>
+    <t>EHS</t>
+  </si>
+  <si>
+    <t>Bladder Diary</t>
+  </si>
+  <si>
+    <t>Kuesioner QOL</t>
+  </si>
+  <si>
+    <t>Kuesioner IIEF</t>
+  </si>
+  <si>
+    <t>Kuesioner EHS</t>
+  </si>
+  <si>
+    <t>Kuesioner Bladder Diary</t>
   </si>
 </sst>
 </file>
@@ -399,7 +429,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="17">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -496,6 +526,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -509,7 +545,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -571,12 +607,42 @@
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -586,31 +652,7 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -914,7 +956,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:DP7"/>
+  <dimension ref="A1:DU7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
@@ -943,195 +985,211 @@
     <col min="42" max="117" width="9.140625" style="1"/>
     <col min="118" max="119" width="15.7109375" style="1" customWidth="1"/>
     <col min="120" max="120" width="12.7109375" style="1" customWidth="1"/>
-    <col min="121" max="16384" width="9.140625" style="1"/>
+    <col min="121" max="125" width="10.7109375" style="1" customWidth="1"/>
+    <col min="126" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:120" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="30"/>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
+    <row r="1" spans="1:125" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="27"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
     </row>
-    <row r="2" spans="1:120" x14ac:dyDescent="0.25">
-      <c r="A2" s="31"/>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
-      <c r="I2" s="31"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="31"/>
+    <row r="2" spans="1:125" x14ac:dyDescent="0.25">
+      <c r="A2" s="28"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="28"/>
+      <c r="K2" s="28"/>
     </row>
-    <row r="3" spans="1:120" x14ac:dyDescent="0.25">
-      <c r="A3" s="32"/>
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
-      <c r="K3" s="32"/>
+    <row r="3" spans="1:125" x14ac:dyDescent="0.25">
+      <c r="A3" s="29"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="29"/>
+      <c r="K3" s="29"/>
     </row>
-    <row r="4" spans="1:120" s="4" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:120" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="33" t="s">
+    <row r="4" spans="1:125" s="4" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:125" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="26" t="s">
+      <c r="B5" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="26"/>
-      <c r="D5" s="26"/>
-      <c r="E5" s="26"/>
-      <c r="F5" s="26"/>
-      <c r="G5" s="26"/>
-      <c r="H5" s="26"/>
-      <c r="I5" s="26"/>
-      <c r="J5" s="26"/>
-      <c r="K5" s="26"/>
-      <c r="L5" s="26"/>
-      <c r="M5" s="26"/>
-      <c r="N5" s="26"/>
-      <c r="O5" s="26"/>
-      <c r="P5" s="26"/>
-      <c r="Q5" s="26"/>
-      <c r="R5" s="26"/>
-      <c r="S5" s="26"/>
-      <c r="T5" s="26"/>
-      <c r="U5" s="26"/>
-      <c r="V5" s="26"/>
-      <c r="W5" s="26"/>
-      <c r="X5" s="26"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="23"/>
+      <c r="I5" s="23"/>
+      <c r="J5" s="23"/>
+      <c r="K5" s="23"/>
+      <c r="L5" s="23"/>
+      <c r="M5" s="23"/>
+      <c r="N5" s="23"/>
+      <c r="O5" s="23"/>
+      <c r="P5" s="23"/>
+      <c r="Q5" s="23"/>
+      <c r="R5" s="23"/>
+      <c r="S5" s="23"/>
+      <c r="T5" s="23"/>
+      <c r="U5" s="23"/>
+      <c r="V5" s="23"/>
+      <c r="W5" s="23"/>
+      <c r="X5" s="23"/>
       <c r="Y5" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="Z5" s="24" t="s">
+      <c r="Z5" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="AA5" s="24"/>
-      <c r="AB5" s="24"/>
-      <c r="AC5" s="24"/>
-      <c r="AD5" s="24"/>
-      <c r="AE5" s="24"/>
-      <c r="AF5" s="24"/>
-      <c r="AG5" s="24"/>
-      <c r="AH5" s="24"/>
-      <c r="AI5" s="24"/>
-      <c r="AJ5" s="24"/>
-      <c r="AK5" s="24"/>
-      <c r="AL5" s="25" t="s">
+      <c r="AA5" s="34"/>
+      <c r="AB5" s="34"/>
+      <c r="AC5" s="34"/>
+      <c r="AD5" s="34"/>
+      <c r="AE5" s="34"/>
+      <c r="AF5" s="34"/>
+      <c r="AG5" s="34"/>
+      <c r="AH5" s="34"/>
+      <c r="AI5" s="34"/>
+      <c r="AJ5" s="34"/>
+      <c r="AK5" s="34"/>
+      <c r="AL5" s="35" t="s">
         <v>40</v>
       </c>
-      <c r="AM5" s="25"/>
-      <c r="AN5" s="25"/>
-      <c r="AO5" s="25"/>
-      <c r="AP5" s="25"/>
-      <c r="AQ5" s="25"/>
-      <c r="AR5" s="25"/>
-      <c r="AS5" s="25"/>
-      <c r="AT5" s="25"/>
-      <c r="AU5" s="25"/>
-      <c r="AV5" s="25"/>
-      <c r="AW5" s="25"/>
-      <c r="AX5" s="25"/>
-      <c r="AY5" s="25"/>
-      <c r="AZ5" s="25"/>
-      <c r="BA5" s="25"/>
-      <c r="BB5" s="25"/>
-      <c r="BC5" s="25"/>
-      <c r="BD5" s="25"/>
-      <c r="BE5" s="25"/>
-      <c r="BF5" s="25"/>
-      <c r="BG5" s="25"/>
-      <c r="BH5" s="25"/>
-      <c r="BI5" s="25"/>
-      <c r="BJ5" s="25"/>
-      <c r="BK5" s="23" t="s">
+      <c r="AM5" s="35"/>
+      <c r="AN5" s="35"/>
+      <c r="AO5" s="35"/>
+      <c r="AP5" s="35"/>
+      <c r="AQ5" s="35"/>
+      <c r="AR5" s="35"/>
+      <c r="AS5" s="35"/>
+      <c r="AT5" s="35"/>
+      <c r="AU5" s="35"/>
+      <c r="AV5" s="35"/>
+      <c r="AW5" s="35"/>
+      <c r="AX5" s="35"/>
+      <c r="AY5" s="35"/>
+      <c r="AZ5" s="35"/>
+      <c r="BA5" s="35"/>
+      <c r="BB5" s="35"/>
+      <c r="BC5" s="35"/>
+      <c r="BD5" s="35"/>
+      <c r="BE5" s="35"/>
+      <c r="BF5" s="35"/>
+      <c r="BG5" s="35"/>
+      <c r="BH5" s="35"/>
+      <c r="BI5" s="35"/>
+      <c r="BJ5" s="35"/>
+      <c r="BK5" s="33" t="s">
         <v>72</v>
       </c>
-      <c r="BL5" s="23"/>
-      <c r="BM5" s="23"/>
-      <c r="BN5" s="23"/>
-      <c r="BO5" s="23"/>
-      <c r="BP5" s="23"/>
-      <c r="BQ5" s="23"/>
-      <c r="BR5" s="27" t="s">
+      <c r="BL5" s="33"/>
+      <c r="BM5" s="33"/>
+      <c r="BN5" s="33"/>
+      <c r="BO5" s="33"/>
+      <c r="BP5" s="33"/>
+      <c r="BQ5" s="33"/>
+      <c r="BR5" s="24" t="s">
         <v>73</v>
       </c>
-      <c r="BS5" s="27"/>
-      <c r="BT5" s="27"/>
-      <c r="BU5" s="27"/>
-      <c r="BV5" s="27"/>
-      <c r="BW5" s="27"/>
-      <c r="BX5" s="27"/>
-      <c r="BY5" s="27"/>
-      <c r="BZ5" s="27"/>
-      <c r="CA5" s="27"/>
-      <c r="CB5" s="27"/>
-      <c r="CC5" s="27"/>
-      <c r="CD5" s="27"/>
-      <c r="CE5" s="27"/>
-      <c r="CF5" s="27"/>
-      <c r="CG5" s="27"/>
-      <c r="CH5" s="27"/>
-      <c r="CI5" s="27"/>
-      <c r="CJ5" s="27"/>
-      <c r="CK5" s="27"/>
-      <c r="CL5" s="27"/>
-      <c r="CM5" s="27"/>
-      <c r="CN5" s="27"/>
-      <c r="CO5" s="27"/>
-      <c r="CP5" s="27"/>
-      <c r="CQ5" s="27"/>
-      <c r="CR5" s="27"/>
-      <c r="CS5" s="27"/>
-      <c r="CT5" s="27"/>
-      <c r="CU5" s="29" t="s">
+      <c r="BS5" s="24"/>
+      <c r="BT5" s="24"/>
+      <c r="BU5" s="24"/>
+      <c r="BV5" s="24"/>
+      <c r="BW5" s="24"/>
+      <c r="BX5" s="24"/>
+      <c r="BY5" s="24"/>
+      <c r="BZ5" s="24"/>
+      <c r="CA5" s="24"/>
+      <c r="CB5" s="24"/>
+      <c r="CC5" s="24"/>
+      <c r="CD5" s="24"/>
+      <c r="CE5" s="24"/>
+      <c r="CF5" s="24"/>
+      <c r="CG5" s="24"/>
+      <c r="CH5" s="24"/>
+      <c r="CI5" s="24"/>
+      <c r="CJ5" s="24"/>
+      <c r="CK5" s="24"/>
+      <c r="CL5" s="24"/>
+      <c r="CM5" s="24"/>
+      <c r="CN5" s="24"/>
+      <c r="CO5" s="24"/>
+      <c r="CP5" s="24"/>
+      <c r="CQ5" s="24"/>
+      <c r="CR5" s="24"/>
+      <c r="CS5" s="24"/>
+      <c r="CT5" s="24"/>
+      <c r="CU5" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="CV5" s="29"/>
-      <c r="CW5" s="29"/>
-      <c r="CX5" s="29"/>
-      <c r="CY5" s="29"/>
-      <c r="CZ5" s="29"/>
-      <c r="DA5" s="29"/>
-      <c r="DB5" s="29"/>
-      <c r="DC5" s="29"/>
-      <c r="DD5" s="29"/>
-      <c r="DE5" s="29"/>
-      <c r="DF5" s="29"/>
-      <c r="DG5" s="29"/>
-      <c r="DH5" s="29"/>
-      <c r="DI5" s="29"/>
-      <c r="DJ5" s="28" t="s">
+      <c r="CV5" s="26"/>
+      <c r="CW5" s="26"/>
+      <c r="CX5" s="26"/>
+      <c r="CY5" s="26"/>
+      <c r="CZ5" s="26"/>
+      <c r="DA5" s="26"/>
+      <c r="DB5" s="26"/>
+      <c r="DC5" s="26"/>
+      <c r="DD5" s="26"/>
+      <c r="DE5" s="26"/>
+      <c r="DF5" s="26"/>
+      <c r="DG5" s="26"/>
+      <c r="DH5" s="26"/>
+      <c r="DI5" s="26"/>
+      <c r="DJ5" s="25" t="s">
         <v>108</v>
       </c>
-      <c r="DK5" s="28"/>
-      <c r="DL5" s="28"/>
-      <c r="DM5" s="28"/>
-      <c r="DN5" s="21" t="s">
+      <c r="DK5" s="25"/>
+      <c r="DL5" s="25"/>
+      <c r="DM5" s="25"/>
+      <c r="DN5" s="32" t="s">
         <v>109</v>
       </c>
-      <c r="DO5" s="21"/>
-      <c r="DP5" s="34" t="s">
+      <c r="DO5" s="32"/>
+      <c r="DP5" s="22" t="s">
         <v>112</v>
       </c>
+      <c r="DQ5" s="21" t="s">
+        <v>113</v>
+      </c>
+      <c r="DR5" s="21" t="s">
+        <v>119</v>
+      </c>
+      <c r="DS5" s="21" t="s">
+        <v>120</v>
+      </c>
+      <c r="DT5" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="DU5" s="21" t="s">
+        <v>122</v>
+      </c>
     </row>
-    <row r="6" spans="1:120" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="33"/>
+    <row r="6" spans="1:125" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="30"/>
       <c r="B6" s="13"/>
       <c r="C6" s="13"/>
       <c r="D6" s="13"/>
@@ -1200,45 +1258,45 @@
       <c r="BO6" s="14"/>
       <c r="BP6" s="14"/>
       <c r="BQ6" s="14"/>
-      <c r="BR6" s="22" t="s">
+      <c r="BR6" s="31" t="s">
         <v>75</v>
       </c>
-      <c r="BS6" s="22"/>
-      <c r="BT6" s="22"/>
-      <c r="BU6" s="22"/>
-      <c r="BV6" s="22"/>
-      <c r="BW6" s="22"/>
-      <c r="BX6" s="22"/>
-      <c r="BY6" s="22"/>
-      <c r="BZ6" s="22"/>
-      <c r="CA6" s="22"/>
-      <c r="CB6" s="22" t="s">
+      <c r="BS6" s="31"/>
+      <c r="BT6" s="31"/>
+      <c r="BU6" s="31"/>
+      <c r="BV6" s="31"/>
+      <c r="BW6" s="31"/>
+      <c r="BX6" s="31"/>
+      <c r="BY6" s="31"/>
+      <c r="BZ6" s="31"/>
+      <c r="CA6" s="31"/>
+      <c r="CB6" s="31" t="s">
         <v>80</v>
       </c>
-      <c r="CC6" s="22"/>
-      <c r="CD6" s="22"/>
-      <c r="CE6" s="22"/>
-      <c r="CF6" s="22" t="s">
+      <c r="CC6" s="31"/>
+      <c r="CD6" s="31"/>
+      <c r="CE6" s="31"/>
+      <c r="CF6" s="31" t="s">
         <v>83</v>
       </c>
-      <c r="CG6" s="22"/>
-      <c r="CH6" s="22"/>
-      <c r="CI6" s="22" t="s">
+      <c r="CG6" s="31"/>
+      <c r="CH6" s="31"/>
+      <c r="CI6" s="31" t="s">
         <v>86</v>
       </c>
-      <c r="CJ6" s="22"/>
-      <c r="CK6" s="22"/>
-      <c r="CL6" s="22"/>
-      <c r="CM6" s="22"/>
-      <c r="CN6" s="22"/>
-      <c r="CO6" s="22"/>
-      <c r="CP6" s="22"/>
-      <c r="CQ6" s="22"/>
-      <c r="CR6" s="22"/>
-      <c r="CS6" s="22" t="s">
+      <c r="CJ6" s="31"/>
+      <c r="CK6" s="31"/>
+      <c r="CL6" s="31"/>
+      <c r="CM6" s="31"/>
+      <c r="CN6" s="31"/>
+      <c r="CO6" s="31"/>
+      <c r="CP6" s="31"/>
+      <c r="CQ6" s="31"/>
+      <c r="CR6" s="31"/>
+      <c r="CS6" s="31" t="s">
         <v>92</v>
       </c>
-      <c r="CT6" s="22"/>
+      <c r="CT6" s="31"/>
       <c r="CU6" s="18"/>
       <c r="CV6" s="18"/>
       <c r="CW6" s="18"/>
@@ -1260,10 +1318,15 @@
       <c r="DM6" s="19"/>
       <c r="DN6" s="20"/>
       <c r="DO6" s="20"/>
-      <c r="DP6" s="34"/>
+      <c r="DP6" s="22"/>
+      <c r="DQ6" s="21"/>
+      <c r="DR6" s="21"/>
+      <c r="DS6" s="21"/>
+      <c r="DT6" s="21"/>
+      <c r="DU6" s="21"/>
     </row>
-    <row r="7" spans="1:120" s="2" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A7" s="33"/>
+    <row r="7" spans="1:125" s="2" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A7" s="30"/>
       <c r="B7" s="3" t="s">
         <v>2</v>
       </c>
@@ -1620,10 +1683,30 @@
       </c>
       <c r="DP7" s="3" t="s">
         <v>112</v>
+      </c>
+      <c r="DQ7" s="36" t="s">
+        <v>114</v>
+      </c>
+      <c r="DR7" s="36" t="s">
+        <v>115</v>
+      </c>
+      <c r="DS7" s="36" t="s">
+        <v>116</v>
+      </c>
+      <c r="DT7" s="36" t="s">
+        <v>117</v>
+      </c>
+      <c r="DU7" s="36" t="s">
+        <v>118</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="DN5:DO5"/>
+    <mergeCell ref="BR6:CA6"/>
+    <mergeCell ref="BK5:BQ5"/>
+    <mergeCell ref="Z5:AK5"/>
+    <mergeCell ref="AL5:BJ5"/>
     <mergeCell ref="B5:X5"/>
     <mergeCell ref="BR5:CT5"/>
     <mergeCell ref="DJ5:DM5"/>
@@ -1636,11 +1719,6 @@
     <mergeCell ref="CF6:CH6"/>
     <mergeCell ref="CI6:CR6"/>
     <mergeCell ref="CS6:CT6"/>
-    <mergeCell ref="DN5:DO5"/>
-    <mergeCell ref="BR6:CA6"/>
-    <mergeCell ref="BK5:BQ5"/>
-    <mergeCell ref="Z5:AK5"/>
-    <mergeCell ref="AL5:BJ5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
OAB : Laporan Pemeriksaan Fisik
</commit_message>
<xml_diff>
--- a/Laravel-InaLUTS/resources/templates/Report_OAB.xlsx
+++ b/Laravel-InaLUTS/resources/templates/Report_OAB.xlsx
@@ -617,136 +617,130 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1051,842 +1045,842 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:EN7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="DP1" workbookViewId="0">
-      <selection activeCell="EN7" sqref="EN7"/>
+    <sheetView tabSelected="1" topLeftCell="DO1" workbookViewId="0">
+      <selection activeCell="EN8" sqref="EN8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="20.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.7109375" style="1" customWidth="1"/>
-    <col min="9" max="10" width="15.7109375" style="1" customWidth="1"/>
-    <col min="11" max="11" width="20.7109375" style="1" customWidth="1"/>
-    <col min="12" max="12" width="16.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="12.7109375" style="1" customWidth="1"/>
-    <col min="15" max="16" width="10.7109375" style="1" customWidth="1"/>
-    <col min="17" max="17" width="8.7109375" style="1" customWidth="1"/>
-    <col min="18" max="25" width="15.7109375" style="1" customWidth="1"/>
-    <col min="26" max="37" width="10.7109375" style="1" customWidth="1"/>
-    <col min="38" max="40" width="9.140625" style="1"/>
-    <col min="41" max="41" width="18" style="1" bestFit="1" customWidth="1"/>
-    <col min="42" max="117" width="9.140625" style="1"/>
-    <col min="118" max="119" width="15.7109375" style="1" customWidth="1"/>
-    <col min="120" max="120" width="12.7109375" style="1" customWidth="1"/>
-    <col min="121" max="125" width="10.7109375" style="1" customWidth="1"/>
-    <col min="126" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="4.7109375" style="19" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" style="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" style="19" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" style="19" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" style="19" customWidth="1"/>
+    <col min="6" max="6" width="20.7109375" style="19" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" style="19" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" style="19" customWidth="1"/>
+    <col min="9" max="10" width="15.7109375" style="19" customWidth="1"/>
+    <col min="11" max="11" width="20.7109375" style="19" customWidth="1"/>
+    <col min="12" max="12" width="16.85546875" style="19" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="12.7109375" style="19" customWidth="1"/>
+    <col min="15" max="16" width="10.7109375" style="19" customWidth="1"/>
+    <col min="17" max="17" width="8.7109375" style="19" customWidth="1"/>
+    <col min="18" max="25" width="15.7109375" style="19" customWidth="1"/>
+    <col min="26" max="37" width="10.7109375" style="19" customWidth="1"/>
+    <col min="38" max="40" width="9.140625" style="19"/>
+    <col min="41" max="41" width="18" style="19" bestFit="1" customWidth="1"/>
+    <col min="42" max="117" width="9.140625" style="19"/>
+    <col min="118" max="119" width="15.7109375" style="19" customWidth="1"/>
+    <col min="120" max="120" width="12.7109375" style="19" customWidth="1"/>
+    <col min="121" max="125" width="10.7109375" style="19" customWidth="1"/>
+    <col min="126" max="16384" width="9.140625" style="19"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:144" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="32"/>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
-      <c r="K1" s="32"/>
+      <c r="A1" s="35"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="35"/>
     </row>
     <row r="2" spans="1:144" x14ac:dyDescent="0.25">
-      <c r="A2" s="33"/>
-      <c r="B2" s="33"/>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
-      <c r="I2" s="33"/>
-      <c r="J2" s="33"/>
-      <c r="K2" s="33"/>
+      <c r="A2" s="36"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36"/>
+      <c r="J2" s="36"/>
+      <c r="K2" s="36"/>
     </row>
     <row r="3" spans="1:144" x14ac:dyDescent="0.25">
-      <c r="A3" s="34"/>
-      <c r="B3" s="34"/>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
-      <c r="F3" s="34"/>
-      <c r="G3" s="34"/>
-      <c r="H3" s="34"/>
-      <c r="I3" s="34"/>
-      <c r="J3" s="34"/>
-      <c r="K3" s="34"/>
+      <c r="A3" s="37"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="37"/>
+      <c r="J3" s="37"/>
+      <c r="K3" s="37"/>
     </row>
-    <row r="4" spans="1:144" s="4" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:144" s="2" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="35" t="s">
+    <row r="4" spans="1:144" s="3" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:144" s="1" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="28" t="s">
+      <c r="B5" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="28"/>
-      <c r="D5" s="28"/>
-      <c r="E5" s="28"/>
-      <c r="F5" s="28"/>
-      <c r="G5" s="28"/>
-      <c r="H5" s="28"/>
-      <c r="I5" s="28"/>
-      <c r="J5" s="28"/>
-      <c r="K5" s="28"/>
-      <c r="L5" s="28"/>
-      <c r="M5" s="28"/>
-      <c r="N5" s="28"/>
-      <c r="O5" s="28"/>
-      <c r="P5" s="28"/>
-      <c r="Q5" s="28"/>
-      <c r="R5" s="28"/>
-      <c r="S5" s="28"/>
-      <c r="T5" s="28"/>
-      <c r="U5" s="28"/>
-      <c r="V5" s="28"/>
-      <c r="W5" s="28"/>
-      <c r="X5" s="28"/>
-      <c r="Y5" s="6" t="s">
+      <c r="C5" s="39"/>
+      <c r="D5" s="39"/>
+      <c r="E5" s="39"/>
+      <c r="F5" s="39"/>
+      <c r="G5" s="39"/>
+      <c r="H5" s="39"/>
+      <c r="I5" s="39"/>
+      <c r="J5" s="39"/>
+      <c r="K5" s="39"/>
+      <c r="L5" s="39"/>
+      <c r="M5" s="39"/>
+      <c r="N5" s="39"/>
+      <c r="O5" s="39"/>
+      <c r="P5" s="39"/>
+      <c r="Q5" s="39"/>
+      <c r="R5" s="39"/>
+      <c r="S5" s="39"/>
+      <c r="T5" s="39"/>
+      <c r="U5" s="39"/>
+      <c r="V5" s="39"/>
+      <c r="W5" s="39"/>
+      <c r="X5" s="39"/>
+      <c r="Y5" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="Z5" s="39" t="s">
+      <c r="Z5" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="AA5" s="39"/>
-      <c r="AB5" s="39"/>
-      <c r="AC5" s="39"/>
-      <c r="AD5" s="39"/>
-      <c r="AE5" s="39"/>
-      <c r="AF5" s="39"/>
-      <c r="AG5" s="39"/>
-      <c r="AH5" s="39"/>
-      <c r="AI5" s="39"/>
-      <c r="AJ5" s="39"/>
-      <c r="AK5" s="39"/>
-      <c r="AL5" s="40" t="s">
+      <c r="AA5" s="29"/>
+      <c r="AB5" s="29"/>
+      <c r="AC5" s="29"/>
+      <c r="AD5" s="29"/>
+      <c r="AE5" s="29"/>
+      <c r="AF5" s="29"/>
+      <c r="AG5" s="29"/>
+      <c r="AH5" s="29"/>
+      <c r="AI5" s="29"/>
+      <c r="AJ5" s="29"/>
+      <c r="AK5" s="29"/>
+      <c r="AL5" s="30" t="s">
         <v>40</v>
       </c>
-      <c r="AM5" s="40"/>
-      <c r="AN5" s="40"/>
-      <c r="AO5" s="40"/>
-      <c r="AP5" s="40"/>
-      <c r="AQ5" s="40"/>
-      <c r="AR5" s="40"/>
-      <c r="AS5" s="40"/>
-      <c r="AT5" s="40"/>
-      <c r="AU5" s="40"/>
-      <c r="AV5" s="40"/>
-      <c r="AW5" s="40"/>
-      <c r="AX5" s="40"/>
-      <c r="AY5" s="40"/>
-      <c r="AZ5" s="40"/>
-      <c r="BA5" s="40"/>
-      <c r="BB5" s="40"/>
-      <c r="BC5" s="40"/>
-      <c r="BD5" s="40"/>
-      <c r="BE5" s="40"/>
-      <c r="BF5" s="40"/>
-      <c r="BG5" s="40"/>
-      <c r="BH5" s="40"/>
-      <c r="BI5" s="40"/>
-      <c r="BJ5" s="40"/>
-      <c r="BK5" s="38" t="s">
+      <c r="AM5" s="30"/>
+      <c r="AN5" s="30"/>
+      <c r="AO5" s="30"/>
+      <c r="AP5" s="30"/>
+      <c r="AQ5" s="30"/>
+      <c r="AR5" s="30"/>
+      <c r="AS5" s="30"/>
+      <c r="AT5" s="30"/>
+      <c r="AU5" s="30"/>
+      <c r="AV5" s="30"/>
+      <c r="AW5" s="30"/>
+      <c r="AX5" s="30"/>
+      <c r="AY5" s="30"/>
+      <c r="AZ5" s="30"/>
+      <c r="BA5" s="30"/>
+      <c r="BB5" s="30"/>
+      <c r="BC5" s="30"/>
+      <c r="BD5" s="30"/>
+      <c r="BE5" s="30"/>
+      <c r="BF5" s="30"/>
+      <c r="BG5" s="30"/>
+      <c r="BH5" s="30"/>
+      <c r="BI5" s="30"/>
+      <c r="BJ5" s="30"/>
+      <c r="BK5" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="BL5" s="38"/>
-      <c r="BM5" s="38"/>
-      <c r="BN5" s="38"/>
-      <c r="BO5" s="38"/>
-      <c r="BP5" s="38"/>
-      <c r="BQ5" s="38"/>
-      <c r="BR5" s="29" t="s">
+      <c r="BL5" s="28"/>
+      <c r="BM5" s="28"/>
+      <c r="BN5" s="28"/>
+      <c r="BO5" s="28"/>
+      <c r="BP5" s="28"/>
+      <c r="BQ5" s="28"/>
+      <c r="BR5" s="32" t="s">
         <v>73</v>
       </c>
-      <c r="BS5" s="29"/>
-      <c r="BT5" s="29"/>
-      <c r="BU5" s="29"/>
-      <c r="BV5" s="29"/>
-      <c r="BW5" s="29"/>
-      <c r="BX5" s="29"/>
-      <c r="BY5" s="29"/>
-      <c r="BZ5" s="29"/>
-      <c r="CA5" s="29"/>
-      <c r="CB5" s="29"/>
-      <c r="CC5" s="29"/>
-      <c r="CD5" s="29"/>
-      <c r="CE5" s="29"/>
-      <c r="CF5" s="29"/>
-      <c r="CG5" s="29"/>
-      <c r="CH5" s="29"/>
-      <c r="CI5" s="29"/>
-      <c r="CJ5" s="29"/>
-      <c r="CK5" s="29"/>
-      <c r="CL5" s="29"/>
-      <c r="CM5" s="29"/>
-      <c r="CN5" s="29"/>
-      <c r="CO5" s="29"/>
-      <c r="CP5" s="29"/>
-      <c r="CQ5" s="29"/>
-      <c r="CR5" s="29"/>
-      <c r="CS5" s="29"/>
-      <c r="CT5" s="29"/>
-      <c r="CU5" s="31" t="s">
+      <c r="BS5" s="32"/>
+      <c r="BT5" s="32"/>
+      <c r="BU5" s="32"/>
+      <c r="BV5" s="32"/>
+      <c r="BW5" s="32"/>
+      <c r="BX5" s="32"/>
+      <c r="BY5" s="32"/>
+      <c r="BZ5" s="32"/>
+      <c r="CA5" s="32"/>
+      <c r="CB5" s="32"/>
+      <c r="CC5" s="32"/>
+      <c r="CD5" s="32"/>
+      <c r="CE5" s="32"/>
+      <c r="CF5" s="32"/>
+      <c r="CG5" s="32"/>
+      <c r="CH5" s="32"/>
+      <c r="CI5" s="32"/>
+      <c r="CJ5" s="32"/>
+      <c r="CK5" s="32"/>
+      <c r="CL5" s="32"/>
+      <c r="CM5" s="32"/>
+      <c r="CN5" s="32"/>
+      <c r="CO5" s="32"/>
+      <c r="CP5" s="32"/>
+      <c r="CQ5" s="32"/>
+      <c r="CR5" s="32"/>
+      <c r="CS5" s="32"/>
+      <c r="CT5" s="32"/>
+      <c r="CU5" s="34" t="s">
         <v>94</v>
       </c>
-      <c r="CV5" s="31"/>
-      <c r="CW5" s="31"/>
-      <c r="CX5" s="31"/>
-      <c r="CY5" s="31"/>
-      <c r="CZ5" s="31"/>
-      <c r="DA5" s="31"/>
-      <c r="DB5" s="31"/>
-      <c r="DC5" s="31"/>
-      <c r="DD5" s="31"/>
-      <c r="DE5" s="31"/>
-      <c r="DF5" s="31"/>
-      <c r="DG5" s="31"/>
-      <c r="DH5" s="31"/>
-      <c r="DI5" s="31"/>
-      <c r="DJ5" s="30" t="s">
+      <c r="CV5" s="34"/>
+      <c r="CW5" s="34"/>
+      <c r="CX5" s="34"/>
+      <c r="CY5" s="34"/>
+      <c r="CZ5" s="34"/>
+      <c r="DA5" s="34"/>
+      <c r="DB5" s="34"/>
+      <c r="DC5" s="34"/>
+      <c r="DD5" s="34"/>
+      <c r="DE5" s="34"/>
+      <c r="DF5" s="34"/>
+      <c r="DG5" s="34"/>
+      <c r="DH5" s="34"/>
+      <c r="DI5" s="34"/>
+      <c r="DJ5" s="33" t="s">
         <v>108</v>
       </c>
-      <c r="DK5" s="30"/>
-      <c r="DL5" s="30"/>
-      <c r="DM5" s="30"/>
-      <c r="DN5" s="37" t="s">
+      <c r="DK5" s="33"/>
+      <c r="DL5" s="33"/>
+      <c r="DM5" s="33"/>
+      <c r="DN5" s="41" t="s">
         <v>109</v>
       </c>
-      <c r="DO5" s="37"/>
-      <c r="DP5" s="23" t="s">
+      <c r="DO5" s="41"/>
+      <c r="DP5" s="17" t="s">
         <v>112</v>
       </c>
-      <c r="DQ5" s="26" t="s">
+      <c r="DQ5" s="16" t="s">
         <v>113</v>
       </c>
-      <c r="DR5" s="26" t="s">
+      <c r="DR5" s="16" t="s">
         <v>118</v>
       </c>
-      <c r="DS5" s="26" t="s">
+      <c r="DS5" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="DT5" s="26" t="s">
+      <c r="DT5" s="16" t="s">
         <v>120</v>
       </c>
-      <c r="DU5" s="27" t="s">
+      <c r="DU5" s="31" t="s">
         <v>121</v>
       </c>
-      <c r="DV5" s="27"/>
-      <c r="DW5" s="27"/>
-      <c r="DX5" s="27"/>
-      <c r="DY5" s="27"/>
-      <c r="DZ5" s="27"/>
-      <c r="EA5" s="27"/>
-      <c r="EB5" s="27"/>
-      <c r="EC5" s="42" t="s">
+      <c r="DV5" s="31"/>
+      <c r="DW5" s="31"/>
+      <c r="DX5" s="31"/>
+      <c r="DY5" s="31"/>
+      <c r="DZ5" s="31"/>
+      <c r="EA5" s="31"/>
+      <c r="EB5" s="31"/>
+      <c r="EC5" s="40" t="s">
         <v>130</v>
       </c>
-      <c r="ED5" s="42"/>
-      <c r="EE5" s="42"/>
-      <c r="EF5" s="42"/>
-      <c r="EG5" s="42"/>
-      <c r="EH5" s="42"/>
-      <c r="EI5" s="42"/>
-      <c r="EJ5" s="42"/>
-      <c r="EK5" s="42"/>
-      <c r="EL5" s="42"/>
-      <c r="EM5" s="42"/>
-      <c r="EN5" s="42"/>
+      <c r="ED5" s="40"/>
+      <c r="EE5" s="40"/>
+      <c r="EF5" s="40"/>
+      <c r="EG5" s="40"/>
+      <c r="EH5" s="40"/>
+      <c r="EI5" s="40"/>
+      <c r="EJ5" s="40"/>
+      <c r="EK5" s="40"/>
+      <c r="EL5" s="40"/>
+      <c r="EM5" s="40"/>
+      <c r="EN5" s="40"/>
     </row>
-    <row r="6" spans="1:144" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="35"/>
-      <c r="B6" s="13"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="13"/>
-      <c r="I6" s="13"/>
-      <c r="J6" s="13"/>
-      <c r="K6" s="13"/>
-      <c r="L6" s="13"/>
-      <c r="M6" s="13"/>
-      <c r="N6" s="13"/>
-      <c r="O6" s="13"/>
-      <c r="P6" s="13"/>
-      <c r="Q6" s="13"/>
-      <c r="R6" s="13"/>
-      <c r="S6" s="13"/>
-      <c r="T6" s="13"/>
-      <c r="U6" s="13"/>
-      <c r="V6" s="13"/>
-      <c r="W6" s="13"/>
-      <c r="X6" s="13"/>
-      <c r="Y6" s="6"/>
-      <c r="Z6" s="11"/>
-      <c r="AA6" s="11"/>
-      <c r="AB6" s="11"/>
-      <c r="AC6" s="11"/>
-      <c r="AD6" s="11"/>
-      <c r="AE6" s="11"/>
-      <c r="AF6" s="11"/>
-      <c r="AG6" s="11"/>
-      <c r="AH6" s="11"/>
-      <c r="AI6" s="11"/>
-      <c r="AJ6" s="11"/>
-      <c r="AK6" s="11"/>
-      <c r="AL6" s="12"/>
-      <c r="AM6" s="12"/>
-      <c r="AN6" s="12"/>
-      <c r="AO6" s="12"/>
-      <c r="AP6" s="12"/>
-      <c r="AQ6" s="12"/>
-      <c r="AR6" s="12"/>
-      <c r="AS6" s="12"/>
-      <c r="AT6" s="12"/>
-      <c r="AU6" s="12"/>
-      <c r="AV6" s="12"/>
-      <c r="AW6" s="12"/>
-      <c r="AX6" s="12"/>
-      <c r="AY6" s="12"/>
-      <c r="AZ6" s="12"/>
-      <c r="BA6" s="12"/>
-      <c r="BB6" s="12"/>
-      <c r="BC6" s="12"/>
-      <c r="BD6" s="12"/>
-      <c r="BE6" s="12"/>
-      <c r="BF6" s="12"/>
-      <c r="BG6" s="12"/>
-      <c r="BH6" s="12"/>
-      <c r="BI6" s="12"/>
-      <c r="BJ6" s="12"/>
-      <c r="BK6" s="14"/>
-      <c r="BL6" s="14"/>
-      <c r="BM6" s="14"/>
-      <c r="BN6" s="14"/>
-      <c r="BO6" s="14"/>
-      <c r="BP6" s="14"/>
-      <c r="BQ6" s="14"/>
-      <c r="BR6" s="36" t="s">
+    <row r="6" spans="1:144" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="38"/>
+      <c r="B6" s="17"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="17"/>
+      <c r="J6" s="17"/>
+      <c r="K6" s="17"/>
+      <c r="L6" s="17"/>
+      <c r="M6" s="17"/>
+      <c r="N6" s="17"/>
+      <c r="O6" s="17"/>
+      <c r="P6" s="17"/>
+      <c r="Q6" s="17"/>
+      <c r="R6" s="17"/>
+      <c r="S6" s="17"/>
+      <c r="T6" s="17"/>
+      <c r="U6" s="17"/>
+      <c r="V6" s="17"/>
+      <c r="W6" s="17"/>
+      <c r="X6" s="17"/>
+      <c r="Y6" s="18"/>
+      <c r="Z6" s="22"/>
+      <c r="AA6" s="22"/>
+      <c r="AB6" s="22"/>
+      <c r="AC6" s="22"/>
+      <c r="AD6" s="22"/>
+      <c r="AE6" s="22"/>
+      <c r="AF6" s="22"/>
+      <c r="AG6" s="22"/>
+      <c r="AH6" s="22"/>
+      <c r="AI6" s="22"/>
+      <c r="AJ6" s="22"/>
+      <c r="AK6" s="22"/>
+      <c r="AL6" s="23"/>
+      <c r="AM6" s="23"/>
+      <c r="AN6" s="23"/>
+      <c r="AO6" s="23"/>
+      <c r="AP6" s="23"/>
+      <c r="AQ6" s="23"/>
+      <c r="AR6" s="23"/>
+      <c r="AS6" s="23"/>
+      <c r="AT6" s="23"/>
+      <c r="AU6" s="23"/>
+      <c r="AV6" s="23"/>
+      <c r="AW6" s="23"/>
+      <c r="AX6" s="23"/>
+      <c r="AY6" s="23"/>
+      <c r="AZ6" s="23"/>
+      <c r="BA6" s="23"/>
+      <c r="BB6" s="23"/>
+      <c r="BC6" s="23"/>
+      <c r="BD6" s="23"/>
+      <c r="BE6" s="23"/>
+      <c r="BF6" s="23"/>
+      <c r="BG6" s="23"/>
+      <c r="BH6" s="23"/>
+      <c r="BI6" s="23"/>
+      <c r="BJ6" s="23"/>
+      <c r="BK6" s="21"/>
+      <c r="BL6" s="21"/>
+      <c r="BM6" s="21"/>
+      <c r="BN6" s="21"/>
+      <c r="BO6" s="21"/>
+      <c r="BP6" s="21"/>
+      <c r="BQ6" s="21"/>
+      <c r="BR6" s="27" t="s">
         <v>75</v>
       </c>
-      <c r="BS6" s="36"/>
-      <c r="BT6" s="36"/>
-      <c r="BU6" s="36"/>
-      <c r="BV6" s="36"/>
-      <c r="BW6" s="36"/>
-      <c r="BX6" s="36"/>
-      <c r="BY6" s="36"/>
-      <c r="BZ6" s="36"/>
-      <c r="CA6" s="36"/>
-      <c r="CB6" s="36" t="s">
+      <c r="BS6" s="27"/>
+      <c r="BT6" s="27"/>
+      <c r="BU6" s="27"/>
+      <c r="BV6" s="27"/>
+      <c r="BW6" s="27"/>
+      <c r="BX6" s="27"/>
+      <c r="BY6" s="27"/>
+      <c r="BZ6" s="27"/>
+      <c r="CA6" s="27"/>
+      <c r="CB6" s="27" t="s">
         <v>80</v>
       </c>
-      <c r="CC6" s="36"/>
-      <c r="CD6" s="36"/>
-      <c r="CE6" s="36"/>
-      <c r="CF6" s="36" t="s">
+      <c r="CC6" s="27"/>
+      <c r="CD6" s="27"/>
+      <c r="CE6" s="27"/>
+      <c r="CF6" s="27" t="s">
         <v>83</v>
       </c>
-      <c r="CG6" s="36"/>
-      <c r="CH6" s="36"/>
-      <c r="CI6" s="36" t="s">
+      <c r="CG6" s="27"/>
+      <c r="CH6" s="27"/>
+      <c r="CI6" s="27" t="s">
         <v>86</v>
       </c>
-      <c r="CJ6" s="36"/>
-      <c r="CK6" s="36"/>
-      <c r="CL6" s="36"/>
-      <c r="CM6" s="36"/>
-      <c r="CN6" s="36"/>
-      <c r="CO6" s="36"/>
-      <c r="CP6" s="36"/>
-      <c r="CQ6" s="36"/>
-      <c r="CR6" s="36"/>
-      <c r="CS6" s="36" t="s">
+      <c r="CJ6" s="27"/>
+      <c r="CK6" s="27"/>
+      <c r="CL6" s="27"/>
+      <c r="CM6" s="27"/>
+      <c r="CN6" s="27"/>
+      <c r="CO6" s="27"/>
+      <c r="CP6" s="27"/>
+      <c r="CQ6" s="27"/>
+      <c r="CR6" s="27"/>
+      <c r="CS6" s="27" t="s">
         <v>92</v>
       </c>
-      <c r="CT6" s="36"/>
-      <c r="CU6" s="18"/>
-      <c r="CV6" s="18"/>
-      <c r="CW6" s="18"/>
-      <c r="CX6" s="18"/>
-      <c r="CY6" s="18"/>
-      <c r="CZ6" s="18"/>
-      <c r="DA6" s="18"/>
-      <c r="DB6" s="18"/>
-      <c r="DC6" s="18"/>
-      <c r="DD6" s="18"/>
-      <c r="DE6" s="18"/>
-      <c r="DF6" s="18"/>
-      <c r="DG6" s="18"/>
-      <c r="DH6" s="18"/>
-      <c r="DI6" s="18"/>
-      <c r="DJ6" s="19"/>
-      <c r="DK6" s="19"/>
-      <c r="DL6" s="19"/>
-      <c r="DM6" s="19"/>
-      <c r="DN6" s="20"/>
-      <c r="DO6" s="20"/>
-      <c r="DP6" s="22"/>
-      <c r="DQ6" s="21"/>
-      <c r="DR6" s="21"/>
-      <c r="DS6" s="21"/>
-      <c r="DT6" s="21"/>
-      <c r="DU6" s="21"/>
-      <c r="DV6" s="24"/>
-      <c r="DW6" s="24"/>
-      <c r="DX6" s="24"/>
-      <c r="DY6" s="24"/>
-      <c r="DZ6" s="24"/>
-      <c r="EA6" s="24"/>
-      <c r="EB6" s="24"/>
-      <c r="EC6" s="43"/>
-      <c r="ED6" s="43"/>
-      <c r="EE6" s="43"/>
-      <c r="EF6" s="43"/>
-      <c r="EG6" s="43"/>
-      <c r="EH6" s="43"/>
-      <c r="EI6" s="43"/>
-      <c r="EJ6" s="43"/>
-      <c r="EK6" s="43"/>
-      <c r="EL6" s="43"/>
-      <c r="EM6" s="43"/>
-      <c r="EN6" s="43"/>
+      <c r="CT6" s="27"/>
+      <c r="CU6" s="11"/>
+      <c r="CV6" s="11"/>
+      <c r="CW6" s="11"/>
+      <c r="CX6" s="11"/>
+      <c r="CY6" s="11"/>
+      <c r="CZ6" s="11"/>
+      <c r="DA6" s="11"/>
+      <c r="DB6" s="11"/>
+      <c r="DC6" s="11"/>
+      <c r="DD6" s="11"/>
+      <c r="DE6" s="11"/>
+      <c r="DF6" s="11"/>
+      <c r="DG6" s="11"/>
+      <c r="DH6" s="11"/>
+      <c r="DI6" s="11"/>
+      <c r="DJ6" s="12"/>
+      <c r="DK6" s="12"/>
+      <c r="DL6" s="12"/>
+      <c r="DM6" s="12"/>
+      <c r="DN6" s="13"/>
+      <c r="DO6" s="13"/>
+      <c r="DP6" s="14"/>
+      <c r="DQ6" s="20"/>
+      <c r="DR6" s="20"/>
+      <c r="DS6" s="20"/>
+      <c r="DT6" s="20"/>
+      <c r="DU6" s="20"/>
+      <c r="DV6" s="20"/>
+      <c r="DW6" s="20"/>
+      <c r="DX6" s="20"/>
+      <c r="DY6" s="20"/>
+      <c r="DZ6" s="20"/>
+      <c r="EA6" s="20"/>
+      <c r="EB6" s="20"/>
+      <c r="EC6" s="25"/>
+      <c r="ED6" s="25"/>
+      <c r="EE6" s="25"/>
+      <c r="EF6" s="25"/>
+      <c r="EG6" s="25"/>
+      <c r="EH6" s="25"/>
+      <c r="EI6" s="25"/>
+      <c r="EJ6" s="25"/>
+      <c r="EK6" s="25"/>
+      <c r="EL6" s="25"/>
+      <c r="EM6" s="25"/>
+      <c r="EN6" s="25"/>
     </row>
-    <row r="7" spans="1:144" s="2" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A7" s="35"/>
-      <c r="B7" s="3" t="s">
+    <row r="7" spans="1:144" s="1" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A7" s="38"/>
+      <c r="B7" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="G7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="H7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I7" s="3" t="s">
+      <c r="I7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="J7" s="3" t="s">
+      <c r="J7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="K7" s="3" t="s">
+      <c r="K7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="L7" s="3" t="s">
+      <c r="L7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="M7" s="3" t="s">
+      <c r="M7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="N7" s="3" t="s">
+      <c r="N7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="O7" s="3" t="s">
+      <c r="O7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="P7" s="3" t="s">
+      <c r="P7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="Q7" s="3" t="s">
+      <c r="Q7" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="R7" s="3" t="s">
+      <c r="R7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="S7" s="3" t="s">
+      <c r="S7" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="T7" s="3" t="s">
+      <c r="T7" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="U7" s="3" t="s">
+      <c r="U7" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="V7" s="3" t="s">
+      <c r="V7" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="W7" s="3" t="s">
+      <c r="W7" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="X7" s="3" t="s">
+      <c r="X7" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="Y7" s="5" t="s">
+      <c r="Y7" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="Z7" s="8" t="s">
+      <c r="Z7" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="AA7" s="8" t="s">
+      <c r="AA7" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="AB7" s="8" t="s">
+      <c r="AB7" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="AC7" s="8" t="s">
+      <c r="AC7" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="AD7" s="8" t="s">
+      <c r="AD7" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="AE7" s="8" t="s">
+      <c r="AE7" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="AF7" s="8" t="s">
+      <c r="AF7" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="AG7" s="8" t="s">
+      <c r="AG7" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="AH7" s="8" t="s">
+      <c r="AH7" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="AI7" s="8" t="s">
+      <c r="AI7" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="AJ7" s="8" t="s">
+      <c r="AJ7" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="AK7" s="8" t="s">
+      <c r="AK7" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="AL7" s="7" t="s">
+      <c r="AL7" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="AM7" s="7" t="s">
+      <c r="AM7" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="AN7" s="7" t="s">
+      <c r="AN7" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="AO7" s="10" t="s">
+      <c r="AO7" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="AP7" s="7" t="s">
+      <c r="AP7" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="AQ7" s="7" t="s">
+      <c r="AQ7" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="AR7" s="7" t="s">
+      <c r="AR7" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="AS7" s="7" t="s">
+      <c r="AS7" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="AT7" s="7" t="s">
+      <c r="AT7" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="AU7" s="7" t="s">
+      <c r="AU7" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="AV7" s="7" t="s">
+      <c r="AV7" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="AW7" s="7" t="s">
+      <c r="AW7" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="AX7" s="7" t="s">
+      <c r="AX7" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="AY7" s="7" t="s">
+      <c r="AY7" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="AZ7" s="9" t="s">
+      <c r="AZ7" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="BA7" s="9" t="s">
+      <c r="BA7" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="BB7" s="9" t="s">
+      <c r="BB7" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="BC7" s="9" t="s">
+      <c r="BC7" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="BD7" s="9" t="s">
+      <c r="BD7" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="BE7" s="9" t="s">
+      <c r="BE7" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="BF7" s="9" t="s">
+      <c r="BF7" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="BG7" s="9" t="s">
+      <c r="BG7" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="BH7" s="9" t="s">
+      <c r="BH7" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="BI7" s="9" t="s">
+      <c r="BI7" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="BJ7" s="9" t="s">
+      <c r="BJ7" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="BK7" s="15" t="s">
+      <c r="BK7" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="BL7" s="15" t="s">
+      <c r="BL7" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="BM7" s="15" t="s">
+      <c r="BM7" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="BN7" s="15" t="s">
+      <c r="BN7" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="BO7" s="15" t="s">
+      <c r="BO7" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="BP7" s="15" t="s">
+      <c r="BP7" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="BQ7" s="15" t="s">
+      <c r="BQ7" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="BR7" s="16" t="s">
+      <c r="BR7" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="BS7" s="16" t="s">
+      <c r="BS7" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="BT7" s="17" t="s">
+      <c r="BT7" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="BU7" s="16" t="s">
+      <c r="BU7" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="BV7" s="17" t="s">
+      <c r="BV7" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="BW7" s="16" t="s">
+      <c r="BW7" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="BX7" s="17" t="s">
+      <c r="BX7" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="BY7" s="16" t="s">
+      <c r="BY7" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="BZ7" s="17" t="s">
+      <c r="BZ7" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="CA7" s="16" t="s">
+      <c r="CA7" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="CB7" s="17" t="s">
+      <c r="CB7" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="CC7" s="16" t="s">
+      <c r="CC7" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="CD7" s="17" t="s">
+      <c r="CD7" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="CE7" s="16" t="s">
+      <c r="CE7" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="CF7" s="17" t="s">
+      <c r="CF7" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="CG7" s="17" t="s">
+      <c r="CG7" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="CH7" s="16" t="s">
+      <c r="CH7" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="CI7" s="17" t="s">
+      <c r="CI7" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="CJ7" s="17" t="s">
+      <c r="CJ7" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="CK7" s="17" t="s">
+      <c r="CK7" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="CL7" s="17" t="s">
+      <c r="CL7" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="CM7" s="17" t="s">
+      <c r="CM7" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="CN7" s="17" t="s">
+      <c r="CN7" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="CO7" s="17" t="s">
+      <c r="CO7" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="CP7" s="17" t="s">
+      <c r="CP7" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="CQ7" s="17" t="s">
+      <c r="CQ7" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="CR7" s="17" t="s">
+      <c r="CR7" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="CS7" s="17" t="s">
+      <c r="CS7" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="CT7" s="17" t="s">
+      <c r="CT7" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="CU7" s="7" t="s">
+      <c r="CU7" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="CV7" s="7" t="s">
+      <c r="CV7" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="CW7" s="7" t="s">
+      <c r="CW7" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="CX7" s="7" t="s">
+      <c r="CX7" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="CY7" s="7" t="s">
+      <c r="CY7" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="CZ7" s="7" t="s">
+      <c r="CZ7" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="DA7" s="7" t="s">
+      <c r="DA7" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="DB7" s="7" t="s">
+      <c r="DB7" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="DC7" s="7" t="s">
+      <c r="DC7" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="DD7" s="7" t="s">
+      <c r="DD7" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="DE7" s="7" t="s">
+      <c r="DE7" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="DF7" s="7" t="s">
+      <c r="DF7" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="DG7" s="7" t="s">
+      <c r="DG7" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="DH7" s="7" t="s">
+      <c r="DH7" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="DI7" s="7" t="s">
+      <c r="DI7" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="DJ7" s="5" t="s">
+      <c r="DJ7" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="DK7" s="5" t="s">
+      <c r="DK7" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="DL7" s="5" t="s">
+      <c r="DL7" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="DM7" s="5" t="s">
+      <c r="DM7" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="DN7" s="8" t="s">
+      <c r="DN7" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="DO7" s="8" t="s">
+      <c r="DO7" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="DP7" s="3" t="s">
+      <c r="DP7" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="DQ7" s="25" t="s">
+      <c r="DQ7" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="DR7" s="25" t="s">
+      <c r="DR7" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="DS7" s="25" t="s">
+      <c r="DS7" s="15" t="s">
         <v>116</v>
       </c>
-      <c r="DT7" s="25" t="s">
+      <c r="DT7" s="15" t="s">
         <v>117</v>
       </c>
-      <c r="DU7" s="25" t="s">
+      <c r="DU7" s="15" t="s">
         <v>122</v>
       </c>
-      <c r="DV7" s="25" t="s">
+      <c r="DV7" s="15" t="s">
         <v>123</v>
       </c>
-      <c r="DW7" s="25" t="s">
+      <c r="DW7" s="15" t="s">
         <v>124</v>
       </c>
-      <c r="DX7" s="25" t="s">
+      <c r="DX7" s="15" t="s">
         <v>125</v>
       </c>
-      <c r="DY7" s="25" t="s">
+      <c r="DY7" s="15" t="s">
         <v>126</v>
       </c>
-      <c r="DZ7" s="25" t="s">
+      <c r="DZ7" s="15" t="s">
         <v>127</v>
       </c>
-      <c r="EA7" s="25" t="s">
+      <c r="EA7" s="15" t="s">
         <v>128</v>
       </c>
-      <c r="EB7" s="25" t="s">
+      <c r="EB7" s="15" t="s">
         <v>129</v>
       </c>
-      <c r="EC7" s="41" t="s">
+      <c r="EC7" s="24" t="s">
         <v>131</v>
       </c>
-      <c r="ED7" s="41" t="s">
+      <c r="ED7" s="24" t="s">
         <v>132</v>
       </c>
-      <c r="EE7" s="41" t="s">
+      <c r="EE7" s="24" t="s">
         <v>133</v>
       </c>
-      <c r="EF7" s="41" t="s">
+      <c r="EF7" s="24" t="s">
         <v>134</v>
       </c>
-      <c r="EG7" s="41" t="s">
+      <c r="EG7" s="24" t="s">
         <v>135</v>
       </c>
-      <c r="EH7" s="41" t="s">
+      <c r="EH7" s="24" t="s">
         <v>136</v>
       </c>
-      <c r="EI7" s="41" t="s">
+      <c r="EI7" s="24" t="s">
         <v>137</v>
       </c>
-      <c r="EJ7" s="41" t="s">
+      <c r="EJ7" s="24" t="s">
         <v>138</v>
       </c>
-      <c r="EK7" s="41" t="s">
+      <c r="EK7" s="24" t="s">
         <v>139</v>
       </c>
-      <c r="EL7" s="41" t="s">
+      <c r="EL7" s="24" t="s">
         <v>140</v>
       </c>
-      <c r="EM7" s="41" t="s">
+      <c r="EM7" s="24" t="s">
         <v>141</v>
       </c>
-      <c r="EN7" s="41" t="s">
+      <c r="EN7" s="24" t="s">
         <v>142</v>
       </c>
     </row>
@@ -1897,20 +1891,20 @@
     <mergeCell ref="CI6:CR6"/>
     <mergeCell ref="CS6:CT6"/>
     <mergeCell ref="DN5:DO5"/>
-    <mergeCell ref="BR6:CA6"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="A2:K2"/>
     <mergeCell ref="A3:K3"/>
     <mergeCell ref="A5:A7"/>
+    <mergeCell ref="B5:X5"/>
     <mergeCell ref="CB6:CE6"/>
     <mergeCell ref="BK5:BQ5"/>
     <mergeCell ref="Z5:AK5"/>
     <mergeCell ref="AL5:BJ5"/>
     <mergeCell ref="DU5:EB5"/>
-    <mergeCell ref="B5:X5"/>
     <mergeCell ref="BR5:CT5"/>
     <mergeCell ref="DJ5:DM5"/>
     <mergeCell ref="CU5:DI5"/>
+    <mergeCell ref="BR6:CA6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
OAB : Update save new pasien
</commit_message>
<xml_diff>
--- a/Laravel-InaLUTS/resources/templates/Report_OAB.xlsx
+++ b/Laravel-InaLUTS/resources/templates/Report_OAB.xlsx
@@ -697,9 +697,30 @@
     <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -719,27 +740,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1045,8 +1045,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:EN7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="DO1" workbookViewId="0">
-      <selection activeCell="EN8" sqref="EN8"/>
+    <sheetView tabSelected="1" topLeftCell="CX1" workbookViewId="0">
+      <selection activeCell="DM8" sqref="DM8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1077,185 +1077,185 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:144" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="35"/>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
-      <c r="K1" s="35"/>
+      <c r="A1" s="30"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
     </row>
     <row r="2" spans="1:144" x14ac:dyDescent="0.25">
-      <c r="A2" s="36"/>
-      <c r="B2" s="36"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
-      <c r="G2" s="36"/>
-      <c r="H2" s="36"/>
-      <c r="I2" s="36"/>
-      <c r="J2" s="36"/>
-      <c r="K2" s="36"/>
+      <c r="A2" s="31"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="31"/>
     </row>
     <row r="3" spans="1:144" x14ac:dyDescent="0.25">
-      <c r="A3" s="37"/>
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
-      <c r="H3" s="37"/>
-      <c r="I3" s="37"/>
-      <c r="J3" s="37"/>
-      <c r="K3" s="37"/>
+      <c r="A3" s="32"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
+      <c r="K3" s="32"/>
     </row>
     <row r="4" spans="1:144" s="3" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="1:144" s="1" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="38" t="s">
+      <c r="A5" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="39" t="s">
+      <c r="B5" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="39"/>
-      <c r="D5" s="39"/>
-      <c r="E5" s="39"/>
-      <c r="F5" s="39"/>
-      <c r="G5" s="39"/>
-      <c r="H5" s="39"/>
-      <c r="I5" s="39"/>
-      <c r="J5" s="39"/>
-      <c r="K5" s="39"/>
-      <c r="L5" s="39"/>
-      <c r="M5" s="39"/>
-      <c r="N5" s="39"/>
-      <c r="O5" s="39"/>
-      <c r="P5" s="39"/>
-      <c r="Q5" s="39"/>
-      <c r="R5" s="39"/>
-      <c r="S5" s="39"/>
-      <c r="T5" s="39"/>
-      <c r="U5" s="39"/>
-      <c r="V5" s="39"/>
-      <c r="W5" s="39"/>
-      <c r="X5" s="39"/>
+      <c r="C5" s="34"/>
+      <c r="D5" s="34"/>
+      <c r="E5" s="34"/>
+      <c r="F5" s="34"/>
+      <c r="G5" s="34"/>
+      <c r="H5" s="34"/>
+      <c r="I5" s="34"/>
+      <c r="J5" s="34"/>
+      <c r="K5" s="34"/>
+      <c r="L5" s="34"/>
+      <c r="M5" s="34"/>
+      <c r="N5" s="34"/>
+      <c r="O5" s="34"/>
+      <c r="P5" s="34"/>
+      <c r="Q5" s="34"/>
+      <c r="R5" s="34"/>
+      <c r="S5" s="34"/>
+      <c r="T5" s="34"/>
+      <c r="U5" s="34"/>
+      <c r="V5" s="34"/>
+      <c r="W5" s="34"/>
+      <c r="X5" s="34"/>
       <c r="Y5" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="Z5" s="29" t="s">
+      <c r="Z5" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="AA5" s="29"/>
-      <c r="AB5" s="29"/>
-      <c r="AC5" s="29"/>
-      <c r="AD5" s="29"/>
-      <c r="AE5" s="29"/>
-      <c r="AF5" s="29"/>
-      <c r="AG5" s="29"/>
-      <c r="AH5" s="29"/>
-      <c r="AI5" s="29"/>
-      <c r="AJ5" s="29"/>
-      <c r="AK5" s="29"/>
-      <c r="AL5" s="30" t="s">
+      <c r="AA5" s="36"/>
+      <c r="AB5" s="36"/>
+      <c r="AC5" s="36"/>
+      <c r="AD5" s="36"/>
+      <c r="AE5" s="36"/>
+      <c r="AF5" s="36"/>
+      <c r="AG5" s="36"/>
+      <c r="AH5" s="36"/>
+      <c r="AI5" s="36"/>
+      <c r="AJ5" s="36"/>
+      <c r="AK5" s="36"/>
+      <c r="AL5" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="AM5" s="30"/>
-      <c r="AN5" s="30"/>
-      <c r="AO5" s="30"/>
-      <c r="AP5" s="30"/>
-      <c r="AQ5" s="30"/>
-      <c r="AR5" s="30"/>
-      <c r="AS5" s="30"/>
-      <c r="AT5" s="30"/>
-      <c r="AU5" s="30"/>
-      <c r="AV5" s="30"/>
-      <c r="AW5" s="30"/>
-      <c r="AX5" s="30"/>
-      <c r="AY5" s="30"/>
-      <c r="AZ5" s="30"/>
-      <c r="BA5" s="30"/>
-      <c r="BB5" s="30"/>
-      <c r="BC5" s="30"/>
-      <c r="BD5" s="30"/>
-      <c r="BE5" s="30"/>
-      <c r="BF5" s="30"/>
-      <c r="BG5" s="30"/>
-      <c r="BH5" s="30"/>
-      <c r="BI5" s="30"/>
-      <c r="BJ5" s="30"/>
-      <c r="BK5" s="28" t="s">
+      <c r="AM5" s="37"/>
+      <c r="AN5" s="37"/>
+      <c r="AO5" s="37"/>
+      <c r="AP5" s="37"/>
+      <c r="AQ5" s="37"/>
+      <c r="AR5" s="37"/>
+      <c r="AS5" s="37"/>
+      <c r="AT5" s="37"/>
+      <c r="AU5" s="37"/>
+      <c r="AV5" s="37"/>
+      <c r="AW5" s="37"/>
+      <c r="AX5" s="37"/>
+      <c r="AY5" s="37"/>
+      <c r="AZ5" s="37"/>
+      <c r="BA5" s="37"/>
+      <c r="BB5" s="37"/>
+      <c r="BC5" s="37"/>
+      <c r="BD5" s="37"/>
+      <c r="BE5" s="37"/>
+      <c r="BF5" s="37"/>
+      <c r="BG5" s="37"/>
+      <c r="BH5" s="37"/>
+      <c r="BI5" s="37"/>
+      <c r="BJ5" s="37"/>
+      <c r="BK5" s="35" t="s">
         <v>72</v>
       </c>
-      <c r="BL5" s="28"/>
-      <c r="BM5" s="28"/>
-      <c r="BN5" s="28"/>
-      <c r="BO5" s="28"/>
-      <c r="BP5" s="28"/>
-      <c r="BQ5" s="28"/>
-      <c r="BR5" s="32" t="s">
+      <c r="BL5" s="35"/>
+      <c r="BM5" s="35"/>
+      <c r="BN5" s="35"/>
+      <c r="BO5" s="35"/>
+      <c r="BP5" s="35"/>
+      <c r="BQ5" s="35"/>
+      <c r="BR5" s="39" t="s">
         <v>73</v>
       </c>
-      <c r="BS5" s="32"/>
-      <c r="BT5" s="32"/>
-      <c r="BU5" s="32"/>
-      <c r="BV5" s="32"/>
-      <c r="BW5" s="32"/>
-      <c r="BX5" s="32"/>
-      <c r="BY5" s="32"/>
-      <c r="BZ5" s="32"/>
-      <c r="CA5" s="32"/>
-      <c r="CB5" s="32"/>
-      <c r="CC5" s="32"/>
-      <c r="CD5" s="32"/>
-      <c r="CE5" s="32"/>
-      <c r="CF5" s="32"/>
-      <c r="CG5" s="32"/>
-      <c r="CH5" s="32"/>
-      <c r="CI5" s="32"/>
-      <c r="CJ5" s="32"/>
-      <c r="CK5" s="32"/>
-      <c r="CL5" s="32"/>
-      <c r="CM5" s="32"/>
-      <c r="CN5" s="32"/>
-      <c r="CO5" s="32"/>
-      <c r="CP5" s="32"/>
-      <c r="CQ5" s="32"/>
-      <c r="CR5" s="32"/>
-      <c r="CS5" s="32"/>
-      <c r="CT5" s="32"/>
-      <c r="CU5" s="34" t="s">
+      <c r="BS5" s="39"/>
+      <c r="BT5" s="39"/>
+      <c r="BU5" s="39"/>
+      <c r="BV5" s="39"/>
+      <c r="BW5" s="39"/>
+      <c r="BX5" s="39"/>
+      <c r="BY5" s="39"/>
+      <c r="BZ5" s="39"/>
+      <c r="CA5" s="39"/>
+      <c r="CB5" s="39"/>
+      <c r="CC5" s="39"/>
+      <c r="CD5" s="39"/>
+      <c r="CE5" s="39"/>
+      <c r="CF5" s="39"/>
+      <c r="CG5" s="39"/>
+      <c r="CH5" s="39"/>
+      <c r="CI5" s="39"/>
+      <c r="CJ5" s="39"/>
+      <c r="CK5" s="39"/>
+      <c r="CL5" s="39"/>
+      <c r="CM5" s="39"/>
+      <c r="CN5" s="39"/>
+      <c r="CO5" s="39"/>
+      <c r="CP5" s="39"/>
+      <c r="CQ5" s="39"/>
+      <c r="CR5" s="39"/>
+      <c r="CS5" s="39"/>
+      <c r="CT5" s="39"/>
+      <c r="CU5" s="41" t="s">
         <v>94</v>
       </c>
-      <c r="CV5" s="34"/>
-      <c r="CW5" s="34"/>
-      <c r="CX5" s="34"/>
-      <c r="CY5" s="34"/>
-      <c r="CZ5" s="34"/>
-      <c r="DA5" s="34"/>
-      <c r="DB5" s="34"/>
-      <c r="DC5" s="34"/>
-      <c r="DD5" s="34"/>
-      <c r="DE5" s="34"/>
-      <c r="DF5" s="34"/>
-      <c r="DG5" s="34"/>
-      <c r="DH5" s="34"/>
-      <c r="DI5" s="34"/>
-      <c r="DJ5" s="33" t="s">
+      <c r="CV5" s="41"/>
+      <c r="CW5" s="41"/>
+      <c r="CX5" s="41"/>
+      <c r="CY5" s="41"/>
+      <c r="CZ5" s="41"/>
+      <c r="DA5" s="41"/>
+      <c r="DB5" s="41"/>
+      <c r="DC5" s="41"/>
+      <c r="DD5" s="41"/>
+      <c r="DE5" s="41"/>
+      <c r="DF5" s="41"/>
+      <c r="DG5" s="41"/>
+      <c r="DH5" s="41"/>
+      <c r="DI5" s="41"/>
+      <c r="DJ5" s="40" t="s">
         <v>108</v>
       </c>
-      <c r="DK5" s="33"/>
-      <c r="DL5" s="33"/>
-      <c r="DM5" s="33"/>
-      <c r="DN5" s="41" t="s">
+      <c r="DK5" s="40"/>
+      <c r="DL5" s="40"/>
+      <c r="DM5" s="40"/>
+      <c r="DN5" s="29" t="s">
         <v>109</v>
       </c>
-      <c r="DO5" s="41"/>
+      <c r="DO5" s="29"/>
       <c r="DP5" s="17" t="s">
         <v>112</v>
       </c>
@@ -1271,33 +1271,33 @@
       <c r="DT5" s="16" t="s">
         <v>120</v>
       </c>
-      <c r="DU5" s="31" t="s">
+      <c r="DU5" s="38" t="s">
         <v>121</v>
       </c>
-      <c r="DV5" s="31"/>
-      <c r="DW5" s="31"/>
-      <c r="DX5" s="31"/>
-      <c r="DY5" s="31"/>
-      <c r="DZ5" s="31"/>
-      <c r="EA5" s="31"/>
-      <c r="EB5" s="31"/>
-      <c r="EC5" s="40" t="s">
+      <c r="DV5" s="38"/>
+      <c r="DW5" s="38"/>
+      <c r="DX5" s="38"/>
+      <c r="DY5" s="38"/>
+      <c r="DZ5" s="38"/>
+      <c r="EA5" s="38"/>
+      <c r="EB5" s="38"/>
+      <c r="EC5" s="27" t="s">
         <v>130</v>
       </c>
-      <c r="ED5" s="40"/>
-      <c r="EE5" s="40"/>
-      <c r="EF5" s="40"/>
-      <c r="EG5" s="40"/>
-      <c r="EH5" s="40"/>
-      <c r="EI5" s="40"/>
-      <c r="EJ5" s="40"/>
-      <c r="EK5" s="40"/>
-      <c r="EL5" s="40"/>
-      <c r="EM5" s="40"/>
-      <c r="EN5" s="40"/>
+      <c r="ED5" s="27"/>
+      <c r="EE5" s="27"/>
+      <c r="EF5" s="27"/>
+      <c r="EG5" s="27"/>
+      <c r="EH5" s="27"/>
+      <c r="EI5" s="27"/>
+      <c r="EJ5" s="27"/>
+      <c r="EK5" s="27"/>
+      <c r="EL5" s="27"/>
+      <c r="EM5" s="27"/>
+      <c r="EN5" s="27"/>
     </row>
     <row r="6" spans="1:144" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="38"/>
+      <c r="A6" s="33"/>
       <c r="B6" s="17"/>
       <c r="C6" s="17"/>
       <c r="D6" s="17"/>
@@ -1366,45 +1366,45 @@
       <c r="BO6" s="21"/>
       <c r="BP6" s="21"/>
       <c r="BQ6" s="21"/>
-      <c r="BR6" s="27" t="s">
+      <c r="BR6" s="28" t="s">
         <v>75</v>
       </c>
-      <c r="BS6" s="27"/>
-      <c r="BT6" s="27"/>
-      <c r="BU6" s="27"/>
-      <c r="BV6" s="27"/>
-      <c r="BW6" s="27"/>
-      <c r="BX6" s="27"/>
-      <c r="BY6" s="27"/>
-      <c r="BZ6" s="27"/>
-      <c r="CA6" s="27"/>
-      <c r="CB6" s="27" t="s">
+      <c r="BS6" s="28"/>
+      <c r="BT6" s="28"/>
+      <c r="BU6" s="28"/>
+      <c r="BV6" s="28"/>
+      <c r="BW6" s="28"/>
+      <c r="BX6" s="28"/>
+      <c r="BY6" s="28"/>
+      <c r="BZ6" s="28"/>
+      <c r="CA6" s="28"/>
+      <c r="CB6" s="28" t="s">
         <v>80</v>
       </c>
-      <c r="CC6" s="27"/>
-      <c r="CD6" s="27"/>
-      <c r="CE6" s="27"/>
-      <c r="CF6" s="27" t="s">
+      <c r="CC6" s="28"/>
+      <c r="CD6" s="28"/>
+      <c r="CE6" s="28"/>
+      <c r="CF6" s="28" t="s">
         <v>83</v>
       </c>
-      <c r="CG6" s="27"/>
-      <c r="CH6" s="27"/>
-      <c r="CI6" s="27" t="s">
+      <c r="CG6" s="28"/>
+      <c r="CH6" s="28"/>
+      <c r="CI6" s="28" t="s">
         <v>86</v>
       </c>
-      <c r="CJ6" s="27"/>
-      <c r="CK6" s="27"/>
-      <c r="CL6" s="27"/>
-      <c r="CM6" s="27"/>
-      <c r="CN6" s="27"/>
-      <c r="CO6" s="27"/>
-      <c r="CP6" s="27"/>
-      <c r="CQ6" s="27"/>
-      <c r="CR6" s="27"/>
-      <c r="CS6" s="27" t="s">
+      <c r="CJ6" s="28"/>
+      <c r="CK6" s="28"/>
+      <c r="CL6" s="28"/>
+      <c r="CM6" s="28"/>
+      <c r="CN6" s="28"/>
+      <c r="CO6" s="28"/>
+      <c r="CP6" s="28"/>
+      <c r="CQ6" s="28"/>
+      <c r="CR6" s="28"/>
+      <c r="CS6" s="28" t="s">
         <v>92</v>
       </c>
-      <c r="CT6" s="27"/>
+      <c r="CT6" s="28"/>
       <c r="CU6" s="11"/>
       <c r="CV6" s="11"/>
       <c r="CW6" s="11"/>
@@ -1453,7 +1453,7 @@
       <c r="EN6" s="25"/>
     </row>
     <row r="7" spans="1:144" s="1" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A7" s="38"/>
+      <c r="A7" s="33"/>
       <c r="B7" s="2" t="s">
         <v>2</v>
       </c>
@@ -1886,16 +1886,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="EC5:EN5"/>
-    <mergeCell ref="CF6:CH6"/>
-    <mergeCell ref="CI6:CR6"/>
-    <mergeCell ref="CS6:CT6"/>
-    <mergeCell ref="DN5:DO5"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="B5:X5"/>
     <mergeCell ref="CB6:CE6"/>
     <mergeCell ref="BK5:BQ5"/>
     <mergeCell ref="Z5:AK5"/>
@@ -1905,6 +1895,16 @@
     <mergeCell ref="DJ5:DM5"/>
     <mergeCell ref="CU5:DI5"/>
     <mergeCell ref="BR6:CA6"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="B5:X5"/>
+    <mergeCell ref="EC5:EN5"/>
+    <mergeCell ref="CF6:CH6"/>
+    <mergeCell ref="CI6:CR6"/>
+    <mergeCell ref="CS6:CT6"/>
+    <mergeCell ref="DN5:DO5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
OAB : Laporan Penunjang Urodinamik, Uroflowmetri, Diagnosis
</commit_message>
<xml_diff>
--- a/Laravel-InaLUTS/resources/templates/Report_OAB.xlsx
+++ b/Laravel-InaLUTS/resources/templates/Report_OAB.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26924"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54B76CB1-FF92-4BAD-960B-FFFEBC5BE2F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Laporan" sheetId="1" r:id="rId1"/>
@@ -14,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="162">
   <si>
     <t>No</t>
   </si>
@@ -443,12 +444,69 @@
   </si>
   <si>
     <t>Prostat</t>
+  </si>
+  <si>
+    <t>Penunjang - Uroflowmetri</t>
+  </si>
+  <si>
+    <t>Voided volume</t>
+  </si>
+  <si>
+    <t>Q max</t>
+  </si>
+  <si>
+    <t>Q ave</t>
+  </si>
+  <si>
+    <t>PVR</t>
+  </si>
+  <si>
+    <t>Voiding time</t>
+  </si>
+  <si>
+    <t>Pemeriksaan urodinamik</t>
+  </si>
+  <si>
+    <t>Penunjang - Urodinamik</t>
+  </si>
+  <si>
+    <t>Kapasitas kandung kemih</t>
+  </si>
+  <si>
+    <t>Compliance</t>
+  </si>
+  <si>
+    <t>Detrusor overactivity</t>
+  </si>
+  <si>
+    <t>Detrusor overactivity incontinence</t>
+  </si>
+  <si>
+    <t>Urodynamic stress urinary incontinence</t>
+  </si>
+  <si>
+    <t>Obstruksi infravesical</t>
+  </si>
+  <si>
+    <t>Detrusor underactivity</t>
+  </si>
+  <si>
+    <t>Disfunctional Voiding</t>
+  </si>
+  <si>
+    <t>DSD</t>
+  </si>
+  <si>
+    <t>Neurogenic Bladder</t>
+  </si>
+  <si>
+    <t>Diagnosis</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -489,7 +547,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="20">
+  <fills count="22">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -604,6 +662,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -617,7 +687,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -697,50 +767,65 @@
     <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -752,14 +837,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -797,7 +885,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -869,7 +957,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1042,41 +1130,41 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:EN7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:FH7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="CX1" workbookViewId="0">
-      <selection activeCell="DM8" sqref="DM8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="4.7109375" style="19" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" style="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" style="19" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" style="19" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" style="19" customWidth="1"/>
-    <col min="6" max="6" width="20.7109375" style="19" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" style="19" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.7109375" style="19" customWidth="1"/>
-    <col min="9" max="10" width="15.7109375" style="19" customWidth="1"/>
-    <col min="11" max="11" width="20.7109375" style="19" customWidth="1"/>
-    <col min="12" max="12" width="16.85546875" style="19" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="12.7109375" style="19" customWidth="1"/>
-    <col min="15" max="16" width="10.7109375" style="19" customWidth="1"/>
-    <col min="17" max="17" width="8.7109375" style="19" customWidth="1"/>
-    <col min="18" max="25" width="15.7109375" style="19" customWidth="1"/>
-    <col min="26" max="37" width="10.7109375" style="19" customWidth="1"/>
-    <col min="38" max="40" width="9.140625" style="19"/>
+    <col min="1" max="1" width="4.7265625" style="19" customWidth="1"/>
+    <col min="2" max="2" width="11.81640625" style="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.7265625" style="19" customWidth="1"/>
+    <col min="4" max="4" width="14.54296875" style="19" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.7265625" style="19" customWidth="1"/>
+    <col min="6" max="6" width="20.7265625" style="19" customWidth="1"/>
+    <col min="7" max="7" width="13.26953125" style="19" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.7265625" style="19" customWidth="1"/>
+    <col min="9" max="10" width="15.7265625" style="19" customWidth="1"/>
+    <col min="11" max="11" width="20.7265625" style="19" customWidth="1"/>
+    <col min="12" max="12" width="16.81640625" style="19" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="12.7265625" style="19" customWidth="1"/>
+    <col min="15" max="16" width="10.7265625" style="19" customWidth="1"/>
+    <col min="17" max="17" width="8.7265625" style="19" customWidth="1"/>
+    <col min="18" max="25" width="15.7265625" style="19" customWidth="1"/>
+    <col min="26" max="37" width="10.7265625" style="19" customWidth="1"/>
+    <col min="38" max="40" width="9.1796875" style="19"/>
     <col min="41" max="41" width="18" style="19" bestFit="1" customWidth="1"/>
-    <col min="42" max="117" width="9.140625" style="19"/>
-    <col min="118" max="119" width="15.7109375" style="19" customWidth="1"/>
-    <col min="120" max="120" width="12.7109375" style="19" customWidth="1"/>
-    <col min="121" max="125" width="10.7109375" style="19" customWidth="1"/>
-    <col min="126" max="16384" width="9.140625" style="19"/>
+    <col min="42" max="117" width="9.1796875" style="19"/>
+    <col min="118" max="119" width="15.7265625" style="19" customWidth="1"/>
+    <col min="120" max="120" width="12.7265625" style="19" customWidth="1"/>
+    <col min="121" max="125" width="10.7265625" style="19" customWidth="1"/>
+    <col min="126" max="16384" width="9.1796875" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:144" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:164" ht="18.5" x14ac:dyDescent="0.35">
       <c r="A1" s="30"/>
       <c r="B1" s="30"/>
       <c r="C1" s="30"/>
@@ -1089,7 +1177,7 @@
       <c r="J1" s="30"/>
       <c r="K1" s="30"/>
     </row>
-    <row r="2" spans="1:144" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:164" x14ac:dyDescent="0.35">
       <c r="A2" s="31"/>
       <c r="B2" s="31"/>
       <c r="C2" s="31"/>
@@ -1102,7 +1190,7 @@
       <c r="J2" s="31"/>
       <c r="K2" s="31"/>
     </row>
-    <row r="3" spans="1:144" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:164" x14ac:dyDescent="0.35">
       <c r="A3" s="32"/>
       <c r="B3" s="32"/>
       <c r="C3" s="32"/>
@@ -1115,8 +1203,8 @@
       <c r="J3" s="32"/>
       <c r="K3" s="32"/>
     </row>
-    <row r="4" spans="1:144" s="3" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:144" s="1" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:164" s="3" customFormat="1" ht="5.15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="5" spans="1:164" s="1" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="33" t="s">
         <v>0</v>
       </c>
@@ -1148,114 +1236,114 @@
       <c r="Y5" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="Z5" s="36" t="s">
+      <c r="Z5" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="AA5" s="36"/>
-      <c r="AB5" s="36"/>
-      <c r="AC5" s="36"/>
-      <c r="AD5" s="36"/>
-      <c r="AE5" s="36"/>
-      <c r="AF5" s="36"/>
-      <c r="AG5" s="36"/>
-      <c r="AH5" s="36"/>
-      <c r="AI5" s="36"/>
-      <c r="AJ5" s="36"/>
-      <c r="AK5" s="36"/>
-      <c r="AL5" s="37" t="s">
+      <c r="AA5" s="38"/>
+      <c r="AB5" s="38"/>
+      <c r="AC5" s="38"/>
+      <c r="AD5" s="38"/>
+      <c r="AE5" s="38"/>
+      <c r="AF5" s="38"/>
+      <c r="AG5" s="38"/>
+      <c r="AH5" s="38"/>
+      <c r="AI5" s="38"/>
+      <c r="AJ5" s="38"/>
+      <c r="AK5" s="38"/>
+      <c r="AL5" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="AM5" s="37"/>
-      <c r="AN5" s="37"/>
-      <c r="AO5" s="37"/>
-      <c r="AP5" s="37"/>
-      <c r="AQ5" s="37"/>
-      <c r="AR5" s="37"/>
-      <c r="AS5" s="37"/>
-      <c r="AT5" s="37"/>
-      <c r="AU5" s="37"/>
-      <c r="AV5" s="37"/>
-      <c r="AW5" s="37"/>
-      <c r="AX5" s="37"/>
-      <c r="AY5" s="37"/>
-      <c r="AZ5" s="37"/>
-      <c r="BA5" s="37"/>
-      <c r="BB5" s="37"/>
-      <c r="BC5" s="37"/>
-      <c r="BD5" s="37"/>
-      <c r="BE5" s="37"/>
-      <c r="BF5" s="37"/>
-      <c r="BG5" s="37"/>
-      <c r="BH5" s="37"/>
-      <c r="BI5" s="37"/>
-      <c r="BJ5" s="37"/>
-      <c r="BK5" s="35" t="s">
+      <c r="AM5" s="39"/>
+      <c r="AN5" s="39"/>
+      <c r="AO5" s="39"/>
+      <c r="AP5" s="39"/>
+      <c r="AQ5" s="39"/>
+      <c r="AR5" s="39"/>
+      <c r="AS5" s="39"/>
+      <c r="AT5" s="39"/>
+      <c r="AU5" s="39"/>
+      <c r="AV5" s="39"/>
+      <c r="AW5" s="39"/>
+      <c r="AX5" s="39"/>
+      <c r="AY5" s="39"/>
+      <c r="AZ5" s="39"/>
+      <c r="BA5" s="39"/>
+      <c r="BB5" s="39"/>
+      <c r="BC5" s="39"/>
+      <c r="BD5" s="39"/>
+      <c r="BE5" s="39"/>
+      <c r="BF5" s="39"/>
+      <c r="BG5" s="39"/>
+      <c r="BH5" s="39"/>
+      <c r="BI5" s="39"/>
+      <c r="BJ5" s="39"/>
+      <c r="BK5" s="37" t="s">
         <v>72</v>
       </c>
-      <c r="BL5" s="35"/>
-      <c r="BM5" s="35"/>
-      <c r="BN5" s="35"/>
-      <c r="BO5" s="35"/>
-      <c r="BP5" s="35"/>
-      <c r="BQ5" s="35"/>
-      <c r="BR5" s="39" t="s">
+      <c r="BL5" s="37"/>
+      <c r="BM5" s="37"/>
+      <c r="BN5" s="37"/>
+      <c r="BO5" s="37"/>
+      <c r="BP5" s="37"/>
+      <c r="BQ5" s="37"/>
+      <c r="BR5" s="35" t="s">
         <v>73</v>
       </c>
-      <c r="BS5" s="39"/>
-      <c r="BT5" s="39"/>
-      <c r="BU5" s="39"/>
-      <c r="BV5" s="39"/>
-      <c r="BW5" s="39"/>
-      <c r="BX5" s="39"/>
-      <c r="BY5" s="39"/>
-      <c r="BZ5" s="39"/>
-      <c r="CA5" s="39"/>
-      <c r="CB5" s="39"/>
-      <c r="CC5" s="39"/>
-      <c r="CD5" s="39"/>
-      <c r="CE5" s="39"/>
-      <c r="CF5" s="39"/>
-      <c r="CG5" s="39"/>
-      <c r="CH5" s="39"/>
-      <c r="CI5" s="39"/>
-      <c r="CJ5" s="39"/>
-      <c r="CK5" s="39"/>
-      <c r="CL5" s="39"/>
-      <c r="CM5" s="39"/>
-      <c r="CN5" s="39"/>
-      <c r="CO5" s="39"/>
-      <c r="CP5" s="39"/>
-      <c r="CQ5" s="39"/>
-      <c r="CR5" s="39"/>
-      <c r="CS5" s="39"/>
-      <c r="CT5" s="39"/>
-      <c r="CU5" s="41" t="s">
+      <c r="BS5" s="35"/>
+      <c r="BT5" s="35"/>
+      <c r="BU5" s="35"/>
+      <c r="BV5" s="35"/>
+      <c r="BW5" s="35"/>
+      <c r="BX5" s="35"/>
+      <c r="BY5" s="35"/>
+      <c r="BZ5" s="35"/>
+      <c r="CA5" s="35"/>
+      <c r="CB5" s="35"/>
+      <c r="CC5" s="35"/>
+      <c r="CD5" s="35"/>
+      <c r="CE5" s="35"/>
+      <c r="CF5" s="35"/>
+      <c r="CG5" s="35"/>
+      <c r="CH5" s="35"/>
+      <c r="CI5" s="35"/>
+      <c r="CJ5" s="35"/>
+      <c r="CK5" s="35"/>
+      <c r="CL5" s="35"/>
+      <c r="CM5" s="35"/>
+      <c r="CN5" s="35"/>
+      <c r="CO5" s="35"/>
+      <c r="CP5" s="35"/>
+      <c r="CQ5" s="35"/>
+      <c r="CR5" s="35"/>
+      <c r="CS5" s="35"/>
+      <c r="CT5" s="35"/>
+      <c r="CU5" s="42" t="s">
         <v>94</v>
       </c>
-      <c r="CV5" s="41"/>
-      <c r="CW5" s="41"/>
-      <c r="CX5" s="41"/>
-      <c r="CY5" s="41"/>
-      <c r="CZ5" s="41"/>
-      <c r="DA5" s="41"/>
-      <c r="DB5" s="41"/>
-      <c r="DC5" s="41"/>
-      <c r="DD5" s="41"/>
-      <c r="DE5" s="41"/>
-      <c r="DF5" s="41"/>
-      <c r="DG5" s="41"/>
-      <c r="DH5" s="41"/>
-      <c r="DI5" s="41"/>
-      <c r="DJ5" s="40" t="s">
+      <c r="CV5" s="42"/>
+      <c r="CW5" s="42"/>
+      <c r="CX5" s="42"/>
+      <c r="CY5" s="42"/>
+      <c r="CZ5" s="42"/>
+      <c r="DA5" s="42"/>
+      <c r="DB5" s="42"/>
+      <c r="DC5" s="42"/>
+      <c r="DD5" s="42"/>
+      <c r="DE5" s="42"/>
+      <c r="DF5" s="42"/>
+      <c r="DG5" s="42"/>
+      <c r="DH5" s="42"/>
+      <c r="DI5" s="42"/>
+      <c r="DJ5" s="41" t="s">
         <v>108</v>
       </c>
-      <c r="DK5" s="40"/>
-      <c r="DL5" s="40"/>
-      <c r="DM5" s="40"/>
-      <c r="DN5" s="29" t="s">
+      <c r="DK5" s="41"/>
+      <c r="DL5" s="41"/>
+      <c r="DM5" s="41"/>
+      <c r="DN5" s="45" t="s">
         <v>109</v>
       </c>
-      <c r="DO5" s="29"/>
+      <c r="DO5" s="45"/>
       <c r="DP5" s="17" t="s">
         <v>112</v>
       </c>
@@ -1271,32 +1359,58 @@
       <c r="DT5" s="16" t="s">
         <v>120</v>
       </c>
-      <c r="DU5" s="38" t="s">
+      <c r="DU5" s="40" t="s">
         <v>121</v>
       </c>
-      <c r="DV5" s="38"/>
-      <c r="DW5" s="38"/>
-      <c r="DX5" s="38"/>
-      <c r="DY5" s="38"/>
-      <c r="DZ5" s="38"/>
-      <c r="EA5" s="38"/>
-      <c r="EB5" s="38"/>
-      <c r="EC5" s="27" t="s">
+      <c r="DV5" s="40"/>
+      <c r="DW5" s="40"/>
+      <c r="DX5" s="40"/>
+      <c r="DY5" s="40"/>
+      <c r="DZ5" s="40"/>
+      <c r="EA5" s="40"/>
+      <c r="EB5" s="40"/>
+      <c r="EC5" s="44" t="s">
         <v>130</v>
       </c>
-      <c r="ED5" s="27"/>
-      <c r="EE5" s="27"/>
-      <c r="EF5" s="27"/>
-      <c r="EG5" s="27"/>
-      <c r="EH5" s="27"/>
-      <c r="EI5" s="27"/>
-      <c r="EJ5" s="27"/>
-      <c r="EK5" s="27"/>
-      <c r="EL5" s="27"/>
-      <c r="EM5" s="27"/>
-      <c r="EN5" s="27"/>
+      <c r="ED5" s="44"/>
+      <c r="EE5" s="44"/>
+      <c r="EF5" s="44"/>
+      <c r="EG5" s="44"/>
+      <c r="EH5" s="44"/>
+      <c r="EI5" s="44"/>
+      <c r="EJ5" s="44"/>
+      <c r="EK5" s="44"/>
+      <c r="EL5" s="44"/>
+      <c r="EM5" s="44"/>
+      <c r="EN5" s="44"/>
+      <c r="EO5" s="43" t="s">
+        <v>143</v>
+      </c>
+      <c r="EP5" s="43"/>
+      <c r="EQ5" s="43"/>
+      <c r="ER5" s="43"/>
+      <c r="ES5" s="43"/>
+      <c r="ET5" s="43"/>
+      <c r="EU5" s="35" t="s">
+        <v>150</v>
+      </c>
+      <c r="EV5" s="35"/>
+      <c r="EW5" s="35"/>
+      <c r="EX5" s="35"/>
+      <c r="EY5" s="35"/>
+      <c r="EZ5" s="35"/>
+      <c r="FA5" s="35"/>
+      <c r="FB5" s="35"/>
+      <c r="FC5" s="35"/>
+      <c r="FD5" s="35"/>
+      <c r="FE5" s="35"/>
+      <c r="FF5" s="35"/>
+      <c r="FG5" s="35"/>
+      <c r="FH5" s="46" t="s">
+        <v>161</v>
+      </c>
     </row>
-    <row r="6" spans="1:144" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:164" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="33"/>
       <c r="B6" s="17"/>
       <c r="C6" s="17"/>
@@ -1366,45 +1480,45 @@
       <c r="BO6" s="21"/>
       <c r="BP6" s="21"/>
       <c r="BQ6" s="21"/>
-      <c r="BR6" s="28" t="s">
+      <c r="BR6" s="36" t="s">
         <v>75</v>
       </c>
-      <c r="BS6" s="28"/>
-      <c r="BT6" s="28"/>
-      <c r="BU6" s="28"/>
-      <c r="BV6" s="28"/>
-      <c r="BW6" s="28"/>
-      <c r="BX6" s="28"/>
-      <c r="BY6" s="28"/>
-      <c r="BZ6" s="28"/>
-      <c r="CA6" s="28"/>
-      <c r="CB6" s="28" t="s">
+      <c r="BS6" s="36"/>
+      <c r="BT6" s="36"/>
+      <c r="BU6" s="36"/>
+      <c r="BV6" s="36"/>
+      <c r="BW6" s="36"/>
+      <c r="BX6" s="36"/>
+      <c r="BY6" s="36"/>
+      <c r="BZ6" s="36"/>
+      <c r="CA6" s="36"/>
+      <c r="CB6" s="36" t="s">
         <v>80</v>
       </c>
-      <c r="CC6" s="28"/>
-      <c r="CD6" s="28"/>
-      <c r="CE6" s="28"/>
-      <c r="CF6" s="28" t="s">
+      <c r="CC6" s="36"/>
+      <c r="CD6" s="36"/>
+      <c r="CE6" s="36"/>
+      <c r="CF6" s="36" t="s">
         <v>83</v>
       </c>
-      <c r="CG6" s="28"/>
-      <c r="CH6" s="28"/>
-      <c r="CI6" s="28" t="s">
+      <c r="CG6" s="36"/>
+      <c r="CH6" s="36"/>
+      <c r="CI6" s="36" t="s">
         <v>86</v>
       </c>
-      <c r="CJ6" s="28"/>
-      <c r="CK6" s="28"/>
-      <c r="CL6" s="28"/>
-      <c r="CM6" s="28"/>
-      <c r="CN6" s="28"/>
-      <c r="CO6" s="28"/>
-      <c r="CP6" s="28"/>
-      <c r="CQ6" s="28"/>
-      <c r="CR6" s="28"/>
-      <c r="CS6" s="28" t="s">
+      <c r="CJ6" s="36"/>
+      <c r="CK6" s="36"/>
+      <c r="CL6" s="36"/>
+      <c r="CM6" s="36"/>
+      <c r="CN6" s="36"/>
+      <c r="CO6" s="36"/>
+      <c r="CP6" s="36"/>
+      <c r="CQ6" s="36"/>
+      <c r="CR6" s="36"/>
+      <c r="CS6" s="36" t="s">
         <v>92</v>
       </c>
-      <c r="CT6" s="28"/>
+      <c r="CT6" s="36"/>
       <c r="CU6" s="11"/>
       <c r="CV6" s="11"/>
       <c r="CW6" s="11"/>
@@ -1451,8 +1565,28 @@
       <c r="EL6" s="25"/>
       <c r="EM6" s="25"/>
       <c r="EN6" s="25"/>
+      <c r="EO6" s="28"/>
+      <c r="EP6" s="28"/>
+      <c r="EQ6" s="28"/>
+      <c r="ER6" s="28"/>
+      <c r="ES6" s="28"/>
+      <c r="ET6" s="28"/>
+      <c r="EU6" s="29"/>
+      <c r="EV6" s="29"/>
+      <c r="EW6" s="29"/>
+      <c r="EX6" s="29"/>
+      <c r="EY6" s="29"/>
+      <c r="EZ6" s="29"/>
+      <c r="FA6" s="29"/>
+      <c r="FB6" s="29"/>
+      <c r="FC6" s="29"/>
+      <c r="FD6" s="29"/>
+      <c r="FE6" s="29"/>
+      <c r="FF6" s="29"/>
+      <c r="FG6" s="29"/>
+      <c r="FH6" s="46"/>
     </row>
-    <row r="7" spans="1:144" s="1" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:164" s="1" customFormat="1" ht="87" x14ac:dyDescent="0.35">
       <c r="A7" s="33"/>
       <c r="B7" s="2" t="s">
         <v>2</v>
@@ -1883,9 +2017,70 @@
       <c r="EN7" s="24" t="s">
         <v>142</v>
       </c>
+      <c r="EO7" s="27" t="s">
+        <v>95</v>
+      </c>
+      <c r="EP7" s="27" t="s">
+        <v>144</v>
+      </c>
+      <c r="EQ7" s="27" t="s">
+        <v>145</v>
+      </c>
+      <c r="ER7" s="27" t="s">
+        <v>146</v>
+      </c>
+      <c r="ES7" s="27" t="s">
+        <v>147</v>
+      </c>
+      <c r="ET7" s="27" t="s">
+        <v>148</v>
+      </c>
+      <c r="EU7" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="EV7" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="EW7" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="EX7" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="EY7" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="EZ7" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="FA7" s="10" t="s">
+        <v>155</v>
+      </c>
+      <c r="FB7" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="FC7" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="FD7" s="10" t="s">
+        <v>158</v>
+      </c>
+      <c r="FE7" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="FF7" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="FG7" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="FH7" s="8" t="s">
+        <v>161</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="19">
+  <mergeCells count="21">
+    <mergeCell ref="EU5:FG5"/>
     <mergeCell ref="CB6:CE6"/>
     <mergeCell ref="BK5:BQ5"/>
     <mergeCell ref="Z5:AK5"/>
@@ -1895,16 +2090,17 @@
     <mergeCell ref="DJ5:DM5"/>
     <mergeCell ref="CU5:DI5"/>
     <mergeCell ref="BR6:CA6"/>
+    <mergeCell ref="EO5:ET5"/>
+    <mergeCell ref="EC5:EN5"/>
+    <mergeCell ref="CF6:CH6"/>
+    <mergeCell ref="CI6:CR6"/>
+    <mergeCell ref="CS6:CT6"/>
+    <mergeCell ref="DN5:DO5"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="A2:K2"/>
     <mergeCell ref="A3:K3"/>
     <mergeCell ref="A5:A7"/>
     <mergeCell ref="B5:X5"/>
-    <mergeCell ref="EC5:EN5"/>
-    <mergeCell ref="CF6:CH6"/>
-    <mergeCell ref="CI6:CR6"/>
-    <mergeCell ref="CS6:CT6"/>
-    <mergeCell ref="DN5:DO5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
OAB : Laporan Pemeriksaan Imaging
</commit_message>
<xml_diff>
--- a/Laravel-InaLUTS/resources/templates/Report_OAB.xlsx
+++ b/Laravel-InaLUTS/resources/templates/Report_OAB.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26924"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54B76CB1-FF92-4BAD-960B-FFFEBC5BE2F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10305"/>
   </bookViews>
   <sheets>
     <sheet name="Laporan" sheetId="1" r:id="rId1"/>
@@ -15,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="172">
   <si>
     <t>No</t>
   </si>
@@ -501,12 +500,42 @@
   </si>
   <si>
     <t>Diagnosis</t>
+  </si>
+  <si>
+    <t>Pemeriksaan Imaging</t>
+  </si>
+  <si>
+    <t>USG (abdominal / transrektal)</t>
+  </si>
+  <si>
+    <t>CT Urografi</t>
+  </si>
+  <si>
+    <t>Ginjal Kanan</t>
+  </si>
+  <si>
+    <t>Hidronefrosis</t>
+  </si>
+  <si>
+    <t>Batu</t>
+  </si>
+  <si>
+    <t>Ginjal Kiri</t>
+  </si>
+  <si>
+    <t>Buli</t>
+  </si>
+  <si>
+    <t>Divertikel</t>
+  </si>
+  <si>
+    <t>Massa intrabuli</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -687,7 +716,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -776,6 +805,45 @@
     <xf numFmtId="0" fontId="1" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -790,42 +858,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -845,9 +877,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -885,7 +917,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -957,7 +989,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1130,220 +1162,222 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:FH7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:FQ7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" topLeftCell="ES1" workbookViewId="0">
+      <selection activeCell="FP8" sqref="FP8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.7265625" style="19" customWidth="1"/>
-    <col min="2" max="2" width="11.81640625" style="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.7265625" style="19" customWidth="1"/>
-    <col min="4" max="4" width="14.54296875" style="19" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.7265625" style="19" customWidth="1"/>
-    <col min="6" max="6" width="20.7265625" style="19" customWidth="1"/>
-    <col min="7" max="7" width="13.26953125" style="19" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.7265625" style="19" customWidth="1"/>
-    <col min="9" max="10" width="15.7265625" style="19" customWidth="1"/>
-    <col min="11" max="11" width="20.7265625" style="19" customWidth="1"/>
-    <col min="12" max="12" width="16.81640625" style="19" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="12.7265625" style="19" customWidth="1"/>
-    <col min="15" max="16" width="10.7265625" style="19" customWidth="1"/>
-    <col min="17" max="17" width="8.7265625" style="19" customWidth="1"/>
-    <col min="18" max="25" width="15.7265625" style="19" customWidth="1"/>
-    <col min="26" max="37" width="10.7265625" style="19" customWidth="1"/>
-    <col min="38" max="40" width="9.1796875" style="19"/>
+    <col min="1" max="1" width="4.7109375" style="19" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" style="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" style="19" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" style="19" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" style="19" customWidth="1"/>
+    <col min="6" max="6" width="20.7109375" style="19" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" style="19" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" style="19" customWidth="1"/>
+    <col min="9" max="10" width="15.7109375" style="19" customWidth="1"/>
+    <col min="11" max="11" width="20.7109375" style="19" customWidth="1"/>
+    <col min="12" max="12" width="16.85546875" style="19" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="12.7109375" style="19" customWidth="1"/>
+    <col min="15" max="16" width="10.7109375" style="19" customWidth="1"/>
+    <col min="17" max="17" width="8.7109375" style="19" customWidth="1"/>
+    <col min="18" max="25" width="15.7109375" style="19" customWidth="1"/>
+    <col min="26" max="37" width="10.7109375" style="19" customWidth="1"/>
+    <col min="38" max="40" width="9.140625" style="19"/>
     <col min="41" max="41" width="18" style="19" bestFit="1" customWidth="1"/>
-    <col min="42" max="117" width="9.1796875" style="19"/>
-    <col min="118" max="119" width="15.7265625" style="19" customWidth="1"/>
-    <col min="120" max="120" width="12.7265625" style="19" customWidth="1"/>
-    <col min="121" max="125" width="10.7265625" style="19" customWidth="1"/>
-    <col min="126" max="16384" width="9.1796875" style="19"/>
+    <col min="42" max="117" width="9.140625" style="19"/>
+    <col min="118" max="119" width="15.7109375" style="19" customWidth="1"/>
+    <col min="120" max="120" width="12.7109375" style="19" customWidth="1"/>
+    <col min="121" max="125" width="10.7109375" style="19" customWidth="1"/>
+    <col min="126" max="163" width="9.140625" style="19"/>
+    <col min="164" max="172" width="9.140625" style="30"/>
+    <col min="173" max="16384" width="9.140625" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:164" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="30"/>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
+    <row r="1" spans="1:173" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="43"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="43"/>
+      <c r="J1" s="43"/>
+      <c r="K1" s="43"/>
     </row>
-    <row r="2" spans="1:164" x14ac:dyDescent="0.35">
-      <c r="A2" s="31"/>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
-      <c r="I2" s="31"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="31"/>
+    <row r="2" spans="1:173" x14ac:dyDescent="0.25">
+      <c r="A2" s="44"/>
+      <c r="B2" s="44"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="44"/>
+      <c r="K2" s="44"/>
     </row>
-    <row r="3" spans="1:164" x14ac:dyDescent="0.35">
-      <c r="A3" s="32"/>
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
-      <c r="K3" s="32"/>
+    <row r="3" spans="1:173" x14ac:dyDescent="0.25">
+      <c r="A3" s="45"/>
+      <c r="B3" s="45"/>
+      <c r="C3" s="45"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="45"/>
+      <c r="G3" s="45"/>
+      <c r="H3" s="45"/>
+      <c r="I3" s="45"/>
+      <c r="J3" s="45"/>
+      <c r="K3" s="45"/>
     </row>
-    <row r="4" spans="1:164" s="3" customFormat="1" ht="5.15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="5" spans="1:164" s="1" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="33" t="s">
+    <row r="4" spans="1:173" s="3" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:173" s="1" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="34" t="s">
+      <c r="B5" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="34"/>
-      <c r="D5" s="34"/>
-      <c r="E5" s="34"/>
-      <c r="F5" s="34"/>
-      <c r="G5" s="34"/>
-      <c r="H5" s="34"/>
-      <c r="I5" s="34"/>
-      <c r="J5" s="34"/>
-      <c r="K5" s="34"/>
-      <c r="L5" s="34"/>
-      <c r="M5" s="34"/>
-      <c r="N5" s="34"/>
-      <c r="O5" s="34"/>
-      <c r="P5" s="34"/>
-      <c r="Q5" s="34"/>
-      <c r="R5" s="34"/>
-      <c r="S5" s="34"/>
-      <c r="T5" s="34"/>
-      <c r="U5" s="34"/>
-      <c r="V5" s="34"/>
-      <c r="W5" s="34"/>
-      <c r="X5" s="34"/>
+      <c r="C5" s="47"/>
+      <c r="D5" s="47"/>
+      <c r="E5" s="47"/>
+      <c r="F5" s="47"/>
+      <c r="G5" s="47"/>
+      <c r="H5" s="47"/>
+      <c r="I5" s="47"/>
+      <c r="J5" s="47"/>
+      <c r="K5" s="47"/>
+      <c r="L5" s="47"/>
+      <c r="M5" s="47"/>
+      <c r="N5" s="47"/>
+      <c r="O5" s="47"/>
+      <c r="P5" s="47"/>
+      <c r="Q5" s="47"/>
+      <c r="R5" s="47"/>
+      <c r="S5" s="47"/>
+      <c r="T5" s="47"/>
+      <c r="U5" s="47"/>
+      <c r="V5" s="47"/>
+      <c r="W5" s="47"/>
+      <c r="X5" s="47"/>
       <c r="Y5" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="Z5" s="38" t="s">
+      <c r="Z5" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="AA5" s="38"/>
-      <c r="AB5" s="38"/>
-      <c r="AC5" s="38"/>
-      <c r="AD5" s="38"/>
-      <c r="AE5" s="38"/>
-      <c r="AF5" s="38"/>
-      <c r="AG5" s="38"/>
-      <c r="AH5" s="38"/>
-      <c r="AI5" s="38"/>
-      <c r="AJ5" s="38"/>
-      <c r="AK5" s="38"/>
-      <c r="AL5" s="39" t="s">
+      <c r="AA5" s="35"/>
+      <c r="AB5" s="35"/>
+      <c r="AC5" s="35"/>
+      <c r="AD5" s="35"/>
+      <c r="AE5" s="35"/>
+      <c r="AF5" s="35"/>
+      <c r="AG5" s="35"/>
+      <c r="AH5" s="35"/>
+      <c r="AI5" s="35"/>
+      <c r="AJ5" s="35"/>
+      <c r="AK5" s="35"/>
+      <c r="AL5" s="36" t="s">
         <v>40</v>
       </c>
-      <c r="AM5" s="39"/>
-      <c r="AN5" s="39"/>
-      <c r="AO5" s="39"/>
-      <c r="AP5" s="39"/>
-      <c r="AQ5" s="39"/>
-      <c r="AR5" s="39"/>
-      <c r="AS5" s="39"/>
-      <c r="AT5" s="39"/>
-      <c r="AU5" s="39"/>
-      <c r="AV5" s="39"/>
-      <c r="AW5" s="39"/>
-      <c r="AX5" s="39"/>
-      <c r="AY5" s="39"/>
-      <c r="AZ5" s="39"/>
-      <c r="BA5" s="39"/>
-      <c r="BB5" s="39"/>
-      <c r="BC5" s="39"/>
-      <c r="BD5" s="39"/>
-      <c r="BE5" s="39"/>
-      <c r="BF5" s="39"/>
-      <c r="BG5" s="39"/>
-      <c r="BH5" s="39"/>
-      <c r="BI5" s="39"/>
-      <c r="BJ5" s="39"/>
-      <c r="BK5" s="37" t="s">
+      <c r="AM5" s="36"/>
+      <c r="AN5" s="36"/>
+      <c r="AO5" s="36"/>
+      <c r="AP5" s="36"/>
+      <c r="AQ5" s="36"/>
+      <c r="AR5" s="36"/>
+      <c r="AS5" s="36"/>
+      <c r="AT5" s="36"/>
+      <c r="AU5" s="36"/>
+      <c r="AV5" s="36"/>
+      <c r="AW5" s="36"/>
+      <c r="AX5" s="36"/>
+      <c r="AY5" s="36"/>
+      <c r="AZ5" s="36"/>
+      <c r="BA5" s="36"/>
+      <c r="BB5" s="36"/>
+      <c r="BC5" s="36"/>
+      <c r="BD5" s="36"/>
+      <c r="BE5" s="36"/>
+      <c r="BF5" s="36"/>
+      <c r="BG5" s="36"/>
+      <c r="BH5" s="36"/>
+      <c r="BI5" s="36"/>
+      <c r="BJ5" s="36"/>
+      <c r="BK5" s="34" t="s">
         <v>72</v>
       </c>
-      <c r="BL5" s="37"/>
-      <c r="BM5" s="37"/>
-      <c r="BN5" s="37"/>
-      <c r="BO5" s="37"/>
-      <c r="BP5" s="37"/>
-      <c r="BQ5" s="37"/>
-      <c r="BR5" s="35" t="s">
+      <c r="BL5" s="34"/>
+      <c r="BM5" s="34"/>
+      <c r="BN5" s="34"/>
+      <c r="BO5" s="34"/>
+      <c r="BP5" s="34"/>
+      <c r="BQ5" s="34"/>
+      <c r="BR5" s="32" t="s">
         <v>73</v>
       </c>
-      <c r="BS5" s="35"/>
-      <c r="BT5" s="35"/>
-      <c r="BU5" s="35"/>
-      <c r="BV5" s="35"/>
-      <c r="BW5" s="35"/>
-      <c r="BX5" s="35"/>
-      <c r="BY5" s="35"/>
-      <c r="BZ5" s="35"/>
-      <c r="CA5" s="35"/>
-      <c r="CB5" s="35"/>
-      <c r="CC5" s="35"/>
-      <c r="CD5" s="35"/>
-      <c r="CE5" s="35"/>
-      <c r="CF5" s="35"/>
-      <c r="CG5" s="35"/>
-      <c r="CH5" s="35"/>
-      <c r="CI5" s="35"/>
-      <c r="CJ5" s="35"/>
-      <c r="CK5" s="35"/>
-      <c r="CL5" s="35"/>
-      <c r="CM5" s="35"/>
-      <c r="CN5" s="35"/>
-      <c r="CO5" s="35"/>
-      <c r="CP5" s="35"/>
-      <c r="CQ5" s="35"/>
-      <c r="CR5" s="35"/>
-      <c r="CS5" s="35"/>
-      <c r="CT5" s="35"/>
-      <c r="CU5" s="42" t="s">
+      <c r="BS5" s="32"/>
+      <c r="BT5" s="32"/>
+      <c r="BU5" s="32"/>
+      <c r="BV5" s="32"/>
+      <c r="BW5" s="32"/>
+      <c r="BX5" s="32"/>
+      <c r="BY5" s="32"/>
+      <c r="BZ5" s="32"/>
+      <c r="CA5" s="32"/>
+      <c r="CB5" s="32"/>
+      <c r="CC5" s="32"/>
+      <c r="CD5" s="32"/>
+      <c r="CE5" s="32"/>
+      <c r="CF5" s="32"/>
+      <c r="CG5" s="32"/>
+      <c r="CH5" s="32"/>
+      <c r="CI5" s="32"/>
+      <c r="CJ5" s="32"/>
+      <c r="CK5" s="32"/>
+      <c r="CL5" s="32"/>
+      <c r="CM5" s="32"/>
+      <c r="CN5" s="32"/>
+      <c r="CO5" s="32"/>
+      <c r="CP5" s="32"/>
+      <c r="CQ5" s="32"/>
+      <c r="CR5" s="32"/>
+      <c r="CS5" s="32"/>
+      <c r="CT5" s="32"/>
+      <c r="CU5" s="39" t="s">
         <v>94</v>
       </c>
-      <c r="CV5" s="42"/>
-      <c r="CW5" s="42"/>
-      <c r="CX5" s="42"/>
-      <c r="CY5" s="42"/>
-      <c r="CZ5" s="42"/>
-      <c r="DA5" s="42"/>
-      <c r="DB5" s="42"/>
-      <c r="DC5" s="42"/>
-      <c r="DD5" s="42"/>
-      <c r="DE5" s="42"/>
-      <c r="DF5" s="42"/>
-      <c r="DG5" s="42"/>
-      <c r="DH5" s="42"/>
-      <c r="DI5" s="42"/>
-      <c r="DJ5" s="41" t="s">
+      <c r="CV5" s="39"/>
+      <c r="CW5" s="39"/>
+      <c r="CX5" s="39"/>
+      <c r="CY5" s="39"/>
+      <c r="CZ5" s="39"/>
+      <c r="DA5" s="39"/>
+      <c r="DB5" s="39"/>
+      <c r="DC5" s="39"/>
+      <c r="DD5" s="39"/>
+      <c r="DE5" s="39"/>
+      <c r="DF5" s="39"/>
+      <c r="DG5" s="39"/>
+      <c r="DH5" s="39"/>
+      <c r="DI5" s="39"/>
+      <c r="DJ5" s="38" t="s">
         <v>108</v>
       </c>
-      <c r="DK5" s="41"/>
-      <c r="DL5" s="41"/>
-      <c r="DM5" s="41"/>
-      <c r="DN5" s="45" t="s">
+      <c r="DK5" s="38"/>
+      <c r="DL5" s="38"/>
+      <c r="DM5" s="38"/>
+      <c r="DN5" s="42" t="s">
         <v>109</v>
       </c>
-      <c r="DO5" s="45"/>
+      <c r="DO5" s="42"/>
       <c r="DP5" s="17" t="s">
         <v>112</v>
       </c>
@@ -1359,59 +1393,70 @@
       <c r="DT5" s="16" t="s">
         <v>120</v>
       </c>
-      <c r="DU5" s="40" t="s">
+      <c r="DU5" s="37" t="s">
         <v>121</v>
       </c>
-      <c r="DV5" s="40"/>
-      <c r="DW5" s="40"/>
-      <c r="DX5" s="40"/>
-      <c r="DY5" s="40"/>
-      <c r="DZ5" s="40"/>
-      <c r="EA5" s="40"/>
-      <c r="EB5" s="40"/>
-      <c r="EC5" s="44" t="s">
+      <c r="DV5" s="37"/>
+      <c r="DW5" s="37"/>
+      <c r="DX5" s="37"/>
+      <c r="DY5" s="37"/>
+      <c r="DZ5" s="37"/>
+      <c r="EA5" s="37"/>
+      <c r="EB5" s="37"/>
+      <c r="EC5" s="41" t="s">
         <v>130</v>
       </c>
-      <c r="ED5" s="44"/>
-      <c r="EE5" s="44"/>
-      <c r="EF5" s="44"/>
-      <c r="EG5" s="44"/>
-      <c r="EH5" s="44"/>
-      <c r="EI5" s="44"/>
-      <c r="EJ5" s="44"/>
-      <c r="EK5" s="44"/>
-      <c r="EL5" s="44"/>
-      <c r="EM5" s="44"/>
-      <c r="EN5" s="44"/>
-      <c r="EO5" s="43" t="s">
+      <c r="ED5" s="41"/>
+      <c r="EE5" s="41"/>
+      <c r="EF5" s="41"/>
+      <c r="EG5" s="41"/>
+      <c r="EH5" s="41"/>
+      <c r="EI5" s="41"/>
+      <c r="EJ5" s="41"/>
+      <c r="EK5" s="41"/>
+      <c r="EL5" s="41"/>
+      <c r="EM5" s="41"/>
+      <c r="EN5" s="41"/>
+      <c r="EO5" s="40" t="s">
         <v>143</v>
       </c>
-      <c r="EP5" s="43"/>
-      <c r="EQ5" s="43"/>
-      <c r="ER5" s="43"/>
-      <c r="ES5" s="43"/>
-      <c r="ET5" s="43"/>
-      <c r="EU5" s="35" t="s">
+      <c r="EP5" s="40"/>
+      <c r="EQ5" s="40"/>
+      <c r="ER5" s="40"/>
+      <c r="ES5" s="40"/>
+      <c r="ET5" s="40"/>
+      <c r="EU5" s="32" t="s">
         <v>150</v>
       </c>
-      <c r="EV5" s="35"/>
-      <c r="EW5" s="35"/>
-      <c r="EX5" s="35"/>
-      <c r="EY5" s="35"/>
-      <c r="EZ5" s="35"/>
-      <c r="FA5" s="35"/>
-      <c r="FB5" s="35"/>
-      <c r="FC5" s="35"/>
-      <c r="FD5" s="35"/>
-      <c r="FE5" s="35"/>
-      <c r="FF5" s="35"/>
-      <c r="FG5" s="35"/>
-      <c r="FH5" s="46" t="s">
+      <c r="EV5" s="32"/>
+      <c r="EW5" s="32"/>
+      <c r="EX5" s="32"/>
+      <c r="EY5" s="32"/>
+      <c r="EZ5" s="32"/>
+      <c r="FA5" s="32"/>
+      <c r="FB5" s="32"/>
+      <c r="FC5" s="32"/>
+      <c r="FD5" s="32"/>
+      <c r="FE5" s="32"/>
+      <c r="FF5" s="32"/>
+      <c r="FG5" s="32"/>
+      <c r="FH5" s="34" t="s">
+        <v>162</v>
+      </c>
+      <c r="FI5" s="34"/>
+      <c r="FJ5" s="34"/>
+      <c r="FK5" s="34"/>
+      <c r="FL5" s="34"/>
+      <c r="FM5" s="34"/>
+      <c r="FN5" s="34"/>
+      <c r="FO5" s="34"/>
+      <c r="FP5" s="34"/>
+      <c r="FQ5" s="11" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="6" spans="1:164" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="33"/>
+    <row r="6" spans="1:173" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="46"/>
       <c r="B6" s="17"/>
       <c r="C6" s="17"/>
       <c r="D6" s="17"/>
@@ -1480,45 +1525,45 @@
       <c r="BO6" s="21"/>
       <c r="BP6" s="21"/>
       <c r="BQ6" s="21"/>
-      <c r="BR6" s="36" t="s">
+      <c r="BR6" s="33" t="s">
         <v>75</v>
       </c>
-      <c r="BS6" s="36"/>
-      <c r="BT6" s="36"/>
-      <c r="BU6" s="36"/>
-      <c r="BV6" s="36"/>
-      <c r="BW6" s="36"/>
-      <c r="BX6" s="36"/>
-      <c r="BY6" s="36"/>
-      <c r="BZ6" s="36"/>
-      <c r="CA6" s="36"/>
-      <c r="CB6" s="36" t="s">
+      <c r="BS6" s="33"/>
+      <c r="BT6" s="33"/>
+      <c r="BU6" s="33"/>
+      <c r="BV6" s="33"/>
+      <c r="BW6" s="33"/>
+      <c r="BX6" s="33"/>
+      <c r="BY6" s="33"/>
+      <c r="BZ6" s="33"/>
+      <c r="CA6" s="33"/>
+      <c r="CB6" s="33" t="s">
         <v>80</v>
       </c>
-      <c r="CC6" s="36"/>
-      <c r="CD6" s="36"/>
-      <c r="CE6" s="36"/>
-      <c r="CF6" s="36" t="s">
+      <c r="CC6" s="33"/>
+      <c r="CD6" s="33"/>
+      <c r="CE6" s="33"/>
+      <c r="CF6" s="33" t="s">
         <v>83</v>
       </c>
-      <c r="CG6" s="36"/>
-      <c r="CH6" s="36"/>
-      <c r="CI6" s="36" t="s">
+      <c r="CG6" s="33"/>
+      <c r="CH6" s="33"/>
+      <c r="CI6" s="33" t="s">
         <v>86</v>
       </c>
-      <c r="CJ6" s="36"/>
-      <c r="CK6" s="36"/>
-      <c r="CL6" s="36"/>
-      <c r="CM6" s="36"/>
-      <c r="CN6" s="36"/>
-      <c r="CO6" s="36"/>
-      <c r="CP6" s="36"/>
-      <c r="CQ6" s="36"/>
-      <c r="CR6" s="36"/>
-      <c r="CS6" s="36" t="s">
+      <c r="CJ6" s="33"/>
+      <c r="CK6" s="33"/>
+      <c r="CL6" s="33"/>
+      <c r="CM6" s="33"/>
+      <c r="CN6" s="33"/>
+      <c r="CO6" s="33"/>
+      <c r="CP6" s="33"/>
+      <c r="CQ6" s="33"/>
+      <c r="CR6" s="33"/>
+      <c r="CS6" s="33" t="s">
         <v>92</v>
       </c>
-      <c r="CT6" s="36"/>
+      <c r="CT6" s="33"/>
       <c r="CU6" s="11"/>
       <c r="CV6" s="11"/>
       <c r="CW6" s="11"/>
@@ -1584,10 +1629,25 @@
       <c r="FE6" s="29"/>
       <c r="FF6" s="29"/>
       <c r="FG6" s="29"/>
-      <c r="FH6" s="46"/>
+      <c r="FH6" s="31"/>
+      <c r="FI6" s="31"/>
+      <c r="FJ6" s="31" t="s">
+        <v>165</v>
+      </c>
+      <c r="FK6" s="31"/>
+      <c r="FL6" s="31" t="s">
+        <v>168</v>
+      </c>
+      <c r="FM6" s="31"/>
+      <c r="FN6" s="31" t="s">
+        <v>169</v>
+      </c>
+      <c r="FO6" s="31"/>
+      <c r="FP6" s="31"/>
+      <c r="FQ6" s="11"/>
     </row>
-    <row r="7" spans="1:164" s="1" customFormat="1" ht="87" x14ac:dyDescent="0.35">
-      <c r="A7" s="33"/>
+    <row r="7" spans="1:173" s="1" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A7" s="46"/>
       <c r="B7" s="2" t="s">
         <v>2</v>
       </c>
@@ -2075,11 +2135,44 @@
         <v>147</v>
       </c>
       <c r="FH7" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="FI7" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="FJ7" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="FK7" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="FL7" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="FM7" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="FN7" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="FO7" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="FP7" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="FQ7" s="5" t="s">
         <v>161</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="21">
+  <mergeCells count="22">
+    <mergeCell ref="FH5:FP5"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="B5:X5"/>
     <mergeCell ref="EU5:FG5"/>
     <mergeCell ref="CB6:CE6"/>
     <mergeCell ref="BK5:BQ5"/>
@@ -2096,11 +2189,6 @@
     <mergeCell ref="CI6:CR6"/>
     <mergeCell ref="CS6:CT6"/>
     <mergeCell ref="DN5:DO5"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="B5:X5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
OAB : Laporan Penunjang
</commit_message>
<xml_diff>
--- a/Laravel-InaLUTS/resources/templates/Report_OAB.xlsx
+++ b/Laravel-InaLUTS/resources/templates/Report_OAB.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="185">
   <si>
     <t>No</t>
   </si>
@@ -530,6 +530,45 @@
   </si>
   <si>
     <t>Massa intrabuli</t>
+  </si>
+  <si>
+    <t>Penunjang</t>
+  </si>
+  <si>
+    <t>Cara mengukur PVR</t>
+  </si>
+  <si>
+    <t>Mukosa buli</t>
+  </si>
+  <si>
+    <t>Trabekulasi</t>
+  </si>
+  <si>
+    <t>Sakulasi Divertikel</t>
+  </si>
+  <si>
+    <t>Kapasitas Buli</t>
+  </si>
+  <si>
+    <t>Tumor</t>
+  </si>
+  <si>
+    <t>Lobus Medius</t>
+  </si>
+  <si>
+    <t>Kissing Lobe</t>
+  </si>
+  <si>
+    <t>Muara Ureter</t>
+  </si>
+  <si>
+    <t>Urethra</t>
+  </si>
+  <si>
+    <t>MUE</t>
+  </si>
+  <si>
+    <t>Lichen Schlerosis</t>
   </si>
 </sst>
 </file>
@@ -811,15 +850,30 @@
     <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -842,21 +896,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1163,10 +1202,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:FQ7"/>
+  <dimension ref="A1:GF7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="ES1" workbookViewId="0">
-      <selection activeCell="FP8" sqref="FP8"/>
+    <sheetView tabSelected="1" topLeftCell="FI1" workbookViewId="0">
+      <selection activeCell="FR8" sqref="FR8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1198,186 +1237,186 @@
     <col min="173" max="16384" width="9.140625" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:173" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="43"/>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-      <c r="I1" s="43"/>
-      <c r="J1" s="43"/>
-      <c r="K1" s="43"/>
+    <row r="1" spans="1:188" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="33"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
     </row>
-    <row r="2" spans="1:173" x14ac:dyDescent="0.25">
-      <c r="A2" s="44"/>
-      <c r="B2" s="44"/>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="44"/>
-      <c r="I2" s="44"/>
-      <c r="J2" s="44"/>
-      <c r="K2" s="44"/>
+    <row r="2" spans="1:188" x14ac:dyDescent="0.25">
+      <c r="A2" s="34"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
+      <c r="I2" s="34"/>
+      <c r="J2" s="34"/>
+      <c r="K2" s="34"/>
     </row>
-    <row r="3" spans="1:173" x14ac:dyDescent="0.25">
-      <c r="A3" s="45"/>
-      <c r="B3" s="45"/>
-      <c r="C3" s="45"/>
-      <c r="D3" s="45"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="45"/>
-      <c r="G3" s="45"/>
-      <c r="H3" s="45"/>
-      <c r="I3" s="45"/>
-      <c r="J3" s="45"/>
-      <c r="K3" s="45"/>
+    <row r="3" spans="1:188" x14ac:dyDescent="0.25">
+      <c r="A3" s="35"/>
+      <c r="B3" s="35"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="35"/>
+      <c r="I3" s="35"/>
+      <c r="J3" s="35"/>
+      <c r="K3" s="35"/>
     </row>
-    <row r="4" spans="1:173" s="3" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:173" s="1" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="46" t="s">
+    <row r="4" spans="1:188" s="3" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:188" s="1" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="47" t="s">
+      <c r="B5" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="47"/>
-      <c r="D5" s="47"/>
-      <c r="E5" s="47"/>
-      <c r="F5" s="47"/>
-      <c r="G5" s="47"/>
-      <c r="H5" s="47"/>
-      <c r="I5" s="47"/>
-      <c r="J5" s="47"/>
-      <c r="K5" s="47"/>
-      <c r="L5" s="47"/>
-      <c r="M5" s="47"/>
-      <c r="N5" s="47"/>
-      <c r="O5" s="47"/>
-      <c r="P5" s="47"/>
-      <c r="Q5" s="47"/>
-      <c r="R5" s="47"/>
-      <c r="S5" s="47"/>
-      <c r="T5" s="47"/>
-      <c r="U5" s="47"/>
-      <c r="V5" s="47"/>
-      <c r="W5" s="47"/>
-      <c r="X5" s="47"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="37"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="37"/>
+      <c r="G5" s="37"/>
+      <c r="H5" s="37"/>
+      <c r="I5" s="37"/>
+      <c r="J5" s="37"/>
+      <c r="K5" s="37"/>
+      <c r="L5" s="37"/>
+      <c r="M5" s="37"/>
+      <c r="N5" s="37"/>
+      <c r="O5" s="37"/>
+      <c r="P5" s="37"/>
+      <c r="Q5" s="37"/>
+      <c r="R5" s="37"/>
+      <c r="S5" s="37"/>
+      <c r="T5" s="37"/>
+      <c r="U5" s="37"/>
+      <c r="V5" s="37"/>
+      <c r="W5" s="37"/>
+      <c r="X5" s="37"/>
       <c r="Y5" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="Z5" s="35" t="s">
+      <c r="Z5" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="AA5" s="35"/>
-      <c r="AB5" s="35"/>
-      <c r="AC5" s="35"/>
-      <c r="AD5" s="35"/>
-      <c r="AE5" s="35"/>
-      <c r="AF5" s="35"/>
-      <c r="AG5" s="35"/>
-      <c r="AH5" s="35"/>
-      <c r="AI5" s="35"/>
-      <c r="AJ5" s="35"/>
-      <c r="AK5" s="35"/>
-      <c r="AL5" s="36" t="s">
+      <c r="AA5" s="40"/>
+      <c r="AB5" s="40"/>
+      <c r="AC5" s="40"/>
+      <c r="AD5" s="40"/>
+      <c r="AE5" s="40"/>
+      <c r="AF5" s="40"/>
+      <c r="AG5" s="40"/>
+      <c r="AH5" s="40"/>
+      <c r="AI5" s="40"/>
+      <c r="AJ5" s="40"/>
+      <c r="AK5" s="40"/>
+      <c r="AL5" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="AM5" s="36"/>
-      <c r="AN5" s="36"/>
-      <c r="AO5" s="36"/>
-      <c r="AP5" s="36"/>
-      <c r="AQ5" s="36"/>
-      <c r="AR5" s="36"/>
-      <c r="AS5" s="36"/>
-      <c r="AT5" s="36"/>
-      <c r="AU5" s="36"/>
-      <c r="AV5" s="36"/>
-      <c r="AW5" s="36"/>
-      <c r="AX5" s="36"/>
-      <c r="AY5" s="36"/>
-      <c r="AZ5" s="36"/>
-      <c r="BA5" s="36"/>
-      <c r="BB5" s="36"/>
-      <c r="BC5" s="36"/>
-      <c r="BD5" s="36"/>
-      <c r="BE5" s="36"/>
-      <c r="BF5" s="36"/>
-      <c r="BG5" s="36"/>
-      <c r="BH5" s="36"/>
-      <c r="BI5" s="36"/>
-      <c r="BJ5" s="36"/>
-      <c r="BK5" s="34" t="s">
+      <c r="AM5" s="41"/>
+      <c r="AN5" s="41"/>
+      <c r="AO5" s="41"/>
+      <c r="AP5" s="41"/>
+      <c r="AQ5" s="41"/>
+      <c r="AR5" s="41"/>
+      <c r="AS5" s="41"/>
+      <c r="AT5" s="41"/>
+      <c r="AU5" s="41"/>
+      <c r="AV5" s="41"/>
+      <c r="AW5" s="41"/>
+      <c r="AX5" s="41"/>
+      <c r="AY5" s="41"/>
+      <c r="AZ5" s="41"/>
+      <c r="BA5" s="41"/>
+      <c r="BB5" s="41"/>
+      <c r="BC5" s="41"/>
+      <c r="BD5" s="41"/>
+      <c r="BE5" s="41"/>
+      <c r="BF5" s="41"/>
+      <c r="BG5" s="41"/>
+      <c r="BH5" s="41"/>
+      <c r="BI5" s="41"/>
+      <c r="BJ5" s="41"/>
+      <c r="BK5" s="32" t="s">
         <v>72</v>
       </c>
-      <c r="BL5" s="34"/>
-      <c r="BM5" s="34"/>
-      <c r="BN5" s="34"/>
-      <c r="BO5" s="34"/>
-      <c r="BP5" s="34"/>
-      <c r="BQ5" s="34"/>
-      <c r="BR5" s="32" t="s">
+      <c r="BL5" s="32"/>
+      <c r="BM5" s="32"/>
+      <c r="BN5" s="32"/>
+      <c r="BO5" s="32"/>
+      <c r="BP5" s="32"/>
+      <c r="BQ5" s="32"/>
+      <c r="BR5" s="38" t="s">
         <v>73</v>
       </c>
-      <c r="BS5" s="32"/>
-      <c r="BT5" s="32"/>
-      <c r="BU5" s="32"/>
-      <c r="BV5" s="32"/>
-      <c r="BW5" s="32"/>
-      <c r="BX5" s="32"/>
-      <c r="BY5" s="32"/>
-      <c r="BZ5" s="32"/>
-      <c r="CA5" s="32"/>
-      <c r="CB5" s="32"/>
-      <c r="CC5" s="32"/>
-      <c r="CD5" s="32"/>
-      <c r="CE5" s="32"/>
-      <c r="CF5" s="32"/>
-      <c r="CG5" s="32"/>
-      <c r="CH5" s="32"/>
-      <c r="CI5" s="32"/>
-      <c r="CJ5" s="32"/>
-      <c r="CK5" s="32"/>
-      <c r="CL5" s="32"/>
-      <c r="CM5" s="32"/>
-      <c r="CN5" s="32"/>
-      <c r="CO5" s="32"/>
-      <c r="CP5" s="32"/>
-      <c r="CQ5" s="32"/>
-      <c r="CR5" s="32"/>
-      <c r="CS5" s="32"/>
-      <c r="CT5" s="32"/>
-      <c r="CU5" s="39" t="s">
+      <c r="BS5" s="38"/>
+      <c r="BT5" s="38"/>
+      <c r="BU5" s="38"/>
+      <c r="BV5" s="38"/>
+      <c r="BW5" s="38"/>
+      <c r="BX5" s="38"/>
+      <c r="BY5" s="38"/>
+      <c r="BZ5" s="38"/>
+      <c r="CA5" s="38"/>
+      <c r="CB5" s="38"/>
+      <c r="CC5" s="38"/>
+      <c r="CD5" s="38"/>
+      <c r="CE5" s="38"/>
+      <c r="CF5" s="38"/>
+      <c r="CG5" s="38"/>
+      <c r="CH5" s="38"/>
+      <c r="CI5" s="38"/>
+      <c r="CJ5" s="38"/>
+      <c r="CK5" s="38"/>
+      <c r="CL5" s="38"/>
+      <c r="CM5" s="38"/>
+      <c r="CN5" s="38"/>
+      <c r="CO5" s="38"/>
+      <c r="CP5" s="38"/>
+      <c r="CQ5" s="38"/>
+      <c r="CR5" s="38"/>
+      <c r="CS5" s="38"/>
+      <c r="CT5" s="38"/>
+      <c r="CU5" s="44" t="s">
         <v>94</v>
       </c>
-      <c r="CV5" s="39"/>
-      <c r="CW5" s="39"/>
-      <c r="CX5" s="39"/>
-      <c r="CY5" s="39"/>
-      <c r="CZ5" s="39"/>
-      <c r="DA5" s="39"/>
-      <c r="DB5" s="39"/>
-      <c r="DC5" s="39"/>
-      <c r="DD5" s="39"/>
-      <c r="DE5" s="39"/>
-      <c r="DF5" s="39"/>
-      <c r="DG5" s="39"/>
-      <c r="DH5" s="39"/>
-      <c r="DI5" s="39"/>
-      <c r="DJ5" s="38" t="s">
+      <c r="CV5" s="44"/>
+      <c r="CW5" s="44"/>
+      <c r="CX5" s="44"/>
+      <c r="CY5" s="44"/>
+      <c r="CZ5" s="44"/>
+      <c r="DA5" s="44"/>
+      <c r="DB5" s="44"/>
+      <c r="DC5" s="44"/>
+      <c r="DD5" s="44"/>
+      <c r="DE5" s="44"/>
+      <c r="DF5" s="44"/>
+      <c r="DG5" s="44"/>
+      <c r="DH5" s="44"/>
+      <c r="DI5" s="44"/>
+      <c r="DJ5" s="43" t="s">
         <v>108</v>
       </c>
-      <c r="DK5" s="38"/>
-      <c r="DL5" s="38"/>
-      <c r="DM5" s="38"/>
-      <c r="DN5" s="42" t="s">
+      <c r="DK5" s="43"/>
+      <c r="DL5" s="43"/>
+      <c r="DM5" s="43"/>
+      <c r="DN5" s="47" t="s">
         <v>109</v>
       </c>
-      <c r="DO5" s="42"/>
+      <c r="DO5" s="47"/>
       <c r="DP5" s="17" t="s">
         <v>112</v>
       </c>
@@ -1393,70 +1432,87 @@
       <c r="DT5" s="16" t="s">
         <v>120</v>
       </c>
-      <c r="DU5" s="37" t="s">
+      <c r="DU5" s="42" t="s">
         <v>121</v>
       </c>
-      <c r="DV5" s="37"/>
-      <c r="DW5" s="37"/>
-      <c r="DX5" s="37"/>
-      <c r="DY5" s="37"/>
-      <c r="DZ5" s="37"/>
-      <c r="EA5" s="37"/>
-      <c r="EB5" s="37"/>
-      <c r="EC5" s="41" t="s">
+      <c r="DV5" s="42"/>
+      <c r="DW5" s="42"/>
+      <c r="DX5" s="42"/>
+      <c r="DY5" s="42"/>
+      <c r="DZ5" s="42"/>
+      <c r="EA5" s="42"/>
+      <c r="EB5" s="42"/>
+      <c r="EC5" s="46" t="s">
         <v>130</v>
       </c>
-      <c r="ED5" s="41"/>
-      <c r="EE5" s="41"/>
-      <c r="EF5" s="41"/>
-      <c r="EG5" s="41"/>
-      <c r="EH5" s="41"/>
-      <c r="EI5" s="41"/>
-      <c r="EJ5" s="41"/>
-      <c r="EK5" s="41"/>
-      <c r="EL5" s="41"/>
-      <c r="EM5" s="41"/>
-      <c r="EN5" s="41"/>
-      <c r="EO5" s="40" t="s">
+      <c r="ED5" s="46"/>
+      <c r="EE5" s="46"/>
+      <c r="EF5" s="46"/>
+      <c r="EG5" s="46"/>
+      <c r="EH5" s="46"/>
+      <c r="EI5" s="46"/>
+      <c r="EJ5" s="46"/>
+      <c r="EK5" s="46"/>
+      <c r="EL5" s="46"/>
+      <c r="EM5" s="46"/>
+      <c r="EN5" s="46"/>
+      <c r="EO5" s="45" t="s">
         <v>143</v>
       </c>
-      <c r="EP5" s="40"/>
-      <c r="EQ5" s="40"/>
-      <c r="ER5" s="40"/>
-      <c r="ES5" s="40"/>
-      <c r="ET5" s="40"/>
-      <c r="EU5" s="32" t="s">
+      <c r="EP5" s="45"/>
+      <c r="EQ5" s="45"/>
+      <c r="ER5" s="45"/>
+      <c r="ES5" s="45"/>
+      <c r="ET5" s="45"/>
+      <c r="EU5" s="38" t="s">
         <v>150</v>
       </c>
-      <c r="EV5" s="32"/>
-      <c r="EW5" s="32"/>
-      <c r="EX5" s="32"/>
-      <c r="EY5" s="32"/>
-      <c r="EZ5" s="32"/>
-      <c r="FA5" s="32"/>
-      <c r="FB5" s="32"/>
-      <c r="FC5" s="32"/>
-      <c r="FD5" s="32"/>
-      <c r="FE5" s="32"/>
-      <c r="FF5" s="32"/>
-      <c r="FG5" s="32"/>
-      <c r="FH5" s="34" t="s">
+      <c r="EV5" s="38"/>
+      <c r="EW5" s="38"/>
+      <c r="EX5" s="38"/>
+      <c r="EY5" s="38"/>
+      <c r="EZ5" s="38"/>
+      <c r="FA5" s="38"/>
+      <c r="FB5" s="38"/>
+      <c r="FC5" s="38"/>
+      <c r="FD5" s="38"/>
+      <c r="FE5" s="38"/>
+      <c r="FF5" s="38"/>
+      <c r="FG5" s="38"/>
+      <c r="FH5" s="32" t="s">
         <v>162</v>
       </c>
-      <c r="FI5" s="34"/>
-      <c r="FJ5" s="34"/>
-      <c r="FK5" s="34"/>
-      <c r="FL5" s="34"/>
-      <c r="FM5" s="34"/>
-      <c r="FN5" s="34"/>
-      <c r="FO5" s="34"/>
-      <c r="FP5" s="34"/>
+      <c r="FI5" s="32"/>
+      <c r="FJ5" s="32"/>
+      <c r="FK5" s="32"/>
+      <c r="FL5" s="32"/>
+      <c r="FM5" s="32"/>
+      <c r="FN5" s="32"/>
+      <c r="FO5" s="32"/>
+      <c r="FP5" s="32"/>
       <c r="FQ5" s="11" t="s">
         <v>161</v>
       </c>
+      <c r="FR5" s="43" t="s">
+        <v>172</v>
+      </c>
+      <c r="FS5" s="43"/>
+      <c r="FT5" s="43"/>
+      <c r="FU5" s="43"/>
+      <c r="FV5" s="43"/>
+      <c r="FW5" s="43"/>
+      <c r="FX5" s="43"/>
+      <c r="FY5" s="43"/>
+      <c r="FZ5" s="43"/>
+      <c r="GA5" s="43"/>
+      <c r="GB5" s="43"/>
+      <c r="GC5" s="43"/>
+      <c r="GD5" s="43"/>
+      <c r="GE5" s="43"/>
+      <c r="GF5" s="43"/>
     </row>
-    <row r="6" spans="1:173" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="46"/>
+    <row r="6" spans="1:188" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="36"/>
       <c r="B6" s="17"/>
       <c r="C6" s="17"/>
       <c r="D6" s="17"/>
@@ -1525,45 +1581,45 @@
       <c r="BO6" s="21"/>
       <c r="BP6" s="21"/>
       <c r="BQ6" s="21"/>
-      <c r="BR6" s="33" t="s">
+      <c r="BR6" s="39" t="s">
         <v>75</v>
       </c>
-      <c r="BS6" s="33"/>
-      <c r="BT6" s="33"/>
-      <c r="BU6" s="33"/>
-      <c r="BV6" s="33"/>
-      <c r="BW6" s="33"/>
-      <c r="BX6" s="33"/>
-      <c r="BY6" s="33"/>
-      <c r="BZ6" s="33"/>
-      <c r="CA6" s="33"/>
-      <c r="CB6" s="33" t="s">
+      <c r="BS6" s="39"/>
+      <c r="BT6" s="39"/>
+      <c r="BU6" s="39"/>
+      <c r="BV6" s="39"/>
+      <c r="BW6" s="39"/>
+      <c r="BX6" s="39"/>
+      <c r="BY6" s="39"/>
+      <c r="BZ6" s="39"/>
+      <c r="CA6" s="39"/>
+      <c r="CB6" s="39" t="s">
         <v>80</v>
       </c>
-      <c r="CC6" s="33"/>
-      <c r="CD6" s="33"/>
-      <c r="CE6" s="33"/>
-      <c r="CF6" s="33" t="s">
+      <c r="CC6" s="39"/>
+      <c r="CD6" s="39"/>
+      <c r="CE6" s="39"/>
+      <c r="CF6" s="39" t="s">
         <v>83</v>
       </c>
-      <c r="CG6" s="33"/>
-      <c r="CH6" s="33"/>
-      <c r="CI6" s="33" t="s">
+      <c r="CG6" s="39"/>
+      <c r="CH6" s="39"/>
+      <c r="CI6" s="39" t="s">
         <v>86</v>
       </c>
-      <c r="CJ6" s="33"/>
-      <c r="CK6" s="33"/>
-      <c r="CL6" s="33"/>
-      <c r="CM6" s="33"/>
-      <c r="CN6" s="33"/>
-      <c r="CO6" s="33"/>
-      <c r="CP6" s="33"/>
-      <c r="CQ6" s="33"/>
-      <c r="CR6" s="33"/>
-      <c r="CS6" s="33" t="s">
+      <c r="CJ6" s="39"/>
+      <c r="CK6" s="39"/>
+      <c r="CL6" s="39"/>
+      <c r="CM6" s="39"/>
+      <c r="CN6" s="39"/>
+      <c r="CO6" s="39"/>
+      <c r="CP6" s="39"/>
+      <c r="CQ6" s="39"/>
+      <c r="CR6" s="39"/>
+      <c r="CS6" s="39" t="s">
         <v>92</v>
       </c>
-      <c r="CT6" s="33"/>
+      <c r="CT6" s="39"/>
       <c r="CU6" s="11"/>
       <c r="CV6" s="11"/>
       <c r="CW6" s="11"/>
@@ -1645,9 +1701,24 @@
       <c r="FO6" s="31"/>
       <c r="FP6" s="31"/>
       <c r="FQ6" s="11"/>
+      <c r="FR6" s="12"/>
+      <c r="FS6" s="12"/>
+      <c r="FT6" s="12"/>
+      <c r="FU6" s="12"/>
+      <c r="FV6" s="12"/>
+      <c r="FW6" s="12"/>
+      <c r="FX6" s="12"/>
+      <c r="FY6" s="12"/>
+      <c r="FZ6" s="12"/>
+      <c r="GA6" s="12"/>
+      <c r="GB6" s="12"/>
+      <c r="GC6" s="12"/>
+      <c r="GD6" s="12"/>
+      <c r="GE6" s="12"/>
+      <c r="GF6" s="12"/>
     </row>
-    <row r="7" spans="1:173" s="1" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A7" s="46"/>
+    <row r="7" spans="1:188" s="1" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A7" s="36"/>
       <c r="B7" s="2" t="s">
         <v>2</v>
       </c>
@@ -2164,9 +2235,61 @@
       <c r="FQ7" s="5" t="s">
         <v>161</v>
       </c>
+      <c r="FR7" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="FS7" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="FT7" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="FU7" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="FV7" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="FW7" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="FX7" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="FY7" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="FZ7" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="GA7" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="GB7" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="GC7" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="GD7" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="GE7" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="GF7" s="4" t="s">
+        <v>184</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="22">
+  <mergeCells count="23">
+    <mergeCell ref="FR5:GF5"/>
+    <mergeCell ref="EO5:ET5"/>
+    <mergeCell ref="EC5:EN5"/>
+    <mergeCell ref="CF6:CH6"/>
+    <mergeCell ref="CI6:CR6"/>
+    <mergeCell ref="CS6:CT6"/>
+    <mergeCell ref="DN5:DO5"/>
     <mergeCell ref="FH5:FP5"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="A2:K2"/>
@@ -2183,12 +2306,6 @@
     <mergeCell ref="DJ5:DM5"/>
     <mergeCell ref="CU5:DI5"/>
     <mergeCell ref="BR6:CA6"/>
-    <mergeCell ref="EO5:ET5"/>
-    <mergeCell ref="EC5:EN5"/>
-    <mergeCell ref="CF6:CH6"/>
-    <mergeCell ref="CI6:CR6"/>
-    <mergeCell ref="CS6:CT6"/>
-    <mergeCell ref="DN5:DO5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
OAB : Laporan Terapi
</commit_message>
<xml_diff>
--- a/Laravel-InaLUTS/resources/templates/Report_OAB.xlsx
+++ b/Laravel-InaLUTS/resources/templates/Report_OAB.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="186">
   <si>
     <t>No</t>
   </si>
@@ -569,6 +569,9 @@
   </si>
   <si>
     <t>Lichen Schlerosis</t>
+  </si>
+  <si>
+    <t>Terapi</t>
   </si>
 </sst>
 </file>
@@ -755,7 +758,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -850,6 +853,24 @@
     <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -871,9 +892,6 @@
     <xf numFmtId="0" fontId="1" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -883,19 +901,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1202,10 +1208,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:GF7"/>
+  <dimension ref="A1:GG500"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="FI1" workbookViewId="0">
-      <selection activeCell="FR8" sqref="FR8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1237,186 +1243,186 @@
     <col min="173" max="16384" width="9.140625" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:188" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="33"/>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
-      <c r="K1" s="33"/>
+    <row r="1" spans="1:189" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="39"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
+      <c r="J1" s="39"/>
+      <c r="K1" s="39"/>
     </row>
-    <row r="2" spans="1:188" x14ac:dyDescent="0.25">
-      <c r="A2" s="34"/>
-      <c r="B2" s="34"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
-      <c r="H2" s="34"/>
-      <c r="I2" s="34"/>
-      <c r="J2" s="34"/>
-      <c r="K2" s="34"/>
+    <row r="2" spans="1:189" x14ac:dyDescent="0.25">
+      <c r="A2" s="40"/>
+      <c r="B2" s="40"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="40"/>
+      <c r="K2" s="40"/>
     </row>
-    <row r="3" spans="1:188" x14ac:dyDescent="0.25">
-      <c r="A3" s="35"/>
-      <c r="B3" s="35"/>
-      <c r="C3" s="35"/>
-      <c r="D3" s="35"/>
-      <c r="E3" s="35"/>
-      <c r="F3" s="35"/>
-      <c r="G3" s="35"/>
-      <c r="H3" s="35"/>
-      <c r="I3" s="35"/>
-      <c r="J3" s="35"/>
-      <c r="K3" s="35"/>
+    <row r="3" spans="1:189" x14ac:dyDescent="0.25">
+      <c r="A3" s="41"/>
+      <c r="B3" s="41"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="41"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="41"/>
+      <c r="I3" s="41"/>
+      <c r="J3" s="41"/>
+      <c r="K3" s="41"/>
     </row>
-    <row r="4" spans="1:188" s="3" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:188" s="1" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="36" t="s">
+    <row r="4" spans="1:189" s="3" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:189" s="1" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="37" t="s">
+      <c r="B5" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="37"/>
-      <c r="D5" s="37"/>
-      <c r="E5" s="37"/>
-      <c r="F5" s="37"/>
-      <c r="G5" s="37"/>
-      <c r="H5" s="37"/>
-      <c r="I5" s="37"/>
-      <c r="J5" s="37"/>
-      <c r="K5" s="37"/>
-      <c r="L5" s="37"/>
-      <c r="M5" s="37"/>
-      <c r="N5" s="37"/>
-      <c r="O5" s="37"/>
-      <c r="P5" s="37"/>
-      <c r="Q5" s="37"/>
-      <c r="R5" s="37"/>
-      <c r="S5" s="37"/>
-      <c r="T5" s="37"/>
-      <c r="U5" s="37"/>
-      <c r="V5" s="37"/>
-      <c r="W5" s="37"/>
-      <c r="X5" s="37"/>
+      <c r="C5" s="43"/>
+      <c r="D5" s="43"/>
+      <c r="E5" s="43"/>
+      <c r="F5" s="43"/>
+      <c r="G5" s="43"/>
+      <c r="H5" s="43"/>
+      <c r="I5" s="43"/>
+      <c r="J5" s="43"/>
+      <c r="K5" s="43"/>
+      <c r="L5" s="43"/>
+      <c r="M5" s="43"/>
+      <c r="N5" s="43"/>
+      <c r="O5" s="43"/>
+      <c r="P5" s="43"/>
+      <c r="Q5" s="43"/>
+      <c r="R5" s="43"/>
+      <c r="S5" s="43"/>
+      <c r="T5" s="43"/>
+      <c r="U5" s="43"/>
+      <c r="V5" s="43"/>
+      <c r="W5" s="43"/>
+      <c r="X5" s="43"/>
       <c r="Y5" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="Z5" s="40" t="s">
+      <c r="Z5" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="AA5" s="40"/>
-      <c r="AB5" s="40"/>
-      <c r="AC5" s="40"/>
-      <c r="AD5" s="40"/>
-      <c r="AE5" s="40"/>
-      <c r="AF5" s="40"/>
-      <c r="AG5" s="40"/>
-      <c r="AH5" s="40"/>
-      <c r="AI5" s="40"/>
-      <c r="AJ5" s="40"/>
-      <c r="AK5" s="40"/>
-      <c r="AL5" s="41" t="s">
+      <c r="AA5" s="45"/>
+      <c r="AB5" s="45"/>
+      <c r="AC5" s="45"/>
+      <c r="AD5" s="45"/>
+      <c r="AE5" s="45"/>
+      <c r="AF5" s="45"/>
+      <c r="AG5" s="45"/>
+      <c r="AH5" s="45"/>
+      <c r="AI5" s="45"/>
+      <c r="AJ5" s="45"/>
+      <c r="AK5" s="45"/>
+      <c r="AL5" s="46" t="s">
         <v>40</v>
       </c>
-      <c r="AM5" s="41"/>
-      <c r="AN5" s="41"/>
-      <c r="AO5" s="41"/>
-      <c r="AP5" s="41"/>
-      <c r="AQ5" s="41"/>
-      <c r="AR5" s="41"/>
-      <c r="AS5" s="41"/>
-      <c r="AT5" s="41"/>
-      <c r="AU5" s="41"/>
-      <c r="AV5" s="41"/>
-      <c r="AW5" s="41"/>
-      <c r="AX5" s="41"/>
-      <c r="AY5" s="41"/>
-      <c r="AZ5" s="41"/>
-      <c r="BA5" s="41"/>
-      <c r="BB5" s="41"/>
-      <c r="BC5" s="41"/>
-      <c r="BD5" s="41"/>
-      <c r="BE5" s="41"/>
-      <c r="BF5" s="41"/>
-      <c r="BG5" s="41"/>
-      <c r="BH5" s="41"/>
-      <c r="BI5" s="41"/>
-      <c r="BJ5" s="41"/>
-      <c r="BK5" s="32" t="s">
+      <c r="AM5" s="46"/>
+      <c r="AN5" s="46"/>
+      <c r="AO5" s="46"/>
+      <c r="AP5" s="46"/>
+      <c r="AQ5" s="46"/>
+      <c r="AR5" s="46"/>
+      <c r="AS5" s="46"/>
+      <c r="AT5" s="46"/>
+      <c r="AU5" s="46"/>
+      <c r="AV5" s="46"/>
+      <c r="AW5" s="46"/>
+      <c r="AX5" s="46"/>
+      <c r="AY5" s="46"/>
+      <c r="AZ5" s="46"/>
+      <c r="BA5" s="46"/>
+      <c r="BB5" s="46"/>
+      <c r="BC5" s="46"/>
+      <c r="BD5" s="46"/>
+      <c r="BE5" s="46"/>
+      <c r="BF5" s="46"/>
+      <c r="BG5" s="46"/>
+      <c r="BH5" s="46"/>
+      <c r="BI5" s="46"/>
+      <c r="BJ5" s="46"/>
+      <c r="BK5" s="38" t="s">
         <v>72</v>
       </c>
-      <c r="BL5" s="32"/>
-      <c r="BM5" s="32"/>
-      <c r="BN5" s="32"/>
-      <c r="BO5" s="32"/>
-      <c r="BP5" s="32"/>
-      <c r="BQ5" s="32"/>
-      <c r="BR5" s="38" t="s">
+      <c r="BL5" s="38"/>
+      <c r="BM5" s="38"/>
+      <c r="BN5" s="38"/>
+      <c r="BO5" s="38"/>
+      <c r="BP5" s="38"/>
+      <c r="BQ5" s="38"/>
+      <c r="BR5" s="44" t="s">
         <v>73</v>
       </c>
-      <c r="BS5" s="38"/>
-      <c r="BT5" s="38"/>
-      <c r="BU5" s="38"/>
-      <c r="BV5" s="38"/>
-      <c r="BW5" s="38"/>
-      <c r="BX5" s="38"/>
-      <c r="BY5" s="38"/>
-      <c r="BZ5" s="38"/>
-      <c r="CA5" s="38"/>
-      <c r="CB5" s="38"/>
-      <c r="CC5" s="38"/>
-      <c r="CD5" s="38"/>
-      <c r="CE5" s="38"/>
-      <c r="CF5" s="38"/>
-      <c r="CG5" s="38"/>
-      <c r="CH5" s="38"/>
-      <c r="CI5" s="38"/>
-      <c r="CJ5" s="38"/>
-      <c r="CK5" s="38"/>
-      <c r="CL5" s="38"/>
-      <c r="CM5" s="38"/>
-      <c r="CN5" s="38"/>
-      <c r="CO5" s="38"/>
-      <c r="CP5" s="38"/>
-      <c r="CQ5" s="38"/>
-      <c r="CR5" s="38"/>
-      <c r="CS5" s="38"/>
-      <c r="CT5" s="38"/>
-      <c r="CU5" s="44" t="s">
+      <c r="BS5" s="44"/>
+      <c r="BT5" s="44"/>
+      <c r="BU5" s="44"/>
+      <c r="BV5" s="44"/>
+      <c r="BW5" s="44"/>
+      <c r="BX5" s="44"/>
+      <c r="BY5" s="44"/>
+      <c r="BZ5" s="44"/>
+      <c r="CA5" s="44"/>
+      <c r="CB5" s="44"/>
+      <c r="CC5" s="44"/>
+      <c r="CD5" s="44"/>
+      <c r="CE5" s="44"/>
+      <c r="CF5" s="44"/>
+      <c r="CG5" s="44"/>
+      <c r="CH5" s="44"/>
+      <c r="CI5" s="44"/>
+      <c r="CJ5" s="44"/>
+      <c r="CK5" s="44"/>
+      <c r="CL5" s="44"/>
+      <c r="CM5" s="44"/>
+      <c r="CN5" s="44"/>
+      <c r="CO5" s="44"/>
+      <c r="CP5" s="44"/>
+      <c r="CQ5" s="44"/>
+      <c r="CR5" s="44"/>
+      <c r="CS5" s="44"/>
+      <c r="CT5" s="44"/>
+      <c r="CU5" s="48" t="s">
         <v>94</v>
       </c>
-      <c r="CV5" s="44"/>
-      <c r="CW5" s="44"/>
-      <c r="CX5" s="44"/>
-      <c r="CY5" s="44"/>
-      <c r="CZ5" s="44"/>
-      <c r="DA5" s="44"/>
-      <c r="DB5" s="44"/>
-      <c r="DC5" s="44"/>
-      <c r="DD5" s="44"/>
-      <c r="DE5" s="44"/>
-      <c r="DF5" s="44"/>
-      <c r="DG5" s="44"/>
-      <c r="DH5" s="44"/>
-      <c r="DI5" s="44"/>
-      <c r="DJ5" s="43" t="s">
+      <c r="CV5" s="48"/>
+      <c r="CW5" s="48"/>
+      <c r="CX5" s="48"/>
+      <c r="CY5" s="48"/>
+      <c r="CZ5" s="48"/>
+      <c r="DA5" s="48"/>
+      <c r="DB5" s="48"/>
+      <c r="DC5" s="48"/>
+      <c r="DD5" s="48"/>
+      <c r="DE5" s="48"/>
+      <c r="DF5" s="48"/>
+      <c r="DG5" s="48"/>
+      <c r="DH5" s="48"/>
+      <c r="DI5" s="48"/>
+      <c r="DJ5" s="33" t="s">
         <v>108</v>
       </c>
-      <c r="DK5" s="43"/>
-      <c r="DL5" s="43"/>
-      <c r="DM5" s="43"/>
-      <c r="DN5" s="47" t="s">
+      <c r="DK5" s="33"/>
+      <c r="DL5" s="33"/>
+      <c r="DM5" s="33"/>
+      <c r="DN5" s="37" t="s">
         <v>109</v>
       </c>
-      <c r="DO5" s="47"/>
+      <c r="DO5" s="37"/>
       <c r="DP5" s="17" t="s">
         <v>112</v>
       </c>
@@ -1432,87 +1438,90 @@
       <c r="DT5" s="16" t="s">
         <v>120</v>
       </c>
-      <c r="DU5" s="42" t="s">
+      <c r="DU5" s="47" t="s">
         <v>121</v>
       </c>
-      <c r="DV5" s="42"/>
-      <c r="DW5" s="42"/>
-      <c r="DX5" s="42"/>
-      <c r="DY5" s="42"/>
-      <c r="DZ5" s="42"/>
-      <c r="EA5" s="42"/>
-      <c r="EB5" s="42"/>
-      <c r="EC5" s="46" t="s">
+      <c r="DV5" s="47"/>
+      <c r="DW5" s="47"/>
+      <c r="DX5" s="47"/>
+      <c r="DY5" s="47"/>
+      <c r="DZ5" s="47"/>
+      <c r="EA5" s="47"/>
+      <c r="EB5" s="47"/>
+      <c r="EC5" s="35" t="s">
         <v>130</v>
       </c>
-      <c r="ED5" s="46"/>
-      <c r="EE5" s="46"/>
-      <c r="EF5" s="46"/>
-      <c r="EG5" s="46"/>
-      <c r="EH5" s="46"/>
-      <c r="EI5" s="46"/>
-      <c r="EJ5" s="46"/>
-      <c r="EK5" s="46"/>
-      <c r="EL5" s="46"/>
-      <c r="EM5" s="46"/>
-      <c r="EN5" s="46"/>
-      <c r="EO5" s="45" t="s">
+      <c r="ED5" s="35"/>
+      <c r="EE5" s="35"/>
+      <c r="EF5" s="35"/>
+      <c r="EG5" s="35"/>
+      <c r="EH5" s="35"/>
+      <c r="EI5" s="35"/>
+      <c r="EJ5" s="35"/>
+      <c r="EK5" s="35"/>
+      <c r="EL5" s="35"/>
+      <c r="EM5" s="35"/>
+      <c r="EN5" s="35"/>
+      <c r="EO5" s="34" t="s">
         <v>143</v>
       </c>
-      <c r="EP5" s="45"/>
-      <c r="EQ5" s="45"/>
-      <c r="ER5" s="45"/>
-      <c r="ES5" s="45"/>
-      <c r="ET5" s="45"/>
-      <c r="EU5" s="38" t="s">
+      <c r="EP5" s="34"/>
+      <c r="EQ5" s="34"/>
+      <c r="ER5" s="34"/>
+      <c r="ES5" s="34"/>
+      <c r="ET5" s="34"/>
+      <c r="EU5" s="44" t="s">
         <v>150</v>
       </c>
-      <c r="EV5" s="38"/>
-      <c r="EW5" s="38"/>
-      <c r="EX5" s="38"/>
-      <c r="EY5" s="38"/>
-      <c r="EZ5" s="38"/>
-      <c r="FA5" s="38"/>
-      <c r="FB5" s="38"/>
-      <c r="FC5" s="38"/>
-      <c r="FD5" s="38"/>
-      <c r="FE5" s="38"/>
-      <c r="FF5" s="38"/>
-      <c r="FG5" s="38"/>
-      <c r="FH5" s="32" t="s">
+      <c r="EV5" s="44"/>
+      <c r="EW5" s="44"/>
+      <c r="EX5" s="44"/>
+      <c r="EY5" s="44"/>
+      <c r="EZ5" s="44"/>
+      <c r="FA5" s="44"/>
+      <c r="FB5" s="44"/>
+      <c r="FC5" s="44"/>
+      <c r="FD5" s="44"/>
+      <c r="FE5" s="44"/>
+      <c r="FF5" s="44"/>
+      <c r="FG5" s="44"/>
+      <c r="FH5" s="38" t="s">
         <v>162</v>
       </c>
-      <c r="FI5" s="32"/>
-      <c r="FJ5" s="32"/>
-      <c r="FK5" s="32"/>
-      <c r="FL5" s="32"/>
-      <c r="FM5" s="32"/>
-      <c r="FN5" s="32"/>
-      <c r="FO5" s="32"/>
-      <c r="FP5" s="32"/>
+      <c r="FI5" s="38"/>
+      <c r="FJ5" s="38"/>
+      <c r="FK5" s="38"/>
+      <c r="FL5" s="38"/>
+      <c r="FM5" s="38"/>
+      <c r="FN5" s="38"/>
+      <c r="FO5" s="38"/>
+      <c r="FP5" s="38"/>
       <c r="FQ5" s="11" t="s">
         <v>161</v>
       </c>
-      <c r="FR5" s="43" t="s">
+      <c r="FR5" s="33" t="s">
         <v>172</v>
       </c>
-      <c r="FS5" s="43"/>
-      <c r="FT5" s="43"/>
-      <c r="FU5" s="43"/>
-      <c r="FV5" s="43"/>
-      <c r="FW5" s="43"/>
-      <c r="FX5" s="43"/>
-      <c r="FY5" s="43"/>
-      <c r="FZ5" s="43"/>
-      <c r="GA5" s="43"/>
-      <c r="GB5" s="43"/>
-      <c r="GC5" s="43"/>
-      <c r="GD5" s="43"/>
-      <c r="GE5" s="43"/>
-      <c r="GF5" s="43"/>
+      <c r="FS5" s="33"/>
+      <c r="FT5" s="33"/>
+      <c r="FU5" s="33"/>
+      <c r="FV5" s="33"/>
+      <c r="FW5" s="33"/>
+      <c r="FX5" s="33"/>
+      <c r="FY5" s="33"/>
+      <c r="FZ5" s="33"/>
+      <c r="GA5" s="33"/>
+      <c r="GB5" s="33"/>
+      <c r="GC5" s="33"/>
+      <c r="GD5" s="33"/>
+      <c r="GE5" s="33"/>
+      <c r="GF5" s="33"/>
+      <c r="GG5" s="13" t="s">
+        <v>185</v>
+      </c>
     </row>
-    <row r="6" spans="1:188" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="36"/>
+    <row r="6" spans="1:189" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="42"/>
       <c r="B6" s="17"/>
       <c r="C6" s="17"/>
       <c r="D6" s="17"/>
@@ -1581,45 +1590,45 @@
       <c r="BO6" s="21"/>
       <c r="BP6" s="21"/>
       <c r="BQ6" s="21"/>
-      <c r="BR6" s="39" t="s">
+      <c r="BR6" s="36" t="s">
         <v>75</v>
       </c>
-      <c r="BS6" s="39"/>
-      <c r="BT6" s="39"/>
-      <c r="BU6" s="39"/>
-      <c r="BV6" s="39"/>
-      <c r="BW6" s="39"/>
-      <c r="BX6" s="39"/>
-      <c r="BY6" s="39"/>
-      <c r="BZ6" s="39"/>
-      <c r="CA6" s="39"/>
-      <c r="CB6" s="39" t="s">
+      <c r="BS6" s="36"/>
+      <c r="BT6" s="36"/>
+      <c r="BU6" s="36"/>
+      <c r="BV6" s="36"/>
+      <c r="BW6" s="36"/>
+      <c r="BX6" s="36"/>
+      <c r="BY6" s="36"/>
+      <c r="BZ6" s="36"/>
+      <c r="CA6" s="36"/>
+      <c r="CB6" s="36" t="s">
         <v>80</v>
       </c>
-      <c r="CC6" s="39"/>
-      <c r="CD6" s="39"/>
-      <c r="CE6" s="39"/>
-      <c r="CF6" s="39" t="s">
+      <c r="CC6" s="36"/>
+      <c r="CD6" s="36"/>
+      <c r="CE6" s="36"/>
+      <c r="CF6" s="36" t="s">
         <v>83</v>
       </c>
-      <c r="CG6" s="39"/>
-      <c r="CH6" s="39"/>
-      <c r="CI6" s="39" t="s">
+      <c r="CG6" s="36"/>
+      <c r="CH6" s="36"/>
+      <c r="CI6" s="36" t="s">
         <v>86</v>
       </c>
-      <c r="CJ6" s="39"/>
-      <c r="CK6" s="39"/>
-      <c r="CL6" s="39"/>
-      <c r="CM6" s="39"/>
-      <c r="CN6" s="39"/>
-      <c r="CO6" s="39"/>
-      <c r="CP6" s="39"/>
-      <c r="CQ6" s="39"/>
-      <c r="CR6" s="39"/>
-      <c r="CS6" s="39" t="s">
+      <c r="CJ6" s="36"/>
+      <c r="CK6" s="36"/>
+      <c r="CL6" s="36"/>
+      <c r="CM6" s="36"/>
+      <c r="CN6" s="36"/>
+      <c r="CO6" s="36"/>
+      <c r="CP6" s="36"/>
+      <c r="CQ6" s="36"/>
+      <c r="CR6" s="36"/>
+      <c r="CS6" s="36" t="s">
         <v>92</v>
       </c>
-      <c r="CT6" s="39"/>
+      <c r="CT6" s="36"/>
       <c r="CU6" s="11"/>
       <c r="CV6" s="11"/>
       <c r="CW6" s="11"/>
@@ -1716,9 +1725,10 @@
       <c r="GD6" s="12"/>
       <c r="GE6" s="12"/>
       <c r="GF6" s="12"/>
+      <c r="GG6" s="13"/>
     </row>
-    <row r="7" spans="1:188" s="1" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A7" s="36"/>
+    <row r="7" spans="1:189" s="1" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A7" s="42"/>
       <c r="B7" s="2" t="s">
         <v>2</v>
       </c>
@@ -2280,23 +2290,505 @@
       <c r="GF7" s="4" t="s">
         <v>184</v>
       </c>
+      <c r="GG7" s="6" t="s">
+        <v>185</v>
+      </c>
     </row>
+    <row r="8" spans="1:189" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:189" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:189" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:189" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:189" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:189" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:189" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:189" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:189" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="17" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="18" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="19" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="20" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="21" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="22" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="23" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="24" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="25" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="26" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="27" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="29" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="30" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="31" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="32" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="33" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="34" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="35" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="37" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="38" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="39" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="40" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="42" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="44" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="45" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="46" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="47" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="48" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="49" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="50" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="51" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="55" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="56" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="57" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="58" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="59" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="60" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="61" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="62" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="63" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="64" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="65" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="66" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="67" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="68" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="69" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="70" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="71" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="72" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="73" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="74" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="75" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="76" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="77" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="78" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="79" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="80" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="81" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="82" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="83" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="84" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="85" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="86" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="87" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="88" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="89" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="90" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="91" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="92" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="93" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="94" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="95" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="96" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="97" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="98" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="99" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="100" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="101" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="102" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="103" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="104" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="105" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="106" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="107" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="108" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="109" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="110" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="111" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="112" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="113" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="114" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="115" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="116" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="117" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="118" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="119" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="120" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="121" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="122" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="123" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="124" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="125" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="126" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="127" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="128" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="129" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="130" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="131" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="132" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="133" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="134" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="135" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="136" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="137" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="138" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="139" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="140" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="141" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="142" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="143" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="144" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="145" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="146" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="147" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="148" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="149" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="150" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="151" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="152" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="153" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="154" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="155" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="156" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="157" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="158" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="159" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="160" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="161" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="162" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="163" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="164" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="165" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="166" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="167" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="168" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="169" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="170" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="171" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="172" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="173" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="174" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="175" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="176" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="177" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="178" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="179" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="180" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="181" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="182" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="183" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="184" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="185" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="186" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="187" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="188" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="189" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="190" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="191" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="192" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="193" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="194" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="195" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="196" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="197" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="198" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="199" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="200" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="201" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="202" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="203" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="204" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="205" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="206" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="207" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="208" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="209" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="210" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="211" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="212" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="213" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="214" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="215" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="216" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="217" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="218" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="219" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="220" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="221" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="222" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="223" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="224" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="225" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="226" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="227" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="228" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="229" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="230" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="231" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="232" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="233" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="234" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="235" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="236" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="237" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="238" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="239" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="240" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="241" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="242" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="243" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="244" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="245" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="246" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="247" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="248" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="249" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="250" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="251" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="252" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="253" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="254" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="255" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="256" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="257" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="258" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="259" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="260" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="261" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="262" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="263" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="264" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="265" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="266" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="267" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="268" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="269" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="270" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="271" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="272" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="273" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="274" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="275" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="276" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="277" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="278" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="279" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="280" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="281" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="282" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="283" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="284" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="285" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="286" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="287" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="288" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="289" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="290" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="291" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="292" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="293" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="294" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="295" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="296" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="297" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="298" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="299" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="300" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="301" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="302" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="303" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="304" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="305" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="306" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="307" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="308" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="309" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="310" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="311" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="312" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="313" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="314" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="315" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="316" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="317" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="318" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="319" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="320" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="321" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="322" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="323" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="324" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="325" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="326" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="327" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="328" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="329" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="330" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="331" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="332" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="333" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="334" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="335" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="336" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="337" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="338" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="339" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="340" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="341" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="342" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="343" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="344" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="345" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="346" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="347" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="348" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="349" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="350" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="351" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="352" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="353" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="354" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="355" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="356" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="357" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="358" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="359" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="360" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="361" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="362" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="363" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="364" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="365" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="366" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="367" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="368" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="369" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="370" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="371" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="372" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="373" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="374" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="375" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="376" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="377" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="378" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="379" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="380" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="381" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="382" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="383" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="384" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="385" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="386" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="387" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="388" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="389" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="390" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="391" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="392" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="393" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="394" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="395" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="396" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="397" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="398" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="399" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="400" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="401" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="402" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="403" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="404" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="405" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="406" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="407" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="408" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="409" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="410" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="411" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="412" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="413" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="414" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="415" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="416" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="417" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="418" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="419" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="420" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="421" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="422" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="423" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="424" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="425" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="426" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="427" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="428" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="429" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="430" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="431" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="432" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="433" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="434" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="435" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="436" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="437" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="438" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="439" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="440" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="441" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="442" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="443" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="444" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="445" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="446" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="447" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="448" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="449" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="450" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="451" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="452" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="453" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="454" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="455" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="456" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="457" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="458" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="459" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="460" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="461" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="462" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="463" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="464" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="465" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="466" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="467" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="468" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="469" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="470" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="471" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="472" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="473" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="474" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="475" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="476" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="477" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="478" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="479" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="480" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="481" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="482" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="483" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="484" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="485" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="486" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="487" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="488" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="489" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="490" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="491" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="492" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="493" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="494" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="495" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="496" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="497" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="498" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="499" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="500" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="FR5:GF5"/>
-    <mergeCell ref="EO5:ET5"/>
-    <mergeCell ref="EC5:EN5"/>
-    <mergeCell ref="CF6:CH6"/>
-    <mergeCell ref="CI6:CR6"/>
-    <mergeCell ref="CS6:CT6"/>
-    <mergeCell ref="DN5:DO5"/>
-    <mergeCell ref="FH5:FP5"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="B5:X5"/>
-    <mergeCell ref="EU5:FG5"/>
     <mergeCell ref="CB6:CE6"/>
     <mergeCell ref="BK5:BQ5"/>
     <mergeCell ref="Z5:AK5"/>
@@ -2306,6 +2798,20 @@
     <mergeCell ref="DJ5:DM5"/>
     <mergeCell ref="CU5:DI5"/>
     <mergeCell ref="BR6:CA6"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="B5:X5"/>
+    <mergeCell ref="FR5:GF5"/>
+    <mergeCell ref="EO5:ET5"/>
+    <mergeCell ref="EC5:EN5"/>
+    <mergeCell ref="CF6:CH6"/>
+    <mergeCell ref="CI6:CR6"/>
+    <mergeCell ref="CS6:CT6"/>
+    <mergeCell ref="DN5:DO5"/>
+    <mergeCell ref="FH5:FP5"/>
+    <mergeCell ref="EU5:FG5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
OAB : Laporan Terapi Modifikasi Gaya Hidup
</commit_message>
<xml_diff>
--- a/Laravel-InaLUTS/resources/templates/Report_OAB.xlsx
+++ b/Laravel-InaLUTS/resources/templates/Report_OAB.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="193">
   <si>
     <t>No</t>
   </si>
@@ -572,6 +572,27 @@
   </si>
   <si>
     <t>Terapi</t>
+  </si>
+  <si>
+    <t>Terapi Modifikasi Gaya Hidup</t>
+  </si>
+  <si>
+    <t>Menurunkan berat badan</t>
+  </si>
+  <si>
+    <t>Penilaian jenis dan jumlah asupan cairan</t>
+  </si>
+  <si>
+    <t>Bladder training</t>
+  </si>
+  <si>
+    <t>Stop merokok</t>
+  </si>
+  <si>
+    <t>Manajemen stress</t>
+  </si>
+  <si>
+    <t>Manajemen komorbid (termasuk konstipasi, PPOK, asma, dll)</t>
   </si>
 </sst>
 </file>
@@ -856,52 +877,52 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1208,10 +1229,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:GG500"/>
+  <dimension ref="A1:GN500"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="GA1" workbookViewId="0">
+      <selection activeCell="GN8" sqref="GN8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1240,189 +1261,196 @@
     <col min="121" max="125" width="10.7109375" style="19" customWidth="1"/>
     <col min="126" max="163" width="9.140625" style="19"/>
     <col min="164" max="172" width="9.140625" style="30"/>
-    <col min="173" max="16384" width="9.140625" style="19"/>
+    <col min="173" max="188" width="9.140625" style="19"/>
+    <col min="189" max="189" width="20.7109375" style="19" customWidth="1"/>
+    <col min="190" max="190" width="10.7109375" style="19" customWidth="1"/>
+    <col min="191" max="192" width="9.140625" style="19"/>
+    <col min="193" max="193" width="20.7109375" style="19" customWidth="1"/>
+    <col min="194" max="195" width="9.140625" style="19"/>
+    <col min="196" max="196" width="20.7109375" style="19" customWidth="1"/>
+    <col min="197" max="16384" width="9.140625" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:189" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="39"/>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
-      <c r="I1" s="39"/>
-      <c r="J1" s="39"/>
-      <c r="K1" s="39"/>
+    <row r="1" spans="1:196" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="41"/>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
+      <c r="J1" s="41"/>
+      <c r="K1" s="41"/>
     </row>
-    <row r="2" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A2" s="40"/>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
-      <c r="J2" s="40"/>
-      <c r="K2" s="40"/>
+    <row r="2" spans="1:196" x14ac:dyDescent="0.25">
+      <c r="A2" s="42"/>
+      <c r="B2" s="42"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="42"/>
+      <c r="K2" s="42"/>
     </row>
-    <row r="3" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A3" s="41"/>
-      <c r="B3" s="41"/>
-      <c r="C3" s="41"/>
-      <c r="D3" s="41"/>
-      <c r="E3" s="41"/>
-      <c r="F3" s="41"/>
-      <c r="G3" s="41"/>
-      <c r="H3" s="41"/>
-      <c r="I3" s="41"/>
-      <c r="J3" s="41"/>
-      <c r="K3" s="41"/>
+    <row r="3" spans="1:196" x14ac:dyDescent="0.25">
+      <c r="A3" s="43"/>
+      <c r="B3" s="43"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="43"/>
+      <c r="J3" s="43"/>
+      <c r="K3" s="43"/>
     </row>
-    <row r="4" spans="1:189" s="3" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:189" s="1" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="42" t="s">
+    <row r="4" spans="1:196" s="3" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:196" s="1" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="43" t="s">
+      <c r="B5" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="43"/>
-      <c r="D5" s="43"/>
-      <c r="E5" s="43"/>
-      <c r="F5" s="43"/>
-      <c r="G5" s="43"/>
-      <c r="H5" s="43"/>
-      <c r="I5" s="43"/>
-      <c r="J5" s="43"/>
-      <c r="K5" s="43"/>
-      <c r="L5" s="43"/>
-      <c r="M5" s="43"/>
-      <c r="N5" s="43"/>
-      <c r="O5" s="43"/>
-      <c r="P5" s="43"/>
-      <c r="Q5" s="43"/>
-      <c r="R5" s="43"/>
-      <c r="S5" s="43"/>
-      <c r="T5" s="43"/>
-      <c r="U5" s="43"/>
-      <c r="V5" s="43"/>
-      <c r="W5" s="43"/>
-      <c r="X5" s="43"/>
+      <c r="C5" s="45"/>
+      <c r="D5" s="45"/>
+      <c r="E5" s="45"/>
+      <c r="F5" s="45"/>
+      <c r="G5" s="45"/>
+      <c r="H5" s="45"/>
+      <c r="I5" s="45"/>
+      <c r="J5" s="45"/>
+      <c r="K5" s="45"/>
+      <c r="L5" s="45"/>
+      <c r="M5" s="45"/>
+      <c r="N5" s="45"/>
+      <c r="O5" s="45"/>
+      <c r="P5" s="45"/>
+      <c r="Q5" s="45"/>
+      <c r="R5" s="45"/>
+      <c r="S5" s="45"/>
+      <c r="T5" s="45"/>
+      <c r="U5" s="45"/>
+      <c r="V5" s="45"/>
+      <c r="W5" s="45"/>
+      <c r="X5" s="45"/>
       <c r="Y5" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="Z5" s="45" t="s">
+      <c r="Z5" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="AA5" s="45"/>
-      <c r="AB5" s="45"/>
-      <c r="AC5" s="45"/>
-      <c r="AD5" s="45"/>
-      <c r="AE5" s="45"/>
-      <c r="AF5" s="45"/>
-      <c r="AG5" s="45"/>
-      <c r="AH5" s="45"/>
-      <c r="AI5" s="45"/>
-      <c r="AJ5" s="45"/>
-      <c r="AK5" s="45"/>
-      <c r="AL5" s="46" t="s">
+      <c r="AA5" s="35"/>
+      <c r="AB5" s="35"/>
+      <c r="AC5" s="35"/>
+      <c r="AD5" s="35"/>
+      <c r="AE5" s="35"/>
+      <c r="AF5" s="35"/>
+      <c r="AG5" s="35"/>
+      <c r="AH5" s="35"/>
+      <c r="AI5" s="35"/>
+      <c r="AJ5" s="35"/>
+      <c r="AK5" s="35"/>
+      <c r="AL5" s="36" t="s">
         <v>40</v>
       </c>
-      <c r="AM5" s="46"/>
-      <c r="AN5" s="46"/>
-      <c r="AO5" s="46"/>
-      <c r="AP5" s="46"/>
-      <c r="AQ5" s="46"/>
-      <c r="AR5" s="46"/>
-      <c r="AS5" s="46"/>
-      <c r="AT5" s="46"/>
-      <c r="AU5" s="46"/>
-      <c r="AV5" s="46"/>
-      <c r="AW5" s="46"/>
-      <c r="AX5" s="46"/>
-      <c r="AY5" s="46"/>
-      <c r="AZ5" s="46"/>
-      <c r="BA5" s="46"/>
-      <c r="BB5" s="46"/>
-      <c r="BC5" s="46"/>
-      <c r="BD5" s="46"/>
-      <c r="BE5" s="46"/>
-      <c r="BF5" s="46"/>
-      <c r="BG5" s="46"/>
-      <c r="BH5" s="46"/>
-      <c r="BI5" s="46"/>
-      <c r="BJ5" s="46"/>
-      <c r="BK5" s="38" t="s">
+      <c r="AM5" s="36"/>
+      <c r="AN5" s="36"/>
+      <c r="AO5" s="36"/>
+      <c r="AP5" s="36"/>
+      <c r="AQ5" s="36"/>
+      <c r="AR5" s="36"/>
+      <c r="AS5" s="36"/>
+      <c r="AT5" s="36"/>
+      <c r="AU5" s="36"/>
+      <c r="AV5" s="36"/>
+      <c r="AW5" s="36"/>
+      <c r="AX5" s="36"/>
+      <c r="AY5" s="36"/>
+      <c r="AZ5" s="36"/>
+      <c r="BA5" s="36"/>
+      <c r="BB5" s="36"/>
+      <c r="BC5" s="36"/>
+      <c r="BD5" s="36"/>
+      <c r="BE5" s="36"/>
+      <c r="BF5" s="36"/>
+      <c r="BG5" s="36"/>
+      <c r="BH5" s="36"/>
+      <c r="BI5" s="36"/>
+      <c r="BJ5" s="36"/>
+      <c r="BK5" s="34" t="s">
         <v>72</v>
       </c>
-      <c r="BL5" s="38"/>
-      <c r="BM5" s="38"/>
-      <c r="BN5" s="38"/>
-      <c r="BO5" s="38"/>
-      <c r="BP5" s="38"/>
-      <c r="BQ5" s="38"/>
-      <c r="BR5" s="44" t="s">
+      <c r="BL5" s="34"/>
+      <c r="BM5" s="34"/>
+      <c r="BN5" s="34"/>
+      <c r="BO5" s="34"/>
+      <c r="BP5" s="34"/>
+      <c r="BQ5" s="34"/>
+      <c r="BR5" s="38" t="s">
         <v>73</v>
       </c>
-      <c r="BS5" s="44"/>
-      <c r="BT5" s="44"/>
-      <c r="BU5" s="44"/>
-      <c r="BV5" s="44"/>
-      <c r="BW5" s="44"/>
-      <c r="BX5" s="44"/>
-      <c r="BY5" s="44"/>
-      <c r="BZ5" s="44"/>
-      <c r="CA5" s="44"/>
-      <c r="CB5" s="44"/>
-      <c r="CC5" s="44"/>
-      <c r="CD5" s="44"/>
-      <c r="CE5" s="44"/>
-      <c r="CF5" s="44"/>
-      <c r="CG5" s="44"/>
-      <c r="CH5" s="44"/>
-      <c r="CI5" s="44"/>
-      <c r="CJ5" s="44"/>
-      <c r="CK5" s="44"/>
-      <c r="CL5" s="44"/>
-      <c r="CM5" s="44"/>
-      <c r="CN5" s="44"/>
-      <c r="CO5" s="44"/>
-      <c r="CP5" s="44"/>
-      <c r="CQ5" s="44"/>
-      <c r="CR5" s="44"/>
-      <c r="CS5" s="44"/>
-      <c r="CT5" s="44"/>
-      <c r="CU5" s="48" t="s">
+      <c r="BS5" s="38"/>
+      <c r="BT5" s="38"/>
+      <c r="BU5" s="38"/>
+      <c r="BV5" s="38"/>
+      <c r="BW5" s="38"/>
+      <c r="BX5" s="38"/>
+      <c r="BY5" s="38"/>
+      <c r="BZ5" s="38"/>
+      <c r="CA5" s="38"/>
+      <c r="CB5" s="38"/>
+      <c r="CC5" s="38"/>
+      <c r="CD5" s="38"/>
+      <c r="CE5" s="38"/>
+      <c r="CF5" s="38"/>
+      <c r="CG5" s="38"/>
+      <c r="CH5" s="38"/>
+      <c r="CI5" s="38"/>
+      <c r="CJ5" s="38"/>
+      <c r="CK5" s="38"/>
+      <c r="CL5" s="38"/>
+      <c r="CM5" s="38"/>
+      <c r="CN5" s="38"/>
+      <c r="CO5" s="38"/>
+      <c r="CP5" s="38"/>
+      <c r="CQ5" s="38"/>
+      <c r="CR5" s="38"/>
+      <c r="CS5" s="38"/>
+      <c r="CT5" s="38"/>
+      <c r="CU5" s="40" t="s">
         <v>94</v>
       </c>
-      <c r="CV5" s="48"/>
-      <c r="CW5" s="48"/>
-      <c r="CX5" s="48"/>
-      <c r="CY5" s="48"/>
-      <c r="CZ5" s="48"/>
-      <c r="DA5" s="48"/>
-      <c r="DB5" s="48"/>
-      <c r="DC5" s="48"/>
-      <c r="DD5" s="48"/>
-      <c r="DE5" s="48"/>
-      <c r="DF5" s="48"/>
-      <c r="DG5" s="48"/>
-      <c r="DH5" s="48"/>
-      <c r="DI5" s="48"/>
-      <c r="DJ5" s="33" t="s">
+      <c r="CV5" s="40"/>
+      <c r="CW5" s="40"/>
+      <c r="CX5" s="40"/>
+      <c r="CY5" s="40"/>
+      <c r="CZ5" s="40"/>
+      <c r="DA5" s="40"/>
+      <c r="DB5" s="40"/>
+      <c r="DC5" s="40"/>
+      <c r="DD5" s="40"/>
+      <c r="DE5" s="40"/>
+      <c r="DF5" s="40"/>
+      <c r="DG5" s="40"/>
+      <c r="DH5" s="40"/>
+      <c r="DI5" s="40"/>
+      <c r="DJ5" s="39" t="s">
         <v>108</v>
       </c>
-      <c r="DK5" s="33"/>
-      <c r="DL5" s="33"/>
-      <c r="DM5" s="33"/>
-      <c r="DN5" s="37" t="s">
+      <c r="DK5" s="39"/>
+      <c r="DL5" s="39"/>
+      <c r="DM5" s="39"/>
+      <c r="DN5" s="48" t="s">
         <v>109</v>
       </c>
-      <c r="DO5" s="37"/>
+      <c r="DO5" s="48"/>
       <c r="DP5" s="17" t="s">
         <v>112</v>
       </c>
@@ -1438,90 +1466,99 @@
       <c r="DT5" s="16" t="s">
         <v>120</v>
       </c>
-      <c r="DU5" s="47" t="s">
+      <c r="DU5" s="37" t="s">
         <v>121</v>
       </c>
-      <c r="DV5" s="47"/>
-      <c r="DW5" s="47"/>
-      <c r="DX5" s="47"/>
-      <c r="DY5" s="47"/>
-      <c r="DZ5" s="47"/>
-      <c r="EA5" s="47"/>
-      <c r="EB5" s="47"/>
-      <c r="EC5" s="35" t="s">
+      <c r="DV5" s="37"/>
+      <c r="DW5" s="37"/>
+      <c r="DX5" s="37"/>
+      <c r="DY5" s="37"/>
+      <c r="DZ5" s="37"/>
+      <c r="EA5" s="37"/>
+      <c r="EB5" s="37"/>
+      <c r="EC5" s="47" t="s">
         <v>130</v>
       </c>
-      <c r="ED5" s="35"/>
-      <c r="EE5" s="35"/>
-      <c r="EF5" s="35"/>
-      <c r="EG5" s="35"/>
-      <c r="EH5" s="35"/>
-      <c r="EI5" s="35"/>
-      <c r="EJ5" s="35"/>
-      <c r="EK5" s="35"/>
-      <c r="EL5" s="35"/>
-      <c r="EM5" s="35"/>
-      <c r="EN5" s="35"/>
-      <c r="EO5" s="34" t="s">
+      <c r="ED5" s="47"/>
+      <c r="EE5" s="47"/>
+      <c r="EF5" s="47"/>
+      <c r="EG5" s="47"/>
+      <c r="EH5" s="47"/>
+      <c r="EI5" s="47"/>
+      <c r="EJ5" s="47"/>
+      <c r="EK5" s="47"/>
+      <c r="EL5" s="47"/>
+      <c r="EM5" s="47"/>
+      <c r="EN5" s="47"/>
+      <c r="EO5" s="46" t="s">
         <v>143</v>
       </c>
-      <c r="EP5" s="34"/>
-      <c r="EQ5" s="34"/>
-      <c r="ER5" s="34"/>
-      <c r="ES5" s="34"/>
-      <c r="ET5" s="34"/>
-      <c r="EU5" s="44" t="s">
+      <c r="EP5" s="46"/>
+      <c r="EQ5" s="46"/>
+      <c r="ER5" s="46"/>
+      <c r="ES5" s="46"/>
+      <c r="ET5" s="46"/>
+      <c r="EU5" s="38" t="s">
         <v>150</v>
       </c>
-      <c r="EV5" s="44"/>
-      <c r="EW5" s="44"/>
-      <c r="EX5" s="44"/>
-      <c r="EY5" s="44"/>
-      <c r="EZ5" s="44"/>
-      <c r="FA5" s="44"/>
-      <c r="FB5" s="44"/>
-      <c r="FC5" s="44"/>
-      <c r="FD5" s="44"/>
-      <c r="FE5" s="44"/>
-      <c r="FF5" s="44"/>
-      <c r="FG5" s="44"/>
-      <c r="FH5" s="38" t="s">
+      <c r="EV5" s="38"/>
+      <c r="EW5" s="38"/>
+      <c r="EX5" s="38"/>
+      <c r="EY5" s="38"/>
+      <c r="EZ5" s="38"/>
+      <c r="FA5" s="38"/>
+      <c r="FB5" s="38"/>
+      <c r="FC5" s="38"/>
+      <c r="FD5" s="38"/>
+      <c r="FE5" s="38"/>
+      <c r="FF5" s="38"/>
+      <c r="FG5" s="38"/>
+      <c r="FH5" s="34" t="s">
         <v>162</v>
       </c>
-      <c r="FI5" s="38"/>
-      <c r="FJ5" s="38"/>
-      <c r="FK5" s="38"/>
-      <c r="FL5" s="38"/>
-      <c r="FM5" s="38"/>
-      <c r="FN5" s="38"/>
-      <c r="FO5" s="38"/>
-      <c r="FP5" s="38"/>
+      <c r="FI5" s="34"/>
+      <c r="FJ5" s="34"/>
+      <c r="FK5" s="34"/>
+      <c r="FL5" s="34"/>
+      <c r="FM5" s="34"/>
+      <c r="FN5" s="34"/>
+      <c r="FO5" s="34"/>
+      <c r="FP5" s="34"/>
       <c r="FQ5" s="11" t="s">
         <v>161</v>
       </c>
-      <c r="FR5" s="33" t="s">
+      <c r="FR5" s="39" t="s">
         <v>172</v>
       </c>
-      <c r="FS5" s="33"/>
-      <c r="FT5" s="33"/>
-      <c r="FU5" s="33"/>
-      <c r="FV5" s="33"/>
-      <c r="FW5" s="33"/>
-      <c r="FX5" s="33"/>
-      <c r="FY5" s="33"/>
-      <c r="FZ5" s="33"/>
-      <c r="GA5" s="33"/>
-      <c r="GB5" s="33"/>
-      <c r="GC5" s="33"/>
-      <c r="GD5" s="33"/>
-      <c r="GE5" s="33"/>
-      <c r="GF5" s="33"/>
+      <c r="FS5" s="39"/>
+      <c r="FT5" s="39"/>
+      <c r="FU5" s="39"/>
+      <c r="FV5" s="39"/>
+      <c r="FW5" s="39"/>
+      <c r="FX5" s="39"/>
+      <c r="FY5" s="39"/>
+      <c r="FZ5" s="39"/>
+      <c r="GA5" s="39"/>
+      <c r="GB5" s="39"/>
+      <c r="GC5" s="39"/>
+      <c r="GD5" s="39"/>
+      <c r="GE5" s="39"/>
+      <c r="GF5" s="39"/>
       <c r="GG5" s="13" t="s">
         <v>185</v>
       </c>
+      <c r="GH5" s="45" t="s">
+        <v>186</v>
+      </c>
+      <c r="GI5" s="45"/>
+      <c r="GJ5" s="45"/>
+      <c r="GK5" s="45"/>
+      <c r="GL5" s="45"/>
+      <c r="GM5" s="45"/>
+      <c r="GN5" s="45"/>
     </row>
-    <row r="6" spans="1:189" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="42"/>
+    <row r="6" spans="1:196" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="44"/>
       <c r="B6" s="17"/>
       <c r="C6" s="17"/>
       <c r="D6" s="17"/>
@@ -1590,45 +1627,45 @@
       <c r="BO6" s="21"/>
       <c r="BP6" s="21"/>
       <c r="BQ6" s="21"/>
-      <c r="BR6" s="36" t="s">
+      <c r="BR6" s="33" t="s">
         <v>75</v>
       </c>
-      <c r="BS6" s="36"/>
-      <c r="BT6" s="36"/>
-      <c r="BU6" s="36"/>
-      <c r="BV6" s="36"/>
-      <c r="BW6" s="36"/>
-      <c r="BX6" s="36"/>
-      <c r="BY6" s="36"/>
-      <c r="BZ6" s="36"/>
-      <c r="CA6" s="36"/>
-      <c r="CB6" s="36" t="s">
+      <c r="BS6" s="33"/>
+      <c r="BT6" s="33"/>
+      <c r="BU6" s="33"/>
+      <c r="BV6" s="33"/>
+      <c r="BW6" s="33"/>
+      <c r="BX6" s="33"/>
+      <c r="BY6" s="33"/>
+      <c r="BZ6" s="33"/>
+      <c r="CA6" s="33"/>
+      <c r="CB6" s="33" t="s">
         <v>80</v>
       </c>
-      <c r="CC6" s="36"/>
-      <c r="CD6" s="36"/>
-      <c r="CE6" s="36"/>
-      <c r="CF6" s="36" t="s">
+      <c r="CC6" s="33"/>
+      <c r="CD6" s="33"/>
+      <c r="CE6" s="33"/>
+      <c r="CF6" s="33" t="s">
         <v>83</v>
       </c>
-      <c r="CG6" s="36"/>
-      <c r="CH6" s="36"/>
-      <c r="CI6" s="36" t="s">
+      <c r="CG6" s="33"/>
+      <c r="CH6" s="33"/>
+      <c r="CI6" s="33" t="s">
         <v>86</v>
       </c>
-      <c r="CJ6" s="36"/>
-      <c r="CK6" s="36"/>
-      <c r="CL6" s="36"/>
-      <c r="CM6" s="36"/>
-      <c r="CN6" s="36"/>
-      <c r="CO6" s="36"/>
-      <c r="CP6" s="36"/>
-      <c r="CQ6" s="36"/>
-      <c r="CR6" s="36"/>
-      <c r="CS6" s="36" t="s">
+      <c r="CJ6" s="33"/>
+      <c r="CK6" s="33"/>
+      <c r="CL6" s="33"/>
+      <c r="CM6" s="33"/>
+      <c r="CN6" s="33"/>
+      <c r="CO6" s="33"/>
+      <c r="CP6" s="33"/>
+      <c r="CQ6" s="33"/>
+      <c r="CR6" s="33"/>
+      <c r="CS6" s="33" t="s">
         <v>92</v>
       </c>
-      <c r="CT6" s="36"/>
+      <c r="CT6" s="33"/>
       <c r="CU6" s="11"/>
       <c r="CV6" s="11"/>
       <c r="CW6" s="11"/>
@@ -1726,9 +1763,16 @@
       <c r="GE6" s="12"/>
       <c r="GF6" s="12"/>
       <c r="GG6" s="13"/>
+      <c r="GH6" s="14"/>
+      <c r="GI6" s="14"/>
+      <c r="GJ6" s="14"/>
+      <c r="GK6" s="14"/>
+      <c r="GL6" s="14"/>
+      <c r="GM6" s="14"/>
+      <c r="GN6" s="14"/>
     </row>
-    <row r="7" spans="1:189" s="1" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A7" s="42"/>
+    <row r="7" spans="1:196" s="1" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A7" s="44"/>
       <c r="B7" s="2" t="s">
         <v>2</v>
       </c>
@@ -2293,16 +2337,37 @@
       <c r="GG7" s="6" t="s">
         <v>185</v>
       </c>
+      <c r="GH7" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="GI7" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="GJ7" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="GK7" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="GL7" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="GM7" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="GN7" s="2" t="s">
+        <v>192</v>
+      </c>
     </row>
-    <row r="8" spans="1:189" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:189" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:189" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:189" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:189" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:189" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:189" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:189" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:189" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:196" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:196" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:196" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:196" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:196" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:196" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:196" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:196" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:196" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="17" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="18" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="19" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -2788,7 +2853,22 @@
     <row r="499" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="500" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="23">
+  <mergeCells count="24">
+    <mergeCell ref="GH5:GN5"/>
+    <mergeCell ref="FR5:GF5"/>
+    <mergeCell ref="EO5:ET5"/>
+    <mergeCell ref="EC5:EN5"/>
+    <mergeCell ref="CF6:CH6"/>
+    <mergeCell ref="CI6:CR6"/>
+    <mergeCell ref="CS6:CT6"/>
+    <mergeCell ref="DN5:DO5"/>
+    <mergeCell ref="FH5:FP5"/>
+    <mergeCell ref="EU5:FG5"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="B5:X5"/>
     <mergeCell ref="CB6:CE6"/>
     <mergeCell ref="BK5:BQ5"/>
     <mergeCell ref="Z5:AK5"/>
@@ -2798,20 +2878,6 @@
     <mergeCell ref="DJ5:DM5"/>
     <mergeCell ref="CU5:DI5"/>
     <mergeCell ref="BR6:CA6"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="B5:X5"/>
-    <mergeCell ref="FR5:GF5"/>
-    <mergeCell ref="EO5:ET5"/>
-    <mergeCell ref="EC5:EN5"/>
-    <mergeCell ref="CF6:CH6"/>
-    <mergeCell ref="CI6:CR6"/>
-    <mergeCell ref="CS6:CT6"/>
-    <mergeCell ref="DN5:DO5"/>
-    <mergeCell ref="FH5:FP5"/>
-    <mergeCell ref="EU5:FG5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
OAB : Laporan Terapi Rehabilitasi
</commit_message>
<xml_diff>
--- a/Laravel-InaLUTS/resources/templates/Report_OAB.xlsx
+++ b/Laravel-InaLUTS/resources/templates/Report_OAB.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="204">
   <si>
     <t>No</t>
   </si>
@@ -593,6 +593,39 @@
   </si>
   <si>
     <t>Manajemen komorbid (termasuk konstipasi, PPOK, asma, dll)</t>
+  </si>
+  <si>
+    <t>Terapi Rehabilitasi</t>
+  </si>
+  <si>
+    <t>Penilaian otot dasar panggul</t>
+  </si>
+  <si>
+    <t>Oxford</t>
+  </si>
+  <si>
+    <t>Biofeedback</t>
+  </si>
+  <si>
+    <t>Max Power</t>
+  </si>
+  <si>
+    <t>Durasi</t>
+  </si>
+  <si>
+    <t>Latihan penguatan otot dasar panggul</t>
+  </si>
+  <si>
+    <t>Latihan relaksasi otot dasar panggul</t>
+  </si>
+  <si>
+    <t>Kursi magnetic</t>
+  </si>
+  <si>
+    <t>PTNS</t>
+  </si>
+  <si>
+    <t>TTNS</t>
   </si>
 </sst>
 </file>
@@ -779,7 +812,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -877,12 +910,45 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -892,37 +958,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1229,10 +1265,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:GN500"/>
+  <dimension ref="A1:HA500"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="GA1" workbookViewId="0">
-      <selection activeCell="GN8" sqref="GN8"/>
+    <sheetView tabSelected="1" topLeftCell="GH1" workbookViewId="0">
+      <selection activeCell="HA8" sqref="HA8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1268,189 +1304,194 @@
     <col min="193" max="193" width="20.7109375" style="19" customWidth="1"/>
     <col min="194" max="195" width="9.140625" style="19"/>
     <col min="196" max="196" width="20.7109375" style="19" customWidth="1"/>
-    <col min="197" max="16384" width="9.140625" style="19"/>
+    <col min="197" max="197" width="10.7109375" style="19" customWidth="1"/>
+    <col min="198" max="201" width="9.140625" style="19"/>
+    <col min="202" max="202" width="10.7109375" style="19" customWidth="1"/>
+    <col min="203" max="206" width="9.140625" style="19"/>
+    <col min="207" max="207" width="10.7109375" style="19" customWidth="1"/>
+    <col min="208" max="16384" width="9.140625" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:196" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="41"/>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
-      <c r="J1" s="41"/>
-      <c r="K1" s="41"/>
+    <row r="1" spans="1:209" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="42"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
+      <c r="K1" s="42"/>
     </row>
-    <row r="2" spans="1:196" x14ac:dyDescent="0.25">
-      <c r="A2" s="42"/>
-      <c r="B2" s="42"/>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="42"/>
-      <c r="G2" s="42"/>
-      <c r="H2" s="42"/>
-      <c r="I2" s="42"/>
-      <c r="J2" s="42"/>
-      <c r="K2" s="42"/>
+    <row r="2" spans="1:209" x14ac:dyDescent="0.25">
+      <c r="A2" s="43"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
+      <c r="K2" s="43"/>
     </row>
-    <row r="3" spans="1:196" x14ac:dyDescent="0.25">
-      <c r="A3" s="43"/>
-      <c r="B3" s="43"/>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="43"/>
-      <c r="K3" s="43"/>
+    <row r="3" spans="1:209" x14ac:dyDescent="0.25">
+      <c r="A3" s="44"/>
+      <c r="B3" s="44"/>
+      <c r="C3" s="44"/>
+      <c r="D3" s="44"/>
+      <c r="E3" s="44"/>
+      <c r="F3" s="44"/>
+      <c r="G3" s="44"/>
+      <c r="H3" s="44"/>
+      <c r="I3" s="44"/>
+      <c r="J3" s="44"/>
+      <c r="K3" s="44"/>
     </row>
-    <row r="4" spans="1:196" s="3" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:196" s="1" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="44" t="s">
+    <row r="4" spans="1:209" s="3" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:209" s="1" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="45" t="s">
+      <c r="B5" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="45"/>
-      <c r="D5" s="45"/>
-      <c r="E5" s="45"/>
-      <c r="F5" s="45"/>
-      <c r="G5" s="45"/>
-      <c r="H5" s="45"/>
-      <c r="I5" s="45"/>
-      <c r="J5" s="45"/>
-      <c r="K5" s="45"/>
-      <c r="L5" s="45"/>
-      <c r="M5" s="45"/>
-      <c r="N5" s="45"/>
-      <c r="O5" s="45"/>
-      <c r="P5" s="45"/>
-      <c r="Q5" s="45"/>
-      <c r="R5" s="45"/>
-      <c r="S5" s="45"/>
-      <c r="T5" s="45"/>
-      <c r="U5" s="45"/>
-      <c r="V5" s="45"/>
-      <c r="W5" s="45"/>
-      <c r="X5" s="45"/>
+      <c r="C5" s="34"/>
+      <c r="D5" s="34"/>
+      <c r="E5" s="34"/>
+      <c r="F5" s="34"/>
+      <c r="G5" s="34"/>
+      <c r="H5" s="34"/>
+      <c r="I5" s="34"/>
+      <c r="J5" s="34"/>
+      <c r="K5" s="34"/>
+      <c r="L5" s="34"/>
+      <c r="M5" s="34"/>
+      <c r="N5" s="34"/>
+      <c r="O5" s="34"/>
+      <c r="P5" s="34"/>
+      <c r="Q5" s="34"/>
+      <c r="R5" s="34"/>
+      <c r="S5" s="34"/>
+      <c r="T5" s="34"/>
+      <c r="U5" s="34"/>
+      <c r="V5" s="34"/>
+      <c r="W5" s="34"/>
+      <c r="X5" s="34"/>
       <c r="Y5" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="Z5" s="35" t="s">
+      <c r="Z5" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="AA5" s="35"/>
-      <c r="AB5" s="35"/>
-      <c r="AC5" s="35"/>
-      <c r="AD5" s="35"/>
-      <c r="AE5" s="35"/>
-      <c r="AF5" s="35"/>
-      <c r="AG5" s="35"/>
-      <c r="AH5" s="35"/>
-      <c r="AI5" s="35"/>
-      <c r="AJ5" s="35"/>
-      <c r="AK5" s="35"/>
-      <c r="AL5" s="36" t="s">
+      <c r="AA5" s="46"/>
+      <c r="AB5" s="46"/>
+      <c r="AC5" s="46"/>
+      <c r="AD5" s="46"/>
+      <c r="AE5" s="46"/>
+      <c r="AF5" s="46"/>
+      <c r="AG5" s="46"/>
+      <c r="AH5" s="46"/>
+      <c r="AI5" s="46"/>
+      <c r="AJ5" s="46"/>
+      <c r="AK5" s="46"/>
+      <c r="AL5" s="47" t="s">
         <v>40</v>
       </c>
-      <c r="AM5" s="36"/>
-      <c r="AN5" s="36"/>
-      <c r="AO5" s="36"/>
-      <c r="AP5" s="36"/>
-      <c r="AQ5" s="36"/>
-      <c r="AR5" s="36"/>
-      <c r="AS5" s="36"/>
-      <c r="AT5" s="36"/>
-      <c r="AU5" s="36"/>
-      <c r="AV5" s="36"/>
-      <c r="AW5" s="36"/>
-      <c r="AX5" s="36"/>
-      <c r="AY5" s="36"/>
-      <c r="AZ5" s="36"/>
-      <c r="BA5" s="36"/>
-      <c r="BB5" s="36"/>
-      <c r="BC5" s="36"/>
-      <c r="BD5" s="36"/>
-      <c r="BE5" s="36"/>
-      <c r="BF5" s="36"/>
-      <c r="BG5" s="36"/>
-      <c r="BH5" s="36"/>
-      <c r="BI5" s="36"/>
-      <c r="BJ5" s="36"/>
-      <c r="BK5" s="34" t="s">
+      <c r="AM5" s="47"/>
+      <c r="AN5" s="47"/>
+      <c r="AO5" s="47"/>
+      <c r="AP5" s="47"/>
+      <c r="AQ5" s="47"/>
+      <c r="AR5" s="47"/>
+      <c r="AS5" s="47"/>
+      <c r="AT5" s="47"/>
+      <c r="AU5" s="47"/>
+      <c r="AV5" s="47"/>
+      <c r="AW5" s="47"/>
+      <c r="AX5" s="47"/>
+      <c r="AY5" s="47"/>
+      <c r="AZ5" s="47"/>
+      <c r="BA5" s="47"/>
+      <c r="BB5" s="47"/>
+      <c r="BC5" s="47"/>
+      <c r="BD5" s="47"/>
+      <c r="BE5" s="47"/>
+      <c r="BF5" s="47"/>
+      <c r="BG5" s="47"/>
+      <c r="BH5" s="47"/>
+      <c r="BI5" s="47"/>
+      <c r="BJ5" s="47"/>
+      <c r="BK5" s="40" t="s">
         <v>72</v>
       </c>
-      <c r="BL5" s="34"/>
-      <c r="BM5" s="34"/>
-      <c r="BN5" s="34"/>
-      <c r="BO5" s="34"/>
-      <c r="BP5" s="34"/>
-      <c r="BQ5" s="34"/>
-      <c r="BR5" s="38" t="s">
+      <c r="BL5" s="40"/>
+      <c r="BM5" s="40"/>
+      <c r="BN5" s="40"/>
+      <c r="BO5" s="40"/>
+      <c r="BP5" s="40"/>
+      <c r="BQ5" s="40"/>
+      <c r="BR5" s="41" t="s">
         <v>73</v>
       </c>
-      <c r="BS5" s="38"/>
-      <c r="BT5" s="38"/>
-      <c r="BU5" s="38"/>
-      <c r="BV5" s="38"/>
-      <c r="BW5" s="38"/>
-      <c r="BX5" s="38"/>
-      <c r="BY5" s="38"/>
-      <c r="BZ5" s="38"/>
-      <c r="CA5" s="38"/>
-      <c r="CB5" s="38"/>
-      <c r="CC5" s="38"/>
-      <c r="CD5" s="38"/>
-      <c r="CE5" s="38"/>
-      <c r="CF5" s="38"/>
-      <c r="CG5" s="38"/>
-      <c r="CH5" s="38"/>
-      <c r="CI5" s="38"/>
-      <c r="CJ5" s="38"/>
-      <c r="CK5" s="38"/>
-      <c r="CL5" s="38"/>
-      <c r="CM5" s="38"/>
-      <c r="CN5" s="38"/>
-      <c r="CO5" s="38"/>
-      <c r="CP5" s="38"/>
-      <c r="CQ5" s="38"/>
-      <c r="CR5" s="38"/>
-      <c r="CS5" s="38"/>
-      <c r="CT5" s="38"/>
-      <c r="CU5" s="40" t="s">
+      <c r="BS5" s="41"/>
+      <c r="BT5" s="41"/>
+      <c r="BU5" s="41"/>
+      <c r="BV5" s="41"/>
+      <c r="BW5" s="41"/>
+      <c r="BX5" s="41"/>
+      <c r="BY5" s="41"/>
+      <c r="BZ5" s="41"/>
+      <c r="CA5" s="41"/>
+      <c r="CB5" s="41"/>
+      <c r="CC5" s="41"/>
+      <c r="CD5" s="41"/>
+      <c r="CE5" s="41"/>
+      <c r="CF5" s="41"/>
+      <c r="CG5" s="41"/>
+      <c r="CH5" s="41"/>
+      <c r="CI5" s="41"/>
+      <c r="CJ5" s="41"/>
+      <c r="CK5" s="41"/>
+      <c r="CL5" s="41"/>
+      <c r="CM5" s="41"/>
+      <c r="CN5" s="41"/>
+      <c r="CO5" s="41"/>
+      <c r="CP5" s="41"/>
+      <c r="CQ5" s="41"/>
+      <c r="CR5" s="41"/>
+      <c r="CS5" s="41"/>
+      <c r="CT5" s="41"/>
+      <c r="CU5" s="49" t="s">
         <v>94</v>
       </c>
-      <c r="CV5" s="40"/>
-      <c r="CW5" s="40"/>
-      <c r="CX5" s="40"/>
-      <c r="CY5" s="40"/>
-      <c r="CZ5" s="40"/>
-      <c r="DA5" s="40"/>
-      <c r="DB5" s="40"/>
-      <c r="DC5" s="40"/>
-      <c r="DD5" s="40"/>
-      <c r="DE5" s="40"/>
-      <c r="DF5" s="40"/>
-      <c r="DG5" s="40"/>
-      <c r="DH5" s="40"/>
-      <c r="DI5" s="40"/>
-      <c r="DJ5" s="39" t="s">
+      <c r="CV5" s="49"/>
+      <c r="CW5" s="49"/>
+      <c r="CX5" s="49"/>
+      <c r="CY5" s="49"/>
+      <c r="CZ5" s="49"/>
+      <c r="DA5" s="49"/>
+      <c r="DB5" s="49"/>
+      <c r="DC5" s="49"/>
+      <c r="DD5" s="49"/>
+      <c r="DE5" s="49"/>
+      <c r="DF5" s="49"/>
+      <c r="DG5" s="49"/>
+      <c r="DH5" s="49"/>
+      <c r="DI5" s="49"/>
+      <c r="DJ5" s="35" t="s">
         <v>108</v>
       </c>
-      <c r="DK5" s="39"/>
-      <c r="DL5" s="39"/>
-      <c r="DM5" s="39"/>
-      <c r="DN5" s="48" t="s">
+      <c r="DK5" s="35"/>
+      <c r="DL5" s="35"/>
+      <c r="DM5" s="35"/>
+      <c r="DN5" s="39" t="s">
         <v>109</v>
       </c>
-      <c r="DO5" s="48"/>
+      <c r="DO5" s="39"/>
       <c r="DP5" s="17" t="s">
         <v>112</v>
       </c>
@@ -1466,99 +1507,114 @@
       <c r="DT5" s="16" t="s">
         <v>120</v>
       </c>
-      <c r="DU5" s="37" t="s">
+      <c r="DU5" s="48" t="s">
         <v>121</v>
       </c>
-      <c r="DV5" s="37"/>
-      <c r="DW5" s="37"/>
-      <c r="DX5" s="37"/>
-      <c r="DY5" s="37"/>
-      <c r="DZ5" s="37"/>
-      <c r="EA5" s="37"/>
-      <c r="EB5" s="37"/>
-      <c r="EC5" s="47" t="s">
+      <c r="DV5" s="48"/>
+      <c r="DW5" s="48"/>
+      <c r="DX5" s="48"/>
+      <c r="DY5" s="48"/>
+      <c r="DZ5" s="48"/>
+      <c r="EA5" s="48"/>
+      <c r="EB5" s="48"/>
+      <c r="EC5" s="37" t="s">
         <v>130</v>
       </c>
-      <c r="ED5" s="47"/>
-      <c r="EE5" s="47"/>
-      <c r="EF5" s="47"/>
-      <c r="EG5" s="47"/>
-      <c r="EH5" s="47"/>
-      <c r="EI5" s="47"/>
-      <c r="EJ5" s="47"/>
-      <c r="EK5" s="47"/>
-      <c r="EL5" s="47"/>
-      <c r="EM5" s="47"/>
-      <c r="EN5" s="47"/>
-      <c r="EO5" s="46" t="s">
+      <c r="ED5" s="37"/>
+      <c r="EE5" s="37"/>
+      <c r="EF5" s="37"/>
+      <c r="EG5" s="37"/>
+      <c r="EH5" s="37"/>
+      <c r="EI5" s="37"/>
+      <c r="EJ5" s="37"/>
+      <c r="EK5" s="37"/>
+      <c r="EL5" s="37"/>
+      <c r="EM5" s="37"/>
+      <c r="EN5" s="37"/>
+      <c r="EO5" s="36" t="s">
         <v>143</v>
       </c>
-      <c r="EP5" s="46"/>
-      <c r="EQ5" s="46"/>
-      <c r="ER5" s="46"/>
-      <c r="ES5" s="46"/>
-      <c r="ET5" s="46"/>
-      <c r="EU5" s="38" t="s">
+      <c r="EP5" s="36"/>
+      <c r="EQ5" s="36"/>
+      <c r="ER5" s="36"/>
+      <c r="ES5" s="36"/>
+      <c r="ET5" s="36"/>
+      <c r="EU5" s="41" t="s">
         <v>150</v>
       </c>
-      <c r="EV5" s="38"/>
-      <c r="EW5" s="38"/>
-      <c r="EX5" s="38"/>
-      <c r="EY5" s="38"/>
-      <c r="EZ5" s="38"/>
-      <c r="FA5" s="38"/>
-      <c r="FB5" s="38"/>
-      <c r="FC5" s="38"/>
-      <c r="FD5" s="38"/>
-      <c r="FE5" s="38"/>
-      <c r="FF5" s="38"/>
-      <c r="FG5" s="38"/>
-      <c r="FH5" s="34" t="s">
+      <c r="EV5" s="41"/>
+      <c r="EW5" s="41"/>
+      <c r="EX5" s="41"/>
+      <c r="EY5" s="41"/>
+      <c r="EZ5" s="41"/>
+      <c r="FA5" s="41"/>
+      <c r="FB5" s="41"/>
+      <c r="FC5" s="41"/>
+      <c r="FD5" s="41"/>
+      <c r="FE5" s="41"/>
+      <c r="FF5" s="41"/>
+      <c r="FG5" s="41"/>
+      <c r="FH5" s="40" t="s">
         <v>162</v>
       </c>
-      <c r="FI5" s="34"/>
-      <c r="FJ5" s="34"/>
-      <c r="FK5" s="34"/>
-      <c r="FL5" s="34"/>
-      <c r="FM5" s="34"/>
-      <c r="FN5" s="34"/>
-      <c r="FO5" s="34"/>
-      <c r="FP5" s="34"/>
+      <c r="FI5" s="40"/>
+      <c r="FJ5" s="40"/>
+      <c r="FK5" s="40"/>
+      <c r="FL5" s="40"/>
+      <c r="FM5" s="40"/>
+      <c r="FN5" s="40"/>
+      <c r="FO5" s="40"/>
+      <c r="FP5" s="40"/>
       <c r="FQ5" s="11" t="s">
         <v>161</v>
       </c>
-      <c r="FR5" s="39" t="s">
+      <c r="FR5" s="35" t="s">
         <v>172</v>
       </c>
-      <c r="FS5" s="39"/>
-      <c r="FT5" s="39"/>
-      <c r="FU5" s="39"/>
-      <c r="FV5" s="39"/>
-      <c r="FW5" s="39"/>
-      <c r="FX5" s="39"/>
-      <c r="FY5" s="39"/>
-      <c r="FZ5" s="39"/>
-      <c r="GA5" s="39"/>
-      <c r="GB5" s="39"/>
-      <c r="GC5" s="39"/>
-      <c r="GD5" s="39"/>
-      <c r="GE5" s="39"/>
-      <c r="GF5" s="39"/>
+      <c r="FS5" s="35"/>
+      <c r="FT5" s="35"/>
+      <c r="FU5" s="35"/>
+      <c r="FV5" s="35"/>
+      <c r="FW5" s="35"/>
+      <c r="FX5" s="35"/>
+      <c r="FY5" s="35"/>
+      <c r="FZ5" s="35"/>
+      <c r="GA5" s="35"/>
+      <c r="GB5" s="35"/>
+      <c r="GC5" s="35"/>
+      <c r="GD5" s="35"/>
+      <c r="GE5" s="35"/>
+      <c r="GF5" s="35"/>
       <c r="GG5" s="13" t="s">
         <v>185</v>
       </c>
-      <c r="GH5" s="45" t="s">
+      <c r="GH5" s="34" t="s">
         <v>186</v>
       </c>
-      <c r="GI5" s="45"/>
-      <c r="GJ5" s="45"/>
-      <c r="GK5" s="45"/>
-      <c r="GL5" s="45"/>
-      <c r="GM5" s="45"/>
-      <c r="GN5" s="45"/>
+      <c r="GI5" s="34"/>
+      <c r="GJ5" s="34"/>
+      <c r="GK5" s="34"/>
+      <c r="GL5" s="34"/>
+      <c r="GM5" s="34"/>
+      <c r="GN5" s="34"/>
+      <c r="GO5" s="48" t="s">
+        <v>193</v>
+      </c>
+      <c r="GP5" s="48"/>
+      <c r="GQ5" s="48"/>
+      <c r="GR5" s="48"/>
+      <c r="GS5" s="48"/>
+      <c r="GT5" s="48"/>
+      <c r="GU5" s="48"/>
+      <c r="GV5" s="48"/>
+      <c r="GW5" s="48"/>
+      <c r="GX5" s="48"/>
+      <c r="GY5" s="48"/>
+      <c r="GZ5" s="48"/>
+      <c r="HA5" s="48"/>
     </row>
-    <row r="6" spans="1:196" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="44"/>
+    <row r="6" spans="1:209" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="45"/>
       <c r="B6" s="17"/>
       <c r="C6" s="17"/>
       <c r="D6" s="17"/>
@@ -1627,45 +1683,45 @@
       <c r="BO6" s="21"/>
       <c r="BP6" s="21"/>
       <c r="BQ6" s="21"/>
-      <c r="BR6" s="33" t="s">
+      <c r="BR6" s="38" t="s">
         <v>75</v>
       </c>
-      <c r="BS6" s="33"/>
-      <c r="BT6" s="33"/>
-      <c r="BU6" s="33"/>
-      <c r="BV6" s="33"/>
-      <c r="BW6" s="33"/>
-      <c r="BX6" s="33"/>
-      <c r="BY6" s="33"/>
-      <c r="BZ6" s="33"/>
-      <c r="CA6" s="33"/>
-      <c r="CB6" s="33" t="s">
+      <c r="BS6" s="38"/>
+      <c r="BT6" s="38"/>
+      <c r="BU6" s="38"/>
+      <c r="BV6" s="38"/>
+      <c r="BW6" s="38"/>
+      <c r="BX6" s="38"/>
+      <c r="BY6" s="38"/>
+      <c r="BZ6" s="38"/>
+      <c r="CA6" s="38"/>
+      <c r="CB6" s="38" t="s">
         <v>80</v>
       </c>
-      <c r="CC6" s="33"/>
-      <c r="CD6" s="33"/>
-      <c r="CE6" s="33"/>
-      <c r="CF6" s="33" t="s">
+      <c r="CC6" s="38"/>
+      <c r="CD6" s="38"/>
+      <c r="CE6" s="38"/>
+      <c r="CF6" s="38" t="s">
         <v>83</v>
       </c>
-      <c r="CG6" s="33"/>
-      <c r="CH6" s="33"/>
-      <c r="CI6" s="33" t="s">
+      <c r="CG6" s="38"/>
+      <c r="CH6" s="38"/>
+      <c r="CI6" s="38" t="s">
         <v>86</v>
       </c>
-      <c r="CJ6" s="33"/>
-      <c r="CK6" s="33"/>
-      <c r="CL6" s="33"/>
-      <c r="CM6" s="33"/>
-      <c r="CN6" s="33"/>
-      <c r="CO6" s="33"/>
-      <c r="CP6" s="33"/>
-      <c r="CQ6" s="33"/>
-      <c r="CR6" s="33"/>
-      <c r="CS6" s="33" t="s">
+      <c r="CJ6" s="38"/>
+      <c r="CK6" s="38"/>
+      <c r="CL6" s="38"/>
+      <c r="CM6" s="38"/>
+      <c r="CN6" s="38"/>
+      <c r="CO6" s="38"/>
+      <c r="CP6" s="38"/>
+      <c r="CQ6" s="38"/>
+      <c r="CR6" s="38"/>
+      <c r="CS6" s="38" t="s">
         <v>92</v>
       </c>
-      <c r="CT6" s="33"/>
+      <c r="CT6" s="38"/>
       <c r="CU6" s="11"/>
       <c r="CV6" s="11"/>
       <c r="CW6" s="11"/>
@@ -1770,9 +1826,22 @@
       <c r="GL6" s="14"/>
       <c r="GM6" s="14"/>
       <c r="GN6" s="14"/>
+      <c r="GO6" s="33"/>
+      <c r="GP6" s="33"/>
+      <c r="GQ6" s="33"/>
+      <c r="GR6" s="33"/>
+      <c r="GS6" s="33"/>
+      <c r="GT6" s="33"/>
+      <c r="GU6" s="33"/>
+      <c r="GV6" s="33"/>
+      <c r="GW6" s="33"/>
+      <c r="GX6" s="33"/>
+      <c r="GY6" s="33"/>
+      <c r="GZ6" s="33"/>
+      <c r="HA6" s="33"/>
     </row>
-    <row r="7" spans="1:196" s="1" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A7" s="44"/>
+    <row r="7" spans="1:209" s="1" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A7" s="45"/>
       <c r="B7" s="2" t="s">
         <v>2</v>
       </c>
@@ -2358,16 +2427,55 @@
       <c r="GN7" s="2" t="s">
         <v>192</v>
       </c>
+      <c r="GO7" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="GP7" s="15" t="s">
+        <v>194</v>
+      </c>
+      <c r="GQ7" s="15" t="s">
+        <v>195</v>
+      </c>
+      <c r="GR7" s="15" t="s">
+        <v>196</v>
+      </c>
+      <c r="GS7" s="15" t="s">
+        <v>197</v>
+      </c>
+      <c r="GT7" s="15" t="s">
+        <v>198</v>
+      </c>
+      <c r="GU7" s="15" t="s">
+        <v>199</v>
+      </c>
+      <c r="GV7" s="15" t="s">
+        <v>200</v>
+      </c>
+      <c r="GW7" s="15" t="s">
+        <v>201</v>
+      </c>
+      <c r="GX7" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="GY7" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="GZ7" s="15" t="s">
+        <v>198</v>
+      </c>
+      <c r="HA7" s="15" t="s">
+        <v>203</v>
+      </c>
     </row>
-    <row r="8" spans="1:196" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:196" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:196" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:196" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:196" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:196" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:196" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:196" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:196" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:209" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:209" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:209" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:209" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:209" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:209" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:209" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:209" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:209" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="17" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="18" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="19" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -2853,7 +2961,22 @@
     <row r="499" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="500" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="24">
+  <mergeCells count="25">
+    <mergeCell ref="GO5:HA5"/>
+    <mergeCell ref="CB6:CE6"/>
+    <mergeCell ref="BK5:BQ5"/>
+    <mergeCell ref="Z5:AK5"/>
+    <mergeCell ref="AL5:BJ5"/>
+    <mergeCell ref="DU5:EB5"/>
+    <mergeCell ref="BR5:CT5"/>
+    <mergeCell ref="DJ5:DM5"/>
+    <mergeCell ref="CU5:DI5"/>
+    <mergeCell ref="BR6:CA6"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="B5:X5"/>
     <mergeCell ref="GH5:GN5"/>
     <mergeCell ref="FR5:GF5"/>
     <mergeCell ref="EO5:ET5"/>
@@ -2864,20 +2987,6 @@
     <mergeCell ref="DN5:DO5"/>
     <mergeCell ref="FH5:FP5"/>
     <mergeCell ref="EU5:FG5"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="B5:X5"/>
-    <mergeCell ref="CB6:CE6"/>
-    <mergeCell ref="BK5:BQ5"/>
-    <mergeCell ref="Z5:AK5"/>
-    <mergeCell ref="AL5:BJ5"/>
-    <mergeCell ref="DU5:EB5"/>
-    <mergeCell ref="BR5:CT5"/>
-    <mergeCell ref="DJ5:DM5"/>
-    <mergeCell ref="CU5:DI5"/>
-    <mergeCell ref="BR6:CA6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
OAB : Laporan Terapi Non-Operatif
</commit_message>
<xml_diff>
--- a/Laravel-InaLUTS/resources/templates/Report_OAB.xlsx
+++ b/Laravel-InaLUTS/resources/templates/Report_OAB.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="211">
   <si>
     <t>No</t>
   </si>
@@ -626,6 +626,27 @@
   </si>
   <si>
     <t>TTNS</t>
+  </si>
+  <si>
+    <t>Terapi Non-Operatif</t>
+  </si>
+  <si>
+    <t>Tatalaksana non operatif</t>
+  </si>
+  <si>
+    <t>Kateter menetap</t>
+  </si>
+  <si>
+    <t>Kateter berkala</t>
+  </si>
+  <si>
+    <t>Penggunaan diapers</t>
+  </si>
+  <si>
+    <t>Penile clamp</t>
+  </si>
+  <si>
+    <t>Kondom kateter</t>
   </si>
 </sst>
 </file>
@@ -913,52 +934,52 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1265,10 +1286,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:HA500"/>
+  <dimension ref="A1:HG500"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="GH1" workbookViewId="0">
-      <selection activeCell="HA8" sqref="HA8"/>
+    <sheetView tabSelected="1" topLeftCell="GI1" workbookViewId="0">
+      <selection activeCell="HB8" sqref="HB8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1312,7 +1333,7 @@
     <col min="208" max="16384" width="9.140625" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:209" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:215" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A1" s="42"/>
       <c r="B1" s="42"/>
       <c r="C1" s="42"/>
@@ -1325,7 +1346,7 @@
       <c r="J1" s="42"/>
       <c r="K1" s="42"/>
     </row>
-    <row r="2" spans="1:209" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:215" x14ac:dyDescent="0.25">
       <c r="A2" s="43"/>
       <c r="B2" s="43"/>
       <c r="C2" s="43"/>
@@ -1338,7 +1359,7 @@
       <c r="J2" s="43"/>
       <c r="K2" s="43"/>
     </row>
-    <row r="3" spans="1:209" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:215" x14ac:dyDescent="0.25">
       <c r="A3" s="44"/>
       <c r="B3" s="44"/>
       <c r="C3" s="44"/>
@@ -1351,147 +1372,147 @@
       <c r="J3" s="44"/>
       <c r="K3" s="44"/>
     </row>
-    <row r="4" spans="1:209" s="3" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:209" s="1" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:215" s="3" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:215" s="1" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="34" t="s">
+      <c r="B5" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="34"/>
-      <c r="D5" s="34"/>
-      <c r="E5" s="34"/>
-      <c r="F5" s="34"/>
-      <c r="G5" s="34"/>
-      <c r="H5" s="34"/>
-      <c r="I5" s="34"/>
-      <c r="J5" s="34"/>
-      <c r="K5" s="34"/>
-      <c r="L5" s="34"/>
-      <c r="M5" s="34"/>
-      <c r="N5" s="34"/>
-      <c r="O5" s="34"/>
-      <c r="P5" s="34"/>
-      <c r="Q5" s="34"/>
-      <c r="R5" s="34"/>
-      <c r="S5" s="34"/>
-      <c r="T5" s="34"/>
-      <c r="U5" s="34"/>
-      <c r="V5" s="34"/>
-      <c r="W5" s="34"/>
-      <c r="X5" s="34"/>
+      <c r="C5" s="46"/>
+      <c r="D5" s="46"/>
+      <c r="E5" s="46"/>
+      <c r="F5" s="46"/>
+      <c r="G5" s="46"/>
+      <c r="H5" s="46"/>
+      <c r="I5" s="46"/>
+      <c r="J5" s="46"/>
+      <c r="K5" s="46"/>
+      <c r="L5" s="46"/>
+      <c r="M5" s="46"/>
+      <c r="N5" s="46"/>
+      <c r="O5" s="46"/>
+      <c r="P5" s="46"/>
+      <c r="Q5" s="46"/>
+      <c r="R5" s="46"/>
+      <c r="S5" s="46"/>
+      <c r="T5" s="46"/>
+      <c r="U5" s="46"/>
+      <c r="V5" s="46"/>
+      <c r="W5" s="46"/>
+      <c r="X5" s="46"/>
       <c r="Y5" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="Z5" s="46" t="s">
+      <c r="Z5" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="AA5" s="46"/>
-      <c r="AB5" s="46"/>
-      <c r="AC5" s="46"/>
-      <c r="AD5" s="46"/>
-      <c r="AE5" s="46"/>
-      <c r="AF5" s="46"/>
-      <c r="AG5" s="46"/>
-      <c r="AH5" s="46"/>
-      <c r="AI5" s="46"/>
-      <c r="AJ5" s="46"/>
-      <c r="AK5" s="46"/>
-      <c r="AL5" s="47" t="s">
+      <c r="AA5" s="37"/>
+      <c r="AB5" s="37"/>
+      <c r="AC5" s="37"/>
+      <c r="AD5" s="37"/>
+      <c r="AE5" s="37"/>
+      <c r="AF5" s="37"/>
+      <c r="AG5" s="37"/>
+      <c r="AH5" s="37"/>
+      <c r="AI5" s="37"/>
+      <c r="AJ5" s="37"/>
+      <c r="AK5" s="37"/>
+      <c r="AL5" s="38" t="s">
         <v>40</v>
       </c>
-      <c r="AM5" s="47"/>
-      <c r="AN5" s="47"/>
-      <c r="AO5" s="47"/>
-      <c r="AP5" s="47"/>
-      <c r="AQ5" s="47"/>
-      <c r="AR5" s="47"/>
-      <c r="AS5" s="47"/>
-      <c r="AT5" s="47"/>
-      <c r="AU5" s="47"/>
-      <c r="AV5" s="47"/>
-      <c r="AW5" s="47"/>
-      <c r="AX5" s="47"/>
-      <c r="AY5" s="47"/>
-      <c r="AZ5" s="47"/>
-      <c r="BA5" s="47"/>
-      <c r="BB5" s="47"/>
-      <c r="BC5" s="47"/>
-      <c r="BD5" s="47"/>
-      <c r="BE5" s="47"/>
-      <c r="BF5" s="47"/>
-      <c r="BG5" s="47"/>
-      <c r="BH5" s="47"/>
-      <c r="BI5" s="47"/>
-      <c r="BJ5" s="47"/>
-      <c r="BK5" s="40" t="s">
+      <c r="AM5" s="38"/>
+      <c r="AN5" s="38"/>
+      <c r="AO5" s="38"/>
+      <c r="AP5" s="38"/>
+      <c r="AQ5" s="38"/>
+      <c r="AR5" s="38"/>
+      <c r="AS5" s="38"/>
+      <c r="AT5" s="38"/>
+      <c r="AU5" s="38"/>
+      <c r="AV5" s="38"/>
+      <c r="AW5" s="38"/>
+      <c r="AX5" s="38"/>
+      <c r="AY5" s="38"/>
+      <c r="AZ5" s="38"/>
+      <c r="BA5" s="38"/>
+      <c r="BB5" s="38"/>
+      <c r="BC5" s="38"/>
+      <c r="BD5" s="38"/>
+      <c r="BE5" s="38"/>
+      <c r="BF5" s="38"/>
+      <c r="BG5" s="38"/>
+      <c r="BH5" s="38"/>
+      <c r="BI5" s="38"/>
+      <c r="BJ5" s="38"/>
+      <c r="BK5" s="36" t="s">
         <v>72</v>
       </c>
-      <c r="BL5" s="40"/>
-      <c r="BM5" s="40"/>
-      <c r="BN5" s="40"/>
-      <c r="BO5" s="40"/>
-      <c r="BP5" s="40"/>
-      <c r="BQ5" s="40"/>
-      <c r="BR5" s="41" t="s">
+      <c r="BL5" s="36"/>
+      <c r="BM5" s="36"/>
+      <c r="BN5" s="36"/>
+      <c r="BO5" s="36"/>
+      <c r="BP5" s="36"/>
+      <c r="BQ5" s="36"/>
+      <c r="BR5" s="39" t="s">
         <v>73</v>
       </c>
-      <c r="BS5" s="41"/>
-      <c r="BT5" s="41"/>
-      <c r="BU5" s="41"/>
-      <c r="BV5" s="41"/>
-      <c r="BW5" s="41"/>
-      <c r="BX5" s="41"/>
-      <c r="BY5" s="41"/>
-      <c r="BZ5" s="41"/>
-      <c r="CA5" s="41"/>
-      <c r="CB5" s="41"/>
-      <c r="CC5" s="41"/>
-      <c r="CD5" s="41"/>
-      <c r="CE5" s="41"/>
-      <c r="CF5" s="41"/>
-      <c r="CG5" s="41"/>
-      <c r="CH5" s="41"/>
-      <c r="CI5" s="41"/>
-      <c r="CJ5" s="41"/>
-      <c r="CK5" s="41"/>
-      <c r="CL5" s="41"/>
-      <c r="CM5" s="41"/>
-      <c r="CN5" s="41"/>
-      <c r="CO5" s="41"/>
-      <c r="CP5" s="41"/>
-      <c r="CQ5" s="41"/>
-      <c r="CR5" s="41"/>
-      <c r="CS5" s="41"/>
-      <c r="CT5" s="41"/>
-      <c r="CU5" s="49" t="s">
+      <c r="BS5" s="39"/>
+      <c r="BT5" s="39"/>
+      <c r="BU5" s="39"/>
+      <c r="BV5" s="39"/>
+      <c r="BW5" s="39"/>
+      <c r="BX5" s="39"/>
+      <c r="BY5" s="39"/>
+      <c r="BZ5" s="39"/>
+      <c r="CA5" s="39"/>
+      <c r="CB5" s="39"/>
+      <c r="CC5" s="39"/>
+      <c r="CD5" s="39"/>
+      <c r="CE5" s="39"/>
+      <c r="CF5" s="39"/>
+      <c r="CG5" s="39"/>
+      <c r="CH5" s="39"/>
+      <c r="CI5" s="39"/>
+      <c r="CJ5" s="39"/>
+      <c r="CK5" s="39"/>
+      <c r="CL5" s="39"/>
+      <c r="CM5" s="39"/>
+      <c r="CN5" s="39"/>
+      <c r="CO5" s="39"/>
+      <c r="CP5" s="39"/>
+      <c r="CQ5" s="39"/>
+      <c r="CR5" s="39"/>
+      <c r="CS5" s="39"/>
+      <c r="CT5" s="39"/>
+      <c r="CU5" s="41" t="s">
         <v>94</v>
       </c>
-      <c r="CV5" s="49"/>
-      <c r="CW5" s="49"/>
-      <c r="CX5" s="49"/>
-      <c r="CY5" s="49"/>
-      <c r="CZ5" s="49"/>
-      <c r="DA5" s="49"/>
-      <c r="DB5" s="49"/>
-      <c r="DC5" s="49"/>
-      <c r="DD5" s="49"/>
-      <c r="DE5" s="49"/>
-      <c r="DF5" s="49"/>
-      <c r="DG5" s="49"/>
-      <c r="DH5" s="49"/>
-      <c r="DI5" s="49"/>
-      <c r="DJ5" s="35" t="s">
+      <c r="CV5" s="41"/>
+      <c r="CW5" s="41"/>
+      <c r="CX5" s="41"/>
+      <c r="CY5" s="41"/>
+      <c r="CZ5" s="41"/>
+      <c r="DA5" s="41"/>
+      <c r="DB5" s="41"/>
+      <c r="DC5" s="41"/>
+      <c r="DD5" s="41"/>
+      <c r="DE5" s="41"/>
+      <c r="DF5" s="41"/>
+      <c r="DG5" s="41"/>
+      <c r="DH5" s="41"/>
+      <c r="DI5" s="41"/>
+      <c r="DJ5" s="40" t="s">
         <v>108</v>
       </c>
-      <c r="DK5" s="35"/>
-      <c r="DL5" s="35"/>
-      <c r="DM5" s="35"/>
-      <c r="DN5" s="39" t="s">
+      <c r="DK5" s="40"/>
+      <c r="DL5" s="40"/>
+      <c r="DM5" s="40"/>
+      <c r="DN5" s="49" t="s">
         <v>109</v>
       </c>
-      <c r="DO5" s="39"/>
+      <c r="DO5" s="49"/>
       <c r="DP5" s="17" t="s">
         <v>112</v>
       </c>
@@ -1507,113 +1528,121 @@
       <c r="DT5" s="16" t="s">
         <v>120</v>
       </c>
-      <c r="DU5" s="48" t="s">
+      <c r="DU5" s="34" t="s">
         <v>121</v>
       </c>
-      <c r="DV5" s="48"/>
-      <c r="DW5" s="48"/>
-      <c r="DX5" s="48"/>
-      <c r="DY5" s="48"/>
-      <c r="DZ5" s="48"/>
-      <c r="EA5" s="48"/>
-      <c r="EB5" s="48"/>
-      <c r="EC5" s="37" t="s">
+      <c r="DV5" s="34"/>
+      <c r="DW5" s="34"/>
+      <c r="DX5" s="34"/>
+      <c r="DY5" s="34"/>
+      <c r="DZ5" s="34"/>
+      <c r="EA5" s="34"/>
+      <c r="EB5" s="34"/>
+      <c r="EC5" s="48" t="s">
         <v>130</v>
       </c>
-      <c r="ED5" s="37"/>
-      <c r="EE5" s="37"/>
-      <c r="EF5" s="37"/>
-      <c r="EG5" s="37"/>
-      <c r="EH5" s="37"/>
-      <c r="EI5" s="37"/>
-      <c r="EJ5" s="37"/>
-      <c r="EK5" s="37"/>
-      <c r="EL5" s="37"/>
-      <c r="EM5" s="37"/>
-      <c r="EN5" s="37"/>
-      <c r="EO5" s="36" t="s">
+      <c r="ED5" s="48"/>
+      <c r="EE5" s="48"/>
+      <c r="EF5" s="48"/>
+      <c r="EG5" s="48"/>
+      <c r="EH5" s="48"/>
+      <c r="EI5" s="48"/>
+      <c r="EJ5" s="48"/>
+      <c r="EK5" s="48"/>
+      <c r="EL5" s="48"/>
+      <c r="EM5" s="48"/>
+      <c r="EN5" s="48"/>
+      <c r="EO5" s="47" t="s">
         <v>143</v>
       </c>
-      <c r="EP5" s="36"/>
-      <c r="EQ5" s="36"/>
-      <c r="ER5" s="36"/>
-      <c r="ES5" s="36"/>
-      <c r="ET5" s="36"/>
-      <c r="EU5" s="41" t="s">
+      <c r="EP5" s="47"/>
+      <c r="EQ5" s="47"/>
+      <c r="ER5" s="47"/>
+      <c r="ES5" s="47"/>
+      <c r="ET5" s="47"/>
+      <c r="EU5" s="39" t="s">
         <v>150</v>
       </c>
-      <c r="EV5" s="41"/>
-      <c r="EW5" s="41"/>
-      <c r="EX5" s="41"/>
-      <c r="EY5" s="41"/>
-      <c r="EZ5" s="41"/>
-      <c r="FA5" s="41"/>
-      <c r="FB5" s="41"/>
-      <c r="FC5" s="41"/>
-      <c r="FD5" s="41"/>
-      <c r="FE5" s="41"/>
-      <c r="FF5" s="41"/>
-      <c r="FG5" s="41"/>
-      <c r="FH5" s="40" t="s">
+      <c r="EV5" s="39"/>
+      <c r="EW5" s="39"/>
+      <c r="EX5" s="39"/>
+      <c r="EY5" s="39"/>
+      <c r="EZ5" s="39"/>
+      <c r="FA5" s="39"/>
+      <c r="FB5" s="39"/>
+      <c r="FC5" s="39"/>
+      <c r="FD5" s="39"/>
+      <c r="FE5" s="39"/>
+      <c r="FF5" s="39"/>
+      <c r="FG5" s="39"/>
+      <c r="FH5" s="36" t="s">
         <v>162</v>
       </c>
-      <c r="FI5" s="40"/>
-      <c r="FJ5" s="40"/>
-      <c r="FK5" s="40"/>
-      <c r="FL5" s="40"/>
-      <c r="FM5" s="40"/>
-      <c r="FN5" s="40"/>
-      <c r="FO5" s="40"/>
-      <c r="FP5" s="40"/>
+      <c r="FI5" s="36"/>
+      <c r="FJ5" s="36"/>
+      <c r="FK5" s="36"/>
+      <c r="FL5" s="36"/>
+      <c r="FM5" s="36"/>
+      <c r="FN5" s="36"/>
+      <c r="FO5" s="36"/>
+      <c r="FP5" s="36"/>
       <c r="FQ5" s="11" t="s">
         <v>161</v>
       </c>
-      <c r="FR5" s="35" t="s">
+      <c r="FR5" s="40" t="s">
         <v>172</v>
       </c>
-      <c r="FS5" s="35"/>
-      <c r="FT5" s="35"/>
-      <c r="FU5" s="35"/>
-      <c r="FV5" s="35"/>
-      <c r="FW5" s="35"/>
-      <c r="FX5" s="35"/>
-      <c r="FY5" s="35"/>
-      <c r="FZ5" s="35"/>
-      <c r="GA5" s="35"/>
-      <c r="GB5" s="35"/>
-      <c r="GC5" s="35"/>
-      <c r="GD5" s="35"/>
-      <c r="GE5" s="35"/>
-      <c r="GF5" s="35"/>
+      <c r="FS5" s="40"/>
+      <c r="FT5" s="40"/>
+      <c r="FU5" s="40"/>
+      <c r="FV5" s="40"/>
+      <c r="FW5" s="40"/>
+      <c r="FX5" s="40"/>
+      <c r="FY5" s="40"/>
+      <c r="FZ5" s="40"/>
+      <c r="GA5" s="40"/>
+      <c r="GB5" s="40"/>
+      <c r="GC5" s="40"/>
+      <c r="GD5" s="40"/>
+      <c r="GE5" s="40"/>
+      <c r="GF5" s="40"/>
       <c r="GG5" s="13" t="s">
         <v>185</v>
       </c>
-      <c r="GH5" s="34" t="s">
+      <c r="GH5" s="46" t="s">
         <v>186</v>
       </c>
-      <c r="GI5" s="34"/>
-      <c r="GJ5" s="34"/>
-      <c r="GK5" s="34"/>
-      <c r="GL5" s="34"/>
-      <c r="GM5" s="34"/>
-      <c r="GN5" s="34"/>
-      <c r="GO5" s="48" t="s">
+      <c r="GI5" s="46"/>
+      <c r="GJ5" s="46"/>
+      <c r="GK5" s="46"/>
+      <c r="GL5" s="46"/>
+      <c r="GM5" s="46"/>
+      <c r="GN5" s="46"/>
+      <c r="GO5" s="34" t="s">
         <v>193</v>
       </c>
-      <c r="GP5" s="48"/>
-      <c r="GQ5" s="48"/>
-      <c r="GR5" s="48"/>
-      <c r="GS5" s="48"/>
-      <c r="GT5" s="48"/>
-      <c r="GU5" s="48"/>
-      <c r="GV5" s="48"/>
-      <c r="GW5" s="48"/>
-      <c r="GX5" s="48"/>
-      <c r="GY5" s="48"/>
-      <c r="GZ5" s="48"/>
-      <c r="HA5" s="48"/>
+      <c r="GP5" s="34"/>
+      <c r="GQ5" s="34"/>
+      <c r="GR5" s="34"/>
+      <c r="GS5" s="34"/>
+      <c r="GT5" s="34"/>
+      <c r="GU5" s="34"/>
+      <c r="GV5" s="34"/>
+      <c r="GW5" s="34"/>
+      <c r="GX5" s="34"/>
+      <c r="GY5" s="34"/>
+      <c r="GZ5" s="34"/>
+      <c r="HA5" s="34"/>
+      <c r="HB5" s="48" t="s">
+        <v>204</v>
+      </c>
+      <c r="HC5" s="48"/>
+      <c r="HD5" s="48"/>
+      <c r="HE5" s="48"/>
+      <c r="HF5" s="48"/>
+      <c r="HG5" s="48"/>
     </row>
-    <row r="6" spans="1:209" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:215" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="45"/>
       <c r="B6" s="17"/>
       <c r="C6" s="17"/>
@@ -1683,45 +1712,45 @@
       <c r="BO6" s="21"/>
       <c r="BP6" s="21"/>
       <c r="BQ6" s="21"/>
-      <c r="BR6" s="38" t="s">
+      <c r="BR6" s="35" t="s">
         <v>75</v>
       </c>
-      <c r="BS6" s="38"/>
-      <c r="BT6" s="38"/>
-      <c r="BU6" s="38"/>
-      <c r="BV6" s="38"/>
-      <c r="BW6" s="38"/>
-      <c r="BX6" s="38"/>
-      <c r="BY6" s="38"/>
-      <c r="BZ6" s="38"/>
-      <c r="CA6" s="38"/>
-      <c r="CB6" s="38" t="s">
+      <c r="BS6" s="35"/>
+      <c r="BT6" s="35"/>
+      <c r="BU6" s="35"/>
+      <c r="BV6" s="35"/>
+      <c r="BW6" s="35"/>
+      <c r="BX6" s="35"/>
+      <c r="BY6" s="35"/>
+      <c r="BZ6" s="35"/>
+      <c r="CA6" s="35"/>
+      <c r="CB6" s="35" t="s">
         <v>80</v>
       </c>
-      <c r="CC6" s="38"/>
-      <c r="CD6" s="38"/>
-      <c r="CE6" s="38"/>
-      <c r="CF6" s="38" t="s">
+      <c r="CC6" s="35"/>
+      <c r="CD6" s="35"/>
+      <c r="CE6" s="35"/>
+      <c r="CF6" s="35" t="s">
         <v>83</v>
       </c>
-      <c r="CG6" s="38"/>
-      <c r="CH6" s="38"/>
-      <c r="CI6" s="38" t="s">
+      <c r="CG6" s="35"/>
+      <c r="CH6" s="35"/>
+      <c r="CI6" s="35" t="s">
         <v>86</v>
       </c>
-      <c r="CJ6" s="38"/>
-      <c r="CK6" s="38"/>
-      <c r="CL6" s="38"/>
-      <c r="CM6" s="38"/>
-      <c r="CN6" s="38"/>
-      <c r="CO6" s="38"/>
-      <c r="CP6" s="38"/>
-      <c r="CQ6" s="38"/>
-      <c r="CR6" s="38"/>
-      <c r="CS6" s="38" t="s">
+      <c r="CJ6" s="35"/>
+      <c r="CK6" s="35"/>
+      <c r="CL6" s="35"/>
+      <c r="CM6" s="35"/>
+      <c r="CN6" s="35"/>
+      <c r="CO6" s="35"/>
+      <c r="CP6" s="35"/>
+      <c r="CQ6" s="35"/>
+      <c r="CR6" s="35"/>
+      <c r="CS6" s="35" t="s">
         <v>92</v>
       </c>
-      <c r="CT6" s="38"/>
+      <c r="CT6" s="35"/>
       <c r="CU6" s="11"/>
       <c r="CV6" s="11"/>
       <c r="CW6" s="11"/>
@@ -1839,8 +1868,14 @@
       <c r="GY6" s="33"/>
       <c r="GZ6" s="33"/>
       <c r="HA6" s="33"/>
+      <c r="HB6" s="25"/>
+      <c r="HC6" s="25"/>
+      <c r="HD6" s="25"/>
+      <c r="HE6" s="25"/>
+      <c r="HF6" s="25"/>
+      <c r="HG6" s="25"/>
     </row>
-    <row r="7" spans="1:209" s="1" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:215" s="1" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A7" s="45"/>
       <c r="B7" s="2" t="s">
         <v>2</v>
@@ -2466,16 +2501,34 @@
       <c r="HA7" s="15" t="s">
         <v>203</v>
       </c>
+      <c r="HB7" s="24" t="s">
+        <v>205</v>
+      </c>
+      <c r="HC7" s="24" t="s">
+        <v>206</v>
+      </c>
+      <c r="HD7" s="24" t="s">
+        <v>207</v>
+      </c>
+      <c r="HE7" s="24" t="s">
+        <v>208</v>
+      </c>
+      <c r="HF7" s="24" t="s">
+        <v>209</v>
+      </c>
+      <c r="HG7" s="24" t="s">
+        <v>210</v>
+      </c>
     </row>
-    <row r="8" spans="1:209" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:209" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:209" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:209" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:209" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:209" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:209" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:209" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:209" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:215" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:215" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:215" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:215" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:215" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:215" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:215" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:215" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:215" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="17" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="18" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="19" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -2961,7 +3014,17 @@
     <row r="499" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="500" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="25">
+  <mergeCells count="26">
+    <mergeCell ref="CS6:CT6"/>
+    <mergeCell ref="DN5:DO5"/>
+    <mergeCell ref="FH5:FP5"/>
+    <mergeCell ref="EU5:FG5"/>
+    <mergeCell ref="HB5:HG5"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="B5:X5"/>
     <mergeCell ref="GO5:HA5"/>
     <mergeCell ref="CB6:CE6"/>
     <mergeCell ref="BK5:BQ5"/>
@@ -2972,21 +3035,12 @@
     <mergeCell ref="DJ5:DM5"/>
     <mergeCell ref="CU5:DI5"/>
     <mergeCell ref="BR6:CA6"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="B5:X5"/>
     <mergeCell ref="GH5:GN5"/>
     <mergeCell ref="FR5:GF5"/>
     <mergeCell ref="EO5:ET5"/>
     <mergeCell ref="EC5:EN5"/>
     <mergeCell ref="CF6:CH6"/>
     <mergeCell ref="CI6:CR6"/>
-    <mergeCell ref="CS6:CT6"/>
-    <mergeCell ref="DN5:DO5"/>
-    <mergeCell ref="FH5:FP5"/>
-    <mergeCell ref="EU5:FG5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
OAB : Laporan Terapi Medikamentosa
</commit_message>
<xml_diff>
--- a/Laravel-InaLUTS/resources/templates/Report_OAB.xlsx
+++ b/Laravel-InaLUTS/resources/templates/Report_OAB.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="215">
   <si>
     <t>No</t>
   </si>
@@ -647,6 +647,18 @@
   </si>
   <si>
     <t>Kondom kateter</t>
+  </si>
+  <si>
+    <t>Terapi Medikamentosa</t>
+  </si>
+  <si>
+    <t>Medikamentosa</t>
+  </si>
+  <si>
+    <t>Anti Muskarinik</t>
+  </si>
+  <si>
+    <t>B3 Agonis</t>
   </si>
 </sst>
 </file>
@@ -934,52 +946,52 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1286,10 +1298,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:HG500"/>
+  <dimension ref="A1:HN500"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="GI1" workbookViewId="0">
-      <selection activeCell="HB8" sqref="HB8"/>
+    <sheetView tabSelected="1" topLeftCell="GU1" workbookViewId="0">
+      <selection activeCell="HO8" sqref="HO8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1330,122 +1342,124 @@
     <col min="202" max="202" width="10.7109375" style="19" customWidth="1"/>
     <col min="203" max="206" width="9.140625" style="19"/>
     <col min="207" max="207" width="10.7109375" style="19" customWidth="1"/>
-    <col min="208" max="16384" width="9.140625" style="19"/>
+    <col min="208" max="221" width="9.140625" style="19"/>
+    <col min="222" max="222" width="12.7109375" style="19" customWidth="1"/>
+    <col min="223" max="16384" width="9.140625" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:215" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="42"/>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
-      <c r="K1" s="42"/>
+    <row r="1" spans="1:222" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="39"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
+      <c r="J1" s="39"/>
+      <c r="K1" s="39"/>
     </row>
-    <row r="2" spans="1:215" x14ac:dyDescent="0.25">
-      <c r="A2" s="43"/>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
-      <c r="K2" s="43"/>
+    <row r="2" spans="1:222" x14ac:dyDescent="0.25">
+      <c r="A2" s="40"/>
+      <c r="B2" s="40"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="40"/>
+      <c r="K2" s="40"/>
     </row>
-    <row r="3" spans="1:215" x14ac:dyDescent="0.25">
-      <c r="A3" s="44"/>
-      <c r="B3" s="44"/>
-      <c r="C3" s="44"/>
-      <c r="D3" s="44"/>
-      <c r="E3" s="44"/>
-      <c r="F3" s="44"/>
-      <c r="G3" s="44"/>
-      <c r="H3" s="44"/>
-      <c r="I3" s="44"/>
-      <c r="J3" s="44"/>
-      <c r="K3" s="44"/>
+    <row r="3" spans="1:222" x14ac:dyDescent="0.25">
+      <c r="A3" s="41"/>
+      <c r="B3" s="41"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="41"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="41"/>
+      <c r="I3" s="41"/>
+      <c r="J3" s="41"/>
+      <c r="K3" s="41"/>
     </row>
-    <row r="4" spans="1:215" s="3" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:215" s="1" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="45" t="s">
+    <row r="4" spans="1:222" s="3" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:222" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="46" t="s">
+      <c r="B5" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="46"/>
-      <c r="D5" s="46"/>
-      <c r="E5" s="46"/>
-      <c r="F5" s="46"/>
-      <c r="G5" s="46"/>
-      <c r="H5" s="46"/>
-      <c r="I5" s="46"/>
-      <c r="J5" s="46"/>
-      <c r="K5" s="46"/>
-      <c r="L5" s="46"/>
-      <c r="M5" s="46"/>
-      <c r="N5" s="46"/>
-      <c r="O5" s="46"/>
-      <c r="P5" s="46"/>
-      <c r="Q5" s="46"/>
-      <c r="R5" s="46"/>
-      <c r="S5" s="46"/>
-      <c r="T5" s="46"/>
-      <c r="U5" s="46"/>
-      <c r="V5" s="46"/>
-      <c r="W5" s="46"/>
-      <c r="X5" s="46"/>
+      <c r="C5" s="43"/>
+      <c r="D5" s="43"/>
+      <c r="E5" s="43"/>
+      <c r="F5" s="43"/>
+      <c r="G5" s="43"/>
+      <c r="H5" s="43"/>
+      <c r="I5" s="43"/>
+      <c r="J5" s="43"/>
+      <c r="K5" s="43"/>
+      <c r="L5" s="43"/>
+      <c r="M5" s="43"/>
+      <c r="N5" s="43"/>
+      <c r="O5" s="43"/>
+      <c r="P5" s="43"/>
+      <c r="Q5" s="43"/>
+      <c r="R5" s="43"/>
+      <c r="S5" s="43"/>
+      <c r="T5" s="43"/>
+      <c r="U5" s="43"/>
+      <c r="V5" s="43"/>
+      <c r="W5" s="43"/>
+      <c r="X5" s="43"/>
       <c r="Y5" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="Z5" s="37" t="s">
+      <c r="Z5" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="AA5" s="37"/>
-      <c r="AB5" s="37"/>
-      <c r="AC5" s="37"/>
-      <c r="AD5" s="37"/>
-      <c r="AE5" s="37"/>
-      <c r="AF5" s="37"/>
-      <c r="AG5" s="37"/>
-      <c r="AH5" s="37"/>
-      <c r="AI5" s="37"/>
-      <c r="AJ5" s="37"/>
-      <c r="AK5" s="37"/>
-      <c r="AL5" s="38" t="s">
+      <c r="AA5" s="45"/>
+      <c r="AB5" s="45"/>
+      <c r="AC5" s="45"/>
+      <c r="AD5" s="45"/>
+      <c r="AE5" s="45"/>
+      <c r="AF5" s="45"/>
+      <c r="AG5" s="45"/>
+      <c r="AH5" s="45"/>
+      <c r="AI5" s="45"/>
+      <c r="AJ5" s="45"/>
+      <c r="AK5" s="45"/>
+      <c r="AL5" s="46" t="s">
         <v>40</v>
       </c>
-      <c r="AM5" s="38"/>
-      <c r="AN5" s="38"/>
-      <c r="AO5" s="38"/>
-      <c r="AP5" s="38"/>
-      <c r="AQ5" s="38"/>
-      <c r="AR5" s="38"/>
-      <c r="AS5" s="38"/>
-      <c r="AT5" s="38"/>
-      <c r="AU5" s="38"/>
-      <c r="AV5" s="38"/>
-      <c r="AW5" s="38"/>
-      <c r="AX5" s="38"/>
-      <c r="AY5" s="38"/>
-      <c r="AZ5" s="38"/>
-      <c r="BA5" s="38"/>
-      <c r="BB5" s="38"/>
-      <c r="BC5" s="38"/>
-      <c r="BD5" s="38"/>
-      <c r="BE5" s="38"/>
-      <c r="BF5" s="38"/>
-      <c r="BG5" s="38"/>
-      <c r="BH5" s="38"/>
-      <c r="BI5" s="38"/>
-      <c r="BJ5" s="38"/>
+      <c r="AM5" s="46"/>
+      <c r="AN5" s="46"/>
+      <c r="AO5" s="46"/>
+      <c r="AP5" s="46"/>
+      <c r="AQ5" s="46"/>
+      <c r="AR5" s="46"/>
+      <c r="AS5" s="46"/>
+      <c r="AT5" s="46"/>
+      <c r="AU5" s="46"/>
+      <c r="AV5" s="46"/>
+      <c r="AW5" s="46"/>
+      <c r="AX5" s="46"/>
+      <c r="AY5" s="46"/>
+      <c r="AZ5" s="46"/>
+      <c r="BA5" s="46"/>
+      <c r="BB5" s="46"/>
+      <c r="BC5" s="46"/>
+      <c r="BD5" s="46"/>
+      <c r="BE5" s="46"/>
+      <c r="BF5" s="46"/>
+      <c r="BG5" s="46"/>
+      <c r="BH5" s="46"/>
+      <c r="BI5" s="46"/>
+      <c r="BJ5" s="46"/>
       <c r="BK5" s="36" t="s">
         <v>72</v>
       </c>
@@ -1455,64 +1469,64 @@
       <c r="BO5" s="36"/>
       <c r="BP5" s="36"/>
       <c r="BQ5" s="36"/>
-      <c r="BR5" s="39" t="s">
+      <c r="BR5" s="37" t="s">
         <v>73</v>
       </c>
-      <c r="BS5" s="39"/>
-      <c r="BT5" s="39"/>
-      <c r="BU5" s="39"/>
-      <c r="BV5" s="39"/>
-      <c r="BW5" s="39"/>
-      <c r="BX5" s="39"/>
-      <c r="BY5" s="39"/>
-      <c r="BZ5" s="39"/>
-      <c r="CA5" s="39"/>
-      <c r="CB5" s="39"/>
-      <c r="CC5" s="39"/>
-      <c r="CD5" s="39"/>
-      <c r="CE5" s="39"/>
-      <c r="CF5" s="39"/>
-      <c r="CG5" s="39"/>
-      <c r="CH5" s="39"/>
-      <c r="CI5" s="39"/>
-      <c r="CJ5" s="39"/>
-      <c r="CK5" s="39"/>
-      <c r="CL5" s="39"/>
-      <c r="CM5" s="39"/>
-      <c r="CN5" s="39"/>
-      <c r="CO5" s="39"/>
-      <c r="CP5" s="39"/>
-      <c r="CQ5" s="39"/>
-      <c r="CR5" s="39"/>
-      <c r="CS5" s="39"/>
-      <c r="CT5" s="39"/>
-      <c r="CU5" s="41" t="s">
+      <c r="BS5" s="37"/>
+      <c r="BT5" s="37"/>
+      <c r="BU5" s="37"/>
+      <c r="BV5" s="37"/>
+      <c r="BW5" s="37"/>
+      <c r="BX5" s="37"/>
+      <c r="BY5" s="37"/>
+      <c r="BZ5" s="37"/>
+      <c r="CA5" s="37"/>
+      <c r="CB5" s="37"/>
+      <c r="CC5" s="37"/>
+      <c r="CD5" s="37"/>
+      <c r="CE5" s="37"/>
+      <c r="CF5" s="37"/>
+      <c r="CG5" s="37"/>
+      <c r="CH5" s="37"/>
+      <c r="CI5" s="37"/>
+      <c r="CJ5" s="37"/>
+      <c r="CK5" s="37"/>
+      <c r="CL5" s="37"/>
+      <c r="CM5" s="37"/>
+      <c r="CN5" s="37"/>
+      <c r="CO5" s="37"/>
+      <c r="CP5" s="37"/>
+      <c r="CQ5" s="37"/>
+      <c r="CR5" s="37"/>
+      <c r="CS5" s="37"/>
+      <c r="CT5" s="37"/>
+      <c r="CU5" s="48" t="s">
         <v>94</v>
       </c>
-      <c r="CV5" s="41"/>
-      <c r="CW5" s="41"/>
-      <c r="CX5" s="41"/>
-      <c r="CY5" s="41"/>
-      <c r="CZ5" s="41"/>
-      <c r="DA5" s="41"/>
-      <c r="DB5" s="41"/>
-      <c r="DC5" s="41"/>
-      <c r="DD5" s="41"/>
-      <c r="DE5" s="41"/>
-      <c r="DF5" s="41"/>
-      <c r="DG5" s="41"/>
-      <c r="DH5" s="41"/>
-      <c r="DI5" s="41"/>
-      <c r="DJ5" s="40" t="s">
+      <c r="CV5" s="48"/>
+      <c r="CW5" s="48"/>
+      <c r="CX5" s="48"/>
+      <c r="CY5" s="48"/>
+      <c r="CZ5" s="48"/>
+      <c r="DA5" s="48"/>
+      <c r="DB5" s="48"/>
+      <c r="DC5" s="48"/>
+      <c r="DD5" s="48"/>
+      <c r="DE5" s="48"/>
+      <c r="DF5" s="48"/>
+      <c r="DG5" s="48"/>
+      <c r="DH5" s="48"/>
+      <c r="DI5" s="48"/>
+      <c r="DJ5" s="47" t="s">
         <v>108</v>
       </c>
-      <c r="DK5" s="40"/>
-      <c r="DL5" s="40"/>
-      <c r="DM5" s="40"/>
-      <c r="DN5" s="49" t="s">
+      <c r="DK5" s="47"/>
+      <c r="DL5" s="47"/>
+      <c r="DM5" s="47"/>
+      <c r="DN5" s="35" t="s">
         <v>109</v>
       </c>
-      <c r="DO5" s="49"/>
+      <c r="DO5" s="35"/>
       <c r="DP5" s="17" t="s">
         <v>112</v>
       </c>
@@ -1528,53 +1542,53 @@
       <c r="DT5" s="16" t="s">
         <v>120</v>
       </c>
-      <c r="DU5" s="34" t="s">
+      <c r="DU5" s="44" t="s">
         <v>121</v>
       </c>
-      <c r="DV5" s="34"/>
-      <c r="DW5" s="34"/>
-      <c r="DX5" s="34"/>
-      <c r="DY5" s="34"/>
-      <c r="DZ5" s="34"/>
-      <c r="EA5" s="34"/>
-      <c r="EB5" s="34"/>
-      <c r="EC5" s="48" t="s">
+      <c r="DV5" s="44"/>
+      <c r="DW5" s="44"/>
+      <c r="DX5" s="44"/>
+      <c r="DY5" s="44"/>
+      <c r="DZ5" s="44"/>
+      <c r="EA5" s="44"/>
+      <c r="EB5" s="44"/>
+      <c r="EC5" s="38" t="s">
         <v>130</v>
       </c>
-      <c r="ED5" s="48"/>
-      <c r="EE5" s="48"/>
-      <c r="EF5" s="48"/>
-      <c r="EG5" s="48"/>
-      <c r="EH5" s="48"/>
-      <c r="EI5" s="48"/>
-      <c r="EJ5" s="48"/>
-      <c r="EK5" s="48"/>
-      <c r="EL5" s="48"/>
-      <c r="EM5" s="48"/>
-      <c r="EN5" s="48"/>
-      <c r="EO5" s="47" t="s">
+      <c r="ED5" s="38"/>
+      <c r="EE5" s="38"/>
+      <c r="EF5" s="38"/>
+      <c r="EG5" s="38"/>
+      <c r="EH5" s="38"/>
+      <c r="EI5" s="38"/>
+      <c r="EJ5" s="38"/>
+      <c r="EK5" s="38"/>
+      <c r="EL5" s="38"/>
+      <c r="EM5" s="38"/>
+      <c r="EN5" s="38"/>
+      <c r="EO5" s="49" t="s">
         <v>143</v>
       </c>
-      <c r="EP5" s="47"/>
-      <c r="EQ5" s="47"/>
-      <c r="ER5" s="47"/>
-      <c r="ES5" s="47"/>
-      <c r="ET5" s="47"/>
-      <c r="EU5" s="39" t="s">
+      <c r="EP5" s="49"/>
+      <c r="EQ5" s="49"/>
+      <c r="ER5" s="49"/>
+      <c r="ES5" s="49"/>
+      <c r="ET5" s="49"/>
+      <c r="EU5" s="37" t="s">
         <v>150</v>
       </c>
-      <c r="EV5" s="39"/>
-      <c r="EW5" s="39"/>
-      <c r="EX5" s="39"/>
-      <c r="EY5" s="39"/>
-      <c r="EZ5" s="39"/>
-      <c r="FA5" s="39"/>
-      <c r="FB5" s="39"/>
-      <c r="FC5" s="39"/>
-      <c r="FD5" s="39"/>
-      <c r="FE5" s="39"/>
-      <c r="FF5" s="39"/>
-      <c r="FG5" s="39"/>
+      <c r="EV5" s="37"/>
+      <c r="EW5" s="37"/>
+      <c r="EX5" s="37"/>
+      <c r="EY5" s="37"/>
+      <c r="EZ5" s="37"/>
+      <c r="FA5" s="37"/>
+      <c r="FB5" s="37"/>
+      <c r="FC5" s="37"/>
+      <c r="FD5" s="37"/>
+      <c r="FE5" s="37"/>
+      <c r="FF5" s="37"/>
+      <c r="FG5" s="37"/>
       <c r="FH5" s="36" t="s">
         <v>162</v>
       </c>
@@ -1589,61 +1603,70 @@
       <c r="FQ5" s="11" t="s">
         <v>161</v>
       </c>
-      <c r="FR5" s="40" t="s">
+      <c r="FR5" s="47" t="s">
         <v>172</v>
       </c>
-      <c r="FS5" s="40"/>
-      <c r="FT5" s="40"/>
-      <c r="FU5" s="40"/>
-      <c r="FV5" s="40"/>
-      <c r="FW5" s="40"/>
-      <c r="FX5" s="40"/>
-      <c r="FY5" s="40"/>
-      <c r="FZ5" s="40"/>
-      <c r="GA5" s="40"/>
-      <c r="GB5" s="40"/>
-      <c r="GC5" s="40"/>
-      <c r="GD5" s="40"/>
-      <c r="GE5" s="40"/>
-      <c r="GF5" s="40"/>
+      <c r="FS5" s="47"/>
+      <c r="FT5" s="47"/>
+      <c r="FU5" s="47"/>
+      <c r="FV5" s="47"/>
+      <c r="FW5" s="47"/>
+      <c r="FX5" s="47"/>
+      <c r="FY5" s="47"/>
+      <c r="FZ5" s="47"/>
+      <c r="GA5" s="47"/>
+      <c r="GB5" s="47"/>
+      <c r="GC5" s="47"/>
+      <c r="GD5" s="47"/>
+      <c r="GE5" s="47"/>
+      <c r="GF5" s="47"/>
       <c r="GG5" s="13" t="s">
         <v>185</v>
       </c>
-      <c r="GH5" s="46" t="s">
+      <c r="GH5" s="43" t="s">
         <v>186</v>
       </c>
-      <c r="GI5" s="46"/>
-      <c r="GJ5" s="46"/>
-      <c r="GK5" s="46"/>
-      <c r="GL5" s="46"/>
-      <c r="GM5" s="46"/>
-      <c r="GN5" s="46"/>
-      <c r="GO5" s="34" t="s">
+      <c r="GI5" s="43"/>
+      <c r="GJ5" s="43"/>
+      <c r="GK5" s="43"/>
+      <c r="GL5" s="43"/>
+      <c r="GM5" s="43"/>
+      <c r="GN5" s="43"/>
+      <c r="GO5" s="44" t="s">
         <v>193</v>
       </c>
-      <c r="GP5" s="34"/>
-      <c r="GQ5" s="34"/>
-      <c r="GR5" s="34"/>
-      <c r="GS5" s="34"/>
-      <c r="GT5" s="34"/>
-      <c r="GU5" s="34"/>
-      <c r="GV5" s="34"/>
-      <c r="GW5" s="34"/>
-      <c r="GX5" s="34"/>
-      <c r="GY5" s="34"/>
-      <c r="GZ5" s="34"/>
-      <c r="HA5" s="34"/>
-      <c r="HB5" s="48" t="s">
+      <c r="GP5" s="44"/>
+      <c r="GQ5" s="44"/>
+      <c r="GR5" s="44"/>
+      <c r="GS5" s="44"/>
+      <c r="GT5" s="44"/>
+      <c r="GU5" s="44"/>
+      <c r="GV5" s="44"/>
+      <c r="GW5" s="44"/>
+      <c r="GX5" s="44"/>
+      <c r="GY5" s="44"/>
+      <c r="GZ5" s="44"/>
+      <c r="HA5" s="44"/>
+      <c r="HB5" s="38" t="s">
         <v>204</v>
       </c>
-      <c r="HC5" s="48"/>
-      <c r="HD5" s="48"/>
-      <c r="HE5" s="48"/>
-      <c r="HF5" s="48"/>
-      <c r="HG5" s="48"/>
+      <c r="HC5" s="38"/>
+      <c r="HD5" s="38"/>
+      <c r="HE5" s="38"/>
+      <c r="HF5" s="38"/>
+      <c r="HG5" s="38"/>
+      <c r="HH5" s="49" t="s">
+        <v>211</v>
+      </c>
+      <c r="HI5" s="49"/>
+      <c r="HJ5" s="49"/>
+      <c r="HK5" s="49"/>
+      <c r="HL5" s="49"/>
+      <c r="HM5" s="49"/>
+      <c r="HN5" s="49"/>
     </row>
-    <row r="6" spans="1:215" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="45"/>
+    <row r="6" spans="1:222" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="42"/>
       <c r="B6" s="17"/>
       <c r="C6" s="17"/>
       <c r="D6" s="17"/>
@@ -1712,45 +1735,45 @@
       <c r="BO6" s="21"/>
       <c r="BP6" s="21"/>
       <c r="BQ6" s="21"/>
-      <c r="BR6" s="35" t="s">
+      <c r="BR6" s="34" t="s">
         <v>75</v>
       </c>
-      <c r="BS6" s="35"/>
-      <c r="BT6" s="35"/>
-      <c r="BU6" s="35"/>
-      <c r="BV6" s="35"/>
-      <c r="BW6" s="35"/>
-      <c r="BX6" s="35"/>
-      <c r="BY6" s="35"/>
-      <c r="BZ6" s="35"/>
-      <c r="CA6" s="35"/>
-      <c r="CB6" s="35" t="s">
+      <c r="BS6" s="34"/>
+      <c r="BT6" s="34"/>
+      <c r="BU6" s="34"/>
+      <c r="BV6" s="34"/>
+      <c r="BW6" s="34"/>
+      <c r="BX6" s="34"/>
+      <c r="BY6" s="34"/>
+      <c r="BZ6" s="34"/>
+      <c r="CA6" s="34"/>
+      <c r="CB6" s="34" t="s">
         <v>80</v>
       </c>
-      <c r="CC6" s="35"/>
-      <c r="CD6" s="35"/>
-      <c r="CE6" s="35"/>
-      <c r="CF6" s="35" t="s">
+      <c r="CC6" s="34"/>
+      <c r="CD6" s="34"/>
+      <c r="CE6" s="34"/>
+      <c r="CF6" s="34" t="s">
         <v>83</v>
       </c>
-      <c r="CG6" s="35"/>
-      <c r="CH6" s="35"/>
-      <c r="CI6" s="35" t="s">
+      <c r="CG6" s="34"/>
+      <c r="CH6" s="34"/>
+      <c r="CI6" s="34" t="s">
         <v>86</v>
       </c>
-      <c r="CJ6" s="35"/>
-      <c r="CK6" s="35"/>
-      <c r="CL6" s="35"/>
-      <c r="CM6" s="35"/>
-      <c r="CN6" s="35"/>
-      <c r="CO6" s="35"/>
-      <c r="CP6" s="35"/>
-      <c r="CQ6" s="35"/>
-      <c r="CR6" s="35"/>
-      <c r="CS6" s="35" t="s">
+      <c r="CJ6" s="34"/>
+      <c r="CK6" s="34"/>
+      <c r="CL6" s="34"/>
+      <c r="CM6" s="34"/>
+      <c r="CN6" s="34"/>
+      <c r="CO6" s="34"/>
+      <c r="CP6" s="34"/>
+      <c r="CQ6" s="34"/>
+      <c r="CR6" s="34"/>
+      <c r="CS6" s="34" t="s">
         <v>92</v>
       </c>
-      <c r="CT6" s="35"/>
+      <c r="CT6" s="34"/>
       <c r="CU6" s="11"/>
       <c r="CV6" s="11"/>
       <c r="CW6" s="11"/>
@@ -1874,9 +1897,20 @@
       <c r="HE6" s="25"/>
       <c r="HF6" s="25"/>
       <c r="HG6" s="25"/>
+      <c r="HH6" s="28"/>
+      <c r="HI6" s="49" t="s">
+        <v>213</v>
+      </c>
+      <c r="HJ6" s="49"/>
+      <c r="HK6" s="49"/>
+      <c r="HL6" s="49"/>
+      <c r="HM6" s="49"/>
+      <c r="HN6" s="28" t="s">
+        <v>214</v>
+      </c>
     </row>
-    <row r="7" spans="1:215" s="1" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A7" s="45"/>
+    <row r="7" spans="1:222" s="1" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A7" s="42"/>
       <c r="B7" s="2" t="s">
         <v>2</v>
       </c>
@@ -2519,16 +2553,37 @@
       <c r="HG7" s="24" t="s">
         <v>210</v>
       </c>
+      <c r="HH7" s="27" t="s">
+        <v>212</v>
+      </c>
+      <c r="HI7" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="HJ7" s="27" t="s">
+        <v>88</v>
+      </c>
+      <c r="HK7" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="HL7" s="27" t="s">
+        <v>89</v>
+      </c>
+      <c r="HM7" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="HN7" s="27" t="s">
+        <v>93</v>
+      </c>
     </row>
-    <row r="8" spans="1:215" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:215" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:215" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:215" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:215" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:215" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:215" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:215" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:215" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:222" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:222" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:222" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:222" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:222" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:222" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:222" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:222" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:222" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="17" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="18" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="19" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -3014,18 +3069,9 @@
     <row r="499" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="500" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="26">
-    <mergeCell ref="CS6:CT6"/>
-    <mergeCell ref="DN5:DO5"/>
-    <mergeCell ref="FH5:FP5"/>
-    <mergeCell ref="EU5:FG5"/>
-    <mergeCell ref="HB5:HG5"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="B5:X5"/>
-    <mergeCell ref="GO5:HA5"/>
+  <mergeCells count="28">
+    <mergeCell ref="HI6:HM6"/>
+    <mergeCell ref="HH5:HN5"/>
     <mergeCell ref="CB6:CE6"/>
     <mergeCell ref="BK5:BQ5"/>
     <mergeCell ref="Z5:AK5"/>
@@ -3035,12 +3081,23 @@
     <mergeCell ref="DJ5:DM5"/>
     <mergeCell ref="CU5:DI5"/>
     <mergeCell ref="BR6:CA6"/>
+    <mergeCell ref="CF6:CH6"/>
+    <mergeCell ref="CI6:CR6"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="B5:X5"/>
+    <mergeCell ref="CS6:CT6"/>
+    <mergeCell ref="DN5:DO5"/>
+    <mergeCell ref="FH5:FP5"/>
+    <mergeCell ref="EU5:FG5"/>
+    <mergeCell ref="HB5:HG5"/>
+    <mergeCell ref="GO5:HA5"/>
     <mergeCell ref="GH5:GN5"/>
     <mergeCell ref="FR5:GF5"/>
     <mergeCell ref="EO5:ET5"/>
     <mergeCell ref="EC5:EN5"/>
-    <mergeCell ref="CF6:CH6"/>
-    <mergeCell ref="CI6:CR6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
OAB : Update report template
</commit_message>
<xml_diff>
--- a/Laravel-InaLUTS/resources/templates/Report_OAB.xlsx
+++ b/Laravel-InaLUTS/resources/templates/Report_OAB.xlsx
@@ -1060,22 +1060,22 @@
     <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1090,7 +1090,13 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1099,22 +1105,16 @@
     <xf numFmtId="0" fontId="1" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1430,8 +1430,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:IK500"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="HQ1" workbookViewId="0">
-      <selection activeCell="IL8" sqref="IL8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1528,31 +1528,31 @@
       <c r="A5" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="44" t="s">
+      <c r="B5" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="44"/>
-      <c r="D5" s="44"/>
-      <c r="E5" s="44"/>
-      <c r="F5" s="44"/>
-      <c r="G5" s="44"/>
-      <c r="H5" s="44"/>
-      <c r="I5" s="44"/>
-      <c r="J5" s="44"/>
-      <c r="K5" s="44"/>
-      <c r="L5" s="44"/>
-      <c r="M5" s="44"/>
-      <c r="N5" s="44"/>
-      <c r="O5" s="44"/>
-      <c r="P5" s="44"/>
-      <c r="Q5" s="44"/>
-      <c r="R5" s="44"/>
-      <c r="S5" s="44"/>
-      <c r="T5" s="44"/>
-      <c r="U5" s="44"/>
-      <c r="V5" s="44"/>
-      <c r="W5" s="44"/>
-      <c r="X5" s="44"/>
+      <c r="C5" s="50"/>
+      <c r="D5" s="50"/>
+      <c r="E5" s="50"/>
+      <c r="F5" s="50"/>
+      <c r="G5" s="50"/>
+      <c r="H5" s="50"/>
+      <c r="I5" s="50"/>
+      <c r="J5" s="50"/>
+      <c r="K5" s="50"/>
+      <c r="L5" s="50"/>
+      <c r="M5" s="50"/>
+      <c r="N5" s="50"/>
+      <c r="O5" s="50"/>
+      <c r="P5" s="50"/>
+      <c r="Q5" s="50"/>
+      <c r="R5" s="50"/>
+      <c r="S5" s="50"/>
+      <c r="T5" s="50"/>
+      <c r="U5" s="50"/>
+      <c r="V5" s="50"/>
+      <c r="W5" s="50"/>
+      <c r="X5" s="50"/>
       <c r="Y5" s="18" t="s">
         <v>25</v>
       </c>
@@ -1597,73 +1597,73 @@
       <c r="BH5" s="56"/>
       <c r="BI5" s="56"/>
       <c r="BJ5" s="56"/>
-      <c r="BK5" s="54" t="s">
+      <c r="BK5" s="41" t="s">
         <v>72</v>
       </c>
-      <c r="BL5" s="54"/>
-      <c r="BM5" s="54"/>
-      <c r="BN5" s="54"/>
-      <c r="BO5" s="54"/>
-      <c r="BP5" s="54"/>
-      <c r="BQ5" s="54"/>
-      <c r="BR5" s="40" t="s">
+      <c r="BL5" s="41"/>
+      <c r="BM5" s="41"/>
+      <c r="BN5" s="41"/>
+      <c r="BO5" s="41"/>
+      <c r="BP5" s="41"/>
+      <c r="BQ5" s="41"/>
+      <c r="BR5" s="42" t="s">
         <v>73</v>
       </c>
-      <c r="BS5" s="40"/>
-      <c r="BT5" s="40"/>
-      <c r="BU5" s="40"/>
-      <c r="BV5" s="40"/>
-      <c r="BW5" s="40"/>
-      <c r="BX5" s="40"/>
-      <c r="BY5" s="40"/>
-      <c r="BZ5" s="40"/>
-      <c r="CA5" s="40"/>
-      <c r="CB5" s="40"/>
-      <c r="CC5" s="40"/>
-      <c r="CD5" s="40"/>
-      <c r="CE5" s="40"/>
-      <c r="CF5" s="40"/>
-      <c r="CG5" s="40"/>
-      <c r="CH5" s="40"/>
-      <c r="CI5" s="40"/>
-      <c r="CJ5" s="40"/>
-      <c r="CK5" s="40"/>
-      <c r="CL5" s="40"/>
-      <c r="CM5" s="40"/>
-      <c r="CN5" s="40"/>
-      <c r="CO5" s="40"/>
-      <c r="CP5" s="40"/>
-      <c r="CQ5" s="40"/>
-      <c r="CR5" s="40"/>
-      <c r="CS5" s="40"/>
-      <c r="CT5" s="40"/>
-      <c r="CU5" s="57" t="s">
+      <c r="BS5" s="42"/>
+      <c r="BT5" s="42"/>
+      <c r="BU5" s="42"/>
+      <c r="BV5" s="42"/>
+      <c r="BW5" s="42"/>
+      <c r="BX5" s="42"/>
+      <c r="BY5" s="42"/>
+      <c r="BZ5" s="42"/>
+      <c r="CA5" s="42"/>
+      <c r="CB5" s="42"/>
+      <c r="CC5" s="42"/>
+      <c r="CD5" s="42"/>
+      <c r="CE5" s="42"/>
+      <c r="CF5" s="42"/>
+      <c r="CG5" s="42"/>
+      <c r="CH5" s="42"/>
+      <c r="CI5" s="42"/>
+      <c r="CJ5" s="42"/>
+      <c r="CK5" s="42"/>
+      <c r="CL5" s="42"/>
+      <c r="CM5" s="42"/>
+      <c r="CN5" s="42"/>
+      <c r="CO5" s="42"/>
+      <c r="CP5" s="42"/>
+      <c r="CQ5" s="42"/>
+      <c r="CR5" s="42"/>
+      <c r="CS5" s="42"/>
+      <c r="CT5" s="42"/>
+      <c r="CU5" s="44" t="s">
         <v>94</v>
       </c>
-      <c r="CV5" s="57"/>
-      <c r="CW5" s="57"/>
-      <c r="CX5" s="57"/>
-      <c r="CY5" s="57"/>
-      <c r="CZ5" s="57"/>
-      <c r="DA5" s="57"/>
-      <c r="DB5" s="57"/>
-      <c r="DC5" s="57"/>
-      <c r="DD5" s="57"/>
-      <c r="DE5" s="57"/>
-      <c r="DF5" s="57"/>
-      <c r="DG5" s="57"/>
-      <c r="DH5" s="57"/>
-      <c r="DI5" s="57"/>
-      <c r="DJ5" s="45" t="s">
+      <c r="CV5" s="44"/>
+      <c r="CW5" s="44"/>
+      <c r="CX5" s="44"/>
+      <c r="CY5" s="44"/>
+      <c r="CZ5" s="44"/>
+      <c r="DA5" s="44"/>
+      <c r="DB5" s="44"/>
+      <c r="DC5" s="44"/>
+      <c r="DD5" s="44"/>
+      <c r="DE5" s="44"/>
+      <c r="DF5" s="44"/>
+      <c r="DG5" s="44"/>
+      <c r="DH5" s="44"/>
+      <c r="DI5" s="44"/>
+      <c r="DJ5" s="43" t="s">
         <v>108</v>
       </c>
-      <c r="DK5" s="45"/>
-      <c r="DL5" s="45"/>
-      <c r="DM5" s="45"/>
-      <c r="DN5" s="58" t="s">
+      <c r="DK5" s="43"/>
+      <c r="DL5" s="43"/>
+      <c r="DM5" s="43"/>
+      <c r="DN5" s="40" t="s">
         <v>109</v>
       </c>
-      <c r="DO5" s="58"/>
+      <c r="DO5" s="40"/>
       <c r="DP5" s="17" t="s">
         <v>112</v>
       </c>
@@ -1679,155 +1679,155 @@
       <c r="DT5" s="16" t="s">
         <v>120</v>
       </c>
-      <c r="DU5" s="43" t="s">
+      <c r="DU5" s="57" t="s">
         <v>121</v>
       </c>
-      <c r="DV5" s="43"/>
-      <c r="DW5" s="43"/>
-      <c r="DX5" s="43"/>
-      <c r="DY5" s="43"/>
-      <c r="DZ5" s="43"/>
-      <c r="EA5" s="43"/>
-      <c r="EB5" s="43"/>
-      <c r="EC5" s="42" t="s">
+      <c r="DV5" s="57"/>
+      <c r="DW5" s="57"/>
+      <c r="DX5" s="57"/>
+      <c r="DY5" s="57"/>
+      <c r="DZ5" s="57"/>
+      <c r="EA5" s="57"/>
+      <c r="EB5" s="57"/>
+      <c r="EC5" s="52" t="s">
         <v>130</v>
       </c>
-      <c r="ED5" s="42"/>
-      <c r="EE5" s="42"/>
-      <c r="EF5" s="42"/>
-      <c r="EG5" s="42"/>
-      <c r="EH5" s="42"/>
-      <c r="EI5" s="42"/>
-      <c r="EJ5" s="42"/>
-      <c r="EK5" s="42"/>
-      <c r="EL5" s="42"/>
-      <c r="EM5" s="42"/>
-      <c r="EN5" s="42"/>
-      <c r="EO5" s="52" t="s">
+      <c r="ED5" s="52"/>
+      <c r="EE5" s="52"/>
+      <c r="EF5" s="52"/>
+      <c r="EG5" s="52"/>
+      <c r="EH5" s="52"/>
+      <c r="EI5" s="52"/>
+      <c r="EJ5" s="52"/>
+      <c r="EK5" s="52"/>
+      <c r="EL5" s="52"/>
+      <c r="EM5" s="52"/>
+      <c r="EN5" s="52"/>
+      <c r="EO5" s="54" t="s">
         <v>215</v>
       </c>
-      <c r="EP5" s="52"/>
-      <c r="EQ5" s="52"/>
-      <c r="ER5" s="52"/>
-      <c r="ES5" s="52"/>
-      <c r="ET5" s="52"/>
-      <c r="EU5" s="52"/>
-      <c r="EV5" s="52"/>
-      <c r="EW5" s="52"/>
-      <c r="EX5" s="52"/>
-      <c r="EY5" s="52"/>
-      <c r="EZ5" s="52"/>
-      <c r="FA5" s="52"/>
-      <c r="FB5" s="52"/>
-      <c r="FC5" s="52"/>
-      <c r="FD5" s="52"/>
-      <c r="FE5" s="52"/>
-      <c r="FF5" s="52"/>
-      <c r="FG5" s="50" t="s">
+      <c r="EP5" s="54"/>
+      <c r="EQ5" s="54"/>
+      <c r="ER5" s="54"/>
+      <c r="ES5" s="54"/>
+      <c r="ET5" s="54"/>
+      <c r="EU5" s="54"/>
+      <c r="EV5" s="54"/>
+      <c r="EW5" s="54"/>
+      <c r="EX5" s="54"/>
+      <c r="EY5" s="54"/>
+      <c r="EZ5" s="54"/>
+      <c r="FA5" s="54"/>
+      <c r="FB5" s="54"/>
+      <c r="FC5" s="54"/>
+      <c r="FD5" s="54"/>
+      <c r="FE5" s="54"/>
+      <c r="FF5" s="54"/>
+      <c r="FG5" s="51" t="s">
         <v>143</v>
       </c>
-      <c r="FH5" s="50"/>
-      <c r="FI5" s="50"/>
-      <c r="FJ5" s="50"/>
-      <c r="FK5" s="50"/>
-      <c r="FL5" s="50"/>
-      <c r="FM5" s="40" t="s">
+      <c r="FH5" s="51"/>
+      <c r="FI5" s="51"/>
+      <c r="FJ5" s="51"/>
+      <c r="FK5" s="51"/>
+      <c r="FL5" s="51"/>
+      <c r="FM5" s="42" t="s">
         <v>150</v>
       </c>
-      <c r="FN5" s="40"/>
-      <c r="FO5" s="40"/>
-      <c r="FP5" s="40"/>
-      <c r="FQ5" s="40"/>
-      <c r="FR5" s="40"/>
-      <c r="FS5" s="40"/>
-      <c r="FT5" s="40"/>
-      <c r="FU5" s="40"/>
-      <c r="FV5" s="40"/>
-      <c r="FW5" s="40"/>
-      <c r="FX5" s="40"/>
-      <c r="FY5" s="40"/>
-      <c r="FZ5" s="54" t="s">
+      <c r="FN5" s="42"/>
+      <c r="FO5" s="42"/>
+      <c r="FP5" s="42"/>
+      <c r="FQ5" s="42"/>
+      <c r="FR5" s="42"/>
+      <c r="FS5" s="42"/>
+      <c r="FT5" s="42"/>
+      <c r="FU5" s="42"/>
+      <c r="FV5" s="42"/>
+      <c r="FW5" s="42"/>
+      <c r="FX5" s="42"/>
+      <c r="FY5" s="42"/>
+      <c r="FZ5" s="41" t="s">
         <v>162</v>
       </c>
-      <c r="GA5" s="54"/>
-      <c r="GB5" s="54"/>
-      <c r="GC5" s="54"/>
-      <c r="GD5" s="54"/>
-      <c r="GE5" s="54"/>
-      <c r="GF5" s="54"/>
-      <c r="GG5" s="54"/>
-      <c r="GH5" s="54"/>
+      <c r="GA5" s="41"/>
+      <c r="GB5" s="41"/>
+      <c r="GC5" s="41"/>
+      <c r="GD5" s="41"/>
+      <c r="GE5" s="41"/>
+      <c r="GF5" s="41"/>
+      <c r="GG5" s="41"/>
+      <c r="GH5" s="41"/>
       <c r="GI5" s="11" t="s">
         <v>161</v>
       </c>
-      <c r="GJ5" s="45" t="s">
+      <c r="GJ5" s="43" t="s">
         <v>172</v>
       </c>
-      <c r="GK5" s="45"/>
-      <c r="GL5" s="45"/>
-      <c r="GM5" s="45"/>
-      <c r="GN5" s="45"/>
-      <c r="GO5" s="45"/>
-      <c r="GP5" s="45"/>
-      <c r="GQ5" s="45"/>
-      <c r="GR5" s="45"/>
-      <c r="GS5" s="45"/>
-      <c r="GT5" s="45"/>
-      <c r="GU5" s="45"/>
-      <c r="GV5" s="45"/>
-      <c r="GW5" s="45"/>
-      <c r="GX5" s="45"/>
+      <c r="GK5" s="43"/>
+      <c r="GL5" s="43"/>
+      <c r="GM5" s="43"/>
+      <c r="GN5" s="43"/>
+      <c r="GO5" s="43"/>
+      <c r="GP5" s="43"/>
+      <c r="GQ5" s="43"/>
+      <c r="GR5" s="43"/>
+      <c r="GS5" s="43"/>
+      <c r="GT5" s="43"/>
+      <c r="GU5" s="43"/>
+      <c r="GV5" s="43"/>
+      <c r="GW5" s="43"/>
+      <c r="GX5" s="43"/>
       <c r="GY5" s="13" t="s">
         <v>185</v>
       </c>
-      <c r="GZ5" s="44" t="s">
+      <c r="GZ5" s="50" t="s">
         <v>186</v>
       </c>
-      <c r="HA5" s="44"/>
-      <c r="HB5" s="44"/>
-      <c r="HC5" s="44"/>
-      <c r="HD5" s="44"/>
-      <c r="HE5" s="44"/>
-      <c r="HF5" s="44"/>
-      <c r="HG5" s="43" t="s">
+      <c r="HA5" s="50"/>
+      <c r="HB5" s="50"/>
+      <c r="HC5" s="50"/>
+      <c r="HD5" s="50"/>
+      <c r="HE5" s="50"/>
+      <c r="HF5" s="50"/>
+      <c r="HG5" s="57" t="s">
         <v>193</v>
       </c>
-      <c r="HH5" s="43"/>
-      <c r="HI5" s="43"/>
-      <c r="HJ5" s="43"/>
-      <c r="HK5" s="43"/>
-      <c r="HL5" s="43"/>
-      <c r="HM5" s="43"/>
-      <c r="HN5" s="43"/>
-      <c r="HO5" s="43"/>
-      <c r="HP5" s="43"/>
-      <c r="HQ5" s="43"/>
-      <c r="HR5" s="43"/>
-      <c r="HS5" s="43"/>
-      <c r="HT5" s="42" t="s">
+      <c r="HH5" s="57"/>
+      <c r="HI5" s="57"/>
+      <c r="HJ5" s="57"/>
+      <c r="HK5" s="57"/>
+      <c r="HL5" s="57"/>
+      <c r="HM5" s="57"/>
+      <c r="HN5" s="57"/>
+      <c r="HO5" s="57"/>
+      <c r="HP5" s="57"/>
+      <c r="HQ5" s="57"/>
+      <c r="HR5" s="57"/>
+      <c r="HS5" s="57"/>
+      <c r="HT5" s="52" t="s">
         <v>204</v>
       </c>
-      <c r="HU5" s="42"/>
-      <c r="HV5" s="42"/>
-      <c r="HW5" s="42"/>
-      <c r="HX5" s="42"/>
-      <c r="HY5" s="42"/>
-      <c r="HZ5" s="50" t="s">
+      <c r="HU5" s="52"/>
+      <c r="HV5" s="52"/>
+      <c r="HW5" s="52"/>
+      <c r="HX5" s="52"/>
+      <c r="HY5" s="52"/>
+      <c r="HZ5" s="51" t="s">
         <v>211</v>
       </c>
-      <c r="IA5" s="50"/>
-      <c r="IB5" s="50"/>
-      <c r="IC5" s="50"/>
-      <c r="ID5" s="50"/>
-      <c r="IE5" s="50"/>
-      <c r="IF5" s="50"/>
-      <c r="IG5" s="40" t="s">
+      <c r="IA5" s="51"/>
+      <c r="IB5" s="51"/>
+      <c r="IC5" s="51"/>
+      <c r="ID5" s="51"/>
+      <c r="IE5" s="51"/>
+      <c r="IF5" s="51"/>
+      <c r="IG5" s="42" t="s">
         <v>233</v>
       </c>
-      <c r="IH5" s="40"/>
-      <c r="II5" s="40"/>
-      <c r="IJ5" s="40"/>
-      <c r="IK5" s="40"/>
+      <c r="IH5" s="42"/>
+      <c r="II5" s="42"/>
+      <c r="IJ5" s="42"/>
+      <c r="IK5" s="42"/>
     </row>
     <row r="6" spans="1:245" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="49"/>
@@ -1899,45 +1899,45 @@
       <c r="BO6" s="21"/>
       <c r="BP6" s="21"/>
       <c r="BQ6" s="21"/>
-      <c r="BR6" s="41" t="s">
+      <c r="BR6" s="45" t="s">
         <v>75</v>
       </c>
-      <c r="BS6" s="41"/>
-      <c r="BT6" s="41"/>
-      <c r="BU6" s="41"/>
-      <c r="BV6" s="41"/>
-      <c r="BW6" s="41"/>
-      <c r="BX6" s="41"/>
-      <c r="BY6" s="41"/>
-      <c r="BZ6" s="41"/>
-      <c r="CA6" s="41"/>
-      <c r="CB6" s="41" t="s">
+      <c r="BS6" s="45"/>
+      <c r="BT6" s="45"/>
+      <c r="BU6" s="45"/>
+      <c r="BV6" s="45"/>
+      <c r="BW6" s="45"/>
+      <c r="BX6" s="45"/>
+      <c r="BY6" s="45"/>
+      <c r="BZ6" s="45"/>
+      <c r="CA6" s="45"/>
+      <c r="CB6" s="45" t="s">
         <v>80</v>
       </c>
-      <c r="CC6" s="41"/>
-      <c r="CD6" s="41"/>
-      <c r="CE6" s="41"/>
-      <c r="CF6" s="41" t="s">
+      <c r="CC6" s="45"/>
+      <c r="CD6" s="45"/>
+      <c r="CE6" s="45"/>
+      <c r="CF6" s="45" t="s">
         <v>83</v>
       </c>
-      <c r="CG6" s="41"/>
-      <c r="CH6" s="41"/>
-      <c r="CI6" s="41" t="s">
+      <c r="CG6" s="45"/>
+      <c r="CH6" s="45"/>
+      <c r="CI6" s="45" t="s">
         <v>86</v>
       </c>
-      <c r="CJ6" s="41"/>
-      <c r="CK6" s="41"/>
-      <c r="CL6" s="41"/>
-      <c r="CM6" s="41"/>
-      <c r="CN6" s="41"/>
-      <c r="CO6" s="41"/>
-      <c r="CP6" s="41"/>
-      <c r="CQ6" s="41"/>
-      <c r="CR6" s="41"/>
-      <c r="CS6" s="41" t="s">
+      <c r="CJ6" s="45"/>
+      <c r="CK6" s="45"/>
+      <c r="CL6" s="45"/>
+      <c r="CM6" s="45"/>
+      <c r="CN6" s="45"/>
+      <c r="CO6" s="45"/>
+      <c r="CP6" s="45"/>
+      <c r="CQ6" s="45"/>
+      <c r="CR6" s="45"/>
+      <c r="CS6" s="45" t="s">
         <v>92</v>
       </c>
-      <c r="CT6" s="41"/>
+      <c r="CT6" s="45"/>
       <c r="CU6" s="11"/>
       <c r="CV6" s="11"/>
       <c r="CW6" s="11"/>
@@ -1991,19 +1991,19 @@
       <c r="ES6" s="35"/>
       <c r="ET6" s="35"/>
       <c r="EU6" s="35"/>
-      <c r="EV6" s="51" t="s">
+      <c r="EV6" s="53" t="s">
         <v>222</v>
       </c>
-      <c r="EW6" s="51"/>
-      <c r="EX6" s="51"/>
-      <c r="EY6" s="51"/>
-      <c r="EZ6" s="51"/>
-      <c r="FA6" s="51"/>
-      <c r="FB6" s="51"/>
-      <c r="FC6" s="51"/>
-      <c r="FD6" s="51"/>
-      <c r="FE6" s="51"/>
-      <c r="FF6" s="51"/>
+      <c r="EW6" s="53"/>
+      <c r="EX6" s="53"/>
+      <c r="EY6" s="53"/>
+      <c r="EZ6" s="53"/>
+      <c r="FA6" s="53"/>
+      <c r="FB6" s="53"/>
+      <c r="FC6" s="53"/>
+      <c r="FD6" s="53"/>
+      <c r="FE6" s="53"/>
+      <c r="FF6" s="53"/>
       <c r="FG6" s="28"/>
       <c r="FH6" s="28"/>
       <c r="FI6" s="28"/>
@@ -2082,21 +2082,21 @@
       <c r="HX6" s="25"/>
       <c r="HY6" s="25"/>
       <c r="HZ6" s="37"/>
-      <c r="IA6" s="53" t="s">
+      <c r="IA6" s="58" t="s">
         <v>213</v>
       </c>
-      <c r="IB6" s="53"/>
-      <c r="IC6" s="53"/>
-      <c r="ID6" s="53"/>
-      <c r="IE6" s="53"/>
+      <c r="IB6" s="58"/>
+      <c r="IC6" s="58"/>
+      <c r="ID6" s="58"/>
+      <c r="IE6" s="58"/>
       <c r="IF6" s="37" t="s">
         <v>214</v>
       </c>
-      <c r="IG6" s="41" t="s">
+      <c r="IG6" s="45" t="s">
         <v>101</v>
       </c>
-      <c r="IH6" s="41"/>
-      <c r="II6" s="41"/>
+      <c r="IH6" s="45"/>
+      <c r="II6" s="45"/>
       <c r="IJ6" s="39"/>
       <c r="IK6" s="39"/>
     </row>
@@ -13683,38 +13683,38 @@
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="DN5:DO5"/>
-    <mergeCell ref="FZ5:GH5"/>
-    <mergeCell ref="BR5:CT5"/>
-    <mergeCell ref="DJ5:DM5"/>
-    <mergeCell ref="CU5:DI5"/>
+    <mergeCell ref="IG6:II6"/>
+    <mergeCell ref="HT5:HY5"/>
+    <mergeCell ref="HG5:HS5"/>
+    <mergeCell ref="GZ5:HF5"/>
+    <mergeCell ref="IA6:IE6"/>
+    <mergeCell ref="HZ5:IF5"/>
+    <mergeCell ref="BK5:BQ5"/>
+    <mergeCell ref="Z5:AK5"/>
+    <mergeCell ref="AL5:BJ5"/>
+    <mergeCell ref="DU5:EB5"/>
+    <mergeCell ref="IG5:IK5"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="B5:X5"/>
     <mergeCell ref="BR6:CA6"/>
     <mergeCell ref="CF6:CH6"/>
     <mergeCell ref="CI6:CR6"/>
     <mergeCell ref="CS6:CT6"/>
     <mergeCell ref="GJ5:GX5"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="B5:X5"/>
     <mergeCell ref="FG5:FL5"/>
     <mergeCell ref="EC5:EN5"/>
     <mergeCell ref="EV6:FF6"/>
     <mergeCell ref="EO5:FF5"/>
     <mergeCell ref="FM5:FY5"/>
     <mergeCell ref="CB6:CE6"/>
-    <mergeCell ref="BK5:BQ5"/>
-    <mergeCell ref="Z5:AK5"/>
-    <mergeCell ref="AL5:BJ5"/>
-    <mergeCell ref="DU5:EB5"/>
-    <mergeCell ref="IG5:IK5"/>
-    <mergeCell ref="IG6:II6"/>
-    <mergeCell ref="HT5:HY5"/>
-    <mergeCell ref="HG5:HS5"/>
-    <mergeCell ref="GZ5:HF5"/>
-    <mergeCell ref="IA6:IE6"/>
-    <mergeCell ref="HZ5:IF5"/>
+    <mergeCell ref="DN5:DO5"/>
+    <mergeCell ref="FZ5:GH5"/>
+    <mergeCell ref="BR5:CT5"/>
+    <mergeCell ref="DJ5:DM5"/>
+    <mergeCell ref="CU5:DI5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
OAB - Update template Report
</commit_message>
<xml_diff>
--- a/Laravel-InaLUTS/resources/templates/Report_OAB.xlsx
+++ b/Laravel-InaLUTS/resources/templates/Report_OAB.xlsx
@@ -1060,22 +1060,34 @@
     <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1090,13 +1102,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1106,15 +1112,9 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1440,8 +1440,7 @@
     <col min="2" max="2" width="11.85546875" style="19" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.7109375" style="19" customWidth="1"/>
     <col min="4" max="4" width="14.5703125" style="19" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" style="19" customWidth="1"/>
-    <col min="6" max="6" width="20.7109375" style="19" customWidth="1"/>
+    <col min="5" max="6" width="20.7109375" style="19" customWidth="1"/>
     <col min="7" max="7" width="13.28515625" style="19" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.7109375" style="19" customWidth="1"/>
     <col min="9" max="10" width="15.7109375" style="19" customWidth="1"/>
@@ -1485,185 +1484,185 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:245" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="46"/>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="46"/>
+      <c r="A1" s="50"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="50"/>
+      <c r="I1" s="50"/>
+      <c r="J1" s="50"/>
+      <c r="K1" s="50"/>
     </row>
     <row r="2" spans="1:245" x14ac:dyDescent="0.25">
-      <c r="A2" s="47"/>
-      <c r="B2" s="47"/>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="47"/>
-      <c r="G2" s="47"/>
-      <c r="H2" s="47"/>
-      <c r="I2" s="47"/>
-      <c r="J2" s="47"/>
-      <c r="K2" s="47"/>
+      <c r="A2" s="51"/>
+      <c r="B2" s="51"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="51"/>
+      <c r="H2" s="51"/>
+      <c r="I2" s="51"/>
+      <c r="J2" s="51"/>
+      <c r="K2" s="51"/>
     </row>
     <row r="3" spans="1:245" x14ac:dyDescent="0.25">
-      <c r="A3" s="48"/>
-      <c r="B3" s="48"/>
-      <c r="C3" s="48"/>
-      <c r="D3" s="48"/>
-      <c r="E3" s="48"/>
-      <c r="F3" s="48"/>
-      <c r="G3" s="48"/>
-      <c r="H3" s="48"/>
-      <c r="I3" s="48"/>
-      <c r="J3" s="48"/>
-      <c r="K3" s="48"/>
+      <c r="A3" s="52"/>
+      <c r="B3" s="52"/>
+      <c r="C3" s="52"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="52"/>
+      <c r="F3" s="52"/>
+      <c r="G3" s="52"/>
+      <c r="H3" s="52"/>
+      <c r="I3" s="52"/>
+      <c r="J3" s="52"/>
+      <c r="K3" s="52"/>
     </row>
     <row r="4" spans="1:245" s="3" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="1:245" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="49" t="s">
+      <c r="A5" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="50" t="s">
+      <c r="B5" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="50"/>
-      <c r="D5" s="50"/>
-      <c r="E5" s="50"/>
-      <c r="F5" s="50"/>
-      <c r="G5" s="50"/>
-      <c r="H5" s="50"/>
-      <c r="I5" s="50"/>
-      <c r="J5" s="50"/>
-      <c r="K5" s="50"/>
-      <c r="L5" s="50"/>
-      <c r="M5" s="50"/>
-      <c r="N5" s="50"/>
-      <c r="O5" s="50"/>
-      <c r="P5" s="50"/>
-      <c r="Q5" s="50"/>
-      <c r="R5" s="50"/>
-      <c r="S5" s="50"/>
-      <c r="T5" s="50"/>
-      <c r="U5" s="50"/>
-      <c r="V5" s="50"/>
-      <c r="W5" s="50"/>
-      <c r="X5" s="50"/>
+      <c r="C5" s="43"/>
+      <c r="D5" s="43"/>
+      <c r="E5" s="43"/>
+      <c r="F5" s="43"/>
+      <c r="G5" s="43"/>
+      <c r="H5" s="43"/>
+      <c r="I5" s="43"/>
+      <c r="J5" s="43"/>
+      <c r="K5" s="43"/>
+      <c r="L5" s="43"/>
+      <c r="M5" s="43"/>
+      <c r="N5" s="43"/>
+      <c r="O5" s="43"/>
+      <c r="P5" s="43"/>
+      <c r="Q5" s="43"/>
+      <c r="R5" s="43"/>
+      <c r="S5" s="43"/>
+      <c r="T5" s="43"/>
+      <c r="U5" s="43"/>
+      <c r="V5" s="43"/>
+      <c r="W5" s="43"/>
+      <c r="X5" s="43"/>
       <c r="Y5" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="Z5" s="55" t="s">
+      <c r="Z5" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="AA5" s="55"/>
-      <c r="AB5" s="55"/>
-      <c r="AC5" s="55"/>
-      <c r="AD5" s="55"/>
-      <c r="AE5" s="55"/>
-      <c r="AF5" s="55"/>
-      <c r="AG5" s="55"/>
-      <c r="AH5" s="55"/>
-      <c r="AI5" s="55"/>
-      <c r="AJ5" s="55"/>
-      <c r="AK5" s="55"/>
-      <c r="AL5" s="56" t="s">
+      <c r="AA5" s="47"/>
+      <c r="AB5" s="47"/>
+      <c r="AC5" s="47"/>
+      <c r="AD5" s="47"/>
+      <c r="AE5" s="47"/>
+      <c r="AF5" s="47"/>
+      <c r="AG5" s="47"/>
+      <c r="AH5" s="47"/>
+      <c r="AI5" s="47"/>
+      <c r="AJ5" s="47"/>
+      <c r="AK5" s="47"/>
+      <c r="AL5" s="48" t="s">
         <v>40</v>
       </c>
-      <c r="AM5" s="56"/>
-      <c r="AN5" s="56"/>
-      <c r="AO5" s="56"/>
-      <c r="AP5" s="56"/>
-      <c r="AQ5" s="56"/>
-      <c r="AR5" s="56"/>
-      <c r="AS5" s="56"/>
-      <c r="AT5" s="56"/>
-      <c r="AU5" s="56"/>
-      <c r="AV5" s="56"/>
-      <c r="AW5" s="56"/>
-      <c r="AX5" s="56"/>
-      <c r="AY5" s="56"/>
-      <c r="AZ5" s="56"/>
-      <c r="BA5" s="56"/>
-      <c r="BB5" s="56"/>
-      <c r="BC5" s="56"/>
-      <c r="BD5" s="56"/>
-      <c r="BE5" s="56"/>
-      <c r="BF5" s="56"/>
-      <c r="BG5" s="56"/>
-      <c r="BH5" s="56"/>
-      <c r="BI5" s="56"/>
-      <c r="BJ5" s="56"/>
-      <c r="BK5" s="41" t="s">
+      <c r="AM5" s="48"/>
+      <c r="AN5" s="48"/>
+      <c r="AO5" s="48"/>
+      <c r="AP5" s="48"/>
+      <c r="AQ5" s="48"/>
+      <c r="AR5" s="48"/>
+      <c r="AS5" s="48"/>
+      <c r="AT5" s="48"/>
+      <c r="AU5" s="48"/>
+      <c r="AV5" s="48"/>
+      <c r="AW5" s="48"/>
+      <c r="AX5" s="48"/>
+      <c r="AY5" s="48"/>
+      <c r="AZ5" s="48"/>
+      <c r="BA5" s="48"/>
+      <c r="BB5" s="48"/>
+      <c r="BC5" s="48"/>
+      <c r="BD5" s="48"/>
+      <c r="BE5" s="48"/>
+      <c r="BF5" s="48"/>
+      <c r="BG5" s="48"/>
+      <c r="BH5" s="48"/>
+      <c r="BI5" s="48"/>
+      <c r="BJ5" s="48"/>
+      <c r="BK5" s="46" t="s">
         <v>72</v>
       </c>
-      <c r="BL5" s="41"/>
-      <c r="BM5" s="41"/>
-      <c r="BN5" s="41"/>
-      <c r="BO5" s="41"/>
-      <c r="BP5" s="41"/>
-      <c r="BQ5" s="41"/>
-      <c r="BR5" s="42" t="s">
+      <c r="BL5" s="46"/>
+      <c r="BM5" s="46"/>
+      <c r="BN5" s="46"/>
+      <c r="BO5" s="46"/>
+      <c r="BP5" s="46"/>
+      <c r="BQ5" s="46"/>
+      <c r="BR5" s="49" t="s">
         <v>73</v>
       </c>
-      <c r="BS5" s="42"/>
-      <c r="BT5" s="42"/>
-      <c r="BU5" s="42"/>
-      <c r="BV5" s="42"/>
-      <c r="BW5" s="42"/>
-      <c r="BX5" s="42"/>
-      <c r="BY5" s="42"/>
-      <c r="BZ5" s="42"/>
-      <c r="CA5" s="42"/>
-      <c r="CB5" s="42"/>
-      <c r="CC5" s="42"/>
-      <c r="CD5" s="42"/>
-      <c r="CE5" s="42"/>
-      <c r="CF5" s="42"/>
-      <c r="CG5" s="42"/>
-      <c r="CH5" s="42"/>
-      <c r="CI5" s="42"/>
-      <c r="CJ5" s="42"/>
-      <c r="CK5" s="42"/>
-      <c r="CL5" s="42"/>
-      <c r="CM5" s="42"/>
-      <c r="CN5" s="42"/>
-      <c r="CO5" s="42"/>
-      <c r="CP5" s="42"/>
-      <c r="CQ5" s="42"/>
-      <c r="CR5" s="42"/>
-      <c r="CS5" s="42"/>
-      <c r="CT5" s="42"/>
-      <c r="CU5" s="44" t="s">
+      <c r="BS5" s="49"/>
+      <c r="BT5" s="49"/>
+      <c r="BU5" s="49"/>
+      <c r="BV5" s="49"/>
+      <c r="BW5" s="49"/>
+      <c r="BX5" s="49"/>
+      <c r="BY5" s="49"/>
+      <c r="BZ5" s="49"/>
+      <c r="CA5" s="49"/>
+      <c r="CB5" s="49"/>
+      <c r="CC5" s="49"/>
+      <c r="CD5" s="49"/>
+      <c r="CE5" s="49"/>
+      <c r="CF5" s="49"/>
+      <c r="CG5" s="49"/>
+      <c r="CH5" s="49"/>
+      <c r="CI5" s="49"/>
+      <c r="CJ5" s="49"/>
+      <c r="CK5" s="49"/>
+      <c r="CL5" s="49"/>
+      <c r="CM5" s="49"/>
+      <c r="CN5" s="49"/>
+      <c r="CO5" s="49"/>
+      <c r="CP5" s="49"/>
+      <c r="CQ5" s="49"/>
+      <c r="CR5" s="49"/>
+      <c r="CS5" s="49"/>
+      <c r="CT5" s="49"/>
+      <c r="CU5" s="58" t="s">
         <v>94</v>
       </c>
-      <c r="CV5" s="44"/>
-      <c r="CW5" s="44"/>
-      <c r="CX5" s="44"/>
-      <c r="CY5" s="44"/>
-      <c r="CZ5" s="44"/>
-      <c r="DA5" s="44"/>
-      <c r="DB5" s="44"/>
-      <c r="DC5" s="44"/>
-      <c r="DD5" s="44"/>
-      <c r="DE5" s="44"/>
-      <c r="DF5" s="44"/>
-      <c r="DG5" s="44"/>
-      <c r="DH5" s="44"/>
-      <c r="DI5" s="44"/>
-      <c r="DJ5" s="43" t="s">
+      <c r="CV5" s="58"/>
+      <c r="CW5" s="58"/>
+      <c r="CX5" s="58"/>
+      <c r="CY5" s="58"/>
+      <c r="CZ5" s="58"/>
+      <c r="DA5" s="58"/>
+      <c r="DB5" s="58"/>
+      <c r="DC5" s="58"/>
+      <c r="DD5" s="58"/>
+      <c r="DE5" s="58"/>
+      <c r="DF5" s="58"/>
+      <c r="DG5" s="58"/>
+      <c r="DH5" s="58"/>
+      <c r="DI5" s="58"/>
+      <c r="DJ5" s="54" t="s">
         <v>108</v>
       </c>
-      <c r="DK5" s="43"/>
-      <c r="DL5" s="43"/>
-      <c r="DM5" s="43"/>
-      <c r="DN5" s="40" t="s">
+      <c r="DK5" s="54"/>
+      <c r="DL5" s="54"/>
+      <c r="DM5" s="54"/>
+      <c r="DN5" s="57" t="s">
         <v>109</v>
       </c>
-      <c r="DO5" s="40"/>
+      <c r="DO5" s="57"/>
       <c r="DP5" s="17" t="s">
         <v>112</v>
       </c>
@@ -1679,158 +1678,158 @@
       <c r="DT5" s="16" t="s">
         <v>120</v>
       </c>
-      <c r="DU5" s="57" t="s">
+      <c r="DU5" s="42" t="s">
         <v>121</v>
       </c>
-      <c r="DV5" s="57"/>
-      <c r="DW5" s="57"/>
-      <c r="DX5" s="57"/>
-      <c r="DY5" s="57"/>
-      <c r="DZ5" s="57"/>
-      <c r="EA5" s="57"/>
-      <c r="EB5" s="57"/>
-      <c r="EC5" s="52" t="s">
+      <c r="DV5" s="42"/>
+      <c r="DW5" s="42"/>
+      <c r="DX5" s="42"/>
+      <c r="DY5" s="42"/>
+      <c r="DZ5" s="42"/>
+      <c r="EA5" s="42"/>
+      <c r="EB5" s="42"/>
+      <c r="EC5" s="41" t="s">
         <v>130</v>
       </c>
-      <c r="ED5" s="52"/>
-      <c r="EE5" s="52"/>
-      <c r="EF5" s="52"/>
-      <c r="EG5" s="52"/>
-      <c r="EH5" s="52"/>
-      <c r="EI5" s="52"/>
-      <c r="EJ5" s="52"/>
-      <c r="EK5" s="52"/>
-      <c r="EL5" s="52"/>
-      <c r="EM5" s="52"/>
-      <c r="EN5" s="52"/>
-      <c r="EO5" s="54" t="s">
+      <c r="ED5" s="41"/>
+      <c r="EE5" s="41"/>
+      <c r="EF5" s="41"/>
+      <c r="EG5" s="41"/>
+      <c r="EH5" s="41"/>
+      <c r="EI5" s="41"/>
+      <c r="EJ5" s="41"/>
+      <c r="EK5" s="41"/>
+      <c r="EL5" s="41"/>
+      <c r="EM5" s="41"/>
+      <c r="EN5" s="41"/>
+      <c r="EO5" s="56" t="s">
         <v>215</v>
       </c>
-      <c r="EP5" s="54"/>
-      <c r="EQ5" s="54"/>
-      <c r="ER5" s="54"/>
-      <c r="ES5" s="54"/>
-      <c r="ET5" s="54"/>
-      <c r="EU5" s="54"/>
-      <c r="EV5" s="54"/>
-      <c r="EW5" s="54"/>
-      <c r="EX5" s="54"/>
-      <c r="EY5" s="54"/>
-      <c r="EZ5" s="54"/>
-      <c r="FA5" s="54"/>
-      <c r="FB5" s="54"/>
-      <c r="FC5" s="54"/>
-      <c r="FD5" s="54"/>
-      <c r="FE5" s="54"/>
-      <c r="FF5" s="54"/>
-      <c r="FG5" s="51" t="s">
+      <c r="EP5" s="56"/>
+      <c r="EQ5" s="56"/>
+      <c r="ER5" s="56"/>
+      <c r="ES5" s="56"/>
+      <c r="ET5" s="56"/>
+      <c r="EU5" s="56"/>
+      <c r="EV5" s="56"/>
+      <c r="EW5" s="56"/>
+      <c r="EX5" s="56"/>
+      <c r="EY5" s="56"/>
+      <c r="EZ5" s="56"/>
+      <c r="FA5" s="56"/>
+      <c r="FB5" s="56"/>
+      <c r="FC5" s="56"/>
+      <c r="FD5" s="56"/>
+      <c r="FE5" s="56"/>
+      <c r="FF5" s="56"/>
+      <c r="FG5" s="45" t="s">
         <v>143</v>
       </c>
-      <c r="FH5" s="51"/>
-      <c r="FI5" s="51"/>
-      <c r="FJ5" s="51"/>
-      <c r="FK5" s="51"/>
-      <c r="FL5" s="51"/>
-      <c r="FM5" s="42" t="s">
+      <c r="FH5" s="45"/>
+      <c r="FI5" s="45"/>
+      <c r="FJ5" s="45"/>
+      <c r="FK5" s="45"/>
+      <c r="FL5" s="45"/>
+      <c r="FM5" s="49" t="s">
         <v>150</v>
       </c>
-      <c r="FN5" s="42"/>
-      <c r="FO5" s="42"/>
-      <c r="FP5" s="42"/>
-      <c r="FQ5" s="42"/>
-      <c r="FR5" s="42"/>
-      <c r="FS5" s="42"/>
-      <c r="FT5" s="42"/>
-      <c r="FU5" s="42"/>
-      <c r="FV5" s="42"/>
-      <c r="FW5" s="42"/>
-      <c r="FX5" s="42"/>
-      <c r="FY5" s="42"/>
-      <c r="FZ5" s="41" t="s">
+      <c r="FN5" s="49"/>
+      <c r="FO5" s="49"/>
+      <c r="FP5" s="49"/>
+      <c r="FQ5" s="49"/>
+      <c r="FR5" s="49"/>
+      <c r="FS5" s="49"/>
+      <c r="FT5" s="49"/>
+      <c r="FU5" s="49"/>
+      <c r="FV5" s="49"/>
+      <c r="FW5" s="49"/>
+      <c r="FX5" s="49"/>
+      <c r="FY5" s="49"/>
+      <c r="FZ5" s="46" t="s">
         <v>162</v>
       </c>
-      <c r="GA5" s="41"/>
-      <c r="GB5" s="41"/>
-      <c r="GC5" s="41"/>
-      <c r="GD5" s="41"/>
-      <c r="GE5" s="41"/>
-      <c r="GF5" s="41"/>
-      <c r="GG5" s="41"/>
-      <c r="GH5" s="41"/>
+      <c r="GA5" s="46"/>
+      <c r="GB5" s="46"/>
+      <c r="GC5" s="46"/>
+      <c r="GD5" s="46"/>
+      <c r="GE5" s="46"/>
+      <c r="GF5" s="46"/>
+      <c r="GG5" s="46"/>
+      <c r="GH5" s="46"/>
       <c r="GI5" s="11" t="s">
         <v>161</v>
       </c>
-      <c r="GJ5" s="43" t="s">
+      <c r="GJ5" s="54" t="s">
         <v>172</v>
       </c>
-      <c r="GK5" s="43"/>
-      <c r="GL5" s="43"/>
-      <c r="GM5" s="43"/>
-      <c r="GN5" s="43"/>
-      <c r="GO5" s="43"/>
-      <c r="GP5" s="43"/>
-      <c r="GQ5" s="43"/>
-      <c r="GR5" s="43"/>
-      <c r="GS5" s="43"/>
-      <c r="GT5" s="43"/>
-      <c r="GU5" s="43"/>
-      <c r="GV5" s="43"/>
-      <c r="GW5" s="43"/>
-      <c r="GX5" s="43"/>
+      <c r="GK5" s="54"/>
+      <c r="GL5" s="54"/>
+      <c r="GM5" s="54"/>
+      <c r="GN5" s="54"/>
+      <c r="GO5" s="54"/>
+      <c r="GP5" s="54"/>
+      <c r="GQ5" s="54"/>
+      <c r="GR5" s="54"/>
+      <c r="GS5" s="54"/>
+      <c r="GT5" s="54"/>
+      <c r="GU5" s="54"/>
+      <c r="GV5" s="54"/>
+      <c r="GW5" s="54"/>
+      <c r="GX5" s="54"/>
       <c r="GY5" s="13" t="s">
         <v>185</v>
       </c>
-      <c r="GZ5" s="50" t="s">
+      <c r="GZ5" s="43" t="s">
         <v>186</v>
       </c>
-      <c r="HA5" s="50"/>
-      <c r="HB5" s="50"/>
-      <c r="HC5" s="50"/>
-      <c r="HD5" s="50"/>
-      <c r="HE5" s="50"/>
-      <c r="HF5" s="50"/>
-      <c r="HG5" s="57" t="s">
+      <c r="HA5" s="43"/>
+      <c r="HB5" s="43"/>
+      <c r="HC5" s="43"/>
+      <c r="HD5" s="43"/>
+      <c r="HE5" s="43"/>
+      <c r="HF5" s="43"/>
+      <c r="HG5" s="42" t="s">
         <v>193</v>
       </c>
-      <c r="HH5" s="57"/>
-      <c r="HI5" s="57"/>
-      <c r="HJ5" s="57"/>
-      <c r="HK5" s="57"/>
-      <c r="HL5" s="57"/>
-      <c r="HM5" s="57"/>
-      <c r="HN5" s="57"/>
-      <c r="HO5" s="57"/>
-      <c r="HP5" s="57"/>
-      <c r="HQ5" s="57"/>
-      <c r="HR5" s="57"/>
-      <c r="HS5" s="57"/>
-      <c r="HT5" s="52" t="s">
+      <c r="HH5" s="42"/>
+      <c r="HI5" s="42"/>
+      <c r="HJ5" s="42"/>
+      <c r="HK5" s="42"/>
+      <c r="HL5" s="42"/>
+      <c r="HM5" s="42"/>
+      <c r="HN5" s="42"/>
+      <c r="HO5" s="42"/>
+      <c r="HP5" s="42"/>
+      <c r="HQ5" s="42"/>
+      <c r="HR5" s="42"/>
+      <c r="HS5" s="42"/>
+      <c r="HT5" s="41" t="s">
         <v>204</v>
       </c>
-      <c r="HU5" s="52"/>
-      <c r="HV5" s="52"/>
-      <c r="HW5" s="52"/>
-      <c r="HX5" s="52"/>
-      <c r="HY5" s="52"/>
-      <c r="HZ5" s="51" t="s">
+      <c r="HU5" s="41"/>
+      <c r="HV5" s="41"/>
+      <c r="HW5" s="41"/>
+      <c r="HX5" s="41"/>
+      <c r="HY5" s="41"/>
+      <c r="HZ5" s="45" t="s">
         <v>211</v>
       </c>
-      <c r="IA5" s="51"/>
-      <c r="IB5" s="51"/>
-      <c r="IC5" s="51"/>
-      <c r="ID5" s="51"/>
-      <c r="IE5" s="51"/>
-      <c r="IF5" s="51"/>
-      <c r="IG5" s="42" t="s">
+      <c r="IA5" s="45"/>
+      <c r="IB5" s="45"/>
+      <c r="IC5" s="45"/>
+      <c r="ID5" s="45"/>
+      <c r="IE5" s="45"/>
+      <c r="IF5" s="45"/>
+      <c r="IG5" s="49" t="s">
         <v>233</v>
       </c>
-      <c r="IH5" s="42"/>
-      <c r="II5" s="42"/>
-      <c r="IJ5" s="42"/>
-      <c r="IK5" s="42"/>
+      <c r="IH5" s="49"/>
+      <c r="II5" s="49"/>
+      <c r="IJ5" s="49"/>
+      <c r="IK5" s="49"/>
     </row>
     <row r="6" spans="1:245" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="49"/>
+      <c r="A6" s="53"/>
       <c r="B6" s="17"/>
       <c r="C6" s="17"/>
       <c r="D6" s="17"/>
@@ -1899,45 +1898,45 @@
       <c r="BO6" s="21"/>
       <c r="BP6" s="21"/>
       <c r="BQ6" s="21"/>
-      <c r="BR6" s="45" t="s">
+      <c r="BR6" s="40" t="s">
         <v>75</v>
       </c>
-      <c r="BS6" s="45"/>
-      <c r="BT6" s="45"/>
-      <c r="BU6" s="45"/>
-      <c r="BV6" s="45"/>
-      <c r="BW6" s="45"/>
-      <c r="BX6" s="45"/>
-      <c r="BY6" s="45"/>
-      <c r="BZ6" s="45"/>
-      <c r="CA6" s="45"/>
-      <c r="CB6" s="45" t="s">
+      <c r="BS6" s="40"/>
+      <c r="BT6" s="40"/>
+      <c r="BU6" s="40"/>
+      <c r="BV6" s="40"/>
+      <c r="BW6" s="40"/>
+      <c r="BX6" s="40"/>
+      <c r="BY6" s="40"/>
+      <c r="BZ6" s="40"/>
+      <c r="CA6" s="40"/>
+      <c r="CB6" s="40" t="s">
         <v>80</v>
       </c>
-      <c r="CC6" s="45"/>
-      <c r="CD6" s="45"/>
-      <c r="CE6" s="45"/>
-      <c r="CF6" s="45" t="s">
+      <c r="CC6" s="40"/>
+      <c r="CD6" s="40"/>
+      <c r="CE6" s="40"/>
+      <c r="CF6" s="40" t="s">
         <v>83</v>
       </c>
-      <c r="CG6" s="45"/>
-      <c r="CH6" s="45"/>
-      <c r="CI6" s="45" t="s">
+      <c r="CG6" s="40"/>
+      <c r="CH6" s="40"/>
+      <c r="CI6" s="40" t="s">
         <v>86</v>
       </c>
-      <c r="CJ6" s="45"/>
-      <c r="CK6" s="45"/>
-      <c r="CL6" s="45"/>
-      <c r="CM6" s="45"/>
-      <c r="CN6" s="45"/>
-      <c r="CO6" s="45"/>
-      <c r="CP6" s="45"/>
-      <c r="CQ6" s="45"/>
-      <c r="CR6" s="45"/>
-      <c r="CS6" s="45" t="s">
+      <c r="CJ6" s="40"/>
+      <c r="CK6" s="40"/>
+      <c r="CL6" s="40"/>
+      <c r="CM6" s="40"/>
+      <c r="CN6" s="40"/>
+      <c r="CO6" s="40"/>
+      <c r="CP6" s="40"/>
+      <c r="CQ6" s="40"/>
+      <c r="CR6" s="40"/>
+      <c r="CS6" s="40" t="s">
         <v>92</v>
       </c>
-      <c r="CT6" s="45"/>
+      <c r="CT6" s="40"/>
       <c r="CU6" s="11"/>
       <c r="CV6" s="11"/>
       <c r="CW6" s="11"/>
@@ -1991,19 +1990,19 @@
       <c r="ES6" s="35"/>
       <c r="ET6" s="35"/>
       <c r="EU6" s="35"/>
-      <c r="EV6" s="53" t="s">
+      <c r="EV6" s="55" t="s">
         <v>222</v>
       </c>
-      <c r="EW6" s="53"/>
-      <c r="EX6" s="53"/>
-      <c r="EY6" s="53"/>
-      <c r="EZ6" s="53"/>
-      <c r="FA6" s="53"/>
-      <c r="FB6" s="53"/>
-      <c r="FC6" s="53"/>
-      <c r="FD6" s="53"/>
-      <c r="FE6" s="53"/>
-      <c r="FF6" s="53"/>
+      <c r="EW6" s="55"/>
+      <c r="EX6" s="55"/>
+      <c r="EY6" s="55"/>
+      <c r="EZ6" s="55"/>
+      <c r="FA6" s="55"/>
+      <c r="FB6" s="55"/>
+      <c r="FC6" s="55"/>
+      <c r="FD6" s="55"/>
+      <c r="FE6" s="55"/>
+      <c r="FF6" s="55"/>
       <c r="FG6" s="28"/>
       <c r="FH6" s="28"/>
       <c r="FI6" s="28"/>
@@ -2082,26 +2081,26 @@
       <c r="HX6" s="25"/>
       <c r="HY6" s="25"/>
       <c r="HZ6" s="37"/>
-      <c r="IA6" s="58" t="s">
+      <c r="IA6" s="44" t="s">
         <v>213</v>
       </c>
-      <c r="IB6" s="58"/>
-      <c r="IC6" s="58"/>
-      <c r="ID6" s="58"/>
-      <c r="IE6" s="58"/>
+      <c r="IB6" s="44"/>
+      <c r="IC6" s="44"/>
+      <c r="ID6" s="44"/>
+      <c r="IE6" s="44"/>
       <c r="IF6" s="37" t="s">
         <v>214</v>
       </c>
-      <c r="IG6" s="45" t="s">
+      <c r="IG6" s="40" t="s">
         <v>101</v>
       </c>
-      <c r="IH6" s="45"/>
-      <c r="II6" s="45"/>
+      <c r="IH6" s="40"/>
+      <c r="II6" s="40"/>
       <c r="IJ6" s="39"/>
       <c r="IK6" s="39"/>
     </row>
     <row r="7" spans="1:245" s="1" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A7" s="49"/>
+      <c r="A7" s="53"/>
       <c r="B7" s="2" t="s">
         <v>2</v>
       </c>
@@ -13683,22 +13682,6 @@
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="IG6:II6"/>
-    <mergeCell ref="HT5:HY5"/>
-    <mergeCell ref="HG5:HS5"/>
-    <mergeCell ref="GZ5:HF5"/>
-    <mergeCell ref="IA6:IE6"/>
-    <mergeCell ref="HZ5:IF5"/>
-    <mergeCell ref="BK5:BQ5"/>
-    <mergeCell ref="Z5:AK5"/>
-    <mergeCell ref="AL5:BJ5"/>
-    <mergeCell ref="DU5:EB5"/>
-    <mergeCell ref="IG5:IK5"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="B5:X5"/>
     <mergeCell ref="BR6:CA6"/>
     <mergeCell ref="CF6:CH6"/>
     <mergeCell ref="CI6:CR6"/>
@@ -13715,6 +13698,22 @@
     <mergeCell ref="BR5:CT5"/>
     <mergeCell ref="DJ5:DM5"/>
     <mergeCell ref="CU5:DI5"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="B5:X5"/>
+    <mergeCell ref="BK5:BQ5"/>
+    <mergeCell ref="Z5:AK5"/>
+    <mergeCell ref="AL5:BJ5"/>
+    <mergeCell ref="DU5:EB5"/>
+    <mergeCell ref="IG5:IK5"/>
+    <mergeCell ref="IG6:II6"/>
+    <mergeCell ref="HT5:HY5"/>
+    <mergeCell ref="HG5:HS5"/>
+    <mergeCell ref="GZ5:HF5"/>
+    <mergeCell ref="IA6:IE6"/>
+    <mergeCell ref="HZ5:IF5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>